<commit_message>
improved signifance test display, gathered results for ai improved prompt
</commit_message>
<xml_diff>
--- a/data/dfs/only_text_256_20/llama3.1.70b/AI_prompt/ReferenceErrorDetection_data_with_prompt_results.xlsx
+++ b/data/dfs/only_text_256_20/llama3.1.70b/AI_prompt/ReferenceErrorDetection_data_with_prompt_results.xlsx
@@ -743,13 +743,10 @@
       </c>
       <c r="AF2" t="inlineStr">
         <is>
-          <t>Here is my evaluation:
-```
-{
+          <t>{
   "label": "Unsubstantiated",
-  "explanation": "The reference article discusses a fault analysis method for three-phase induction motors using spiking neural P systems, which does not relate to reducing irreversibility or optimizing energy-consumed devices. The article focuses on motor fault prediction and diagnosis, making it unrelated to the cited claim."
-}
-```</t>
+  "explanation": "The reference article does not support the statement about reducing irreversibility or optimizing energy-consumed devices. The abstract and provided excerpts focus on a fault analysis method for three-phase induction motors using spiking neural P systems, which is unrelated to the topic of reducing irreversibility or optimizing energy consumption."
+}</t>
         </is>
       </c>
     </row>
@@ -899,7 +896,14 @@
           <t>['The evaluations of nanofluid thermo-physical properties through various experimental studies, have been followed by the numerical works; which had tried to predict the properties by using the suitable correlations. These correlations outputs might show some detour versus experimental ones; however less costs of researchers encouraged researchers to follow that field to present more accurate correlations at various working conditions  [9] [10] [11] [12] [13] [14] [15] [16] [17] [18] . The expensive steps of stabilize and dispersing the nanoparticles, are able to be ignored through the numerical works; moreover all the nanofluid behaviors can be predicted by a simple optimization approach according to the available empirical results. Among these optimization approaches, the artificial neural network (ANN) was used in many studies to predict the nanofluid properties especially for its thermal conductivity and viscosity. Moreover appropriate accuracy of this method encouraged researchers to develop more new models of ANN to have better consistency with the existence physical conditions of a nanofluid flow . In the following, 24 dissimilar ANN methods are examined at present work by introducing the suitable architectures and training algorithms of these using approaches.', 'Introduction\nThe mixture composed of nanoparticles dispersed through a base liquid, which is called nanofluid, plays a significant role in MEMS &amp; NEMS. It should be mentioned that the nanoparticles concentration have be small to avoid from undesired behaviors such as settlements. The Brownian motions of nanoparticles are able to increase the convection mechanism through the base fluid; however their main important effect would be improve the mixture effective thermal conductivity. That implies the better performance of nanoparticles with more thermal conductivity coefficient. This fact has been reported in many articles for various types of nanoparticles  [1] [2] [3] [4] [5] [6] [7] [8] . Meanwhile, the amount of nanoparticles concentration has an important influence on the mixture thermal behavior especially at different values of working temperature. Other effective thermo-physical properties can be addressed as like the nanoparticles density, specific heat and their shapes and diameters. It is well known that in addition of nanofluid thermal conductivity, the mixture effective viscosity should be evaluated due to its performance in a flow pumping power; so that a large number of works can be referred concerned these aspects of nanofluid properties.', 'To do this, the MSEs between the targets and the ANN outputs of the examined methods are evaluated while the results would be supported by the appropriate sensitivity analysis.\n\nProblem statement\nThe artificial neural network (ANN) optimization method is evaluated according to the experimental results of Bahrami et al.  [10]  concerned the hybrid non-Newtonian nanofluid of iron (Fe) and copper oxide (CuO) in a binary mixture of water and ethylene glycol (see Fig.  1 ). They reported the mixture dynamic viscosity, µ (mPa.s), versus shear rate, γ (1/s), at different amounts of nanoparticles volume fraction (φ = 0.25 to 1.5%) and temperate (T = 25 to 50 • C). Present work novelty is demonstrated by providing 24 dissimilar ANN methods to introduce the suitable architectures and training algorithms for them . The mean squared errors (MSEs) between the targets and ANN outputs are evaluated to present the best optimization approach among them. Meanwhile the results would be supported by the appropriate sensitivity analysis to have better statistical visual presentation.\n\nFeed-forward multilayer ANN\nArtificial Neural Networks (ANNs) are appropriate tools for the function approximation.']</t>
         </is>
       </c>
-      <c r="AF3" t="inlineStr"/>
+      <c r="AF3" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article does not mention heat exchange devices or their efficiency, which is the focus of the citation statement. Instead, it discusses the development and evaluation of artificial neural networks (ANNs) for predicting nanofluid properties, specifically thermal conductivity and viscosity."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -1047,7 +1051,14 @@
           <t>['Note when patients have undergone different medication for swelling, paronychia or skin disorders. Our blood lipid calculation (TC, TG, HDL-C) findings and our photochemical recommendation Dongle and the acquisition (LDL-C) results are available for 78 patients. The correspondence curve for our photochemical guidelines In the photo 4. The concentration for the TC study can be shown to be between 0.9405, 0.271 and 0.895 and vary between 2.63 mmol/l and 6.96 mmol/l TG calculation concentration. The coefficient of intercept -0.08 is 0.94 mmol/L at a median length of 4.35 mmol/L and the coefficient of association is 0.9345. For HDL-C measurement, the standard ranges from 1.2 mmol/L to 3.3 mmol/L with a pitch of 0.91, 0.17 intercept and 0.952 coefficient of correlation.', 'ICNADBE 2021 Journal of Physics: Conference Series 1937 (2021) 012038 IOP Publishing doi:10.1088/1742-6596/1937/1/012038 7 . However, the use of multiple blood samples may contribute to other substances interfering that cause discrepancies Coefficients of reflection and degrade test outcomes of the IoMT blood lipid measuring unit miniaturized. However, it remains within the tolerance range considering such a problem. Next, high (H), medium (M) and low samples (L) Blood lipid concentration was added to monitor for reliability and repeatability by CV percent of our proposed photochemical dongle (coefficient of variation). There are the following: For 3 years, repetitive sample experiments have been performed. As illustrated Table  1  indicates an average mean of 4.027% of the cv. Displaying good photochemical dongle efficiency and reproducibility. The photochemical examination of future work further changes should be made in strip layout to limit testing error.', '2 is used to patch the chromomeric agent previously dropped at the three channels workplace. The coating was then baked at 38°C in a drying box for around 1.5 hour (Dry-401, Bioline Laboratory,India). As Fig reveals  . 2(d) , the sensing block for temperature can support to maintain purely biological temperature conditions experience. The calculation of photochemical reactions and consistent results can also be correct. The photochemical dongles are connected with the OTG cable to the Smartphone and the sensed data is sent directly to the power source in real time.\n\nDISCUSSION AND RESULT\nPhotochemical blood performance of the suggested IoMT a distinction was made of the lipid data acquisition dongle Hitachi Biochemical Analyzer 5260 with a commercial tool. To prepare a report, we have prepared 78 samples for the procedure in 78 patients with fingertips and venous blood. For comparison research, the fingertip blood obtained by the disposable needles was. Professionals use two amounts of their hands when there is little oxygen while extracting blood. Note when patients have undergone different medication for swelling, paronychia or skin disorders.']</t>
         </is>
       </c>
-      <c r="AF4" t="inlineStr"/>
+      <c r="AF4" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article does not mention flavonoids, phenolic acids, or their relative content in any phase, which are the key claims made in the citation statement. The article is focused on a smartphone-based blood lipid data acquisition dongle and its application in measuring blood lipid levels."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -1195,7 +1206,14 @@
           <t>['The second study analyzed 325 patients with 173 in the propofol group and 152 in the sevoflurane group. No difference was observed in the overall 5-year survival rate between two groups, although the propofol group did have a lower rate of cancer recurrence (p = 0.037)  [48] . The third study collected 2645 cases, which included 2589 in the volatile anesthesia group and 56 in the propofol group. There was no significant difference between the groups in terms of postoperative recurrence or survival probability  [49] . Taken together, these studies suggest that propofol may either improve overall survival rates or lower the rate of cancer recurrence, but the evidence is not overwhelming. It is good to consider the limitations of these studies. First, there is the inherent limitation of retrospective studies in that they do not standardize clinical care and do not randomize patient groups. Therefore, the effects of confounding factors and selection bias cannot be easily eliminated. Second, one of the studies (Lee et al.  [49] ) had a relative small patient population and another (Kim et al.', 'The effect could be attributable to either the vertebral block, propofol or both  [46] .\n\nPropofol and clinical trials in breast cancer\nThree retrospective studies have compared propofol with volatile anesthetic agents on clinical outcomes of patients undergoing breast cancer surgery (Table  2 ). The first study, published in 2014 by Enlund and colleagues, reviewed surgical data from 1837 breast cancer patients with 620 in the propofol group and 1217 in the sevoflurane group. Differences in overall survival rates (propofol vs sevoflurane) for breast cancer were 3% (95% confidence interval, 1 to 4%, p &lt; 0.001) at 1 year, and 2% (-2 to 6%, non-significant) at 5 years, in favor of propofol. However, the observed differences were eliminated after adjustment for confounders (history of cardiac ischemia was 1.8 times more likely in the sevoflurane group)  [47] .', 'Therefore, the free propofol concentration employed in the in vitro cell culture experiments may be 50-500 times that of the clinical concentrations. This would be a lethal dose for humans. Future in vitro experiments should be designed to take protein binding into account.\n\nPropofol and the immune system\nSurgical trauma is associated with an increase of cytokines and stress hormones in the plasma during the vulnerable peri-operative period  [17] . This stress response  induces transient suppression of cell-mediated immunity, the primary immune-defense against the invasion of tumor cells and micro-metastasis  [33] . Surgery and anesthesia could suppress the immune response by activating the hypothalamic-pituitary-adrenal axis and the sympathetic nervous system  [34] . Anesthetics may also directly affect the functions of immune cells, including natural killer (NK) cells, cytotoxic T cells, mononuclear cells and dendritic cells  [35, 36] . NK cells are large, granular cytotoxic lymphocytes that naturally recognize malignant cells, and induce lysis without prior sensitization. Low perioperative levels of NK activity are associated with an increased cancer related morbidity and mortality in humans  [37] .']</t>
         </is>
       </c>
-      <c r="AF5" t="inlineStr"/>
+      <c r="AF5" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article does not support the claim about remimazolam tosylate's properties or its comparison with dexmedetomidine and propofol. The article primarily discusses the effects of propofol on breast cancer cells, the immune system, and patient outcomes, without mentioning remimazolam tosylate or the specific comparisons made in the citation statement."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -1344,7 +1362,16 @@
           <t>['In the table, China\'s intermediary centrality is lower than that of the United Kingdom and even France, which ranks sixth in publications, the analysis believes that academic exchange activities are mainly caused by the country\'s geographic location, lower than the academic exchanges between European and American countries  [17] .\n\nDistribution of institutions\nThrough the analysis of the distribution of research institutions, in addition to getting rid of the overall situation of the country, we can explore the current key research institutions in this field, this is the focus of academic research in this field, it is also convenient for researchers to understand the distribution of research forces in this field. The node type selects "Organization" and other parameters default, obtain the research collinear map of ceramic textile institutions (Fig.  2 ), in the co-occurrence network diagram, the number of occurrences of the node size indicator is high, reflecting the important status of the research institution, the more connections indicate the greater the number of partnerships, the thicker the connections indicate the stronger the degree of cooperation.', "As can be seen from the figure, the most frequent ones are Donghua Univ (Donghua University), Dalian Polytech Univ (Dalian University of Technology), Chinese Acad Sc (Chinese Academy of Sciences), Chonbuk Natl Univ (Chonbuk National University, South Korea), these institutions are all located in East Asia, it can be seen that the research on the application of ceramics in the textile field in East Asia is located in the world's leading area. At the same time, it can be seen from the figure that there are fewer cooperative relations among major institutions, the cooperation relationship is not close,  and the cooperation in the field of ceramic textile application in Asia and Europe needs to be strengthened in particular  [18] .\n\nResearch direction\nIn order to better express the application research direction of ceramics in textiles, use the search results of the WoS core database to make a research direction map, as can be seen from Fig.  3 , the research direction of ceramics in textiles has been applied in many fields, the most are engineering, materials science, architecture, equipment, physics, business economy.", "China is a leading country in the publication of ceramics in textile applications, but the earliest included in the WoS core library was in 2008, and it was later included, it should be affected by the language and the degree of internationalization of our country, but it also reflects the rapid development of China's ceramic textile field in recent years. The country with the earliest documents included in the WoS core database is the United Kingdom, and its total documents are second only to China, ranking second  [16] . In addition, the centrality in Cite space can reflect the intermediary status of academic research. Centrality is a measure of how connected a particular node is in the entire network, it refers to a certain point in the network, and the ratio of the shortest path connecting these two points to the total number of shortest path lines between these two points, nodes with high centrality are usually the main nodes in the entire network and are used to connect different research topics."]</t>
         </is>
       </c>
-      <c r="AF6" t="inlineStr"/>
+      <c r="AF6" t="inlineStr">
+        <is>
+          <t>Here is my evaluation:
+{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article does not mention anything related to routing algorithms, Manhattan distance, or transmission delay. It appears to be a scientometric analysis of ceramic materials in textile applications and has no relevance to the statement made in the citing article."
+}
+Let me know if you have any questions or need further clarification!</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1493,7 +1520,14 @@
           <t>["When it is explored, the textile manufacturing technology, textile manufacturing, and textile manufacturing industry are used as the subject keywords, and the search result was found to be 4123. Then, select 'Article (thesis)' as the article type. After invalid and duplicate data is screened and delimited, a total of 2852 related research articles in the global textile manufacturing and apparel industry from 2010 to 2019 are    [23] . In the knowledge network, key nodes occupy a key position, which can show the influence and relevance of nodes. Centrality can describe the accurate number of the key node size, which represents the frequency of this keyword node showing in the researched literature group, that is, the larger the key node shown in the map, the greater its frequency in the article group, which means that the greater the degree of its association with the vocabulary node appearing in other articles, the more frequent the information exchange  [24] [25] [26] .", "direction in the textile manufacturing technical field, which shows the importance of environmental issues in academia. In addition, the last tag word shows that the research on smart textile manufacturing in this field will exists as a research focus for a long time in the future.\n\n| Analysis of core authors\nUsually, the high-quality literature of the core authors reflects the research direction of the field, so through the research on the core authors of the retrieved literature can know the development focus of the textile manufacturing technical field. By setting the relevant parameters in the CiteSpace, and analysing 2852 articles, the core author relationship map of the textile manufacturing technical field from 2010 to 2019 can be obtained, as shown in Figure  8 . In the core author relationship map, the size of the node indicates the amount of publication of the author's literature, and the connection of the node indicates the cooperation between the authors. Through statistics, as shown in Figure  8 , the top ten core authors have published a total of 1111 articles in the past 10 years.", 'Moreover, the analysis of the keyword information in recent years indicates that textile manufacturing materials have gradually developed into nanoparticles and composite materials, which is a signal that textile manufacturing technology is gradually becoming intelligent.\n\n| Dynamic analysis of research hotspots\nA hot spot refers to a node that one thing develops rapidly or suddenly appears in a short period of time, which is a new research trend in academia. It emphasises the new development direction of industrial knowledge, and is also a feature of suddenness in time and space in the literature  [27] . Hotspots are generally the latest research directions. The time when each hotspot appears is the time when the research changes and is an important symbol of the dynamic development and evolution of the knowledge network. To more clearly know the continuation of the key research content in the textile manufacturing technology field in time, the time zone view is further drawn  [28] [29] [30] . The time zone view focuses on analysing the evolution of knowledge from the time dimension, so that the update and mutual influence of literature can be more clearly displayed  [31] .  direction in the textile manufacturing technical field, which shows the importance of environmental issues in academia.']</t>
         </is>
       </c>
-      <c r="AF7" t="inlineStr"/>
+      <c r="AF7" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article does not support the citation statement as it discusses the knowledge map visualization of technology hotspots and development trends in China's textile manufacturing industry, while the citation statement refers to calculating recommended trust values in a wireless sensor energy network. The abstract and provided excerpts do not mention trust management or wireless sensor networks, indicating that the reference article is unrelated to the cited topic."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1641,7 +1675,14 @@
           <t>['Our results on TNF cytokine corroborate other recent studies and highlight the complexity of the immune response against T. cruzi in chronic CD. As perspectives, we aim to address the mechanisms of TNFR activity in the peripheral blood cell from Chagas disease patients. Studies on cytokine profiles and frequency of receptors involved in apoptosis would also contribute to a better understanding of the immunopathology of chronic Chagas disease. \n\nCRediT authorship contribution statement\n\n\nDiego\n\n\nDeclaration of Competing Interest\nThe authors declare that they have no known competing financial interests or personal relationships that could have appeared to influence the work reported in this paper.', 'Therefore, evaluating soluble receptors, which are inhibitors of this cytokine, may improve the understanding of the chronic clinical evolution of the infection as well as the search for new immunological biomarkers.\n\nMaterials and methods\nPopulation and study site -This study was conducted in accordance with the recommendations of the FIOCRUZ/PE committee (CAAE: 0022.0.095.000-07 and 0032.095.000-10). All subjects signed written informed consent forms in accordance with the the guidelines of CNS Resolution 466/2012 of the National Health Council/Ministry of Health of Brazil.. One-hundred and thirty-two patients chronic with Chagas disease were selected at the Outpatient Clinic for Chagas Disease and Cardiac Insufficiency of the Cardiac Emergency Department of Pernambuco (PROCAPE)/University of Pernambuco (UPE). Individuals who had received previous treatment with Benznidazole and/or who presented with digestive complaints were excluded from the study. The clinical classification was performed by cardiologists following the II Brazilian Consensus on Chagas disease  (Dias et al., 2016) .', "Statistical Analysis -Variables were presented as descriptive measures: mean, median and standard deviation. The distribution of the data was evaluated by the D'Agostino-Pearson test, where it was verified that the data were non-parametric. Later, the Kruskal-Wallis test was used to evaluate the difference between the groups. Once the association was verified, the Mann-Whitney test was used for quantitative comparisons of receptors and cytokine between groups. The evaluation of correlations between TNFR1/2 versus TNF, TNFR1 versus TNFR2 and TNFR1/ 2, and TNF versus left ventricular ejection fraction (LVEF) was performed using the Spearman correlation test. Statistical analysis was performed using GraphPad Prism 5.0 software (GraphPad, San Diego, CA, USA) and data were considered significant when p &lt; 0.05.\n\nResults\nChagas disease patients have increased soluble TNF receptors levels -We found that sTNFR1 and sTNFR2 are elevated in chronic carriers of Chagas disease when compared to non-infected individuals (NI) (Fig."]</t>
         </is>
       </c>
-      <c r="AF8" t="inlineStr"/>
+      <c r="AF8" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article does not mention anything related to term translation, enriching term entries, or improving the quality of terms and term translation. The article is focused on the immunopathology of chronic Chagas disease, specifically the relationship between soluble TNF receptors and TNF in patients with the disease."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1789,7 +1830,14 @@
           <t>['The continuous variables were represented by mean ± SD. The correlation was analyzed by Pearson correlation, and a p value of 0.05 or lower was considered to be statistically significant. Statistical analyses were performed by IBM SPSS Statistics for Windows, version 26 (IBM Corp., Armonk, N.Y., USA).\n\nResults\n\n\nPatient Characteristics\nThe mean age of 44 patients was 50.8 years (SD, 14.8; range, 7-71). Among 44 patient, 22 (50%) patients were diagnosed with neuroendocrine tumors, of which 9 patients with pancreatic NET, 8 patients with rectal NET, and 5 patients with other or unknown origins. Twelve patients (27%) were diagnosed as pheochromocytoma or paraganglioma. Other 10 (23%) patients were diagnosed with other tumors except NET including meningioma. Demographics and diagnosis of patients were summarized in Table  1 . BGL of 44 patients were 107.5 ± 37.5 mg/dL (70-145 mg/dL), and the distribution of BGL is shown in Fig.  2 .', 'The ratio between SUVmax of the pancreas uncinate process and SUVmean of the normal pancreas body showed a significant negative correlation with BGL (r = -0.40, p = 0.01), and the ratio between SUVmax of the pancreas uncinate process and BP SUVmean also showed a significant negative correlation with BGL (r = -0.34, p = 0.02). However, two volume measurements on 68 Ga-DOTA-TOC PET were not significantly correlated with BGL: r = 0.274 and p = 0.068 for the correlation between SV 2.5 and BGL and r = -0.15 and p = 0.32 for the correlation between SV 40% and BGL. There was no significant correlation between patient age and SUVmax of the pancreas uncinate process (r = -0.17, p = 0.27). Representative cases with high and low BGL are shown in Fig.  3 . The result of correlation analysis between BGL and 68 Ga-DOTA-TOC PET parameters is shown in Fig.  4 .', 'Because PP is affected by glycemic conditions, we evaluated whether glycemia was associated with 68 Ga-DOTA-TOC uptake in the pancreas uncinate process. We found a correlation between blood glucose level (BGL) and 68 Ga-DOTA-TOC uptake in the pancreas uncinate process. While a significant negative correlation between BGL level and SUV parameters of 68 Ga-DOTA-TOC uptake was found, volume measurements defined by PET showed no significant correlation with BGL. Our findings imply that BGL could affect SSTR expression in the PP cells enriched in the pancreas uncinate process. Since SSTR is not fixed on cell membrane and is a dynamic structure capable of functions such as internalization, trafficking, and recycling  [11, 12] , rapid molecular response in SSTR expression could be triggered by glycemic conditions. Of note, volume measurements were not correlated with BGL. It suggested the tissue volume of PP cell rich islets in the pancreas could not be rapidly changed according to the glycemic condition. Moreover, it implied that glycemic conditions affect the functional activity of PP cells which might be represented by SSTR expression rather than increased volume of PP cell enriched region.']</t>
         </is>
       </c>
-      <c r="AF9" t="inlineStr"/>
+      <c r="AF9" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article does not mention anything related to 'Correlation between English Translation Ability and Students’ Performance'. The content is focused on the correlation between blood glucose levels and 68Ga-DOTA-TOC uptake in the pancreas uncinate process, which has no apparent connection to translation ability or students' performance."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1938,7 +1986,14 @@
           <t>['Although synonymous codon substitution does not alter amino acid sequence, the nucleotide sequence is then changed and is likely to affect the mRNA level in terms of transcription activity and mRNA stability  (Hia and Takeuchi, 2021) . It has been pointed out there was a potential correlation between gene sequence and transcription speed. Specific nucleotide pentamers (5 consecutive nucleotide bases) tended to have a specific transcription rate which was highly conserved in different genes  (Cohen et al., 2018) . Besides, a correlation between codon usage bias and nuclear RNA levels has also been reported in the genome of N. crassa. A batch of transcription factors or histone transmethylases might be involved in supporting this correlation  (Zhao et al., 2021) . In vivo studies in N. crassa showed that the transcriptional activity of luciferase increased with codon optimization, which was unrelated with translation. The inner mechanism was further revealed as reduced gene silencing marker H3K9me3 levels in codon optimized sequences  (Larrondo et al., 2012; Zhou et al., 2016) .', 'This may be explained by recent discoveries that besides translation speed, codon usage bias also regulates protein folding and function. For example, synonymous mutations on E. coli EgFABP1 coding gene changed the protein solubility ranging from 52% to 95%  (Cortazzo et al., 2002)  and codon optimization of Suf1 affected the efficiency of protein folding, which could be rescued by low temperature treatment  (Zhang et al., 2009) . In addition to E. coli, codon optimization of cyanobacteria circadian clock genes KaiB and KaiC also affected their functions in circadian clock regulation  (Xu et al., 2013) . Besides prokaryotes, the effect of codon bias on protein structure and function in eukaryotes has also been reported. Early studies in some gene candidates associated single-nucleotide silent mutation with protein functions, such as human period genes and sleep preference, MDR1 gene and substrate specificity  (Kimchi-Sarfaty et al., 2007; Carpen et al., 2006) .', 'In 2013, codon usage bias was shown to regulate co-translational folding and protein function by taking the N. crassa circadian clock core component FRQ as an example  (Zhou et al., 2013) . After that, the influence of codon bias on protein structure and function was subsequently confirmed on D. melanogaster circadian clock core component dPER and N. crassa Cross Pathway Control Protein 1 (CPC-1)  (Fu et al., 2016; Lyu and Liu, 2020) . In addition, a significant negative correlation between codon usage bias and protein structural disorder was identified in the genomes of five model organisms: E. coli, N. crassa, S. cerevisiae, C. elegans and D. melanogaster. The use of non-optimal codons in some regions may be a mechanism to reduce translation speed and provide enough folding time  (Zhou et al., 2015) . Compared with translation, the influence of codon usage bias on transcription has been overlooked for years.']</t>
         </is>
       </c>
-      <c r="AF10" t="inlineStr"/>
+      <c r="AF10" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article does not support the citation statement. The article discusses the relationship between codon usage bias and protein expression, structure, and function, but does not mention students' behavioral participation, cognitive participation, emotional participation, or translation performance in high school translation classrooms."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -2093,7 +2148,14 @@
           <t>['The optimality of re-triages was estimated at Trauma System level (percent of transfers to closest high-level TC) and at center level (percent of NTCs that re-triages to closest high-level TC for 90% of transfers).\n\nRESULTS:\nIn the CA Trauma System 81.2% of re-triages were to the closest high-level TC. However, at the individual center level, only four NTCs (1.8%) re-triaged 90% of transfers to the closest high-level TC. When there was &lt;50 miles of driving distance between NTC and TC, 74% of 1,216 non-optimal ground transfers could have reduced transfer times between 1-61 minutes had they re-triaged to the closest high-level TC. When there was 50 miles, 99% of non-optimal transfers could have been reduced by 1-324 minutes by driving or flying to the nearest high-level TC. CONCLUSION: The CA trauma system had satisfactory optimality in 2016. Optimization of re-triage to closest TC could improve performance of CA trauma system.', 'Optimization of re-triage to closest TC could improve performance of CA trauma system. Outcomes in Trauma Population of Nonagenarians Admitted to a Surgical Service vs Non-surgical: Experience at a Level I Trauma Center Charles Kung C Hu, MD, FACS, Daniel Jeremy Cucher, MD Dignity Health Chandler Regional Medical Center, Chandler, AZ INTRODUCTION: As the population ages, the number of patient over 90 years of age is increasing. This creates many challenges in providing care for the most vulnerable segment of the population. The aim of the study is to characterize and to compare outcomes of nonagenarians admitted to surgical service (trauma or orthopedic) vs non-surgical service (hospitalist).\n\nMETHODS:\nA retrospective review of trauma patients 90 years and older who were admitted from March 2014 to December 2020. The patients were divided into two groups: those admitted to a surgical service (trauma or orthopedic) and those admitted to a nonsurgical service (hospitalist). A total of 888 patients were found.\n\nRESULTS:\nThe ISS score is statistically higher for patients admitted to trauma or orthopedic service than to the hospitalists.', 'CONCLUSION: Changing the circuit while on ECMO support was associated with longer ECMO duration, higher mortality, and higher bleeding complications.\n\nOptimality of Re-triage of Under-triaged Severely Injured Patients in California\nAlona Furmanchuk, PhD, Kelsey Rydland, PhD, Abel Kho, MD, Anne M Stey, MD, MSc Northwestern University, Chicago, IL Northwestern, Chicago, IL INTRODUCTION: Re-triage is a complex process where nontrauma centers (NTC) transfer under-triaged severely injured patients to high-level trauma centers (TC). The process requires calling multiple high-level centers to accept the patient, coordinating transport and providing comprehensive hand-off. This study sought to quantify the optimality re-triage between NTC and TC in California.\n\nMETHODS:\nWe conducted an observational cohort study utilizing 2016 California Office of Statewide Health and Planning Data of severely injured adults. Network analysis based on the ground transportation and air ambulance data was employed to estimate the total distance and time from NTC to TC for each transfer.']</t>
         </is>
       </c>
-      <c r="AF11" t="inlineStr"/>
+      <c r="AF11" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article does not support the statement about a significant positive correlation between behavioral participation and translation performance. The article actually discusses extracorporeal membrane oxygenation (ECMO) in children and neonates, and its findings are unrelated to the variables mentioned in the citation statement."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -2241,7 +2303,14 @@
           <t>["environment  [5] -  [7]  because a high node density and a large communication overhead are required. Typical examples of range-free algorithms include Amorphous  [8] , Distance Vector-Hop(DV-Hop)  [9] , Multi Dimentional Scaling Map(MDS-MAP)  [10] , Distance Vector-short(DV-short)  [11]  and Approximate Point in Triangulation Test(APTT)  [12] . Moreover, many scholars have proposed using the connectiveness between nodes to determine a target's current movement position and predict its next position. Bayesianestimation-based filtering algorithms such as the Particle Filter(PF)  [13] , Extended Kalman Filter(EKF)  [14] , Extended Kalman Particle Filter(EKPF)  [15] , Unscented Kalman Filter(UKF)  [16]  and Hybrid Iterated Kalman Particle Filter(HIKPF)  [17]  are representative of this scenario.", 'The drift theory was used to design a Monte Carlo procedure in a Markov chain, causing the particle samples to be similar to observations. The particle swarm optimization (PSO) proposed in  [12]  measures the distance between nodes, and the measurement error was contained in the observation function of the motion noise. As a result, the positions of objects were determined by a weighted aggregation and by maximizing the PSO. Hou et al.  [27]  proposed an improved cubature PF algorithm that uses the least squares to estimate the prior states of target nodes. The cubature Kalman filter and Gauss-Newton iterative methods were used to measure the posterior state. This work provided the suggested distribution for the PF and improved the positioning accuracy. Vázquez and Míguez  [28]  introduced a distributed PF algorithm based on the posterior probability and combined it with Bayesian estimation. Experimentally, this method is superior to the distributed PF in terms of the positioning accuracy and robustness. In summary, most existing works combined the range-based and range-free methods and used additional auxiliary filters to improve the positioning accuracy.', 'However, they did not consider the particle degradation problem and ignored the influence of various intricate environmental factors (such as the number of deployed nodes, the mobility, and the path loss factor) and PF parameters (such as the number of generated particles, the noise variation and the particle population mobility) on the positioning accuracy of the target node. In addition, they were limited by their computational complexity and convergence speed, hindering them from being applicable in a large-scale and complex environment.\n\nIII. PROPOSED ALGORITHM\nThe target node periodically broadcasts beacon packets to neighboring nodes, and each beacon packet contains its identification number and location coordinates. When the number of beacon packets exceeds a specified threshold, the node is determined to be the centroid of a polygon. Correspondingly, the centroids of its neighboring nodes are viewed as its estimation. Although the traditional PF algorithm can perform node position estimation in non-linear and non-Gaussian WSNs, it has the particle degradation problem which means particles in the higher likelihood region have bigger weights and particles that do not intersect with the prior distribution region have weights close to 0. This problem can be well addressed by predicting the posterior distribution of high-quality particle populations. PQP algorithm can be applied in this respect.']</t>
         </is>
       </c>
-      <c r="AF12" t="inlineStr"/>
+      <c r="AF12" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article does not mention a hybrid artificial bee colony algorithm, nor does it discuss any application or proposal related to such an algorithm. The content provided focuses on target positioning in large-scale WSNs using particle centroid drift and comparisons with existing range-free algorithms."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -2389,7 +2458,14 @@
           <t>['As with many novel technologies, the high cost and bulky design of current CSLM devices are considered to be major barriers. Efforts, such as miniaturizing the device and lowering the cost of production can facilitate wider adoption. In addition, extensive training in both the acquisition and the interpretation of CSLM images is needed. Like dermoscopy, there is a steep learning curve to master the interpretation of CSLM images. Lastly, the technology has intrinsic limitations where CSLM evaluation can give rise to false-positive or falsenegative results.  64, 78, 79  \n\nHigh-Resolution Ultrasound\nMedical ultrasonography is an ultrasound-based diagnostic imaging modality used to visualize body tissue in real time. Modern ultrasound devices are both portable and relatively inexpensive when compared with other imaging modalities. The ultrasound technology is based on pulse-echo systems in which acoustic pulses are generated by a transducer and propagated to the body tissue. The return waves (echo) from the tissue are detected and converted into images for visual inspection. The resolution of the image and depth of tissue penetration is largely dependent on the frequency of the ultrasound transducer.', 'Despite its clinical efficacy, dermoscopy has several shortcomings. As mentioned previously, extensive training in the interpretation and analysis of dermoscopic structures and patterns is needed. A steep learning curve often discourages many clinicians from routinely using the device in daily practice. Also, some subset of melanomas (MMs), such as amelanotic/hypomelanotic MMs that lack pigmentations and dermoscopic structures, are exceedingly difficult to diagnose with dermoscopy. Moreover, its role in detecting MMs Ͻ 6 mm remains in debate.  38, 39  Nevertheless, for these difficult  lesions, clinicians can perform short-term mole monitoring by taking dermoscopic photos of the concerning lesions.  30, 40  Computer-Assisted Diagnostic Systems The combination of TBP and dermoscopy has improved diagnostic accuracy, but there are still significant numbers of pigmented lesions that pose a diagnostic challenge. To further improve diagnostic accuracy, various research groups in the world have been engaged in developing equipment and analytical software that can provide objective evaluations and even diagnoses of pigmented skin lesions, especially melanoma.', 'In general, the dermoscopic image qualities from PD and NPD are relatively similar. The major difference is that surface dermoscopic structures (eg, comedone-like openings, milia-like cysts and blue white veil) are better observed with NPD. In contrast, deep structures (eg, vessels) are better seen with PD.  29  The clinical utility of dermoscopy in aiding the diagnosis of melanoma is well documented. A list of these benefits are described in Table  1 .  30  Among these benefits, increased diagnostic accuracy is the most important feature. In the hands of experienced users, dermoscopy increases the diagnostic accuracy by more than 40%.  31  This improvement has been verified by several meta-analyses.  23, 32, 33  For patients, the improvement in diagnostic accuracy directly translates into an improvement of the benign/malignant biopsy ratio.  34  Terushkin et al  35  have shown that a group of clinicians performed fewer biopsies as their dermoscopic acumen increased. Increasing diagnostic confidence is another valuable benefit that appeals to practitioners.']</t>
         </is>
       </c>
-      <c r="AF13" t="inlineStr"/>
+      <c r="AF13" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article does not mention university-enterprise cooperation, practical teaching platforms, or talent training systems. The content of the article focuses on noninvasive imaging technologies for diagnosing melanoma, which is unrelated to the statement in question."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -2537,7 +2613,14 @@
           <t>['e comparison results of key security are shown in Table 2. It can be seen from Table  2  that the key security of the proposed IIBE algorithm is the highest. en, compare the computational complexity of different algorithms, as shown in Table  3 . It can be seen from Table  3  that, compared with other algorithms, the computational complexity of the proposed IIBE algorithm in system initialization, helping device, and user key update is reduced from O (log N) to o (1), which means that the complexity of the proposed IIBE algorithm is the lowest.\n\nExperimental Results and Analysis\n4.1. Experimental Setup. In the experiment, the WSN node adopts CC2530 sensor network node of TI (Texas instruments) company  [30] , which has an enhanced C51 single chip microcomputer and 8k RAM storage space, and is powered by two No.5 batteries  [31, 32] . WSN nodes are shown in Figure  4 . e actual network topology of IIBE is shown in Figure  5 . Settings of WSN network parameters are shown in Table  4 .', 'e calculation method of data reception rate  [33]  is as follows: Pr � \U0010ff50 n i�0 n (i)receive \U0010ff50 n i�0 n (i)send , ( 1 ) where n (i) receive represents the number of data received by the server from ith node and b represents the number of data sent by ith node. On CC2530 WSN node, the data receiving rates of several methods with 30-bit key are tested, and about 40,000 experimental data are obtained. e statistical fitting curve of the results is shown in Figure  7 . It can be seen from Figure  7  that when the network scale increases, the trend of traffic not only depends on the algorithm itself but also is greatly affected by the network layout. e random distribution method adopted in the experiment makes some nodes close to the coordinator Initialization Server Calculate sP as a public parameter and disclose it to all nodes Save the public parameter sP and the node private key E. key E Node Sending sP Encryption and decryption &amp; authentication Server Get plaintext D=f (m) Node Choose r at random and calculate rP.', 'NS2 simulation results show that this method is effective in preventing flooding attacks. However, this method only signs the data transmitted by nodes to prevent flooding attacks and has limited preventive effect on data eavesdropping attacks, so it needs to be combined with other encryption methods in practical applications. Rachkidy et al.  [23]  proposed a method of data storage combined with homomorphic encryption for some wireless sensor networks with insensitive real-time data, which is called DIOS. In some WSN (such as underwater sensor networks), people are more concerned about the whole data, rather than the data at a certain time. In view of this situation and considering that a large amount of data may cause loss to the sensor nodes if it is transmitted for a long time and a long distance, this literature puts forward that the data should be stored in a relay node in advance and preprocessed, so as to avoid the scattered and uninterrupted transmission of data. At the same time, homomorphic encryption is adopted to ensure security. is method is effective in some occasions, saving energy, and data can be stored safely. However, it is not suitable for most net-laying environments and has certain limitations.']</t>
         </is>
       </c>
-      <c r="AF14" t="inlineStr"/>
+      <c r="AF14" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article does not mention the regularization term of l_2 parametric or any concept related to reducing parameter space and avoiding overfitting. The article focuses on an improved identity-based encryption algorithm for wireless sensor network security, which is unrelated to the citation statement."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -2686,7 +2769,14 @@
           <t>['e comparison results of key security are shown in Table 2. It can be seen from Table  2  that the key security of the proposed IIBE algorithm is the highest. en, compare the computational complexity of different algorithms, as shown in Table  3 . It can be seen from Table  3  that, compared with other algorithms, the computational complexity of the proposed IIBE algorithm in system initialization, helping device, and user key update is reduced from O (log N) to o (1), which means that the complexity of the proposed IIBE algorithm is the lowest.\n\nExperimental Results and Analysis\n4.1. Experimental Setup. In the experiment, the WSN node adopts CC2530 sensor network node of TI (Texas instruments) company  [30] , which has an enhanced C51 single chip microcomputer and 8k RAM storage space, and is powered by two No.5 batteries  [31, 32] . WSN nodes are shown in Figure  4 . e actual network topology of IIBE is shown in Figure  5 . Settings of WSN network parameters are shown in Table  4 .', 'e calculation method of data reception rate  [33]  is as follows: Pr � \U0010ff50 n i�0 n (i)receive \U0010ff50 n i�0 n (i)send , ( 1 ) where n (i) receive represents the number of data received by the server from ith node and b represents the number of data sent by ith node. On CC2530 WSN node, the data receiving rates of several methods with 30-bit key are tested, and about 40,000 experimental data are obtained. e statistical fitting curve of the results is shown in Figure  7 . It can be seen from Figure  7  that when the network scale increases, the trend of traffic not only depends on the algorithm itself but also is greatly affected by the network layout. e random distribution method adopted in the experiment makes some nodes close to the coordinator Initialization Server Calculate sP as a public parameter and disclose it to all nodes Save the public parameter sP and the node private key E. key E Node Sending sP Encryption and decryption &amp; authentication Server Get plaintext D=f (m) Node Choose r at random and calculate rP.', 'NS2 simulation results show that this method is effective in preventing flooding attacks. However, this method only signs the data transmitted by nodes to prevent flooding attacks and has limited preventive effect on data eavesdropping attacks, so it needs to be combined with other encryption methods in practical applications. Rachkidy et al.  [23]  proposed a method of data storage combined with homomorphic encryption for some wireless sensor networks with insensitive real-time data, which is called DIOS. In some WSN (such as underwater sensor networks), people are more concerned about the whole data, rather than the data at a certain time. In view of this situation and considering that a large amount of data may cause loss to the sensor nodes if it is transmitted for a long time and a long distance, this literature puts forward that the data should be stored in a relay node in advance and preprocessed, so as to avoid the scattered and uninterrupted transmission of data. At the same time, homomorphic encryption is adopted to ensure security. is method is effective in some occasions, saving energy, and data can be stored safely. However, it is not suitable for most net-laying environments and has certain limitations.']</t>
         </is>
       </c>
-      <c r="AF15" t="inlineStr"/>
+      <c r="AF15" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article does not mention 2D pose estimation or the uncertainty of 3D pose estimation. The content appears to be focused on Wireless Sensor Networks (WSN) security, specifically an improved identity-based encryption algorithm (IIBE). There is no apparent connection between the citation statement and the provided reference article."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -2834,7 +2924,14 @@
           <t>['Introduction\nThe novel coronavirus disease (COVID-19) continues to spread worldwide, posing a dangerous threat to public health. By November 2021, there were about 250 million confirmed cases worldwide and well over 5 million deaths. In the past year, nonpharmaceutical interventions (e.g. cancelling mass gathering activities, travel restrictions, and mandating social distancing) were implemented by countries to reduce the transmission of COVID-19  (Dinleyici et al., 2020; Liu, 2021 Liu, , 2020)) . In the meanwhile, health experts recognize COVID-19 vaccination as one of the most important measures for combating COVID-19 infection  (Dinleyici et al., 2020) . Recently, the distribution of COVID-19 vaccines has begun in many countries, such as the United States, Russia, and China  (Smith et al., 2020) . However, an alarming number of people are highly suspicious of the safety and efficacy of COVID-19 vaccines and refuse immunization, a behavior defined as vaccine hesitancy  (Featherstone et al., 2019; Getman et al., 2018) .', "Several limitations of this study should be noted. First, single-item measures were used to investigate participants' COVID-19 information exposure on traditional news media, online news media, and social media, and this might incur measurement errors. Future research should use multiple items to ensure adequate reliability (e.g. internal consistency). Second, the cross-sectional study design might preclude an assessment of causality between COVID-19 information exposure, trust in government, vaccine confidence, and vaccine hesitancy. Scholars can use longitudinal research designs or experimental methods to better understand the relationships. Third, the data of this study was collected through an online survey which might be influenced by sampling bias, and the results cannot be generalized. For instance, the survey was available to respondents who are active online, and the sample of this study is skewed toward a highly educated population. Scholars should use probability sampling methods to research a diverse population and obtain higher-quality findings.\n\nConclusion\nDuring the crisis of COVID-19 pandemic, mass media play a salient role that potentially influences people's decision-making processes regarding the COVID-19 vaccination.", "The statistically acknowledged (p&lt;.05) indirect path and unacknowledged (aka non-significant) direct path form indirect-only mediation  (Zhao et al., 2010; Jiang et al., 2021) . One plausible reason is that social media contain a fair amount of misinformation that was closely related to public health  (Bode &amp; Vraga, 2018; Chou et al., 2018) . Given that COVID-19 vaccine development was compressed in time, and news about temporary side effects of the vaccines has been reported and raised global concerns, it is worrying that misinformation and unsubstantiated rumors about COVID-19 and vaccines against the disease were spread widely on the internet  (Duffy, 2020; Liu &amp; Huang, 2020) . Individuals who relied on social media for COVID-19 related information were more likely to be misinformed by disinformation about COVID-19 vaccines  (Burki, 2020; Wilson &amp; Wiysonge, 2020) . The spread of disinformation and misinformation about COVID-19 vaccines on social media can weaken people's confidence in vaccine safety and increase vaccine hesitancy."]</t>
         </is>
       </c>
-      <c r="AF16" t="inlineStr"/>
+      <c r="AF16" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article does not mention global warming or carbon dioxide pollution, which are the main topics of the citation statement. Instead, it focuses on COVID-19 information exposure, vaccine hesitancy, and trust in government. The provided excerpts do not contain any relevant information that supports the claim about global warming."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -2982,7 +3079,14 @@
           <t>["Accordingly, the U p can be considered a powerful tool for monitoring and detecting the damage in the adhesive joints in which the variation in the area enclosed by the hysteresis cycle is too small to cause a large change in the U d , E'' and tan δ. On the other hand, the predicted normalized potential energy of both NE and SiC-SAs show relatively less agreement with the experimental results, as shown in Figure  20 (b). Again, this behavior was attributed to the insignificant loss in the joint stiffness during stage II (main portion of joint life) that contrary to Zhang sigmoid model assumption. Hence, many efforts are required to develop analytical models that capable to monitoring and predicting the variation in the stiffness degradation as well as the increasing rate in the potential energy under low or moderate fatigue loading and thus, help in preventing the catastrophic failure of the joint without warning.\n\nConclusions\nIn this study, fatigue results of the scarf adhesive joints (SAJs) fabricated using neat epoxy (NE), and SiC and Al 2 O 3 -nanocomposite adhesives were extensively analyzed regarding the effect of the adhesive materials, bond thickness (0.17 mm and 0.25 mm) on fatigue lives and dynamic behavior.", "The scatter in the fatigue life was investigated using the two parameter Weibull function. Safe fatigue lives of the NE, SiC, and Al 2 O 3 -SAJs were estimated at different reliability levels. The following conclusions are drawn from this study. The measured potential energy (area under loading curve) was increased with the increase of the stress level (σ max ) as consequence of increasing the thermal and mechanical interfacial damages in the SAJs. This result is consistent with decreasing the storage modulus (E'), which has a linear inverse relationship with Potential energy (U p ). Potential energy (U p ) was used for the first time (except author works) for monitoring and predicting the damage in the adhesive joints in which the variation in the area enclosed by the hysteresis loop is too small to cause a large change in the factor (tan δ), loss modulus (E''), and dissipated energy (U d ). Zhang model predicts well the experimental measurements of the potential energy and storage modulus (E 0 ) specially at higher stress levels (i.e., high damage) at which they follow a sigmoid curve with constant increasing/ decreasing rates during the most lifetime of the joint.", 'In general, the S-N curves can be used for prediction the joint life, but they do not give indication about the damage initiation, propagation, and the dynamic parameters during the lifetime of the joint that will be investigated in the following sections. Statistical analysis. Table  5  shows the computed Weibull parameters (α and β), Mean lives (N m ) and coefficient of variation (CV%). The Weibull parameters were used to draw the Weibull fatigue life distributions of the SiC-SAJs at different stress levels, as shown by the representative example in Figure  8 . It is obvious from Figure  8  that the lowest slopes (i.e., higher scatter) were observed at the intermediate stress levels (66.7 MPa and 70.7 MPa) compared to those of the minimum (55.5 MPa) and maximum (75.0 MPa) stress levels. These observations are consistent with the estimated CV% in Table  5 .']</t>
         </is>
       </c>
-      <c r="AF17" t="inlineStr"/>
+      <c r="AF17" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article does not mention WebGIS technology, spatial databases, or ecological environment resource data management, which are the key components of the citation statement. The article appears to focus on fatigue damage in adhesive joints and nanocomposites, unrelated to the topic of the citing article."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -3131,7 +3235,14 @@
           <t>['In the table, China\'s intermediary centrality is lower than that of the United Kingdom and even France, which ranks sixth in publications, the analysis believes that academic exchange activities are mainly caused by the country\'s geographic location, lower than the academic exchanges between European and American countries  [17] .\n\nDistribution of institutions\nThrough the analysis of the distribution of research institutions, in addition to getting rid of the overall situation of the country, we can explore the current key research institutions in this field, this is the focus of academic research in this field, it is also convenient for researchers to understand the distribution of research forces in this field. The node type selects "Organization" and other parameters default, obtain the research collinear map of ceramic textile institutions (Fig.  2 ), in the co-occurrence network diagram, the number of occurrences of the node size indicator is high, reflecting the important status of the research institution, the more connections indicate the greater the number of partnerships, the thicker the connections indicate the stronger the degree of cooperation.', "As can be seen from the figure, the most frequent ones are Donghua Univ (Donghua University), Dalian Polytech Univ (Dalian University of Technology), Chinese Acad Sc (Chinese Academy of Sciences), Chonbuk Natl Univ (Chonbuk National University, South Korea), these institutions are all located in East Asia, it can be seen that the research on the application of ceramics in the textile field in East Asia is located in the world's leading area. At the same time, it can be seen from the figure that there are fewer cooperative relations among major institutions, the cooperation relationship is not close,  and the cooperation in the field of ceramic textile application in Asia and Europe needs to be strengthened in particular  [18] .\n\nResearch direction\nIn order to better express the application research direction of ceramics in textiles, use the search results of the WoS core database to make a research direction map, as can be seen from Fig.  3 , the research direction of ceramics in textiles has been applied in many fields, the most are engineering, materials science, architecture, equipment, physics, business economy.", "China is a leading country in the publication of ceramics in textile applications, but the earliest included in the WoS core library was in 2008, and it was later included, it should be affected by the language and the degree of internationalization of our country, but it also reflects the rapid development of China's ceramic textile field in recent years. The country with the earliest documents included in the WoS core database is the United Kingdom, and its total documents are second only to China, ranking second  [16] . In addition, the centrality in Cite space can reflect the intermediary status of academic research. Centrality is a measure of how connected a particular node is in the entire network, it refers to a certain point in the network, and the ratio of the shortest path connecting these two points to the total number of shortest path lines between these two points, nodes with high centrality are usually the main nodes in the entire network and are used to connect different research topics."]</t>
         </is>
       </c>
-      <c r="AF18" t="inlineStr"/>
+      <c r="AF18" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article does not mention anything about generating weight vectors or parameters of excitation functions randomly. The article appears to be about analyzing research hotspots in ceramic materials for textile applications, and the provided excerpts do not relate to the statement being evaluated."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -3419,7 +3530,14 @@
           <t>['In addition, such conventional technologies use integrated security management methods that manage the logs of security products on different models. In particular, firewalls, intrusion detection/prevention systems, and anti-virus technologies are focused on the development of the platform technology needed to apply signature or blacklist-based detection methods to 10Gbp-level high-performance networks. Also, the changes in the key technologies to counter cyber-attacks were based on integrated security management technologies, and it is expected that an intelligent security analysis model using big data will be the prominent topic of the future. By seamlessly integrating security equipment that has previously been operated separately and managing them as a whole, it will be possible to conduct an intelligent analysis of security threats, which will allow us to predict future problems in parallel with behavior-based analysis, to prevent and remove security risks. Big data security analysis methods will allow the threats of attacks that have not been resolved to be addressed, utilizing the security system that will ensure seamless responses to the latest cyber-attacks. The correlation analysis of big data through these security systems will reveal the unknown patterns of the attacks and support decision-making. By implementing a high-performance pattern matching algorithm through the behavior-based signature database, it would be possible to make comparisons at a higher speed.', 'In Chapter 2 of this article, the author conducted a literature review that describes the evolution of cyber-attack technologies, which is followed by Chapter 3 in which the intelligent security analysis method utilizing big data is presented. In Chapter 4, the author explains the intelligent behavioral analysis and verification methods. Finally, Chapter 5 provides the conclusion and suggestions for future research.\n\nLiterature review\n1. The Evolution of Cyber-Attacks With the evolution of the technologies used in cyber-attacks, they are now considered one of the major threats against the country and society. One of the most commonly used types of cyber-attack is the APT (Advanced Persistent Threat) attack. An APT attack continuously attacks its target with the goal of stealing industrial secrets, classified military intel, and customer information, etc. In addition, as this attack is used for major information leakage, control system attacks, and cyber terrorism, the threat of cyber-targeted attacks targeting major information and communication infrastructure is increasing.', 'detection analysis is the main technology\n\nData &amp; User Monitoring\nMonitoring data/user activity, including user and data context, is an essential skill for intrusion detection and misuse detection, and is fundamentally required for monitoring privileged users and sensitive data access\n\nApplication monitoring\nSince application vulnerabilities are the main target of targeted attacks, the activity monitoring technology of abnormal applications\n\nAnalytics\nA core technology for big data security analysis that analyzes the characteristics of various source information and determines whether there is an abnormality using machine learning, data mining, and network mining techniques, which are traditional methods of big data analysis\n\nBehavior-Based Intelligent Security Analysis Methods and Verification Results\nIn this study, security threats are classified by reconstructing the records of persistent attacks recorded in security solutions, servers, applications, and other events to enable a response to cyber-attacks in real time. That is, the researcher intends to study a behaviorbased intelligent security analysis method in which detection rules can be used to understand the relationships of the events before and after an attack. This behavior-based technology will allow attacks to be predicted before they happen, making it possible to make an immediate decision.\n\nBehavior-based Intelligent Security Analysis\nAn attacker uses various cyber-attack tools to get the information he or she wants.']</t>
         </is>
       </c>
-      <c r="AF20" t="inlineStr"/>
+      <c r="AF20" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article primarily focuses on intelligent security analysis methods utilizing big data, discussing topics like cyber threats, APT attacks, and behavior-based security analysis. There is no mention of an identifiable technology device with advanced technology as claimed in the citation statement."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -3567,7 +3685,14 @@
           <t>['A systems analyst must keep in mind that excessive energy output could harm the human body. Even still, Theorem 4 in Section 3) shows that there are no unique optimal solutions to Problem (3). X 1 (A, b) is an infinite set of optimum solution to Problem (3), sometimes known as X 1 (A, b). As a result, we use an unlimited set of X 1 (A, b) values to look for the most ideal solution, which employs a second optimization objective  (Shang et al., 2014) . In the above definition, optimizing the second objective given X 1 (A, b). Constraint reuse is a secondlevel issue. To increase non-operational base stations, we must reduce operational base stations. When base stations fail, their maintenance costs fall. The second goal is to reduce base station operating costs. While a non-functional base station has no electro-magnetic strength, a functional base station does. For instance, in order to keep the zero norm of the vector x = (x 1 , x 2 , x 3 , x 4 . . .', "Aim 1 in Problems (3)-(  4 ) is to keep electromagnetic waves intensity as low as possible, whereas objective 2 is to keep base station operating expenses as low as possible. Problem (3) can be solved using the idea of a minimal solution matrix presented by Yang et al. While Yang's method fails to provide the whole solution set to the problem, this paper will prove that (3). We could not employ Yang's methods in the original study since it did not address the bi-level problem. This study seeks to discover the best possible solution to the problem stated above, which is bi-level objective programming (3), (4). The final section of Section 3 looks at the ideal solution set for Problem (3) and measures its quality by utilizing a minimum-maximum norm solution matrix. This chapter studies the problem at the second level (4). We use the set of minimum-norm solutions to solve the problem (4). We have included a mathematical example in Section 5 to show how and why our proposed method might be implemented and would produce accurate results. Section 4 discusses several forms of management requirements in order to highlight multiple kinds of bi-level difficulties.", "Additionally, system administrators may have additional requirements that must be taken into consideration when single-level optimization is employed.  Yang et al. examined  single-level min-max programming using a BT-P2P file-sharing system  (Rastogi et al., 2015; Bulanov et al., 2004) .  Guu et al. developed  bi-level optimization to achieve a balance of realistic management requirements  (Bjorklund et al., 2003; Pedrycz, 1985) . As per further explored difficult managerial requirements by creating a three-tiered optimization problem for the firm  (Stamou and Tzafestas, 2001; Shieh, 2007) . Their solution for bilevel optimization with max-product fuzzy relation inequalities included wireless communication. The goals' aspects allow for both management qualities. Fairness was applied to the wireless communication station system. Growing numbers of individuals utilize wireless communication. Signals, data, and information are delivered by fixed emission basic stations. Start from the premise to n EBSs, for example, A 1 , A 2 , . . .. An (see Fig."]</t>
         </is>
       </c>
-      <c r="AF21" t="inlineStr"/>
+      <c r="AF21" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article does not support the statement about parties having further experience and understanding of evaluation objectives and system objectives. The article primarily discusses bi-level optimization models for energy efficiency in wireless transmission station systems, with no mention of public management problem classification or evaluation objectives."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -3717,7 +3842,18 @@
           <t>['They obtained domain-related models with adjustable budgets in terms of the number of parameters and computational complexity. To adjust the computational complexity of the network, they adopted a pretrained architecture to derive a specialized deep model for each domain and then incorporated a budget-aware adapter to select the most relevant feature channel to better process the data from the new domain. Among recent works, there are also some studies that improve domain adaptability through adversarial learning. They decompose a deep network into feature extractor and classifier components and then train each component by tuning its partner  (Xu, Chen, Zuo, Yan, &amp; Lin, 2018) . They either use a deep cocktail network (DCTN) to deploy multidirectional adversarial learning to minimize the difference between the targets and multidomain data  (Ganin et al., 2016)  or use domain-specific representation learning  (Schoenauer-Sebag et al., 2019) , where the data come from similar but heterogeneous distributions.', 'This article focuses on multidomain data in heterogeneous networks, which plays an important role in maintaining the operation of the Internet and protecting Internet of Things devices, especially the privacy and security of a large number of dense mobile users. Future work includes solving the Lagrangian function to find an accurate solution instead of an approximate solution and further improving the ability to detect samples with approximate distributions. CRediT authorship contribution statement Peng An: Supervision, Reviewing. Zhiyuan Wang: Writing -original draft, Model implementation, Experimentation. Chunjiong Zhang: Conceptualization, Methodology, Data curation, Experimentation, Visualization, Editing.', 'Although multidomain machine learning solves the problem of domain adaptability to some extent through assumptions about specific data distributions, the performance of most models is poor in practice because they ignore the nature of data skewness and lack a process that effectively determines the robustness of multidomain data. It is claimed that ignoring the inconsistency of the data size and the heterogeneity of the data distribution generated by network traffic will have a serious impact on the detection results and may even mislead the entire machine learning process. In contrast to existing works, the current study focuses on extracting the hidden relationship between data that are not independent and identically distributed (non-IID) and unbalanced data and performing robust optimization on data from different domains so that the proposed scheme can further improve domain adaptability without relying on assumptions about the data distribution.\n\nProposed framework\n\n\nSystem overview\nThe purpose of this research is to perform effective anomaly detection on network intrusion samples from different domains. The key problem to be solved is the feature learning and reconstruction of high-dimensional multidomain data. However, most of the current studies using single-channel networks cannot capture the hidden spatial information of data in different domains, and the features of the reconstructed errors do not include the differential representation of heterogeneous distributions.']</t>
         </is>
       </c>
-      <c r="AF22" t="inlineStr"/>
+      <c r="AF22" t="inlineStr">
+        <is>
+          <t>Here is my evaluation:
+```
+{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article (11) focuses on cyberattack detection using ensemble unsupervised autoencoders and Gaussian mixture models, which has no apparent connection to urban resilience, urban planning, or construction. The provided excerpts do not mention any of these topics."
+}
+```
+This is because the citation statement mentions urban resilience and planning, but the reference article appears to be about a completely different topic (cyberattack detection).</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -3866,7 +4002,14 @@
           <t>["specificity (Sp), precision, accuracy (Acc) and Matthew's Correlation Coefficient (MCC): Sn ¼ TP TP þ FN Sp ¼ TN TN þ FP Precision ¼ TP TP þ FP Acc ¼ TP þ TN TP þ TN þ FP þ FN MCC ¼ TP Â TN À FP Â FN ffiffiffiffiffiffiffiffiffiffiffiffiffiffiffiffiffiffiffiffiffiffiffiffiffiffiffiffiffiffiffiffiffiffiffiffiffiffiffiffiffiffiffiffiffiffiffiffiffiffiffiffiffiffiffiffiffiffiffiffiffiffiffiffiffiffiffiffiffiffiffiffiffiffiffiffiffiffiffiffiffiffiffiffiffiffiffiffiffiffiffiffiffiffiffiffiffiffiffiffiffiffiffiffiffiffi ðTP þ FPÞ Â ðTP þ FNÞ Â ðTN þ FPÞ Â ðTN þ FNÞ p where TP, TN, FP and FN denote the numbers of true positives (correctly predicted cleavage sites), true negatives (correctly predicted 3 Results and discussion On the other hand, if the target dataset is large or the number of parameters is small,", "We provide a detailed description of how these data were encoded into the inputs for the DeepCleave's network in Supplementary Methods section in Supplementary Materials. We compare the predictive quality of these approaches on the training and independent test datasets in Supplementary Tables  S7  and  S8 , respectively. Results reveal that majority of these input types, except for the putative secondary structure, can be used to predict the cleavage sites reasonably well. The average AUCs computed over the 12 proteases equal 0.605 for the putative secondary structure, 0.766 for CKSAAP, 0.798 for the putative solvent accessibility, 0.806 for the PSSM and conservation scores, 0.922 when using the BLOSUM62 matrix-derived inputs and 0.947 when using the one-hot encoding from DeepCleave. Similar trend is true when using the average MCC, with the corresponding values equal 0.181, 0.463, 0.527, 0.510, 0.732 and 0.828.", '4E  and  F ). The UMAP plots demonstrate that the DeepCleave framework learns informative feature representations from the one-hot encoding that is easy to extract from the input protein chains. However, even the results at the 2nd fully connected layer show overlap between some cleavage points associated with different caspases. This is not surprising since some sites are cleaved by several different proteases. In addition, we obtain similar results when using another visualization tool, t-SNE (van der  Maaten and Hinton, 2008) . The t-SNE plots are shown in Supplementary Figure  S3 . To sum up, our empirical results in Sections 3.1-3.3 suggest that the models trained on the protease-family cleavage data can be used to develop accurate cleavage prediction models.\n\nFeature representation in the DeepCleave predictor\n\n\nComparison of predictive performance on the test dataset\nWe compare the predictive performance of the protease-specific DeepCleave models on the independent test dataset (up to 20% similarity with the training dataset) against state-of-the-art prediction tools that have been developed for the caspase and MMP cleavage sites prediction.']</t>
         </is>
       </c>
-      <c r="AF23" t="inlineStr"/>
+      <c r="AF23" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article does not mention or address the problem of difficulty in arranging classes and summarizing grades under high-level management. The content appears to be focused on a deep learning predictor for protease-specific substrates and cleavage sites, which is unrelated to the statement from the citing article."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -4021,7 +4164,14 @@
           <t>['QALY: quality-adjusted life of years; SA: sensitivity analysis.\n\n5\nFootnotes:\n\n6\n* Within each analysis, the intervention in bold is the intervention which is considered to be most cost-effective under the NICE £20,000 per QALY decision rule.\n\n7\n† Assuming different cancer progression rate for patients receiving different interventions. The cancer progression rates for patients who received surgery were calibrated from published 8 literature (Table  1 ). The cancer progression rates for patients who received RFA were calculated based on the RR (RFA vs surgery) reported by a recently published meta-analysis of five trials 9 including 742 patients: 1.42 for local progression and 1.36 for regional/distant progression  [60] . The short-term cancer progression rate for patients who receiving SABR was obtained from the 10 CtE scheme. The exponential distribution provided the closest fit to the data for both local and regional/distant progression: from no progression to local recurrence (monthly transition 11 rate=3.00%), and from no progression to regional/distant recurrence (monthly transition rate=1.01%)).', '856 2.5806 ---2 2 RFA 11,132 2.5811 --Extendedly dominated 3 3 Surgery 12,489 2.8795 1,357 0.2984 4,548 1 1 SA 4: Different cancer progression rate and different mortality rate for patients receiving different interventions ** (base case assumes same cancer progression rate and same mortality rate for all three interventions) Intervention Cost (£) QALY Incremental cost Incremental QALY ICER Ranking of NMB (WTP=20,000 per QALY) Ranking of NMB (WTP=30,000 per QALY) SABR 12,159 2.2607 --Dominated 3 3 RFA 11,661 2.5403 ---2 2 Surgery 12,489 2.8795 828 0.3392 £2,440 1 1 Abbreviations: ICER: Incremental cost-effectiveness ratio; NMB: net monetary benefit; QALY: quality-adjusted life of years; SA: sensitivity analysis.', '[53] Progression free with SAEs 0.40 [52, 54, 55] 0.50 [56, 57] Local progression 0.65 [52, 54, 55] 0.63 [24] Parameters Liver oligometastases HCC Value Reference Value Reference Regional/ distant progression 0.19 [52, 54, 55] 0.40 [58] Footnotes: * A complete list of all parameters used in the model, their fixed values, ranges, distributions and references are reported in Appendix B. Abbreviations: ICER: Incremental cost-effectiveness ratio; NMB: net monetary benefit; QALY: quality-adjusted life of years; SA: sensitivity analysis; WTP: willingness to pay threshold. Footnotes: * Within each analysis, the intervention in bold is the intervention which is considered to be most cost-effective under the NICE £20,000 per QALY decision rule. † Assuming different cancer progression rate for patients receiving different interventions. The cancer progression rates for patients who received surgery were calibrated from published literature (Table  1 ).']</t>
         </is>
       </c>
-      <c r="AF24" t="inlineStr"/>
+      <c r="AF24" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article does not mention anything about nursing-sensitive quality indicators, three-level quality control of nursing departments, or head nurses. It appears to be focused on a cost-effectiveness analysis of different treatments for liver cancer and hepatocellular carcinoma."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -4169,7 +4319,17 @@
           <t>['Use of stereo earphones also allows differentiation between positive and negative (reverse) signals by ear. After the advent of modern ultrasound techniques combining high-resolution imaging, color Doppler imaging and pulsed Doppler, listening to the signals has been generally abandoned in favor of adjusting the recording situation and optimizing signals by visual control of the Doppler spectrum. Indeed, modern ultrasound systems do not provide an output for audible signals anymore and the quality of built-in loudspeakers is usually very poor.', 'Analyses of the FFTs were done in the frequency range from 150 Hz, corresponding to the limit of earphones used by the sonographer, to 10,007 Hz, representing the frequency of the band stop of recording. An auditory feature, the high frequency cut-off band was identified within the frequency range  [14] . Based on the results of our previous experimental study  [9] , this high-frequency cut-off (MAX peak-15 dB ) was defined as the frequency band where the energy level had decreased by 15 dB from its maximum level, i. e. from the MAX peak value ( • " Fig.  1 ). The primary outcome variable was the composite adverse pregnancy outcome including perinatal death, operative delivery for fetal distress and admission for treatment in the neonatal intensive care unit. The risk for a negative outcome, given a certain value for artery PI, auditory parameter MAX peak-15 dB, or combination of PI and MAX peak-15 dB , was calculated using logistic regression analysis.', 'Recently, we have developed and validated in an animal experimental model a method for objective analysis of the Doppler sound spectrum  [9] . Subsequently, in a human pilot study, we compared the audio analysis and the traditional waveform analysis of umbilical artery Doppler signals before and after maternal steroid treatment  [10] . The auditory parameter reflected the changes in the umbilical artery circulation more sensitively than the PI did. Our hypothesis is that the auditory analysis of umbilical artery Doppler sound spectrum might be an additional tool in the evaluation of fetal circulation in high-risk pregnancies. The aim of the present study was to retrospectively apply the new auditory parameter on a group of high-risk pregnancies with various degrees of placental insufficiency in order to investigate its possible usefulness.\n\nMaterials and Methods\n\n\n!\nThe study group comprised 127 singleton high-risk pregnancies with gestational age ranging from 23 to 39 weeks. They were referred for Doppler ultrasound examination according to the clinical fetal surveillance program.']</t>
         </is>
       </c>
-      <c r="AF25" t="inlineStr"/>
+      <c r="AF25" t="inlineStr">
+        <is>
+          <t>Here is my evaluation:
+```
+{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article does not discuss sound perception or the internal processing of received sound through the brain, which are the key concepts in the citation statement. Instead, it focuses on Doppler audio signal analysis for evaluating umbilical artery circulation in high-risk pregnancies."
+}
+```</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -4317,7 +4477,14 @@
           <t>['3a ). SAP was expressed in all major subsets of human T cells (CD4 + , CD45RO + , CD45RA + and CD8 + ) (Fig.  3c ), in the T-cell tumour cell line Jurkat, and in the Burkitt lymphoma line Raji which is positive in the Epstein±Barr virus (EBV). No transcripts were detected in the EBV + Burkitt lymphomas Namalwa or BL41/B95-8, the EBV-transformed cell line X50-7, the EBV + marmoset cell lines B95-8 and FF41, the EBV -Burkitt lymphoma BJAB, or in the pre-B ALL lines LAZ 221 and NALM 6 (Fig.  3 , and data not shown). Figure  2  Characterization of the human and murine SAP proteins and their interactions with SLAM. a, Jurkat cells and human peripheral blood lymphocytes (PBL) were lysed and postnuclear lysates (1 mg ml -1 ) were immunoprecipitated (IP) with a rabbit antiserum directed against human SAP or with a control serum (3 ml).', 'c, hSAP exon 1, exon 2, exon 3 and exon 4 and BRCA1 exon 2 were ampli®ed by PCR from genomic DNA from patients A1, B1, B2 and B3, and from the cell line Raji. DNA products were resolved on a 2% agarose gel. phosphorylation of Y281 was not required for binding of the two polypeptide chains. However, we found that the SH2 domain of SAP was functionally intact as it could be puri®ed on a Sepharose± phosphotyrosine column (data not shown). In addition, four SAP mutants with deletions in the tail domain (Fig.  1 ) and co-transfected with the CD8±SLAM3 chimaera were able to interact with the short cytoplasmic domain of SLAM3, which contained the Y281 segment (Fig.  7d ). Collectively these results show that SLAM interacts with SAP through part of its SH2 domain.', 'Collectively, our results show that, unlike SLAM, SAP is primarily expressed in T cells. SAP is encoded by the XLP disease gene By using a 45-kb pBAC clone that contained all four exons of murine SAP (Fig.  1 ), the SAP gene was localized within band A5.1 of the murine X chromosome (C.W., J.S. and C.T., manuscript in preparation). Because of synteny between murine band A5.1 and human Xq25, where the locus for the immune de®ciency X-linked lymphoproliferative disease (XLP) had been mapped 8±11 , we investigated whether the SAP gene could be involved in this disease. Moreover, the observation that in XLP uncontrolled B-cell proliferation following EBV infection often leads to fatal infectious mononucleosis, malignant lymphomas, hypogammaglobulinaemia or aplastic anaemia  11, 12  was in agreement with the involvement of SLAM in T $ B-cell interactions.']</t>
         </is>
       </c>
-      <c r="AF26" t="inlineStr"/>
+      <c r="AF26" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article does not mention SAPR/3 system, ERP application systems, or any related concepts. Instead, it discusses a protein called SAP (SH2D1A) and its role in regulating signals induced through the co-receptor SLAM, which is unrelated to the citation statement."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -4465,7 +4632,14 @@
           <t>['e comparison results of key security are shown in Table 2. It can be seen from Table  2  that the key security of the proposed IIBE algorithm is the highest. en, compare the computational complexity of different algorithms, as shown in Table  3 . It can be seen from Table  3  that, compared with other algorithms, the computational complexity of the proposed IIBE algorithm in system initialization, helping device, and user key update is reduced from O (log N) to o (1), which means that the complexity of the proposed IIBE algorithm is the lowest.\n\nExperimental Results and Analysis\n4.1. Experimental Setup. In the experiment, the WSN node adopts CC2530 sensor network node of TI (Texas instruments) company  [30] , which has an enhanced C51 single chip microcomputer and 8k RAM storage space, and is powered by two No.5 batteries  [31, 32] . WSN nodes are shown in Figure  4 . e actual network topology of IIBE is shown in Figure  5 . Settings of WSN network parameters are shown in Table  4 .', 'e calculation method of data reception rate  [33]  is as follows: Pr � \U0010ff50 n i�0 n (i)receive \U0010ff50 n i�0 n (i)send , ( 1 ) where n (i) receive represents the number of data received by the server from ith node and b represents the number of data sent by ith node. On CC2530 WSN node, the data receiving rates of several methods with 30-bit key are tested, and about 40,000 experimental data are obtained. e statistical fitting curve of the results is shown in Figure  7 . It can be seen from Figure  7  that when the network scale increases, the trend of traffic not only depends on the algorithm itself but also is greatly affected by the network layout. e random distribution method adopted in the experiment makes some nodes close to the coordinator Initialization Server Calculate sP as a public parameter and disclose it to all nodes Save the public parameter sP and the node private key E. key E Node Sending sP Encryption and decryption &amp; authentication Server Get plaintext D=f (m) Node Choose r at random and calculate rP.', 'NS2 simulation results show that this method is effective in preventing flooding attacks. However, this method only signs the data transmitted by nodes to prevent flooding attacks and has limited preventive effect on data eavesdropping attacks, so it needs to be combined with other encryption methods in practical applications. Rachkidy et al.  [23]  proposed a method of data storage combined with homomorphic encryption for some wireless sensor networks with insensitive real-time data, which is called DIOS. In some WSN (such as underwater sensor networks), people are more concerned about the whole data, rather than the data at a certain time. In view of this situation and considering that a large amount of data may cause loss to the sensor nodes if it is transmitted for a long time and a long distance, this literature puts forward that the data should be stored in a relay node in advance and preprocessed, so as to avoid the scattered and uninterrupted transmission of data. At the same time, homomorphic encryption is adopted to ensure security. is method is effective in some occasions, saving energy, and data can be stored safely. However, it is not suitable for most net-laying environments and has certain limitations.']</t>
         </is>
       </c>
-      <c r="AF27" t="inlineStr"/>
+      <c r="AF27" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article does not mention cartoon rendering algorithms or ink texture mapping. The abstract and excerpts discuss wireless sensor networks (WSN), identity-based encryption, and network security, which are unrelated to the citation statement about traditional cartoon rendering algorithms."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -4613,7 +4787,14 @@
           <t>['If all features are fused blindly, the dimension of the feature vector will be greatly increased, which not only increases the computation effort and storage but may also reduce the recognition performance. Moreover, features differ in their physical meanings and usages. A hierarchical recognition method handles different features by different classifiers. When designing classifiers at different levels, the classifier must be optimized by considering the physical meanings and statistical distributions of the features. For example, features such as target size and scattering center can be classified by a simple threshold discriminant classifier or a decision tree classifier, whereas the structural and statistical features of the scattering centers can be discriminated by a support vector machine classifier. Before making the final decision, the results of different classifiers can be combined by an ensemble classification method.  For adaptive feature extraction, we can exploit the end-to-end capability of deep neural networks. Deep learning avoids the high dependence of the traditional machine learning algorithm on human experience  [118] [119] [120] [121] . Deep neural networks include deep autoencoders, deep convolution neural networks, and deep recurrent neural networks. Among these, the deep convolution neural network is most commonly used.', 'Some outcomes of these studies are elaborated below. First, the classical point-target detector was modified for range-spread targets by the energy integration detector and the M out of N (M/N ) detector. The typical scattering density dependent generalized likelihood ratio test (SDD-GLRT) detector  [39] , which consists of a nonlinear map followed by an integrator along the range cells, detects a range-spread target among white Gaussian noise. If the scattering density parameter is known, the performance of SDD-GLRT improves. However, the efficiency of SDD-GLRT solutions is decreased by the exponential and logarithmic operations. The M/N detector is a typical double-threshold detector of spatially distributed targets. Owing to its efficient structure, this detector can be easily realized in engineering and has been widely applied. Therefore, it has attracted much interest and has been often modified to improve its robustness and efficiency  [40, 41, 55] .', 'Al- Long T, et al. Sci China Inf Sci April 2019 Vol. 62 040301:11 YES EM iteration NO Establish initial value set Target detection Update target feature status Calculating multivariate information log likelihood function expectation Optimizing multivariate information log likelihood function expectation Update target motion status Calculating the multivariate association condition posterior probability Discriminant convergence Predict feature state Predict motion state E Step M Step Prediction of c th ~ath frames Prediction of Prediction of a th ~bth frames a th ~bth frames though the classical multi-target association method directly processes the associated data, it does not form a closed-loop structure; rather, the information flows in the observation-target and target-track associations are unidirectional, meaning that the former cannot obtain the a priori information fed back by the latter. When the numbers of false alarms and missed detections are significant, the observationtarget association will largely deviate, decreasing the accuracy of the target-parameter estimation. These errors will accumulate over time and the target-track correlation process will eventually fail.']</t>
         </is>
       </c>
-      <c r="AF28" t="inlineStr"/>
+      <c r="AF28" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article does not mention DenseNet classification model or its architecture with multiple blocks and feature map propagation, which is the claim made in the citation statement. The excerpts provided focus on radar target detection, tracking, imaging, and recognition, and discuss various signal processing algorithms and techniques, but do not mention DenseNet or any related concepts."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -4761,7 +4942,14 @@
           <t>["Visual sensing automation used vehicular networking with sensors. The emergence of 'sensor on wheels' in-car brings the additional features to driver-assisted systems integrated in present-day vehicle designs  (Manapragada and Kluesing 2014) . Welding is a thermal processing method; sensing using infra-red (IR) thermal image and camera are most extensively employed for monitoring and control of the welding process  (Chandrasekhar et al. 2015) . Based on advanced technologies such as data communication techniques, sensor networks, and radiofrequency identification, it is then presented in  Liu et al. (2017) . Figure  1  shows the illustration of the image transmission process through the wireless channel. During image acquisition, the received signal needs to be reformatted to obtain the original image transmitted, but this signal would also include redundant information  (Karakus et al. 2013) . Hence, a precise compression technique required to remove such unnecessary data from input signals. Signals are represented as a sparse or compressible form across various domains  (Zhang et al. 2012) .", 'from the image pixel P i = a i , b i , c i , … , z i and construct the random measurable for i given by where P i = (P i ) T are the predictor features variables, x i are the responses, and τ, υ are the recovering parameters for predic- tion accuracy and interpretability. The module determines a sub-set of the covariates (Eq. 4) to accomplish both of these objectives by driving the aggregate of the absolute estimation of the relapse coefficients to be a lower sum than a fixed worth that stimulates specific coefficients to be set to zero. By selecting these coefficients with prediction accuracy and interpreting the parameters, the random variables can be easily identified and reconstructed in the final stage. To protect these variables from the various cipher attacks, the need for encryption mechanism which explained in the following section. Step 3 Construction of the security matrix The security matrix having a 2-D discrete-time dynamical system obtained from the Eq.', 'Wireless channel is random and having multiple reflectors in the environment that leads in fading. Multiple reflections generate multiple paths for a visual signal transmission from the transmitter to the receiver termed as multipath propagation  (Watteyne et al. 2010) . Multipath propagation results a high fluctuations in the phase and amplitude of the signal. Hence modulating the signal is an essential need while transmitting into the channel. Interleaving techniques are essential to combat the effect of bursty errors due to fading, interference and multipath propagation in wireless communication  (Kohno et al. 1995) . By using linear minimum mean square error (LMMSE) equalization at the receiver, the system analyzed by using helical and chaotic Image Acquistation (Pre-processing) Image Formatting transmitter Wireless Channel\n\nImage deformatting Output Image\n\n\nFig. 2 Image transmission using the CS technique\n\n\nInput Image\nImage Acquistation (Pre-processing)\n\nImage Formatting transmitter Wireless Channel\n\n\nImage deformatting Post processing Output Image\n\n\nCompressive Sensing(CS)\n\n\nReconstruction of CS\ninterleaving  (El-Bakary et al. 2013) .']</t>
         </is>
       </c>
-      <c r="AF29" t="inlineStr"/>
+      <c r="AF29" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article does not mention converting texts to lowercase, removing URLs, or using RegEx expressions for text pre-processing. The article focuses on image transmission and compression in visual sensor networks, which is unrelated to the cited statement about text processing."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -4916,7 +5104,15 @@
           <t>['Introduction\nDegree of compression, distortion size, when images are downloaded from the web  (Mahesh et al., 2016; Stolfo, 1997; Talukder and Harada, 2010) , are some of the aspects to note. Compression leads to deterioration of the image content, so pre-processing approaches such as optimization, segmentation and representation need to be performed to address these consistency-based issues  (Oh and Lei, 2012) . Once preprocessed, the image gets formatted through various techniques, resulting under digital form. These digital signals consume large space and more time when it moves through a wireless channel  (Yang et al., 2016) . The following Figure  1  shows the image transmission process through the channel. The prepared sign should be reformatted during image handling to get the first transmitted image, yet this sign will likewise give repetitive data  (Manapragada and Kluesing, 2014) . It is additionally imperative to give an appropriate pressure procedure to take out such repetitive information  (Qaisar et al., 2013) .', 'The savvy module would likewise diminish the requirement for new sifting techniques, which ingest additional time, here. The Corvus corone module gives improved vitality effective and stable two-way image transmission through its quantization procedure along assurance and the transmission organize. The framework regard this research summed up as follows. Section 2 arrangements along related exploration works. Section 3 talked about the proposed technique. Section 4 examined about the outcome and execution assessment of this exploration and end under Section 5.  Liao et al. (2017)  introduced another strategy for detachable data stowing ceaselessly under mixed pictures using CS and discrete Fourier change. As exhibited through that framework, CS used just to pack and encode the parts containing the puzzle message under the wake of hiding the mystery message. The estimation number for CS entertainment decreases monotonically along the decrease of weight rate. To keep the picture not sensationally expanded, the weight rate must be a little respect. Under this manner, along the diminishing of the estimation number for CS diversion, it is unimaginable to totally address implanted data and recoup exceptional picture.  Ahmad et al.', 'Under equation (  4 ), the module select just a subset of the gave covariates to accomplish both of these objectives through constraining the whole of the outright estimation of the relapse coefficients to be not exactly a fixed worth, which powers certain coefficients to be set to zero, viably picking a less complex model that does exclude those coefficients. X N i¼1 1 N P i ¼ 1; X N i¼1 1 N P i 2 ¼ 0: Through choosing these coefficients along expectation precision and decipher the parameters, the arbitrary factors can be effortlessly recognized and reproduced under the last stage. To shield these factors from the different figure assaults, the requirement for the encryption is emerging that can be clarified under the accompanying procedure.']</t>
         </is>
       </c>
-      <c r="AF30" t="inlineStr"/>
+      <c r="AF30" t="inlineStr">
+        <is>
+          <t>Here is my evaluation:
+{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article does not mention converting texts to lowercase or removing URLs using a RegEx expression in Python. The article focuses on image transmission, compression, and security in wireless sensor networks, which is unrelated to the citation statement about text pre-processing."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -5067,7 +5263,14 @@
           <t>['The evaluation and comparison results paraded that the proposed module achieves the process within 1.42 s along an enhanced channel capacity of 96.684 and leads to the less BER value of 0.0003 compared to the other techniques respectively.', 'Figure  3  shows the proposed two-way helpful image transmission model. In addition, the dispersion and dispersion of a Tughlaq property in a booby ringer is used as a planning condition in quantization, claiming to see only those familiar along the language of the pixies so that the image bits. Image attackers later provide high security to image bits. To send these pieces along bending without a signal, at that point, the idea of modulation for broadcasting in the MIMO channel needs to be met, which is allowed to arrive in the full-duplex channel that communicates in two ways. The additive white Gaussian noise (AWGN) is added when communicating through the channel, so it can be properly squeezed into the remaking stage to retrieve the first encoded bits. Appropriately, in this proposed module, the use of mid-rate bit coding of modulation can reproduce the first fragments along their clock property through realizing the state of the first pieces and the paired clutter state. As a result, clever modules will reduce the need for new separation strategies, which burn along extra time, here.', "For that Manchester's clock recovery is used to decode the original signal. Then the random variable that is selected at the initial stage is recovered using the forecasting and integrality function of the regression theory (Figs.  13, 14) . After decrypting the random variables through the chaotic values of the tinkering bell would result in the below Fig.  15 . The outcome of the original image after reshaping the obtained value is shown through the Fig.  16 . Fig. 16 Receveid output images From Fig.  16 , it is proved that using the proposed Corvus Coron module, the input image that is transmitted through the user through a two-way communication channel receives less energy, is safer and encapsulates less energy and Finally reconstructs the output image. The input image is then evaluated seven parameters to evaluate the performance results of the proposed module as shown below.\n\nPerformance Analysis\nThis section presents the performance evaluation proposed approach in various parameters like PSNR (Peak to Signal Noise Ratio), SNR (Signal to Noise Ratio), Channel Capacity, BER (Bit Error Rate), Time, etc."]</t>
         </is>
       </c>
-      <c r="AF31" t="inlineStr"/>
+      <c r="AF31" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article does not mention a hybrid-based fake news detection model or any related concepts. Instead, it focuses on two-way image transmission using the Corvus Coron module over Wireless Sensor Networks (WSN). The abstract and excerpts provided do not support the citation statement from the citing article."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -5215,7 +5418,14 @@
           <t>['The total number of offensive and defensive resources S A and S D are two key factors affecting the level of system vulnerability during the game phase. The sensitivity analysis of them is shown in Fig.  9 . The simulation results and the analysis conclusions of this section can help guide the CPS defenders of the distribution network with distributed collaborative control mode and choose how to invest the appropriate amount of defense resources according to the CPS attack and defense environment. In the game phase, in addition to the influencing factors of the network attack and defense, the dynamic convergence process of the distributed collaborative control itself will also affect the system vulnerability assessment results. The following is a description of the influence mechanism through the simulation example and then the sensitivity analysis.  The simulation analysis of the impact of network attack time and control scheduling commands on the vulnerability of distribution network CPS. The simulation results are shown in Fig.  10 , where the scheduling ratio is defined as the ratio of the reference power P ref to the maximum allowable output of the VPP, which shows that the VPP dynamically adjusts according to each control scheduling command, and the attack and defense game is performed at each moment.', 'In this article, it was named as time-dependent detection. The other type was cross validation through the correlation between the different sensors of the system to achieve the purpose of detection. This article named it space-dependent detection.\n\nB. Time-Dependent and Spatially Correlated Detection Models\nThe main members of the steel product traceability system include steel companies, distribution, product users, quality regulators, etc. The information of the steel enterprise includes the registration information of the enterprise, the raw material composition of the product, the production process data of the product, the product quality data, etc. The information of the distribution includes the batch, packaging, and the logistics date, etc. The information on the product user includes the required product category, use, quality traceability, etc. As a result, a part of the data relationship between the product manufacturing chain and the supply chain is shown in Fig.  2 , and when a problem occurs at a node, the impact can be traced back or up along the data relationship network to improve the product supply and related dispute resolution efficiency. At present, the graph computing system generally adopts the node centered programming model or interface.', "Corresponding system vulnerability: It can be seen from the figure that in the process of VPP accepting a certain instruction P ref scheduling, the system vulnerability changes obviously at the beginning stage and gradually becomes fixed after a period of time; meanwhile, as the P ref increases, the system vulnerability gradually increases. Upgrade: This is because under the new scheduling command, each DG will initially adjust its own output quickly, and P ref is positively correlated with the value of the scheduling command. According to this, the grid defender can prearm according to the VPP scheduling situation and reasonably plan the investment timing of the defense resources according to the vulnerability of the system. It can be seen that the control system has strong fault tolerance under a certain (structure and size) parameter perturbation and maintains the system's strong defensiveness. According to the different definitions of performance, it can be divided into stable robustness and performance robustness. The defense robustness obtained in this article not only has its own stable robustness but also has the performance robustness.\n\nIV. CONCLUSION\nIn this article, the reliability of CPS was studied, and an automatic online evaluation method of CPS reliability based on machine learning was proposed."]</t>
         </is>
       </c>
-      <c r="AF32" t="inlineStr"/>
+      <c r="AF32" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article does not mention dyslexia, children's reading abilities, or school success. The abstract and provided excerpts focus on industrial IoT systems, artificial intelligence, and cyber-physical systems, which are unrelated to the topic of the citation statement."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -5363,7 +5573,14 @@
           <t>["Introduction\nLife without internet has almost become impossible in the present day and age. The potential of internet is enormous and its growth has been reflected in the functioning of business models pertaining to education, entertainment, healthcare and all the various types of organizations around the world. However, use of internet in every sphere of human life has its own challenges. The most significant challenge deals with data security. Network intrusion is a situation of security breach due to unauthorized access in a computational network. The process of identifying the different types of intrusions in a network is performed by an intrusion detection system (IDS)  [1] . The attacks in the IDS can be categorized as Probe attack, DoS attack, R2L attack, U2R attack. In probe attack, the unauthorized personnel 'sniffs' the network and identifies the vulnerabilities of a particular target resource. As an example, the attacker can use an uncommon port number as the identification with other IP addresses to attack on different ports. The DoS attacks are targeted to make the network resources unavailable by flooding unnecessary data packets by the attacker.", 'Apart from the popular machine learning techniques extreme learning machine (ELM) and NSL knowledge discovery data mining have been identified as a standard for the evaluation of intrusion detection mechanisms in the network  [7] . Researchers have also implemented random forest classifier on the IDS dataset sample. Such approaches have helped in the experimentation of datasets and analysing effects of malicious attacks considering various perspectives and dimensions  [8] . It is well known that applications of machine learning has a successful track record of automatically detecting and classifying intrusions both at network and host level in the quickest time frame. However, it is also essential to consider the volatility and ever changing characteristics of the malicious attacks involving larger volumes of stake holders. This issue needs to be resolved providing scalability. Moreover, the available datasets require continuous updates based on the dynamic characteristics of malware attacks. Several researchers have suggested the implementation of deep learning models and deep neural networks (DNN) for the development of flexible and dynamic IDS that would be capable of efficiently detecting and classifying capricious network attacks  [9] [10] [11] .', 'The results of the DNN model reveal potential of high dimensional feature representation of the IDS data when fed into hidden layers in comparison to the other machine learning approaches. Based on the performance of the DNN model, the authors have proposed a scalable hybrid IDS-AlertNet system that would efficiently monitor network traffic and proactively send alert on cyber attacks. In coordination with the use of DNN, convolutional neural network algorithms have also been identified as an advanced and superior technology for extraction of features in an intrusion dataset for the classification purposes  [12] . There exists almost eleven datasets namely DARPA, KDD99, ISC2012 and ADFA13, which have been used for classification and analysis of intrusion datasets. However, most of these datasets fail to incorporate network traffic diversity, volume and versatility related information on malicious attacks. Moreover, there are cases of anonymous packet information, insufficient payload information, lack of features and metadata  [13] . The classical machine learning algorithms when applied to the biased public and biased datasets fail to yield accurate results making them impractical to be used in real-time situations. The authors hence have split the datasets in a disjoint fashion across multiple time scales for the purpose of training and testing of the ML model.']</t>
         </is>
       </c>
-      <c r="AF33" t="inlineStr"/>
+      <c r="AF33" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article (Reference Number: 3) does not mention dyslexic students, learning and reading abilities, or achievement levels in social life areas. Instead, it focuses on intrusion detection systems and a proposed hybrid PCA-firefly based XGBoost classification model for network security. The abstract and provided excerpts do not address the topic mentioned in the citation statement."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -5511,7 +5728,14 @@
           <t>["Table  3  compares the results when derived stress factors in the highest stressful time are classified as top 1 and top 3. As the first is stricter, the F1 results are 15.2% smaller than the latter, mainly due to a decrease in the recall by 9.56 points.\n\nEvaluation with the State-of-the-Art Approach to Personal Event Identification\nWhile there are no methods to recognizing young people with traumatic periods and challenging events in the research on the traumatic era, our linguistic system of stressors is similar to that of the state-of-the-art predictive approach to the recognition of personal life events Table  4 . It analyzes the stressor incidents found that the overall traumatic times (not restricted to the aspect of the school life). It counts the number of instances of any stressor overall observed cumulative stress times for each student and measures their occurrence rate by the amount / overall stressful duration. Table  5  indicates the total student event rates of grades. The highest stressors among both classes are self-awareness and school life. This is consistent with the migrant children's psychological study and leads to problems with the inner cognitions of migrant children in school lives.", '1  General structure of stress analysis be most readily overlooked while the evaluation and prevention activities take place  (Marsac et al. 2014) . PTSS work for childhood injuries typically explores separation predictors, sometimes ignoring possibly significant experiences. This paper presents a new framework that utilizes the Bio-Psycho-Social System (BPSS) and reflects on emergency care incidents peri trauma processes. Knowing the connections between bio-psycho-social factors during peripheral trauma that inform the early detection of risky children, prevention measures and clinical care. Recommendations for further studies are addressed, including the need for the analysis of PTSS in the sense of many causes. Throughout their everyday lives, school-age children experience a lot of tension, which can trigger psychological and physical difficulties  (White 2012) . Stress Management focused on awareness is an adult awareness-centered system of practices successful. This research aimed to evaluate the effectiveness of awareness training with schoolgirls in yoga to reduce the experience of tension, to improve coping skills, self-esteem and self-regulation. Students in grades four and five have been selected and selectively allocated to participation and waitlist monitoring classes from two high schools.', "Table  1  mentions several common events, their duration, the frequency of student performance assessment and the overall frequencies in the observed 3 years. As these activities are regular and graduation, students in the same grade have the same experiences each year as in previous years. Through month on average there will be 2-stressor activities for every student school.\n\nPosting Behaviour\nIt recognizes 124 students who are Tencent Weibo superiors (registered in Taicang Senior High School before 1 January 2012) that have published more than 100 entries in the microblog. Each student is anonymous, and every post is accessible. A total of 29,232 posts have been written between 1 January 2012 and 1 February 2015. The average number for postal services is 236, a maximum of 1387 and a minimum of 104. In each school, Table  2  displays the number of active students over 3 years, students 'roles and stressor activities. The number of users, communications and stress events involved in user research is provided in Table  2 ."]</t>
         </is>
       </c>
-      <c r="AF34" t="inlineStr"/>
+      <c r="AF34" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article does not support the statement that direct support from teachers for dyslexic students is limited. The article actually focuses on recognizing stressful periods and events of urban migrant children, analyzing their microblog posts to detect stressors, and developing a model to study postings during stressful activities in schools. There is no mention of dyslexia or teacher support."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -5659,7 +5883,14 @@
           <t>["Under the trend of artificial intelligence, the communication between human and computer becomes easier and easier. Therefore, vigorously promoting the research of facial expression recognition technology is of great value to the development of individuals and society  [8] ,  [9] . The facial expression recognition is a technology which uses computer as an assistant tool and combines it with specific algorithms to judge the inner emotion of the human face expression. The facial expression recognition is also applied to the medical field. To know the effect of new antidepressants, more accurate drug evaluation can be made according to the daily record of patients' facial expressions. In the treatment of autistic children, facial expression recognition can be used to help interpret the emotions of  VOLUME 7, 2019  This work is licensed under a Creative Commons Attribution 4.0 License. For more information, see  http://creativecommons.org/licenses/by/4.0/  autistic children and help doctors understand themselves. Psychological changes in autistic children, so as to develop more accurate treatment programs  [10] .", 'I. INTRODUCTION\nHuman-computer interaction technology refers to a kind of technology which takes computer equipment as the medium, so as to realize the interaction between human and computer. In the recent years, with the rapid development of pattern recognition and artificial intelligence, more and more research has been conducted in the field of human-computer interaction technology  [1] ,  [2] . The facial expression recognition, as an important means of intelligent human-computer interaction, has a broad application background. It has been applied in the fields of assistant medicine, distance education, interactive games and public security  [3] -  [5] . The facial expression recognition extracts the information representing the facial expression features from the original input facial expression images through computer image The associate editor coordinating the review of this manuscript and approving it for publication was Yongtao Hao. processing technology, and classifies the facial expression features according to human emotional expression, such as happiness, surprise, aversion and neutrality  [6] ,  [7] . The facial expression recognition plays an important role in the research of emotional quantification. Under the trend of artificial intelligence, the communication between human and computer becomes easier and easier.', "The application of facial expression recognition in teaching field can enable the teaching system to capture and record students' emotional changes in learning, and provide better reference for teachers to teach students in accordance with their aptitude. The application of facial expression recognition in traffic field can be used to judge the fatigue state of pilots or drivers, and to avoid the occurrence of traffic hazards by technical means. Applying facial expression recognition to daily life, life management robots can understand people's mental state and intention according to facial expression recognition, and then make appropriate responses, thus enhancing the experience of human-computer interaction. In the recent years, the development of facial expression recognition technologies has been rapid and many scholars have contributed to the development of facial expression recognition  [11] ,  [12] . Among them, the Massachusetts Institute of Technology Media Laboratory and Japan's Art Media Information Science Laboratory are representative. The research of expression recognition in computer field mainly focuses on the feature extraction and feature classification. The so-called feature extraction refers to extracting features that can be used for classification from input pictures or video streams  [13] ,  [14] . There are many methods of feature extraction."]</t>
         </is>
       </c>
-      <c r="AF35" t="inlineStr"/>
+      <c r="AF35" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article does not support the statement about AI-based E-learning being a crucial platform for dyslexic students. The article is focused on facial expression recognition using convolutional neural networks and image edge computing, with no mention of e-learning or dyslexia."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -5807,7 +6038,14 @@
           <t>["Several DLbased techniques are designed to examine the retinal fundus images and to develop automated Computer-Aided Diagnosis (CAD) models for DR  [8] [9] [10] [11] [12] [13] [14] [15] [16] [17] [18] [19] [20] [21] [22] . A novel technology was designed in the literature  [8]  to determine the disease intensity under cloud and IoT applications. This technique was applied to predict the seriousness of the illness. The above technology was deployed to take unique care of student's and children's health. In this study, a programmatic health information, termed as student data, was created with the help of reputed UCI Repository as well as sensors employed in medical domain. This was deployed also to forecast diverse ailments which have been influenced by student with severity. Followed by, several other classification models were applied to predict different types of diseases. The major application of this algorithm is the determination of prediction accuracy using few attributes like F-measure, specificity as well as sensitivity. Consequently, it is evident that the presented technique outperformed with respect to prediction accuracy when compared with previous methodologies.", 'Kakria et al.  [18]  employed a novel online health care observation technology to monitor the remote heart patients often using mobile phones and wearable sensors. Subsequently, Kim et al.  [19]  established a technique to monitor the emergency scenario under the application of content of motion tracking disease patients. Some other models are also found in Jebaseeli et al.  [20] . Roychowdhury et al.  [21]  developed a new DREAM: Diabetic Retinopathy Analysis Using Machine Learning model which investigates the fundus images with varying illumination and fields of view. The severity level of DR can be generated by the use of ML models such as Gaussian Mixture model (GMM), k-nearest neighbor (kNN), support vector machine (SVM), and AdaBoost. Among the classifiers, GMM and kNN are found to be effective while classifying bright and red lesions respectively. Adal et al.  [22]  has developed a robust and flexible method to automatically detect the longitudinal retinal modifications because of small red lesions through the utilization of the normalized fundus images. It reduces the illumination differences and enhances the contrast level of small retinal features.', 'Hence, the variables associated with these normal distributions could be derived using, m X l jC¼c ¼ 1 N c X N c l¼1 x l (21) s 2 X l jC¼c ¼ 1 N c X N c l¼1 x l 2 Àm 2 (22) where N c denotes the count of instance where C ¼ c whereas N represents the number of overall examples applied in training. By estimating P C ¼ c ð Þ for every class, it becomes simple by applying relevant frequencies in the form of, P C ¼ c ð Þ¼ N c N (23) Finally, the classifier outcome by the proposed model is notified to the user using the cloud database server and smart phones.\n\nPerformance Validation\n\n\nDataset Description\nFor experimentation purposes, a benchmark MESSIDOR DR Dataset was used which had a total of 1,200 color fundus images with annotations in Excel file  [24] . The details related to the dataset is shown in the Tab. 1 and the images can be graded into different levels namely level 1, level 2 and level 3. Fig.']</t>
         </is>
       </c>
-      <c r="AF36" t="inlineStr"/>
+      <c r="AF36" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article does not mention E-learning resources or their development for regular students' capabilities and needs. The abstract and excerpts focus on an IoT-Cloud based intelligent computer-aided diagnosis of Diabetic Retinopathy using deep learning, which is unrelated to the citation statement."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -5955,7 +6193,14 @@
           <t>['We define , xy n f as: , ( ),( ) x y x y n ff \uf061\uf062 \uf02b\uf02b \uf03d Where \uf061 and \uf062 are the constant having the values either D \uf02b or D \uf02d depending upon the value of n as, 0, -D 1 -D, 0 2 , 0, +D 3 +D, 0 4 n n n n \uf061\uf062 \uf03d \uf0ec \uf0ef \uf03d \uf0ef \uf03d \uf0ed \uf03d \uf0ef \uf0ef \uf03d \uf0ee We used three directions (clock wise 0 \uf061 \uf03d , diagonal 1 \uf061 \uf03d and anticlockwise 2 \uf061 \uf03d ) to encode the relationship of each diagonal from , ij n Q for find the local diagonal maxima and minima. Figure 2 (b) depicts the first order adjacent derivatives for \uf061 \uf03d 0, 1 and 2 respectively.', 'To facilitate high performance classification, in this paper, we used only adjacent neighbours because it reduces the dimension of the descriptor and contain most of the local edge information. The remaining sections of this research paper include, section 2 proposes a descriptor based fingerprint classification model using local adjacent extrema pattern. Section 3 describes about SVM. 1234567890 14th ICSET-2017 IOP Publishing IOP Conf. Series: Materials Science and Engineering 263 (2017) 042143 doi:10.1088/1757-899X/263/4/042143 Section 4 presents classification results and performance analysis. Finally, Section 5 concludes the paper.\n\nLocal Adjacent Extrema Pattern\nLocal adjacent extrema pattern has derived as a new feature descriptor for fingerprint classification form center pixel and its local neighbours. The first order local adjacent derivative is used to extract the local adjacent extrema (maxima and minima) pattern. The connection of local adjacent extrema with the center pixel plays a major role to encode the LAEP descriptor. Local adjacent extrema are extracted of any center pixel by using first order local adjacent derivatives.', 'Local adjacent extrema are extracted of any center pixel by using first order local adjacent derivatives. , ij LAEP pattern for center pixel , ij Q Let , ij Q be the center pixel and its corresponding th n diagonal neighbours , ij n Q at a distance D , where [1,4] n\uf0ce and , ij Q is the pixel at th i row and th j column of any gray scaled image M having 1 m rows and 2 m columns. Let , ij n I and , ij I be the intensity value of , ij n Q and , ij Q respectively as shown in Figure 2(a).']</t>
         </is>
       </c>
-      <c r="AF37" t="inlineStr"/>
+      <c r="AF37" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article does not mention dyslexia or any related hypotheses, instead focusing on fingerprint image classification using a Local Adjacent Extrema Pattern (LAEP) descriptor. The abstract and provided excerpts do not provide any support for the statement about interpreting adaptation information based on cutting-edge dyslexia hypotheses."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -6103,7 +6348,14 @@
           <t>['From the analysis, it is known that the implemented ADCHS technique is 20% better than both the ACHS and FACHS methods. Figure  7  shows the statistical analysis of the implemented ADCHS algorithm and conventional ACHS and FACHS algorithms, by considering the CH count that is selected at each particular round. In the final round 2000, a sum of 10 CHs is selected in the implemented ADCHS algorithm. The figure legibly exposes the statement that the count of CHs that is chosen with the implemented ADCHS algorithm goes beyond the traditional ACHS and FACHS algorithms.\n\nCHS performance\nThe bar chart for the contrast of the traditional FACHS and ACHS algorithms and the implemented ADCHS algorithm by means of the distance among CHs is revealed in Figure  8 . A node is converted to a CH merely when the associates belonging to a certain cluster display the lowest distance with the CH. In the implemented ADCHS algorithm, the distance among the CHs is less than that of the traditional techniques. Figure  9  illustrates the distance among the alive nodes of the traditional and implemented methods.', 'Figure  4  demonstrates the convergence graph concerning the number of iterations. From Figure  4 , the convergence analysis for the proposed ADCHS method concerning the number of iteration is 8.3% better than the ACHS method and 2.7% better than the FACHS method. Thus, the capability of the proposed ADCHS method is proved to be better when compared with the existing methods: % ð Þ=\n\nCost function of the implemented technique À Cost function of the conventional technique Cost function of the conventional technique ð20Þ\nThe iteration is continued until it attains at the dead node. From Figure  5 , the statistical analysis of the proposed ADCHS technique with respect to the number of nodes can be determined. From the analysis, it is known that the implemented method is 16.6% superior to the ACHS method and 22.2% superior to the FACHS technique. Hence, it is shown that the proposed ADCHS method offers an increased number of alive nodes with an  increase in the number of nodes. Similarly, from Figure  6 , the normalized network energy in terms of the number of rounds is obtained.', 'Thus, the capability of the proposed ADCHS algorithm is verified. Table  6  summarizes the analysis on alive nodes and normalized network energy by varying the limits of the scout bee size for population size 25.\n\nConclusion\nIn a WSN, choosing and optimally positioning the CH is the main feature. CH routing is executed between the base    station and the sensor node for data interaction. A principle dynamic scout bee (DS) has been incorporated along with the ACHS technique to produce several scout bee solutions for choosing the CH that signifies the WSN. The presentation demonstrated by the implemented ADCHS method has been verified with the two major factors of routing methods, energy and distance. The results acquired following the testing of the implemented ADCHS technique have been distinguished with the ACHS and FACHS techniques by means of the number of alive nodes and energy in network. The implemented ADCHS technique has been established to offer less consumption of energy, along with an increase in the number of alive nodes at every iteration compared with the conventional ACHS and FACHS algorithms.']</t>
         </is>
       </c>
-      <c r="AF38" t="inlineStr"/>
+      <c r="AF38" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article does not mention analyzing the productivity of reading skills in students, nor does it discuss dyslexia. The content focuses on optimizing cluster head selection for energy-efficient sensor routing using Artificial Bee Colony algorithms, which is unrelated to the citation statement."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -6251,7 +6503,14 @@
           <t>["As technological solutions contributing to the development of a sustainable environment may allow progressive socioeconomic changes for environmental sustainability  (Cazorla-Montero et al., 2019; Bazan-Krzywoszańska et al., 2019) . These traditionally established technical approaches for water management and sustainable practice often reflect standard water governance  (How et al., 2020) . The Sustainability Index (SI) analyses the efficiency of different water policies and the environment and the system's capacity to reduce its vulnerability using artificial intelligent techniques  (Prabakaran et al., 2019; Wang et al., 2019) . The index shows that the system has a higher adaptive capacity for a suggested policy that makes the system more ecological effective  (Goralski and Tan, 2020) . The sustainability index integrates performance standards that capture the basin's important and long-awaited sustainabilities  (Cernev and Fenner, 2020)  for environment management using AI  (Zhang et al., 2019) .", 'The rest of the paper is organized as follows: Section 1 and Section 2 discussed the introduction and related works on sustainable development of water environment based on ecological engineering intelligent planning. In Section 3, Adaptive Intelligent Dynamic Water Resource Planning (AIDWRP) has been proposed. In Section 4, the numerical results have been analyzed, and the consistency of the data is evaluated. Finally, Section 5 concludes the research paper with a future perspective.\n\nRelated works\nAjay Gajanan Bhave et al.  (Fritz et al., 2019)  introduced the Decision-Making Under uncertainty (DMUU) approach for water resource planning. A water supply model is satisfactorily optimized and validated with the observed streamflow. In model simulations, almost all conditions increased the potential to meet such performance metrics without adaptation. The change options partly compensate for the effects of change, and the sequence of choices in adaptation processes according to stakeholder priorities impacts metric fulfillment. Early emphasis on agricultural demand control increases robustness and trade-offs between intra-basin water quality and basin-wide water availability. They prove that the best balance between demand and water supply is prone to future uncertainty and changes. Qiang  Wang et al.', "The index allows it more comfortable to compare policies as the performance criteria for effective environmental planning and management  (Qian et al., 2019; Sachs et al., 2019) . Fig.  1  shows the sustainable water resource management and its impacts. As inferred from Fig.  1 . The current water availability needs an effective resource management solution to satisfy the supply and demand ratio based on the food cycle. The water demand is rising, and the river basin's water management challenges exceeded their carrying ability, contributing to clear inconsistencies between supply and demand due to climatic changes  (Abdo and Zeadally, 2020) . Local water conservation aims at creating resilience in towns and cities that are living, efficient, and safe. Evaluation of sustainable water resources management requires responsibility for the actual overhead expense of water management. Water resources management has to be responsible. Socio-economic and environmental dimensions that are also not readily expressed in the quantitative principles needed for comprehensive planning, decision making, monitoring, and assessment Evaluation models include potential environmental sustainability metrics, which are used in comparing management strategies in different organizations and ecosystems for site modeling analyses to help individual administrators and policymakers to measure progress towards sustainable practices."]</t>
         </is>
       </c>
-      <c r="AF39" t="inlineStr"/>
+      <c r="AF39" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article does not support the statement about Xiang et al. analyzing teachers' attitudes to dyslexia and its impact on teacher standards and students' academic success. The title, abstract, and provided excerpts are focused on urban water resource management using artificial intelligence techniques and do not mention dyslexia or education-related topics."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -6399,7 +6658,14 @@
           <t>["Since then, F(a, b; c; x) and its special cases and gen-eralizations have attracted attention of many researchers, and was studied deeply in various fields  [2, 5, 9, 11-18, 20, 22, 23, 26, 30, 31, 35-37, 40, 45, 46, 48] . A lot of geometrical and analytic properties, and inequalities of the Gaussian hypergeometric function have been obtained  [3, 6-8, 19, 29, 32, 34, 38, 49] . Recently, in order to investigate the Ramanujan's generalized modular equation in number theory, Landen inequalities, Ramanujan cubic transformation inequalities, and several other quadratic transformation inequalities for zero-balanced hypergeometric function have been proved in  [27, 28, 32, 39, 42] .", 'Moreover, very recently in  [33] , some Landen-type inequalities for a class of Gaussian hypergeometric function 2 F 1 (a, b; (a + b + 1)/2; x) (a, b &gt; 0), which can be viewed as a generalization of Landen identities of the complete elliptic integrals of the first kind F 1 2 , 1 2 ; 1; 4r (1 + r) 2 = (1 + r)F 1 2 , 1 2 ; 1; r 2 , have also been proved. As an application, the analogs of duplication inequalities for the generalized Grötzsch ring function with two parameters  [33]   μ a,b (r) = B(a, b) 2 F(a, b; (a + b + 1)/2; 1 -r 2 ) F(a, b; (a + b + 1)/2; r 2 ) , r ∈ (0, 1), (1.6) have been derived.', 'For instance, using the quadratic transformation formula  [24, (15.8.15) ,  (15.8.21) ] F 1 4 , 3 4 ; 1; 8r(1 + r) (1 + 3r) 2 = √ 1 + 3rF 1 4 , 3 4 ; 1; r 2 , (1.3) Wang and Chu  [32]  found the maximal regions of the (a, b)-plane in the first quadrant such that inequality F a, b; a + b; 8r(1 + r) (1 + 3r) 2 ≤ √ 1 + 3rF a, b; a + b; r 2 (1.4) or its reversed inequality F a, b; a + b; 8r(1 + r) (1 + 3r) 2 ≥ √ 1 + 3rF a, b; a + b; r 2 (1.5) holds for each r ∈ (0, 1).']</t>
         </is>
       </c>
-      <c r="AF40" t="inlineStr"/>
+      <c r="AF40" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article focuses on quadratic transformation inequalities for Gaussian hypergeometric function and its applications in number theory, while the citation statement is about recent developments in various fields having a significant impact on human health and life. There is no apparent connection between the topics discussed in the reference article and the claim made in the citation statement."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -6555,7 +6821,14 @@
           <t>['\uf6dc\uf63d\uf63c,\uf641\uf63f\uf6dc,\uf63f\uf639\uf63a,\uf641\uf63f\uf63ex -\uf6dc\uf641,\uf641\uf63d\uf63b,\uf63e\uf6dc\uf640,\uf63f\uf63e\uf63e,\uf63c\uf63f\uf63c.', '\uf63e\uf63e\uf63c,\uf63e\uf63b\uf63b,\uf639\uf6dc\uf640,\uf63f\uf641\uf63c,\uf640\uf63e\uf63cx \uf63d + \uf6dc\uf63f,\uf63f\uf6dc\uf640,\uf63a\uf63a\uf63d,\uf63d\uf63e\uf63e,\uf63c\uf63b\uf63f,\uf641\uf63d\uf63bx \uf63c + \uf640,\uf6dc\uf63a\uf639,\uf63a\uf63b\uf63a,\uf641\uf641\uf63f,\uf63f\uf63e\uf641,\uf63c\uf6dc\uf63ax \uf63b + \uf63a,\uf639\uf640\uf6dc,\uf63a\uf640\uf6dc,\uf6dc\uf63a\uf641,\uf641\uf63a\uf63f,\uf641\uf639\uf640x \uf63a + \uf6dc\uf63f\uf641,\uf6dc\uf63d\uf63c,', '\uf639\uf639\uf63d,\uf63d\uf641\uf63f,\uf63b\uf640\uf63b,\uf63a\uf63d\uf639x \uf641 + \uf63b,\uf641\uf63d\uf63c,\uf63e\uf6dc\uf641,\uf63e\uf641\uf6dc,\uf63f\uf639\uf639x \uf640 + \uf641,\uf640\uf639\uf639,\uf63b\uf63c\uf63e,\uf63e\uf63c\uf63a,\uf640\uf63d\uf63dx \uf63f + \uf6dc\uf63e,\uf639\uf63d\uf640,\uf640\uf639\uf640,\uf63d\uf63e\uf639,\uf639\uf640\uf63dx \uf63e + \uf6dc\uf63f,\uf63f\uf63b\uf6dc,\uf639\uf641\uf63a,\uf639\uf63d\uf641,\uf641\uf63a\uf63ex \uf63d + \uf6dc\uf63b,']</t>
         </is>
       </c>
-      <c r="AF41" t="inlineStr"/>
+      <c r="AF41" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article focuses on monotonicity properties of a function involving the psi function and its applications to bound the psi function and its derivatives. There is no mention or implication of any impact on human health or life, which is the claim in the citation statement related to this reference."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -6703,7 +6976,14 @@
           <t>['The accuracy of variants to identify severity of bug reports by using feature selection. From Tables  3 4 5 6 , it can be found that the performance of identifying severity of bug reports by using four FS and four IS approaches all works much better than the original experiment, except identifying severity of DS-E4 by four IS approaches. For example, as shown in Table  3  and  4 , the accuracy and F-measure of CHI with 70% as the ratio of the final number of words to identify severity of bug reports for DS-E1 is 0.79 and 0.79. And, the accuracy and F-measure of original bug reports to identify severity of bug reports for DS-E1 is 0.78 and 0.75. The average best performance of TABLE 4. The F-measure of variants to identify of bug reports by using feature selection. four feature selection (OneR, IG, CHI, RF) are better than four instance selection (CNN, MCS, ENN, ICF) approaches to identify the severity of bug reports.', 'High-dimension is caused by the bug reports are submitted by testers from all over the world, and for each tester, the understanding and natural language description of bugs are different, which could result in large-scale and low-quality bug reports in bug repositories  [1] . A number of problems may arise due to the large-scale and low-quality, such as extensive computation and a decline in predictive performance. Class imbalance occurs when the number of bug reports in one class (majority-class) is obviously more than the other class (minority-class). This problem is more prevalent in bug repository (such Eclipse, Mozilla, and GNOME), where the proportion of severe bug reports is relatively larger than nonsevere bug reports. The primary drawback of imbalanced dataset is that traditional classification algorithms tend to misclassify minority-class bug reports as majority-class bug reports. Some investigators have try to solve these problem  [9] ,  [17] -  [19] . For the high-dimension problem, Gao et al.  [17]  presents six filter-based feature ranking techniques to reduce the number of available software metrics. Xuan et al.', 'From the Tables  11  and  12 , we can get that, using RSMOTE with data reduction (FS→IS) to identify the severity of bug reports could not only balance the imbalance distribution of bug reports, but also reduce bug report dimension and the word dimension at the same time. There could reduce the impact of noise on identifying the severity of bug reports, while reducing reduce bug report dimension and the word dimension. RQ5. Can the multi-classifier fuzzy-integral with RSMOTE approach outperform state-of-the-art approaches? As discussed in regard to RQ4, RSMOTE with data reduction (FS→IS) can effectively improve the performance of identifying the severity of bug reports. in order to solve the random sampling uncertainty of RSMOTE, we use FC-FI approach to ensemble multi-RSMOTE. To better demonstrate the superiority of FC-FI approach, in this experiment, we compared the fusion of multi-RSMOTE with fuzzy integral approach with three classic classifier ensemble approaches: voting, bagging, and AdaBoost. In order to compare the performance of integrated methods, we use the balanced dataset obtained from RSMOTE approach.']</t>
         </is>
       </c>
-      <c r="AF42" t="inlineStr"/>
+      <c r="AF42" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article does not support the statement about coordination chemistry having a great latent capacity to provide compounds with multiple mechanisms associated with DNA binding, redox reactivity, and different geometries. The article actually discusses bug report classification, feature selection, and ensemble learning techniques for identifying severity of bug reports in software systems."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -6851,7 +7131,14 @@
           <t>['Introduction\nAn extensive amount of research has been focused on developing a viable, safe and efficient technique for hydrogen storage. Most importantly, various hydrogen storage materials, such as the light metal hydride and their complexes, have been extensively explored over the recent years. 1, 2 Among these materials, aluminium hydride (AlH 3 ) is one of the most promising candidates due to its high theoretical hydrogen storage capacity (10.08 wt. %) and low decomposition temperature (100-200 °С).  [3] [4] [5] [6] [7] [8]  Compared to other metal hydride or hydrogen storage materials, AlH 3 is an ideal candidate for a wide array of applications, such as solid rocket propellant and hydrogen-fuel cells.  [9] [10] [11]  Hence, several research groups have investigated the synthesis methods and hydrogenstorage performance of AlH 3 polymorphs.', 'This solid state mechanochemical method has also been adopted for use by other researchers to produce nanosized α-AlH 3 composite.  [27] [28] [29] [30] [31]  Because of its widespread use, it is evident that mechanochemical method is a valid and wellestablished method for the synthesis of nano-sized α-AlH 3 composite. However, it has been reported that the metallic Al forms during the room temperature ball milling, which can be partially attributed to the heterogeneity of solid-state reaction and leads to the decomposition of AlH 3 . Though the cryo-milling process has the potential to prevent the AlH 3 from dehydriding, the much lower temperature also raises technical challenges on large-scale production of α-AlH 3 . Ionic liquids (ILs) are considered as promising environmentfriendly solvents in organic synthesis and offer distinct advantages, such as non-flammability, low volatility, low toxicity and high thermal and chemical stability. 32, 33 ILs are also extremely important because they can be used as a solvent in catalyst-free reactions.', '21  Birke et al. have suggested that the mechanochemical method offers distinct economic benefits, such as a low energy of consumption and utilization of cost-effective reagents.  22  Moreover, it has been demonstrated by Tigineh et al. that the mechanochemical process is solvent-free and consumes less energy, which makes them greener and sustainable than the conventional solution-based processes.  23  Furthermore, Park et al. have demonstrated that the dry-nature of the mechanochemical method makes it compatible with the current push to greenchemistry alternatives by avoiding the use of expensive and hazardous organic solvents during the synthesis process.  24  Thus, this method is considered as a powerful tool to employ solid-state reactions for metal hydrides synthesis. Based on the drawbacks of above-mentioned wet chemical techniques, Brinks et al. have employed a mechanochemical method to synthesize AlH 3 .  14  It has been demonstrated that the AlH 3 /LiCl composite can be synthesized by a mechanically assisted reaction, between LiAlH 4 and AlCl 3 at room temperature and 77 K.  14  The reaction can be described by Eqn. (4).']</t>
         </is>
       </c>
-      <c r="AF43" t="inlineStr"/>
+      <c r="AF43" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article does not support the statement that metal complexes have been widely studied and potentially used in gene regulation, probing of DNA specific structures and interactions, and the design of therapeutic agents. The article actually discusses the mechanochemical synthesis of α-AlH3 nano-composites for hydrogen storage applications and does not mention gene regulation or therapeutic agents."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -6999,7 +7286,14 @@
           <t>['Introduction\nHydrogen, as a clean and renewable energy source, has received wide attention  [1] [2] [3] . However, the major obstacle for a widespread hydrogen utilization is the challenges in storage  [4] . The hydrogen storage technology includes gas storage, liquid storage and solid-state hydrogen storage method which is different from other storage technologies such as CO 2 adsorption and storage technology  [1, 5, 6] . Solidstate hydrogen storage methods offer advantages, such as the lower safety risk, over high-pressure and cryogenic approaches  [7] . Additionally, solid materials have excellent volumetric and gravitational storage capacities. Therefore, a lot of efforts have been undertaken in research and development of solid-state hydrogen storage materials as well as storage systems  [8] [9] [10] [11] [12] [13] [14] [15] [16] . Research of safe, recyclable and cheap hydrogen storage materials, such as the light metal hydrides and their complexes, is the focus of the most recent studies; however, several issues still remain unsolved  [4, [10] [11] [12] .', "To date, mechanochemical milling has been successfully used for the solid-state synthesis of AlH 3  [40, [60] [61] [62] [63] . Mechanochemical method for AlD 3 synthesis was employed by Brinks  [40] . AlD 3 mixture of various polymorphs was synthesized by mechanically-assisted reaction between LiAlD 4 and AlCl 3 at 77 K and room temperature (see Eq. (  4 ))  [36] . 3LiAlD 4(s) + AlCl 3(s) → 4AlD 3 +3LiCl (4) Lately, Paskevicius obtained a mixture of several polymorphs of AlH 3 (α-, α'-, and γ) by a mechanochemical reaction of LiAlH 4 and AlCl 3  [61] . The final crystalline size of AlH 3 was 15-17 nm.", "For example, Ma demonstrated that presence TiF 3 significantly enhanced dehydrogenation of MgH 2  [64] . Ismail confirmed catalytic role of Ti-containing compounds for performance of NaAlH 4 -TiF 3 system and promotes dehydrogenation of NaAlH 4  [65] . Balema  [66, 67]  recently demonstrated synthesis of Li 3 AlH 6 using solid state reaction at ambient temperatures, which proceeded faster with addition of TiCl 4 . Moreover, Sartori  [63]  added FeF 3 to the cryomilled LiAlD 4 /AlCl 3 mixture to accelerate nucleation of the as-milled product and alter its α/α'-AlH 3 ratio. This could be attributed to the isostructure between FeF 3 and α'-AlH 3 which may lead to larger amount of α'-AlH 3 in the as-milled product  [63] ."]</t>
         </is>
       </c>
-      <c r="AF44" t="inlineStr"/>
+      <c r="AF44" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article does not support the citation statement. The article discusses the synthesis and properties of alpha-aluminum hydride, a hydrogen storage material, and does not mention metal complexes or their applications in gene regulation, DNA probing, or therapeutic agents."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -7150,7 +7444,14 @@
           <t>['ID3 is one of the major algorithms of decision tree which was used in this study.\n\nBagging-ID3\nBagging (Bootstrap aggregating) is a popular approach proposed by Bremen  [24, 25]  which is considered as an ensemble meta-algorithm to build classification models. This resampling-based technique can be incorporated into various classification algorithms or regression methods. This incorporation resulted in reducing the variance associated with the prediction models, and thereby improves the predictive performance of these models. Bagging consists of creating numerous bootstrap replicates of the learning set by drawing "B" simple random samples with replacement (bootstrap samples) from the learning set and using these as new learning sets. Then, the considered prediction model is applied to each "B" bootstrap sample (i.e. new learning sets). To construct the final model, the results (i.e. the "B" built models) subsequently are combined into an ensemble by averaging for regression and simple voting for classification  [26] [27] [28] . In fact, the true strength of bagging approach is for unstable models, such as decision trees and neural networks. Unstable models are sensitive to small alterations in the dataset.', 'Thus, a tremendous performance from this classifier should not be expected.\n\nNaive Bayes\nApplying Naive Bayes classifier, each new sample is assigned to the most probable class based on the Bayes decision making. The probability functions of the classes are empirically estimated from the training data. In spite of the low computational complexity, this method has a relatively high performance  [20] .\n\nIterative dichotomiser-3\nDecision trees are powerful and effective approaches to create a classification model. This method is a flow-chart-like tree structure, where a tree is constructed by the "if-then" rules (i.e. A logical sequence of questions) extracted from the training data  [9, 21] . A new case can be classified by starting at the root of the tree and moving through it until a leaf is encountered. Decision trees have become one of the most widely applied methods among numerous classification approaches, because these are white box models with easy-to-interpret results. In addition, its construction does not need any domain knowledge or parameter setting and thus is appropriate for exploratory knowledge discovery  [22, 23] .', "Unstable models are sensitive to small alterations in the dataset. Hence, training the same model on two slightly different training sets might result in substantially different models (i.e. The models with different parameters similar overall accuracies)  [25, 29] . Thus, bagging can be a good solution to overcome this problem. In order to overcome unstably of the ID3, classifier bagging can be incorporated into the ID3 and emerge Bagging-ID3 classifier.\n\nFeature selection\nFeature selection is one of the important steps in a classification problem. In reality, there are usually many redundant features which do not have any contributions in discriminating classes. Moreover, redundant features increase the complexity of the classification algorithm. Thus, they may have an effect on the performance of the model and may decrease its accuracy as well. There are two main approaches for performing dimensionality reduction of high dimensional data  [18] . The first approach is feature extraction, which focuses on transforming the existing features into a lower dimensional space. Most feature extraction methods have been based on two major linear techniques: principal components analysis and Fisher's linear discriminant analysis  [16, 18] ."]</t>
         </is>
       </c>
-      <c r="AF45" t="inlineStr"/>
+      <c r="AF45" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article (2) does not support the statement that advances in molecular technology allow plant taxonomists to use molecular techniques for exploring plant groupings. The article is focused on applying pattern recognition tools for classifying acute coronary syndrome, with no mention of molecular technology or plant taxonomy."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -7301,7 +7602,14 @@
           <t>['Other review, case-control, cohort, and intervention studies were excluded from the list of articles. The studies were then reviewed based on fourphase PRISMA (2009. STROBE checklist was used to review studies. This checklist consists of various methodological aspects, including study objectives, determination of appropriate sample size, type of study, sampling method, research population, data collection method, definition of variables and procedure, study data collection tool, study objectives, statistical tests, and findings. Accordingly, a maximum quality evaluation score of 32 was considered and articles with scores below 14 were excluded from the study.\n\nStatistical analysis\nData were analyzed using Comprehensive Meta-analysis software (Biostat, Englewood, NJ, USA version 3), the heterogeneity of the studies was assessed using the I 2 test and probability of publication bias Funnel chart using Egger test and significance level 0.05 and also to investigate the effects of potential factors on heterogeneity of studies from Meta-regression test.', "Background\nOlder adult is an inevitable biological process that affects all living things and is associated with unpleasant experiences in some cases  [1] . The aging process refers to the gradual decline in the function of the body's systems, including cardiovascular, respiratory, genitourinary, endocrine glands, and immune system  [2] . Social, economic, and scientific developments in recent years have increased life expectancy and reduced mortality rates, leading to an increase in the world's older adult population  [3] . The older adult population is estimated to be doubled during next 40 years in the world  [4] . Today, aging has become a major global phenomenon and according to WHO statistics, the number of older adult in Southwest Asian countries, including Iran, will reach 15% of the total population by 2030  [5] . Other reports suggest that the number of people aged ≥60 years will increase from 841 million people in 2013 to 1.2 billion people in 2025, with 70% of them living in developing countries and 8 out of every 10 older adult people in the world are expected to live in developing areas by 2050  [6] .", 'The search process was carried out using the keywords Older adult, Depression, Mood Disorders, Types of Depression, Severe Depression and their English equivalents and their possible combinations, search engine using both English and Persian words and (AND) and (OR) operators were used in combination to provide more comprehensive access to all articles, therefore, the OR operator was used to check for common names for disorders such as (Older adult OR Aging), (depression OR Depressive Disorder), (mood disorders OR Affective Disorders). The AND operator was also used among the keywords (Older adult AND depression AND severe depression) by matching words in the MeSH browser.\n\nEvaluation of articles and quality control\nAll articles were first collected using the selected keywords and a list of abstracts was prepared after the search was completed. After hiding the article specifications, including the name of the magazine and the author, the full text of the articles was made available to the reviewers. Each article was studied independently by two reviewers and if the article was excluded, the reason was mentioned. Articles in Persian and English extracted from cross-sectional studies on the prevalence and of severe depression in Iranian older adult met the inclusion criteria.']</t>
         </is>
       </c>
-      <c r="AF46" t="inlineStr"/>
+      <c r="AF46" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article (3) does not support the statement 'Plant taxonomists may now use molecular techniques to explore plant groupings thanks to advances in molecular technology'. The article is actually about the prevalence of severe depression in Iranian older adults and does not mention molecular techniques, plant taxonomy, or any related topics."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -7449,7 +7757,14 @@
           <t>['As visits by large bees or empidines   Considering how frequently interactions between empidines and numerous flowering plant species have been reported in the literature since Darwin  [13, [26] [27] [28] [29] [30] [31] [32] [33] [34] [35] [36] , it is surprising that their role in the reproductive success of those plants had never been addressed. They are obligate floral-visitors with more than 2000 described species worldwide which, contrary to the commonly accepted assumptions that they are generalists and poor pollinators, could reveal high levels of specialization and the same pollination efficiency as bees. Their high abundance and diversity throughout the favourable season suggest that they are important pollinators in mountains and at high latitudes  [14] . Like empidine dance flies, numerous species of calliphorids, conopids, muscids, anthomyids, tabanids and many other fly families depend on nectar and pollen for feeding. In habitats where bees are unable to thrive, flies often represent the predominant biotic vector carrying pollen grains from one flower to another, and therefore the main potential pollinators. Competing interests.', 'Flies (Diptera) represent the most conspicuous group of flower-visitors and potential pollinators after bees  [5] [6] [7] , especially in cool to cold habitats of high altitude or latitude where wild bees become naturally scarcer  [8] [9] [10] [11] [12] [13] [14] . However, most studies including dipterans address only flower visitation frequencies, which King et al.  [15]  consider a poor proxy for pollinator effectiveness. Visitors are indeed not always pollinators, a visit being likely to enhance the reproductive success of a plant only when it results in conspecific pollen deposition on its stigma. Therefore, direct measures of pollinator effectiveness and plant reproductive success should be performed, respectively, through single-visit stigmatic pollen deposition and seed set after single-visit experiments  [16, 17] . To our knowledge, very few studies include such experiments on flower-visiting Diptera, although some of them challenge the common assumption that bees are the best pollinators: e.g.', 'hoverflies can pollinate strawberries as efficiently as bees  [18] , and a blowfly (Calliphoridae) was shown to be as efficient as honeybees and other flower-visitors together in pollinating hybrid carrots  [19] . Moreover, the first study comparing syrphids with other Diptera found no differences in pollen-loads or specialization  [20] . Those results cast light on the lack of knowledge about the role played by most flower-visiting fly families in the pollination of angiosperms. To assess the effectiveness of dipterans as pollinators of a wild plant relative to other foraging insects, we used Geranium sylvaticum L. and its flower-visitors as a model, in a subalpine environment where wild bees are scarce. Our objectives were: (i) to quantify the visitor cortege of G. sylvaticum; (ii) to assess the pollination effectiveness of the main flower-visitors using single-visit seed set experiments; (iii) to test whether pollination effectiveness was related to species identity or species traits, such as body size and visit duration.']</t>
         </is>
       </c>
-      <c r="AF47" t="inlineStr"/>
+      <c r="AF47" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article discusses the pollination effectiveness of empidine dance flies and bees on Geranium sylvaticum, but does not provide information on Rindera members or honeybees as pollinators. The citation statement mentions specific types of pollinators (honeybees) and plants (Rindera members), which are not addressed in the reference article."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -7597,7 +7912,16 @@
           <t>["Kearns (1990)  inferred that G. richardsonii was self-incompatible or required a minimum threshold quantity of pollen for successful self-fertilization based on a limited number of hand crosses. Recent hand pollination experiments (K. O'Malley, C. Williams, and M. Kuchenreuther, unpublished data) have shown that G. richardsonii does self and suffers inbreeding depression in fruit and seed set. Although autogamy appears rare in G. richardsonii, because of its large, asynchronous floral display, geitonogamy may contribute significantly to selfing in this species. We estimated the proportion of pollen received from geitonogamy as the difference in pollen receipt on stigmas of emasculated target flowers on emasculated (E) and unemasculated (U) plants in the geitonogamy experiment. In 1997 there was 19% and in 1998 42% more pollen received by flowers on unemasculated plants. Therefore, although hermaphrodites do receive over two times more pollen than females (see above), most is geitonogamous self-pollen.", "These estimates also appear to reflect actual levels of selfing occurring in the field. Genetic estimates of selfing rates, including geitonogamy, in open-pollinated hermaphrodites  (Ritland and Jain, 1981)  from four populations of G. richardsonii at RMBL ranged from 51 to 67% (mean ϭ 61%) (K. O'Malley, C. Williams, and M. Kuchenreuther, unpublished data).  Agren and Willson (1991)  estimated that the selfing rates in two populations of Geranium maculatum were 60 and 73%, based on inbreeding depression. Similarly high selfing rates have been found in hermaphrodites of other gynodioecious species (23-25% in Limnanthes douglasii-  Kesseli and Jain, 1984; 11-76% in Bidens-Sun and Ganders, 1986; 18-61% in Salvia pratensis, Van Treuren et al., 1993; 88-100% in Chionographis japonica-Maki, 1993; .", 'Further studies of the magnitude of inbreeding depression on seed production and progeny fitness are in progress to determine how differences in pollination affect the relative fitness of females and hermaphrodites in this species. In addition, since the relative success of females at receiving pollen declines as their frequency in the population increases, selection opposing females may occur at high female frequencies due to pollen limitation. Understanding the maintenance of gynodioecy in G. richardsonii will depend on quantifying patterns of resource allocation, selfing rates, inbreeding depression, and pollen limitation in the context of the frequency of floral morphs. These studies are currently underway in natural populations of Geranium richardsonii spanning a wide range of floral morph frequencies.\n\nLITERATURE CITED']</t>
         </is>
       </c>
-      <c r="AF48" t="inlineStr"/>
+      <c r="AF48" t="inlineStr">
+        <is>
+          <t>Here is my evaluation:
+{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article discusses the relationship between pollination, self-fertilization, and gynodioecy in Geranium richardsonii, but does not mention Rindera or shared alleles related to self-pollination. The study focuses on the differences in resource allocation and selfing rates between female and hermaphroditic plants of G. richardsonii, which is a different species from Rindera."
+}
+Note that I only evaluated the portion of the citation statement corresponding to reference 1, and did not consider any other parts of the citing article or references.</t>
+        </is>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -7745,7 +8069,14 @@
           <t>['17  Interestingly, epigenetically dysregulated lncRNAs displayed substantially higher expression levels and lower expression variation compared with other lncRNAs in all three breast cancer subtypes (p &lt; 0.05). Consistently, we observed higher expression levels and lower expression variation of epigenetically dysregulated PCGs compared with other PCGs in the basal and claudin-low subtypes (p &lt; 0.05; Figure  S2B ). These results suggest that epigenetically dysregulated lncRNAs are stably expressed in breast cancer subtypes and may be suitable as potential biomarkers for breast cancer.  18  Epigenetically dysregulated lncRNAs at enhancer elements contributing to cancer subtype-specific functions The genomic distribution of epi-lncRNAs showed that abnormal histone modifications H3K27ac (47.91%), H3K4me3 (25.95%), and H3K4me1 (15.11%) within enhancers (77.77%) mainly contribute to dysregulation of lncRNAs in the basal subtype.', '15,16 859 (53.1%) and 27 (1.6%) epi-lncRNAs belonged to intergenic lncRNAs and overlapping lncRNAs, respectively. Structural analysis revealed that epigenetic-dysregulated overlapping lncRNAs had higher exon, intron. and isoform number, longer intron and gene length, and shorter exon length (p &lt; 0.05; Figure  S2A ). These results suggest that lncRNAs with complex splicing patterns are more likely regulated by aberrant epigenetic modifications. In addition, we compared the expression level and expression variation of epi-lncRNAs with other lncRNAs to characterize the expression pattern of epigenetically dysregulated lncRNAs. The coefficient of variation (CV) was used to assess expression variation of genes among patients with breast cancer. lncRNAs showed substantially lower expression levels than did PCGs in all three breast cancer subtypes, which has been described in previous studies.', 'RESULTS\nIdentifying epigenetically dysregulated lncRNAs and proteincoding genes (PCGs) in breast cancer subtypes Our goal was to analyze the relationship between lncRNA expression and epigenetic alterations in breast cancer subtypes. We focused on differentially expressed lncRNAs and looked for differences in three breast cancer subtypes compared with normal breast tissue or cell lines using DESeq2. 318 (2.50%), 2,493 (19.59%), and 3,414 (24.62%) lncRNAs were differentially expressed in luminal, basal, and claudin-low subtypes, respectively (false discovery rate [FDR] &lt; 0.05). We also identified 2,141 (11.54%), 7,582 (40.85%), and 9,851 (51.87%) differentially expressed PCGs in luminal, basal, and claudin-low subtypes, respectively. Epigenetic changes have been reported in a number of PCGs in breast cancer subtypes.  8  We hypothesized that aberrant epigenetic modifications might play a crucial role in regulating lncRNAs in breast cancer.']</t>
         </is>
       </c>
-      <c r="AF49" t="inlineStr"/>
+      <c r="AF49" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article does not mention anything about changes in environment leading to variation in genetic diversity levels among populations or the adaptability of populations with little variability. The article focuses on epigenetic alterations of long non-coding RNAs (lncRNAs) in breast cancer subtypes and their potential as prognostic biomarkers, which is unrelated to the statement being evaluated."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -7893,7 +8224,14 @@
           <t>['A lower mitochondrial volume is associated with the Warburg effect, which also contributes to tumor progression,  44  as well as being a critical metabolic characteristic of cell stemness restoration,  45  while both stemness maintenance and the Warburg effect contribute to sorafenib resistance.  46, 47  Another recent study  48  suggested that mitochondrial TXNRD3 confers drug resistance via a redox-mediated mechanism, further supporting the findings of our current study. In addition, the alterations of biological redox couples vary in different cell lines, suggesting a cell line-specific, but generally reductive reprogramming in sorafenib-resistant cells and OE-PGC1β cells, compared with their controls. Mitochondrial biogenesis is a complex process.  21  Mitochondrial biogenesis is regulated by the transcriptional family of PGC1, which is composed of PGC1α, PGC1-related coactivator, and PGC1β. These proteins interact with other transcription factors involved in mitochondrial gene expression to regulate genes encoding proteins Fig.  5  The role of UBQLN1 regulated PGC1β degradation in sorafenib resistance.', '20  Recently, mitochondrial biogenesis was shown to be tightly linked to ROS production.  21  Studies found that the upregulation of mitochondrial content resulted in higher ROS levels under stress.  22, 23  Whether mitochondrial biogenesis-mediated ROS levels play a role in sorafenib resistance in HCC remains to be determined. In this study, we found alleviated ROS responses in sorafenibresistant HCC cells due to decreased mitochondrial biogenesis. Mechanistic studies revealed that upregulation of UBQLN1 in sorafenib-resistant HCC cells expedited the proteasome-mediated protein degradation of peroxisome proliferator-activated receptor γ coactivator 1β (PGC1β), contributing to decreased mitochondrial biogenesis and ROS generation, finally inducing sorafenib resistance. These findings may provide a novel mechanism involving mitochondrial biogenesis and ROS homeostasis in sorafenib resistance, which may offer new therapeutic targets and strategies for HCC patients.\n\nRESULTS\n\n\nDecreased ROS levels in sorafenib-resistant HCC cells\nTo mimic the biological process of sorafenib resistance in HCC patients, an in vitro model was established in this study, as described previously.', '30  Mitochondria and cellular homeostasis are accurately coordinated by mitochondrial biogenesis and clearance. To elucidate the underlying mechanisms of the reduced mitochondrial content in resistant cells, we first evaluated mitochondria degradation. Mitophagy is a principle mechanism for mitochondria degradation and reduction of ROS stress.  31  We measured mitophagy levels in parental and resistant cells, and found that LC3II (reflects autophagic activity) levels were lower in resistant cells under sorafenib treatment, with or without chloroquine (a classic inhibitor of autophagy that alters the acidic environment of lysosomes thus blocks the binding of autophagosomes to lysosomes; Fig.  3a ,  b ). Moreover, levels of the mitophagy-specific markers PARKIN and PINK were also reduced in resistant cells (Fig.  3c ,  d ). Fluorescence imaging further revealed a lower autophagic flux in resistant cells than parental cells under sorafenib treatment (Fig.  3e ). These results indicated that mitophagy was decreased in resistant cells under sorafenib treatment, which is unlikely to explain the lower mitochondrial content in resistant cells.']</t>
         </is>
       </c>
-      <c r="AF50" t="inlineStr"/>
+      <c r="AF50" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article does not support the statement. It discusses sorafenib resistance and mitochondrial biogenesis in hepatocellular carcinoma, but does not mention genetic diversity levels or adaptation among populations. The topic is unrelated to the citing article's statement about environmental changes leading to variation in genetic diversity."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -8042,7 +8380,14 @@
           <t>['Although the structural design of LOGC cathodes could be further improved via optimization of the entire electrochemical system, this work could shed light on developing high-performance cathode materials for DIBs.', 'For the calculations, we search the global minimum of each phase by enumerating the anion intercalation stage, anion arrangement, and initial graphite layer distance. Therefore, the blue dots on the convex hull represent the most stable anion intercalation configurations at each PF 6 À content x, a species produced during the chargedischarge process. At x 0.5, we find at least three two-phase reactions upon anion intercalation into graphite, where the anion arrangement goes from stage VIII to IV to II. At x = 0.33, the formation energy of stage III is slightly above the convex hull, indicating a decomposition reaction into stage IV and II. While at 0.5 x 0.8, solid-solution reactions take place within stage II, until the final two-phase reaction between stage II and I at 0.8 x 1.', 'Developing cost-effective energy storage systems is pivotally important in the implementation of intermittent renewable energy sources (e.g., solar and wind). Although lithiumion batteries (LIBs) have been widely used in portable and automotive energy storage systems, the scarcity and uneven distribution of lithium element in Earths crust limit their large-scale applications. \n[1]  Non-lithium batteries such as sodium-ion batteries (SIBs),  [2]  potassium-ion batteries (KIBs),  [3]  and aluminum-ion batteries (AIBs),  [4]  therefore, have attracted increasing research interests. However, the search for cation-intercalating cathode materials for these non-lithium rocking-chair batteries is challenging due to the larger ionic radius (e.g., Na + and K + ) or higher charge density (e.g., Mg 2+ and Ca 2+ ) of post-lithium cations.']</t>
         </is>
       </c>
-      <c r="AF51" t="inlineStr"/>
+      <c r="AF51" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article does not mention allelic richness loss, population differentiation, genetic drift, or inbreeding depression. Instead, it focuses on the development of high-capacity dual-ion batteries and discusses topics related to energy storage systems."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -8190,7 +8535,16 @@
           <t>['v) PEs are more conducive to realizing high ionic conductivity for the transfer of Na + ions and K + ions at room temperature or even at low temperature than ISEs, due to the large ionic radii of active ions and different ion migration mechanism between PEs and ISEs.  [92]  vi) PEs also have some other merits of lightweight, high-volume utilization, and good film-forming ability.  [90]  To further improve the electrochemical properties of PEs, it is of significance to get fundamental insight into the migration mechanism and transfer kinetics of active ions in PEs. It is generally accepted that the Li + -ion migration in PEs is affected by the fracture/formation of coordination bonds in the segmented movement of polymer chains, which mainly occurs in the amorphous region of the polymer matrices.  [93]  For example, Li + ions first locate at the active site provided by the polar group of PEs (e.g., \ue0c6O\ue0c6 in PEO).', '2. High cation migration number (T + ≈ 1). The cation migration number is a measure of the cation mobility in the PEs relative to the anion.  [91]  Reverse movement of anions without being deposited on the electrodes can cause concentration polarization, which results in increased internal impedances and reduced discharge voltages. Single ion conductive PE is used to limit the anion and increase the cation conductivity by covalently binding the anion to the polymer chain or adding an anion acceptor.  [204]  Therefore, how to restrict the migration Reproduced with permission.  [179]  Copyright 2018, Wiley-VCH. d) Schematic illustration of the failure mechanism of the Sn anode in the liquid electrolyte and the protection mechanism of the gel PE. Reproduced with permission.  [203]  Copyright 2020, American Chemical Society. of anions in PEs is a key issue. However, note that different from in "rocking-chair" battery systems, in a DIB system, active ions include both cations and anions, which needs a comparable ion transfer kinetics for cations and anions. 3.', "Besides, previously reported studies on the transfer kinetics of Li + ions in PEs have shown that the smaller particle size of nanofillers is beneficial to allow faster transfer kinetics of cations.  [87]  However, the agglomeration of nanoscale oxides quickly takes place to form larger particles. In order to avoid the agglomeration, Wei's group  [114]  reported a carbon quantum dots (CQDs, 2.0-3.0 nm) with high dispersion by a simple synthesis method (the synthesis mechanism was schematically shown in Figure  5b ), and the addition of the CQDs endowed the PEObased SPE with an ionic conductivity of 7.2 × 10 -5 S cm -1 at ambient temperature. Such enhanced effect could be explained by that introducing smaller and more dispersed CQDs enhanced the dissociation of Na-salts, so that the crystal size of polymer was reduced and accompanied by the expanded amorphous region (Figure  5b )."]</t>
         </is>
       </c>
-      <c r="AF52" t="inlineStr"/>
+      <c r="AF52" t="inlineStr">
+        <is>
+          <t>Here is my evaluation:
+{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article does not mention allelic richness loss, population differentiation, genetic drift, or inbreeding depression. Instead, it discusses polymer electrolytes for sodium/potassium-ion batteries and their properties, mechanisms, and applications. The topic is unrelated to the citation statement."
+}
+Note that I only evaluated the portion of the citation statement corresponding to reference 7, which does not support the claim made in the citing article.</t>
+        </is>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -8338,7 +8692,14 @@
           <t>['These markers have been used in DNA fingerprinting, conservation biology, identification and determination of species relationships in many plants  [16, 17] . G. molle grows in different regions of Iran and comprises many local geographical populations. Therefore, the present study was performed for the first time in the country to investigate the genetic structure and diversity of these local populations. The results of present study may have positive effect on conservation strategy and future breeding of this medicinally important plant. We used ISSR molecular markers in the present study as these markers were shown to be informative for genetic diversity and population structure studies  [18] [19] [20] .\n\nMATERIALS AND METHODS\n\n\nPlant Materials\nFor morphometric studies we used 132 plant specimens (5-12 samples from each populations), and for ISSR analysis, we used 109. Different references were used for the correct identification of species (G. molle),  [4, 8, 10, 21, 22] . Details of sampling sites are mentioned (Table  1 , Fig.  1 ). Voucher specimens are deposited in Herbarium of Shahid Beheshti University (HSBU).', 'The populations, divergence may be accompanied by local adaptation. When we use multilocus molecular markers (such as SSR, AFLP, RAPD, ISSR, etc.) for population genetic studies we understand that these are neutral molecular markers (they are not directly acting as adaptive genes), but they may be linked to a gene or a genetic region with adaptive value  [26] . Therefore, combination of genetic divergence, limited gene flow and local adaptation have played role in diversification of G. molle population in the country. An ecotype is a distinct set of genotypes (or populations) within a species, resulting from adaptation to local environmental conditions, but which are capable of inter breeding with other ecotypes of the same species  [46] . Ecotypes are populations adapted to local conditions, at a variety of spatial and temporal scales. Creation of a ecotype is very important because this type of variation has adaptive value for each species and increases biodiversity in the ecosystems. Matching ecotypes to local conditions increases restoration success.', "The Mantel test was performe as implemented in PAST ver. 2.17  [23, 24] . For this, Nei genetic distance was determined for ISSR data, while Geographic distance of PAST was determined for geographical data. It is calculated based on the sum of the paired differences among both longitude as well as latitude coordinates of the studied populations. AMOVA (Analysis of molecular variance) test (with 1000 permutations) as implemented in GenAlex 6.4  [28]  and Nei,s Gst analysis as implemented in Geno-Dive ver.2 (2013)  [29]  were used to show genetic difference of the populations. Moreover, populations, genetic differentiation was studied by G'ST est = standardized measure of genetic differentiation  [30]  and D_est = Jost measure of differentiation  [31] . The genetic structure of populations was studied by Bayesian based model STRUCTURE analysis  [32]  and maximum likelihood-based method of K-Means clustering of GenoDive ver. 2. (2013). For STRUCTURE analysis, data were scored as dominant markers  [33] ."]</t>
         </is>
       </c>
-      <c r="AF53" t="inlineStr"/>
+      <c r="AF53" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Substantiated",
+  "explanation": "The reference article supports the use of ISSR in measuring genetic variation and relationships, which is a part of the statement. The abstract and excerpts mention the use of ISSR molecular markers to investigate genetic structure and diversity, and its effectiveness in population structure studies."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -8486,7 +8847,14 @@
           <t>['20  \n\nInfluence of JP on bacterial diversity\nThe high-quality clean reads were &gt;98.50% for all six samples, indicating a good sequencing depth for fecal microbiota gene analysis (Table  S1  †). The flat curves of the base sequence and mass distribution demonstrated higher accuracy (Fig.  S1a † ). Using MEGAHIT software to assemble effective reads, the default length of KMER should be 21, 41, 61, 81, 99, and the length of contigs could exceed 600 in each group when the sum value reaches 90% of the total length of fragment (Table  S2  †). Using the ReefSeq database in NCBI, fecal microbial genes were indexed and the species annotated using Meta-Othello. The species annotation and abundance information for each sample were counted, and a species abundance information table obtained in Fig.  2 . Among the classifiable sequences in different groups, Proteobacteria, Firmicutes, Bacteroidetes, Actinobacteria, Ascomycota, and Basidiomycota were represented the dominant lineages in the samples.', "PCR products were purified (AMPure XP system) and libraries were analyzed for size distribution using the Agilent-2100 Bioanalyzer and quantified using real-time PCR. The clustering of indexcoded samples was performed on a c-Bot Cluster Generation System according to manufacturer's instructions. After cluster generation, library preparations were sequenced on an Illumina HiSeq platform and paired-end reads were generated.  24  Quality trimming is an essential step to generate high confidence of variant calling. Raw reads were processed to generate high quality clean reads according to four stringent filtering standards: (i) removing reads with ≥10% unidentified nucleo-\n\nPaper\nFood &amp; Function tides; (ii) removing reads with &gt;50% bases having low quality scores of ≤20; and (iii) removing reads aligned to the barcode adapter. The high-quality reads were clustered into operational taxonomic units (OTUs) using CD-HIT software. The OTUs that reached a 97% nucleotide similarity level were used for further analysis.  20, 25  \n\nDe novo assembly and gene predictions\nOpen Reading Frame (ORFs) were predicted based on final assembly contigs using MetaGeneMark.", "Predicted ORFs ≥ 300 bp in length from all samples were pooled and combined based on ≥95% identity and 90% read coverage using CD-HIT to reduce the number of redundant genes for downstream assembly. The reads were re-arrayed to predict genes using BWA to count reads numbers. Finally, gene catalogues were obtained from non-redundant genes with gene reads counts &gt;2. 30,31\n\nTaxonomical assignment and functional classification\nAfter read filtering, clean reads were used to generate taxonomic profiles using a k-Mer-based taxonomic classifier. This approach employs a novel data structure called l-Othello, which supports efficient querying of taxonomic information from NCBI, using reads k-Mer signatures of 31 bp in length. All unique ORFs were annotated using DIAMOND to the functional databases: Kyoto Encyclopedia of Genes and Genomes (KEGG) and Gene Ontology (GO).  31  \n\nStatistical analysis\nThe results were expressed as mean ± SEM where applicable. GraphPad Prism 6.0 software was used for statistical analysis. Statistical significances for group differences were analyzed by ANOVA followed by Duncan's test.\n\nResults"]</t>
         </is>
       </c>
-      <c r="AF54" t="inlineStr"/>
+      <c r="AF54" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article does not mention the importance of a species' genetic variety to its survival, which is the claim being evaluated. The article actually focuses on the modulatory effects of jujube polysaccharides on intestinal microbiota and their potential in preventing colorectal cancer, with no relevance to genetic diversity or species survival."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -8634,7 +9002,14 @@
           <t>['2015a) , which suggested that sequence signaling is very important for m 6 A sites. Recently, a novel, singlebase-resolution technique, miCLIP-seq  (Ke et al. 2015; Linder et al. 2015) , was also established, which prompted a new wave of research on computational methods of m 6 A identification  (Xiang et al. 2016; Zhou et al. 2016) . Notably, m 6 A sites have methylation-specific surroundings, with the topology of a DRACH (where D = A, G, or U; R = A or G; and H = A, C, or U) consensus motif and a GAC consensus motif localized near stop codons, in 3 ′ -UTRs, within long internal exons, and at 5 ′ -UTRs  (Meyer et al. 2012; Schwartz et al. 2013; Li et al. 2014; Luo et al. 2014; Zhou et al. 2016) .', 'Other improved works in terms of prediction accuracy on the two data sets were also presented  (Chen et al. 2017b; Xing et al. 2017) . Recently, Zhou et al. established an m 6 A data set from published single-nucleotideresolution maps of human and mouse m 6 A sites  (Ke et al. 2015; Linder et al. 2015) . They then developed an m 6 A predictor named SRAMP  (Zhou et al. 2016) , which simply uses three sequence-derived features with Random Forest classifiers. Following this work,  Xiang et al. (2016)  improved the predictive performance by integrating multiple sequence features, including positional binary nucleotide sequence encoding, nucleotide pair spectrum encoding, positionspecific encoding, and k-mer nucleotide frequency encoding. These methods were used with conventional features in position and frequency statistics, with the sliding window being limited to a narrow region and focusing on only a single species. Additionally, there was a lack of independent testing, which resulted in overfitting.', ', 2018;; He et al. 2018) . However, in this context, there is a major problem regarding construction of the training data set. Specifically, low-quality negative samples cause low generalizability of the model, resulting in poor performance when applied to novel data. In addition, the compatibility of prediction methods in different species also remains a problem, so researchers cannot currently be certain that cross-species predictions are accurate. The yeast data set  (Schwartz et al. 2013)  and Arabidopsis data set  (Luo et al. 2014)  are two benchmark data sets for the computational prediction of m 6 A. Focusing on the Arabidopsis data set, Chen and coworkers first proposed a support vector machine-based method to identify m 6 A sites. Soon afterwards, they proposed a predictor called "iRNA-Methyl"  (Chen et al. 2015b ) on a near singlenucleotide resolution yeast data set. Chen and coworkers represented RNA sequences using "pseudo-dinucleotide composition," which focuses on the physiochemical properties of RNA.']</t>
         </is>
       </c>
-      <c r="AF55" t="inlineStr"/>
+      <c r="AF55" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article does not mention inter-simple sequence repeat (ISSR) molecular markers, nor does it relate to the development of molecular marker techniques. The content is focused on N6-methyladenosine sites prediction from mRNA sequences using deep learning techniques."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -8782,7 +9157,14 @@
           <t>['According to ALI ESMAIL AL-SNAFI  (2017)  showed that Erodium cicutarium contained Tannin, catechins, gallic and elagic acids, sugars (glucose, galactose, fructose), amino acids (glycine, alanine, proline, histidine, tryptophan, tyrosine, glutamic acid), vitamins K and C, and wide range of essential and volatile oils. Chromosome counts of 2n=20, 36, 40, 48, and 54 have been reported for the species. The most commonly reported counts from western Europe and non-native areas, where the species has become naturalized, have been n=10, 20; 2n=20, 40 (e.g.  WARBURG, 1938; HEISER and WHITAKER 1948; LARSEN, 1958) . The flowers of E. cicutarium subsp.', '1986; HULTE´N and FRIES, 1986) . Although the species requires moisture from rainfall or irrigation for optimal germination, established plants are drought tolerant and can survive periodic arid conditions  (BLACKSHAW and HARKER, 1998a; BUSSO et al., 1998; BROOKS and BERRY, 2006) . In arid and semi-arid regions, E. cicutarium has had some importance as a forage plant on ranges in California and Arizona  (ANONYMOUS, 1939; BUSSO et al. 1998; GEORGE et al. 2006) ; and is an important grazing plant and source of protein supplements to straw for ruminants in semi deserts and wastelands of the Middle East  (AL-MASRI, 2007) . In Turkey, the species is gathered as a food plant in the Aegean region  (BILGIR, 1982) .', 'Moreover, due to extensive morphological variability of this species in the country, there is possibility of having infra-specific taxonomic forms in this species. Therefore, we carried out population genetic analysis and morphometric study of 15 geographical populations for the first time in the country. Different methods of DNA fingerprinting have proved to be a useful tool with a wide range of applications in plant population studies, such as detection of genetic variation within and between populations, characterization of clones, analysis of breeding systems, and analysis of ecogeographical variation  (DAHLGREN, 1980) . For genetic study, we used the inter-retrotransposon amplified polymorphism (IRAP) method that displays insertional polymorphisms by amplifying the segments of DNA between two retrotransposons. It has been used in numerous studies of genetic diversity  (SMYKAL et al., 2011) .\n\nMATERIALS AND METHODS\n\n\nPlant materials\nA total of 102 individuals were sampled representing 15 natural populations of E. cicutarium in East Azerbaijan, Lorestan, Kermanshah, Gilan and Ardabil Provinces of Iran during July-Agust 2018 (Table  1 ).']</t>
         </is>
       </c>
-      <c r="AF56" t="inlineStr"/>
+      <c r="AF56" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article does not mention the antibacterial, anti-inflammatory, anthelmintic, analgesic, and diuretic properties of Cordia myxa L. or its treatment of various diseases as stated in the citation. The article actually focuses on the population genetic structure, genetic diversity, and morphological variability of Erodium cicutarium, a different plant species."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -8930,7 +9312,14 @@
           <t>['20  \n\nInfluence of JP on bacterial diversity\nThe high-quality clean reads were &gt;98.50% for all six samples, indicating a good sequencing depth for fecal microbiota gene analysis (Table  S1  †). The flat curves of the base sequence and mass distribution demonstrated higher accuracy (Fig.  S1a † ). Using MEGAHIT software to assemble effective reads, the default length of KMER should be 21, 41, 61, 81, 99, and the length of contigs could exceed 600 in each group when the sum value reaches 90% of the total length of fragment (Table  S2  †). Using the ReefSeq database in NCBI, fecal microbial genes were indexed and the species annotated using Meta-Othello. The species annotation and abundance information for each sample were counted, and a species abundance information table obtained in Fig.  2 . Among the classifiable sequences in different groups, Proteobacteria, Firmicutes, Bacteroidetes, Actinobacteria, Ascomycota, and Basidiomycota were represented the dominant lineages in the samples.', "PCR products were purified (AMPure XP system) and libraries were analyzed for size distribution using the Agilent-2100 Bioanalyzer and quantified using real-time PCR. The clustering of indexcoded samples was performed on a c-Bot Cluster Generation System according to manufacturer's instructions. After cluster generation, library preparations were sequenced on an Illumina HiSeq platform and paired-end reads were generated.  24  Quality trimming is an essential step to generate high confidence of variant calling. Raw reads were processed to generate high quality clean reads according to four stringent filtering standards: (i) removing reads with ≥10% unidentified nucleo-\n\nPaper\nFood &amp; Function tides; (ii) removing reads with &gt;50% bases having low quality scores of ≤20; and (iii) removing reads aligned to the barcode adapter. The high-quality reads were clustered into operational taxonomic units (OTUs) using CD-HIT software. The OTUs that reached a 97% nucleotide similarity level were used for further analysis.  20, 25  \n\nDe novo assembly and gene predictions\nOpen Reading Frame (ORFs) were predicted based on final assembly contigs using MetaGeneMark.", "Predicted ORFs ≥ 300 bp in length from all samples were pooled and combined based on ≥95% identity and 90% read coverage using CD-HIT to reduce the number of redundant genes for downstream assembly. The reads were re-arrayed to predict genes using BWA to count reads numbers. Finally, gene catalogues were obtained from non-redundant genes with gene reads counts &gt;2. 30,31\n\nTaxonomical assignment and functional classification\nAfter read filtering, clean reads were used to generate taxonomic profiles using a k-Mer-based taxonomic classifier. This approach employs a novel data structure called l-Othello, which supports efficient querying of taxonomic information from NCBI, using reads k-Mer signatures of 31 bp in length. All unique ORFs were annotated using DIAMOND to the functional databases: Kyoto Encyclopedia of Genes and Genomes (KEGG) and Gene Ontology (GO).  31  \n\nStatistical analysis\nThe results were expressed as mean ± SEM where applicable. GraphPad Prism 6.0 software was used for statistical analysis. Statistical significances for group differences were analyzed by ANOVA followed by Duncan's test.\n\nResults"]</t>
         </is>
       </c>
-      <c r="AF57" t="inlineStr"/>
+      <c r="AF57" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article (5) does not support the statement about using multiple data sets for phylogenetic inference. The article is actually focused on metagenomic analysis of gut microbiota and the effects of jujube polysaccharides on intestinal microbiota in a colorectal cancer mouse model, which is unrelated to phylogenetic inference."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -9222,7 +9611,14 @@
           <t>['Except for TiO 2 , various types of photocatalysts were reported in these years, such as titanate  [7, 8] , AM 2 O 4 (A = Cu and Zn, M = Al, Cr, Mn, Fe and Co)  [9, 10] , tantalite (niobate)  [11, 12] , sulphide  [13, 14] , ferrite  [15, 16]  and some oxide semiconductor  [17] [18] [19] [20] [21] [22] . BiFeO 3 is a perovskite-type multiferroic compound, which shows potential applications in spintronics devices due to its high ferroelectric and magnetic phase transitions, as well as large remanent polarization at room temperature  [23] [24] [25] . Moreover, it shows excellently photovoltaic effect and photocatalytic activity because that it can absorb a wide range of sunlight corresponding to its small E g  [26] [27] [28] .', "For the applications in the photocatalyst field, one of advantages of BiFeO 3 is its excellently magnetic property. It is known that the separation of photocatalysts is essential after the photocatalytic process. Generally, coagulation, flocculation and sedimentation are widely used in the separation process although they are complex and expensive  [29, 30] . But the separation process will be easy if the photocatalyst has the magnetism. It means that the photocatalyst can be separated easily by applying an exterior magnetic field. There are some reports for BiFeO 3 in photocatalytic degradation of organic pollutants in water  [27, 28, [31] [32] [33] [34] [35] [36] [37] ]. Chen's work shows that the hydrothermally-synthesized BiFeO 3 nanocrystals have excellently photocatalytic activity for methyl orange degradation under visible light irradiation and the surface oxygen vacancies enhance the photocatalytic activity effectively  [37] .", 'To find out the mechanism of the higher photocatalytic activity of BiFeO 3 :Gd 3+ , a series of physical and chemical properties of BiFeO 3 and BiFeO 3 :Gd 3+ were investigated and compared. Fig.  3  shows the microstructural analysis of BiFeO 3 (Fig.  3A ) and BiFeO 3 :Gd 3+ (Fig.  3B ). The SEM images show that a large number of  irregular nanoparticles were produced by the sol-gel process. There are agglomerations between particles. But the agglomeration does not influence the band gap of samples  [34] . In the sol-gel synthesis, the complexing ligands of precursor xerogel wrote over the produced nanocrystals and thus prevented the agglomeration. But the subsequent calcination induced the evaporation of citrate complexing agents. Thus, the nanocrystals agglomerated and grow to be larger due to their high surface energy. These led to the final microstructure of the synthesized photocatalysts. Fig.  3C  and Fig.']</t>
         </is>
       </c>
-      <c r="AF59" t="inlineStr"/>
+      <c r="AF59" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article does not support the statement that metal-based complexes suffer from shortcomings such as drug resistance and high toxicity. The article actually discusses the enhancement of photocatalytic hydrogen production of BiFeO3 by Gd3+ doping, which is unrelated to the topic of metal-based complexes as anticancer reagents."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -9370,7 +9766,14 @@
           <t>['Introduction\nMetal-organic frameworks (MOFs), self-assembled from metal ions (or metal clusters) and organic ligands, have attracted considerable attention during the last two decades owing to their fascinating physical and chemical properties, such as high specific surface areas, tunable structures and porosities, as well as designable functionality  [1] . Therefore, MOFs, which serve as the functional materials, have exhibited huge potential applications in diverse areas  [2, 3] , including gas storage  [4] , adsorption/separation  [5] , supercapacitor  [6] , drug delivery  [7] , sensing  [8]  and catalysis  [9] . Notably, porosity is an essential feature in MOFs, which plays a vital role in functionalization like the diffusion and mass transfer of substrates/products  [10, 11] . However, the pore sizes of the majority of MOFs have been reported to be within a micropore range (pore size \\ 2 nm) during the last few decades  [4, 12, 13] .', 'Besides, a couple of new methods are also available, such as ionic liquids assisted synthesis  [22] , modulator-induced-defect-formation  [23]  and a spray-drying technology  [24] . Typically, HP-MOFs synthesized by these methods are characterized by the superiorities of tunable mesoporosity and abundant active sites  [25] . However, these approaches mostly require harsh experimental conditions and tedious downstream treatments (such as a long reaction time at high temperature and pressure and/or special apparatus)  [26, 27] , which is energy-consuming and may lead to pollution, a risk of explosion and a low production rate  [28] [29] [30] . For instance, the space-time yields (STYs, kg m -3 d -1 ) are usually below 300 kg m -3 d -1 for products synthesized within several hours  [28] . Recently, Huo groups reported the room-temperature synthesis of HP-MOFs (HKUST-1) with a high STY (2035 kg m -3 d -1 ) by controlling either the synthesis time or the copper source, for the first time  [31] .', '(  1 ) STY ¼ m MOF V solution Á s Â 1:44 Â 10 6 ð1Þ where m MOF represents the powder mass (g) of the HP-MOFs, V solution represents the total volume (cm 3 ) of the mixture, and s represents the reaction time (min).\n\nResults and discussion\nFigure  1a  shows the wide-angle XRD patterns of the HP-Cu-BTC sample synthesized with a cooperative template method and the C-Cu-BTC, as well as the simulated XRD pattern of Cu-BTC single-crystal. It can be clearly observed from Fig.  1a  that the XRD patterns of the as-synthesized HP-Cu-BTC are consistent with those of C-Cu-BTC and the simulated Cu-BTC, indicating that the obtained product is topologically identical to Cu-BTC crystal  [29] . Moreover, the sharp XRD peaks of HP-Cu-BTC confirm fine crystallinity  [37] . The crystal structure of HP-Cu-BTC was further characterized using FT-IR spectroscopy. As shown in Fig.']</t>
         </is>
       </c>
-      <c r="AF60" t="inlineStr"/>
+      <c r="AF60" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article primarily focuses on the synthesis and properties of hierarchically porous metal-organic frameworks (HP-MOFs), but does not explicitly discuss coordination polymers (CPs) as a class of materials. While MOFs are mentioned, which could be considered a type of CP, the article's scope is more specific to HP-MOFs and their synthesis, rather than providing a general overview or definition of CPs."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -9518,7 +9921,14 @@
           <t>['In this regard, scholars from all over the world have carried out studies on waste minimization, multiple utilization and harmlessness from the perspectives of waste management methods  [11] , management mode  [12] , optimization process  [13] , recycling  [14] ,  [15] . Among waste, construction waste is the most important component of construction waste, including broken concrete blocks, bricks and so on  [16] . It is one of the most necessary research to reduce environmental pollution by secondary utilization after crushing. However, construction waste cannot be recycled and reused in a full sense  [17] ,  [18] . When it is damaged to a certain extent, it will not be reused. It can only be treated by landfill or open-air stacking. It is one of the important means to solve the problem at present, including effectively judging the damage degree of construction waste, reducing unnecessary secondary treatment and misjudgement of multiple utilization, and making comprehensive use of valuable components  [19] . As a common waste of construction waste, recycled aggregate concrete aggregate has a lot of research on the development and application all over the world  [20] .', 'Based on this, the acoustic emission waveforms of fatigue crack propagation  [6] ,  [7] , the influence of acoustic emission sensors on the acoustic emission waveforms of fatigue crack propagation of thinwalled aerospace specimens  [8] , and the relationship between crop acoustic emission and disease stress are studied with the abnormal change propagation characteristics captured by the evolution of acoustic emission waveforms  [9] . In recent years, economic development has led to the growth of various types of construction, while the corresponding waste is also increasing. Construction waste, which most seriously affects the environment, has become one of the focuses of research. Secondary pollution is becoming more and more serious due to construction waste increasingly diversified and the impact of construction waste on the environment is permanent and cumulative. Since the 21st century, the amount of urban construction waste has gradually increased, and now it accounts for about 35% of the total amount of urban waste  [10] . For various reasons, most of the construction waste is directly transported to the suburbs without treatment and is disposed of by open-air stacking or landfill, which seriously threatens the safety of the ecological environment.', 'The recycled aggregate concrete is studied through a lot of experiments. It is found that the recycled aggregate concrete has high crushing index, low density, high porosity, enhanced water absorption, low aggregate strength and weak bonding ability. The shear strength and compressive strength test showed that the recycled aggregate perforated brick material showed obvious brittleness  [14] ,  [21] ,  [22] . By measuring the low modulus of elasticity of recycled coarse aggregate concrete relative to ordinary concrete, Etxeberria et al. analyzed the effect of material sequence in concrete production (made of recycled aggregate) on improving its splitting tensile strength  [23] . To some extent, these studies have played a positive role in the reuse of construction waste. However, in practical application, such as the increase of wall cracks has become the bottleneck of the development of this new construction material.']</t>
         </is>
       </c>
-      <c r="AF61" t="inlineStr"/>
+      <c r="AF61" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article (9) does not mention coordination polymers or any related concepts. The title and abstract focus on acoustic emission signal processing technology, and the provided excerpts discuss topics such as waste minimization, construction waste management, and recycled aggregate concrete, which are unrelated to the statement about coordination polymers."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -9666,7 +10076,14 @@
           <t>["In  (ADARAMOLA, 2018) , an investigation study is made to transmit data traffic efficiently in cities in the presence of various challenges. The selected metrics are the packet delivery ratio (PDR), end-to-end delay and routing overhead.\n\nProposed model\nThe examination in VANETs can be employed to enhance the transportation framework, provide chain management, in addition to logistics through estimating numerous parameters about the roadways, vehicles, as well as drivers. The collection of data needs sensors in the roadways as well as vehicles which learns the traffic level, climatic conditions, working of the vehicle, and reaction of drivers to the dynamic conditions. In a million miles of streets, billions of vehicles, as well as driver's data are, gathered in several years, the sheer count of data points is astonishing. It is just at this point, using modern Big Data technologies, i.e., a large amount of data can be investigated in shorter time duration for it to be valuable. Out of this massive selection of data, it is needed to construct adaptive methods to assist transportation organizations to decide on the selection of optimal routes with the best time to delivery, safety, cost, and fuel utilization.", 'When calculating traffic conditions during poor climatic conditions, logistics organization can provide an optimal path which allows best routes for proper time delivery. There is a requirement of creating models that may foresee regardless of whether accidents are probably going to happen due to the nature of street as well as driver reaction, in the long run prompting more secure streets. This research has uncovered various advantages such as high safety, low transportation cost, user-friendly, and predictable material deliverance for producing, that is particularly critical for modern just-in-time manufacturing. An individual application can be employed to create or generate different kinds of data which is established quickly and has to process rapidly. The conventional relational databases cannot handle this massive quantity of data, and there is a requirement of efficient methods to manage it. Hadoop is an open-source environment which processes the high volume of information  (Barlow, 2013) . At the point, when an organization requires saving of large measure of data, they have two choices: use a large machine by additional CPU, RAM, disk space and so forth otherwise discuss with database sellers for better solutions. But, each of the two choices has their issues, and there is a tradeoff over securing a big device.', 'A Hadoop cluster scales computation capacity, storage capacity as well as I/O bandwidth through the inclusion of commodity servers  (L€ ammel, 2008) . It can toutilize the available commodity of hardware, consequently, the computation cost to construct the Hadoop cluster be low. To execute a Map Reduce program, a small Hadoop cluster is required which might incorporate a master node as well as many worker nodes. The master node contains a JobTracker, TaskTracker Name-Node as well as DataNode. A slave otherwise worker node behaves as a DataNode as well as TaskTracker, although it is probable to comprise data-only worker nodes as well as compute-only worker nodes"  (Lind et al., 1999) . MapReduce programming model involves a series of steps which are listed below  (L€ ammel, 2008) : Iteration on the input Calculation of key/value pairs out off every piece of input Clustering entire intermittent ranges via key Iteration on the resultant group Reducing every class The estimation involves a collection of input key/value pairs, as well as it produces a collection of output key/value pairs. Two functions, map in addition to reduce, are employed to describe the estimation.']</t>
         </is>
       </c>
-      <c r="AF62" t="inlineStr"/>
+      <c r="AF62" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article primarily focuses on the application of big data technology and ant colony optimization in vehicular ad hoc networks for smart cities, with no mention of education management or professional teams. The abstract and excerpts do not provide any relevant information that supports the claim about a professional team with theoretical knowledge and practical skills in education management."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -9815,7 +10232,14 @@
           <t>["In this case, it is necessary to solve Navier-Stokes equations  [32] [33] [34] [35] . In this regard's conservation equations for continuity, energy and momentum are used to solve the materials flow. Equations (  1 )-(3) indicated that the continuity, energy and momentum, respectively: ∂u i ∂x i = 0 (1) u indicated plastic velocity of material and i = 1, 2 and 3 presenting x, y and z direction.", 'The simulation procedure was done on the commercially ANSYS FLUENT software under the computational fluid dynamics (CFD) approach. The simulation domain dimension and geometry are defined according to the experimental tests, as shown in Figure  1a . A 3D Cartesian system for the welded material (WM) and the FSW tools was established. All geometries and process parameters were selected according to the experimental tests. The origin was set at the middle point of the FSW tool shoulder. The x-axis indicated the welding direction, and the z-axis indicated the FSW tool normal axis. The FSW tool had rotational movement, and the interior domain was set to move according to the welding tool speed. The interior domain had the same velocity as the welding tool by the velocity inlet side. The sidewalls, along with the top and bottom, had the same velocity as the velocity of the inlet. The outer plate of the workpiece was set at zero pressure to avoid the reverse flow at the pressure outlet. The WM is assumed to be a non-Newtonian single-phase fluid representing the quasi-static thermal and fluid flow boundary problem.', '∂u i u j ∂x i = - ∂P ∂x j + ∂ ∂x i µ ∂u j ∂x i + µ ∂u i ∂x i -ρu 1 ∂u j ∂x j (2) 1 i j j j i i j i i i j u u u u u P u x x x x x x μ μ ρ ∂ ∂ ∂ \uf0e6 \uf0f6 ∂ ∂ ∂ = - + + - \uf0e7 \uf0f7 ∂ ∂ ∂ ∂ ∂ ∂ \uf0e8 \uf0f8 (2) In Equation (  2 ), the ρ, P and u1, presented density, pressure and welding velocity, respectively.']</t>
         </is>
       </c>
-      <c r="AF63" t="inlineStr"/>
+      <c r="AF63" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article does not mention the SIMPLE scheme or a convergence metric of 10–6. The provided excerpts discuss Navier-Stokes equations, simulation procedures using ANSYS FLUENT software, and boundary conditions for the FSW process, but do not support the statement about pressure–velocity coupling."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -9963,7 +10387,14 @@
           <t>['Point of view research papers confirmed the need for a calibration process but the calibration methods were different  (Kleidorfer et    ΔV ¼ P þ S i þ G i À ETa À I À S 0 À G 0 ± T (1) where ΔV ¼ storage capacity variation; P ¼ precipitation; S i ¼ surface water infiltration; G i ¼ surface water infiltration; ETa ¼ actual evapotranspiration; I ¼ infiltration; S 0 ¼ surface water seepage; G 0 ¼ surface water seepage; T ¼ tidal current. The surface flow rate will be obtained using the Manning equation.', 'Infiltration coefficients, the amount of permeable and impermeable lands were the components that need to uncer-   2 . The calibration of the model continues until it is determined by statistical indicators that the results of the calibrated model are in good agreement with the measured data. To evaluate the models from the statistical indicators of EFF model efficiency, the mean of the second root of the error is RMSE, the normalized RMSE (NRMSE), the residual mass coefficient of CRM.', 'EFF ¼ 1 À P n i¼1 (O m À O c ) 2 P n i¼1 (O m À O m ) 2 0 B B B @ 1 C C C A × 100 (7) RMSE ¼ 1 À P n i¼1 (O m À O c ) 2 n 0 B B @ 1 C C A 1 2 (8) CRM ¼ 1 À P n i¼1 O m À P n i¼1 O c P n i¼1 O m 0 B B B @ 1 C C C A × 100 (9) where O m is the measured value, O c is the calibrated value, n is the number of samples used and O is the average value of the observed parameter.  The percentage of permeability PPer À 30%-þ 30% percentage of water received is transferred to the transport module. In the next step, transport module that is composed of a set of units with transfer and processing features including pipes, channels, etc., which is embodied in the combination of nodes and connections.']</t>
         </is>
       </c>
-      <c r="AF64" t="inlineStr"/>
+      <c r="AF64" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article does not mention anything related to numerical methods or schemes for pressure-velocity coupling. The abstract and provided excerpts focus on stormwater management, hydrological frameworks, and urban water allocation systems, which are unrelated to the citation statement."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -10111,7 +10542,14 @@
           <t>['An interface can be used to transmit the load  [32]  . As a result, the VESTA software used HOMO-LUMO to determine the most likely mechanism of Al-MOF formation  [33]  . Using the Gauss-09 quantum chemistry package, kinetic and thermochemical data were estimated at the theoretical DFT level  [34]  . Since absolute values of the enthalpy and Gibbs free energy of the molecule can be obtained by theoretical calculation, the enthalpy of the reaction and the Gibbs energy of each possible reaction are obtained by using these energy values  [35]  . The CA ineludible C = C, C -H, H -O, and C -O bonds must be taken into account during the interaction with the aluminium precursor. The optimization of appropriate molecules was carried out using the B3LYP theory by the 6-31 G set  [15]  . Gaussian 09 was used to make the estimates  [36]  . All optimized structures of S. hortensis were confirmed to have minimal energy compatibility.', 'The samples were heated upto 700 °C at the rate of 10 °C/min. The Brunauer-Emmett-Teller (BET) model used the nitrogen adsorption/desorption isotherms (at the temperature of 196 °C) after the separation at 200 °C and 10-5 mm Hg for at least 4 h to estimate surface-specific regions. The mesoporous size distribution and total mesoporous volume were estimated using the modified Barrett-Joyner-Halenda (BJH) method. GC-MS analysis was also performed using a Thermoquest-Finigan gas chromatograph (equipped with a DB-1 column silica capillary column (60 m * 0.25 mm i.d.; film thickness = 0.25 μm) with four polarization of TRACE mass. Helium tracer was employed as a carrier gas with an ionization voltage equal to 70 eV. The ion source and interface temperatures were 200 °C and 250 °C, respectively.', 'Density functional theory (DFT)\nDensity functional theory (DFT) (i.e., a ground-state theory used to determine the ground states of a quantum system in order to estimate relevant values, such as ground state energy) is an intriguing and powerful tool  [30]  . The particle density of a system with interacting N particles is used as the original value in DFT instead of the wave function  [31]  . Frontier orbital energy gap is the subtraction of the highest occupied molecular orbital (HOMO) to the lowest unoccupied molecular orbit (LUMO). The Frontier orbital energy gap could be used to determine the interaction between different species. Harmonic vibrational waves were calculated using second-order analytical derivatives to confirm the convergence of minimums on the potential surface and to evaluate the zero-vibration contrast energy. As shown in Fig.  2  , in the finitecharge regime at one of the metal/molecule interfaces, the role of non-boundary modes is important, as these channels provide additional channels through which they can be used. An interface can be used to transmit the load  [32]  .']</t>
         </is>
       </c>
-      <c r="AF65" t="inlineStr"/>
+      <c r="AF65" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article does not mention pressure–velocity coupling or the SIMPLE scheme, nor does it discuss convergence metrics or numerical values like 10−6. The content is focused on metal-organic frameworks, their synthesis, and characterization, which is unrelated to the citation statement."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -10259,7 +10697,14 @@
           <t>['2  too. Initial configuration is shown in Fig.  2a . Figure  2b  shows the pressure contours and material flow fields at t = 5.25 µs, when the detonation front reaches the end of the donor HE charge. Pressure on the detonation wave front in the donor charge is 22.1 GPa. Material flow fields and decomposition contours at t = 5.25 µs are shown in Fig.  2c . When this wave enters the silicon carbide rod, it produces a wave with front pressure of 28.1 GPa. At the same time, the initial pressure of the shock wave front in water is only 19.1 GPa. These two waves continue to propagate towards the acceptor HE charge, with the wave in the rod moving ahead of the wave in water. At t = 8.50 µs the wave in the rod reaches the acceptor HE charge with an amplitude of 3.6 GPa and initiates a compression wave without a shock front in it with an amplitude of 2 GPa. The degree of decomposition of the acceptor charge equals zero (see Fig.  2d ,  e ).', 'It was modified in paper  [14] . The reaction rate law contains three terms to model the ignition of hot spots by shock compression, the slow growth of reaction from these isolated hot spots, and the rapid completion of reaction as the hot spots coalesce. dα/dt = I (1 -α) b (ρ/ρ 0 -1 -a) x + G 1 (1 -α) c α d p y + G 2 (1 -α) e α g p z where α is the fraction reacted (degree of HE decomposition), t is time, ρ is the current density, ρ 0 is the initial density, p is pressure, and I, G 1 , G 2 , a, b, c, d, e, g, x, y, and z are constants. The parameter a is the critical compression that is used to prohibit ignition until a certain degree of compression (or a certain input pressure) has been reached. This parameter provides the ability to calculate HE desensitization after precursor wave loading.', 'Analysis of the wave processes occurring during the initiation of the acceptor HE charge has been performed. Peculiarities of the wave processes in the gap test assemblies that can influence the results of sensitivity measurements have been studied. In particular, it has been established that precursor waves in gap test assemblies can influence the detonation transmission distance. It is also shown that the presence of the identification steel specimen can lead to erroneous results when using the gap test due to possible initiation of acceptor HE charge by the wave reflected from the specimen. Summarizing the foregoing, we would like to recommend when analyzing the gap test results to take into account the possibility of acceptor charge desensitization by precursor waves, and its possible initiation by the wave reflected from an identification specimen.']</t>
         </is>
       </c>
-      <c r="AF66" t="inlineStr"/>
+      <c r="AF66" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article discusses numerical simulations of high explosive charge desensitization in gap test assemblies and has no relation to students' study arrangements or learning efficiency. The topics are entirely unrelated."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -10408,7 +10853,17 @@
           <t>["Besides the technical analysis methods, many conventional numeric forecasting models have been proposed by financial researchers, such as Engle's  [17]  autoregressive conditional heteroscedasticity (ARCH) model, Bollerslev's  [6]  generalized ARCH (GARCH) model, Box and Jenkins'  [7]  autoregressive moving average (ARMA) model, and the autoregressive integrated moving average model (ARIMA). In recent decades, many researchers have employed another approach to financial forecasting: artificial intelligence algorithms In 1990, Kinoto et al.  [29]  developed a prediction system for the stock market by using a neural network. Nikolopoulos and Fellrath  [32]  combined genetic algorithms (GAs) and a neural network to develop a hybrid expert system for investment decisions. Kim and Han  [27]  proposed a genetic algorithms approach in order to feature discretization and the determination of connection weights for artificial neural networks (ANNs) to predict the stock price index. Huarng and Yu  [25]  applied a backpropagation neural network to establish fuzzy relationships in fuzzy time series for forecasting stock prices.", "The rest of this paper is organized, as follows: Section 2 introduces the related works; Section 3 demonstrates the proposed model and algorithm; Section 4 evaluates the performance of the proposed model and describes the findings; and Section 5 draws conclusions and proposes recommendations for future research.\n\nRelated works\nThis section reviews related works of technical analysis, cumulative probability distribution approach, minimize entropy principle approach, rough set theory, and genetic algorithms.\n\nTechnical analysis\nTechnical analysis is an attempt to predict future stock price movements by analyzing a past sequence of stock prices  [39] . It relies on charts and looks for particular configurations that are supposed to have predictive value. Analysts focus on investor psychology, which represents common investors' responses to certain price formations and price movements, to analyze the fluctuations of stock market. The price at which investors are willing to buy or sell depends on personal expectation. If investors expect the security price to rise, they will buy it; if investors expect the security price to fall, they will sell it. These simple statements are the cause for a major challenge in setting security prices, because they refer to human expec-tations and attitudes  [39] .", '** Denotes that correlation is significant at the 0.05 level using 2-tailed test. *** Denotes that correlation is significant at the 0.01 level. it is clear that the proposed model surpasses the other three models (Buy-and-Hold, RST and GAs) in each testing period, except 2005. These stock return evaluations demonstrate the outstanding performance of the proposed model.\n\nFindings and conclusions\nThis paper has proposed a new hybrid model, based on four novel methods (CDPA, MEPA, RST and GA), to promote stock market forecasting performance. From the performance evaluation data in the above section, we can conclude that the main objective of this paper has been reached. Furthermore, by examining the performance data carefully, we also ascertain that four important findings for the proposed model emerge, as follows: (1) The proposed model produces a positive stock return, whether the market is bullish or bearish.']</t>
         </is>
       </c>
-      <c r="AF67" t="inlineStr"/>
+      <c r="AF67" t="inlineStr">
+        <is>
+          <t>Here is my evaluation in JSON format:
+```
+{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article does not discuss 'confirmation choice' at all. It focuses on proposing a hybrid forecasting model for stock price trends using rough sets theory and genetic algorithms, which is unrelated to the citation statement."
+}
+```</t>
+        </is>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -10557,7 +11012,14 @@
           <t>['In this paper, it is shown that EM-ELMs can also be cast as a particular case of SAOCIF. In particular, EM-ELMs can easily be extended to test some number of random candidates at each step and select the best of them, as SAOCIF does. Moreover, it is demonstrated that the cost of the computation of the optimal output-layer weights in the originally proposed EM-ELMs can be improved if it is replaced by the one included in SAOCIF. In addition, there are still a lot of applications about ELM in other areas. An improved ELM method was proposed for soft sensing modeling by  Chang et al. (2007) . By adding a kind of sorting neurons into the hidden layer of the single hidden layer feedforward neural network (SLFN), a new SLFN structure was proposed. The method provided a new approach to build soft sensing models, and it was successfully applied to the soft sensing modeling the of cell concentration for the Nosiheptied fermentation process to realize the online prediction of the cell concentration.  Pan et al.', 'Extreme learning machine is used in the fields such as signal processing  (Mao 2002) , automatic control  (Mao and Huang 2005) , image processing  (Huang et al. 2011) , market analysis, aviation and aerospace and medical diagnosis  (Shang et al. 2005) , etc. A new human face recognition algorithm based on bidirectional two dimensional principal component analysis (B2DPCA) and ELM is proposed by  Mohammed et al. (2011) . The method is based on curvelet image decomposition of human faces and a subband that exhibits a maximum standard deviation is dimensionally reduced using an improved dimensionality reduction technique. Discriminative feature sets are generated using B2DPCA to ascertain classification accuracy. Other notable contributions of the proposed work include significant improvements in classification rate, up to hundred folds reduction in training time and minimal dependence on the number of prototypes. Many researchers using the ELM to solve the compete phenomena in the whole nature and society, such as the winner-take-all (WTA) competition which is widely observed in both inanimate and biological media and society. Then,  Li et al.', 'The data sets include actual results and its related factors. During training, the influence factors and the corresponding results will be put into ELM for training, through an iteration to complete learning process. Then, with the trained ELM to predict, only need to input and the training data set is similar to the influencing factors. ELM model can be obtained the prediction results according to the memory. Extreme learning machine is an easy to use and effective algorithm for single hidden layer feedforward neural network. The traditional neural network learning algorithm (e.g. BP algorithm) need to set up lots of artificial network training parameters, and can easily lead to local optimal solution. ELM algorithm only need to set the number of hidden layer nodes, in the algorithm implementation process does not need to adjust the network input weights and hidden biases, and generates a unique optimal solution, with advantages of fast learning speed and generalization performance.\n\nModel of ELM\nFor N arbitrary distinct samples (x i , t i ), where x i = [x i1 , x i2 , . . . , x in ] T ∈ R n and t i = [t i1 , t i2 , . . .']</t>
         </is>
       </c>
-      <c r="AF68" t="inlineStr"/>
+      <c r="AF68" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article does not support the statement about individual finance score models being created to sort candidates based on attributes like age, pay, and marital condition. The article discusses Extreme Learning Machine (ELM) algorithms, their applications, and advantages, but does not mention finance score models or candidate sorting."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -10705,7 +11167,17 @@
           <t>['Marini and Walczak (2011)  proposed a discrete binary-coded implementation of the PSO algorithm to identify and select variables with a significant clustering tendency. In particular, to cope with the problems that can arise when performing variable selection on data sets with a high number of variables, and to account for the possibility of using the method also for purely exploratory purposes, an unsupervised approach was used, where the fitness was computed based on hierarchical clustering models. The characteristics of the method were shown on two simulated data sets and on a real megavariate data set coming from the analysis of genomic microarrays. They conclude that in all cases, PSO allowed them to explore different subspaces and to discover meaningful structures in the analyzed data. Based on these considerations, it is apparent that the use of PSO can represent a very promising option to deal with the problem of finding groups in a multivariate data set in a relatively straightforward and reliable way. This approach could be very useful to cope with biomarker identification in the fields of genomics, proteomics or metabolomics. Lotfi  Shahreza et al.', 'The outcome of the study clearly indicates that the proposed composite model and approach of this neural network clustering based PSO can be used as an attractive means for load characteristics to obtain the global load model for describing the nonlinear characteristics of the electric load. It will automatically produce the If-Then rules, whose premise parameters and consequent parameters are adjusted by using a Back-Propagation algorithm in combination with the least squares method. The simulation results also show the feasibility of the method.  Paterlini and Krink (2006)  introduced two algorithms for numerical optimization, namely particle swarm optimization (PSO) and differential evolution (DE). DE is clearly and consistently superior compared with the genetic algorithm (GA) for hard clustering problems.  Abraham et al. (2007)  introduced a method for clustering complex and linearly nonseparable datasets, without any prior knowledge of the number of naturally occurring clusters. The proposed method is based on an improved variant of the particle swarm optimization (PSO) algorithm.  Ahmadi et al (2007)  reported that, when the data set is large and has a high dimension, the time single swarm is incapable of exploring the entire solution space.', '2003; Parsons et al. 2004) . Variable selection in clustering has been approached from different perspectives: density-based methods such as  (Agrawal et al. 1998; Chan and Hall 2010; Raftery and Dean 2006) , model-based methods such as  (Pan and Shen 2007; Wang ans Zhu 2008) , and criterion-based methods such as  (Witten and Tibshirani 2010; Raftery and Dean 2006) . Many algorithms for large data sets have been proposed in the literature using different techniques. However, conventional algorithms have some shortcomings such as the slowness of the convergence and the sensitivity to initialization values, etc. and they still require much investigation to improve performance and efficiency. Clustering methods such as the K-means algorithm, soft clustering based on mixed models, hierarchical clustering, and spectral clustering have been developed and have proven to be successful in many real world applications  (Kriegel et al. 2009; Luxburg 2007; Steinbach et al. 2003; Parsons et al. 2004; Zhou and Shi 2011) .']</t>
         </is>
       </c>
-      <c r="AF69" t="inlineStr"/>
+      <c r="AF69" t="inlineStr">
+        <is>
+          <t>Here is my evaluation:
+```
+{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article does not mention individual finance score models, candidate attributes such as age or pay, or conjugal condition. The article focuses on particle swarm optimization algorithms and clustering high-dimensional data, which appears unrelated to the citing statement."
+}
+```</t>
+        </is>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -10853,7 +11325,14 @@
           <t>['Finally, some additional components could be included in the future agenda for CF: researchers should focus more on multiple objectives rather than single objectives, the dynamic nature of the CF should be included when more comprehensive models are taken into account reflecting reality; more attention should be given to PSO and ACO as both seem promising methodologies for CF; uncertainty in part/machine utilisation could be studied by employing fuzzy theory; hybrid metaheuristics are powerful tools which should be employed more frequently for complex systems such CF.', 'It is worth noting that these papers were selected to be included in this review as their contribution towards CF covers a large spectrum of research directions over the last ten years. All papers have been classified based on different methodologies employed such as mathematical programming, heuristics/metaheuristics and artificial intelligence approaches and their contribution discussed. For the purpose of this section a comparison and evaluation of the CF formulations is carried out. Table  1  presents a numbered list of CF reference sources and Table  2  a comparison of these numbered sources based on major criteria. The latter involves major objectives and constraints included, solution approaches employed, maximum size of problem data solved, identification of whether the optimum value or deviation from the optimum solution is provided when largest problem solved and whether methodology has been compared to other existing methodologies and finally implementation tools adopted. Major objectives are identified as minimisation of intercellular movements, machine/load utilisation and numerous cost considerations such as: machine operating cost, machine modification costs, machine (re)configuration cost, subcontracting cost, machine setup cost, inventory holding cost, replacement costs of defective parts.', "In order to be able to evaluate those methodologies and obtain overall performance criteria, i.e. applicability, practicability, there is still a need for objectively comparing them on benchmark problems. All CF approaches that have been proposed have been tested with a variety of problem sizes and in some cases compared with existing methodologies. An additional stage which would complement the process of evaluating results would be to use industrial data to test a proposed formulation's stability and ability for reconfiguration when real situations are encountered. The main focus of the CF problem is to group parts into part families and machines into machine cells when certain objective functions are taken into account. In the past, it has been suggested by  Selim et al. (1998) , that to achieve the goal of creating efficient manufacturing cells it is imperative to go beyond just grouping parts and machines by adding workers and tools as third and fourth dimensions to parts and machines respectively to meet industrial specifications. To the best knowledge of the authors the latter has not been examined during the last decade by any CF study, hence more attention should be given to utilising workers and tools."]</t>
         </is>
       </c>
-      <c r="AF70" t="inlineStr"/>
+      <c r="AF70" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article (22) does not support the statement about individual finance score advantages. The article actually focuses on cell formation problems in manufacturing systems, discussing various methodologies and their evaluation, without any mention of individual finance scores or related concepts."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -11001,7 +11480,14 @@
           <t>['Thus we use the class memberships to construct the new representation of the image. Based on this new presentation, we could gain an accurate retrieval of images from a image database  [12] -  [14] . A kernel classifier is used to measure the membership of an image to a special image class. The number of images in each class is always tremendous, thus the training of kernel classifier may takes a long time  [15] -  [18] . To solve this problem, an efficient algorithm is needed. In this paper, we develope a new iterative algorithm to learn the kernel classifier, which is an efficient fast implementation of support vector machine (SVM)  [19] -  [21] . We try to develop the fast algorithm by using both the stochastic learning strategy  [22] -  [24]  and the support vector approximation technology  [25] ,  [26] . The developed classifier is fast and robust, which makes the learning from a large number of images possible. Because the training images are input into the algorithm one by one, thus it does not takes much memory, and it is also a online algorithm.', 'We write the objective function in  (3)  as O(α) = 1 2 α 2 2 + C 1 N N i=1 (f (x i ), y i ) = 1 2 α α + C 1 N N i=1 β i 1 -y i α K(•, x i ) (5) β i is defined as β i = 1, if 1 -y i α K(•, x i ) ≥ 0 0, e l s e (6) We try to use the gradient descent method  [43] -  [45]  to update the classifier parameter α in an iterative algorithm. However, for the hinge loss has no close form of derivative with regarding to α, thus we fix β i as the previous one.', 'When the training image number N is large, the computational cost could be very expensive. α t = α t-1 -τ t ∂O(α) ∂α α=α t-1 = α t-1 -τ t α t-1 -C 1 N N i=1 β t-1 i y i K(•, x i ) = 1 -τ t α t-1 -τ t C 1 N N i=1 β t-1 i y i K(•, x i ) (9) 1) Fast updating method: To accelerate the updating procedure, we develop a novel and efficient algorithm for this problem. The training images are given to the algorithm one by one. In each iteration, only one image is used. We assume that in t-th iteration, x i t is used, and the objective function is constructed using only x i t as O(α) = 1 2 α 2 2 + C (f (x i t ), y i t ) = 1 2 α α + Cβ i t 1 -y i t α K(•,']</t>
         </is>
       </c>
-      <c r="AF71" t="inlineStr"/>
+      <c r="AF71" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article does not mention the use of Genetic Algorithm (GA) or any other streamlining instruments for optimizing element subset and model parameter. The article focuses on a novel image representation method using kernel classification, and the excerpts provided discuss the learning of kernel classifiers and an efficient algorithm for training them."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -11149,7 +11635,14 @@
           <t>['Our proposed algorithm MTPS exhibits shorter running time than others, except for the OASIS and OMKS, suggesting that MTPS provides a comparably efficient way against the problem, and shows a promising improvement space for the future work.\n\nIV. CONCLUSION AND FUTURE WORKS\nIn this paper we study the problem of similarity learning for content-based image retrieval. The critical novelty of this work is it learns the similarity to maximize the top precision measure over the training set. We model the learning problem as a support top irrelevant database image weighting problem to obtain the optimal similarity function. The experiments over some benchmark databases show its advantages over other similarity learning methods. In the future, we will investigate to use some other similarity function as similarity measure instead of linear function, such as Bayesian network  [12] ,  [13] ,  [14] , and also to develop novel algorithms of other machine learning problems and applications besides similarity learning, to maximize top precision measure, such as importance sampling  [15] ,  [16] ,  [17] , portfolio choices  [18] ,  [19] , multimedia technology  [20] ,  [21] ,  [22] ,  [23] ,', '( 5 ) Thus the loss function for each (z i , x j ) i,j:yij =1 is, ℓ(z i , x j ; W ) = max 0, max k:y ik =0 s(z i , x k ) -s(z i , x j ) + 1 = max 0, max k:y ik =0 z ⊤ i W (x k -x j ) + 1 . (6) The optimization problem is modeled as, min W,ξij |i,j:y ij =1 \uf8f1 \uf8f2 \uf8f3 1 2 W 2 F + C i,j:yij =1 ξ ij \uf8fc \uf8fd \uf8fe , s.t. ∀i, j : y ij = 1, ξ ij ≥ 0, ξ ij ≥ z ⊤ i W (x k -x j ) + 1, (7) where ξ ij is slack variable of (6), 1 2 W 2 F is the squared Frobenius norm of W to prevent the over-fitting problem, and C is the tradeoff parameter.', 'To fill the gap between similarity learning and top precision optimization in the problem of content-based image retrieval, we propose a problem of top precision-optimal similarity learning, together with a corresponding solution using a novel algorithm. Our contributions in this paper are divided into two parts, which are given as followed. The proposed problem is to learn a similarity function to compare a query image against a database image. With the similarity scores between query and database images, when retrieval task is performed, we can obtain a maximum top precision measure. The problem is to adjust the parameters of the similarity function, so that the top precision can be maximized. The proposed novel similarity function learning algorithm is to maximize the top precision over a training set of query images and a database of images. We design the similarity function as a linear function of the two feature vectors of a query image and a database image. To learn the parameter matrix of the similarity function, we propose to maximize the top precision for each query, and parallelly minimize the squared Frobenius norm of the parameter matrix in order to prevent the emergence of the over-fitting problem. The optimization problem is modeled by a hinge loss and solved as a quadratic programming.']</t>
         </is>
       </c>
-      <c r="AF72" t="inlineStr"/>
+      <c r="AF72" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article focuses on content-based image retrieval, proposing a novel similarity learning method to optimize top precision performance measure. It does not mention utilizing GA (Genetic Algorithm) for optimizing show parameters and information highlights, which is the claim made in the citation statement."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -11297,7 +11790,14 @@
           <t>['(Incheon, Korea), and GE Healthcare UK Ltd. (Little Chalfont, UK), respectively. Deionized water was used as the solvent for PVA. A 15 μm polyethylene terephthalate (PET) film was supplied by Soojoung Co., Ltd. (Gwangju, Korea). A highabsorbance pad with a three-layered structure of gauze/supersorbent polymer (polyacrylamide)/gauze was purchased from Yuhan Kimberly Co., Ltd. (Daejeon, Korea). Fabrication of pH indicator First, BCP was immobilized on a filter paper using the absorption method (9) by simply immersing the filter paper in 20 mL BCP/PVA/deionized water solution (0.03 g/10 g/90 mL) for 1 h at ambient temperature. Then, the BCP/PVA/filter paper was dried in an oven at 70 o C for 24 h. The filter paper impregnated with BCP and PVA was then cut to the desired shape and size and placed on the PET film.', 'As shown in Fig.  1 , the pH indicator in this study was designed as a three-layered structure with a super-absorbent pad, which was used to prevent direct contact of the dye with the chicken breast and to improve the color change sensitivity of BCP. The effectiveness of the pH indicator was examined by attaching it to the surface of chicken breasts stored at 4 and 10 o C. The indicator response was correlated with pH, volatile basic nitrogen (VBN) content, bacterial growth, and changes in the surface color of the chicken breast. This color-based pH indicator was successfully prepared and tested for the visual monitoring of the real-time freshness of chicken breast in direct contact mode.\n\nMaterials and Methods\nMaterials BCP (dye content 90%) as the dye, 98.0-99.5% hydrolyzed PVA (average molecular weight: 17,500 g/mol) as the binder, and filter paper (Whatman TM Filter Paper No. 42; Whatman plc, Maidstone, UK) as the indicator carrier were purchased from Sigma-Aldrich Co. (St. Louis, MI, USA), OCI Co., Ltd. (Incheon, Korea), and GE Healthcare UK Ltd.', 'As expected, the as-prepared pH indicator shows good response to pH change on the surface of the chicken breast and accumulation of VBN species during storage. Furthermore, there are no visual differences in color changes between the samples stored at 4 and 10 o C, i.e., the visual color of the pH indicator changes only according to pH on the surface of the chicken breast. No migration of the dye from the indicator onto the surface of the chicken breast is detected after 10 days of storage. This indicates that the BCP dye is successfully entrapped within the highabsorbance materials and filter paper in our system, and that the asprepared pH indicators do not show migration problems in our product-indicator direct-contact system. The pH-responsive color change of the as-prepared indicator shows excellent response to pH change on the surface of the chicken breast and the VBN contents, which are strongly correlated to the proliferation of spoilage microorganisms. Thus, the quick and direct detection of chicken breast spoilage by the pH indicator attached to its surface is highly feasible using the pH responsive freshness indicator developed in this study.']</t>
         </is>
       </c>
-      <c r="AF73" t="inlineStr"/>
+      <c r="AF73" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article discusses a pH indicator for monitoring the freshness of chicken breast meat, but does not mention λ exonuclease, streptavidin-gold nanoparticle complexes (SA-AuNPs), or alkaline phosphatase (ALP) at all. The topic and content are unrelated to the statement from the citing article."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -11445,7 +11945,14 @@
           <t>['Such molecules have been tailored to exhibit specific properties for the utilization as molecular pressure sensors,  23  pH-sensitive molecular probes,  24  supersoft elastomers,  25  and therapeutic delivery vehicles.  [26] [27] [28]   The unique shape and easily controlled dimensions (from tens to hundreds of nanometers) of molecular bottlebrushes render them particularly useful as molecular building blocks for generating nanostructured materials by (  1 ) single-molecule manipulation to create well-defined nano-objects, (2) solution self-assembly to produce larger aggregates with different morphologies, and (3) melt self-assembly to fabricate periodic nanomaterials with large domain spacings. In each of these applications, the peculiar properties of bottlebrush copolymers enable the synthesis of previously inaccessible materials in a controlled and predictable fashion. The molecular templating method based on bottlebrush copolymers combines excellent dimensional control of solid templating methods and scalability of self-assembly approaches to provide a robust platform for the construction of 1D nanoobjects with tunable dimensions (Figure  2 ). A molecular bottlebrush can be viewed as a covalently preassembled cylindrical polymer micelle.', '58  Predominantly lamellae morphologies were observed even for highly asymmetric bottlebrush block copolymers (f PLA = 0.3) where the asymmetry was achieved by different length backbones. Interestingly, the obtained d-spacings coincided with the calculated end-to-end distances of a bottlebrush backbone, assuming a fully stretched conformation (Figure  4 ). Grubbs et al. also has shown that the domain spacings for poly(n-butyl acrylate)-polylactide bottle-brush block copolymers were in close agreement with the contour length of a single polymer chain.  59  These observations suggest interdigitated packing of bottlebrush block copolymers, but more studies are necessary to understand the phenomenon. The morphology of blocky bottlebrushes can be manipulated by perturbing their cylindrical shape with the use of different length branches on each side of the bottlebrush. Such asymmetric molecules have been shown to pack into cylindrical microstructures, which upon removal of the minority PLA component provide nanoporous materials with enlarged pores (d pore &gt; 50 nm),  60  difficult to achieve from linear block copolymer precursors.', '29  Muller et al. designed a strategy to produce superparamagnetic nanocylinders by using core-shell bottlebrush copolymers with a poly(acrylic acid) core and a poly(n-butyl acrylate) shell (Figure  2 ).  30  Oxidation of the complexed salts inside the core produced magnetic nanoparticle aggregates, whose dimensions replicated those of the precursor bottlebrushes. Core-shell bottlebrush copolymer templates have also been used to generate magnetite  31  and CdSe 32 nanoparticle arrays, and CdSe  33  and silica  34  nanowires. Porous nanostructures can be produced by peripheral crosslinking and subsequent core removal of core-shell bottlebrushes (Figure  2b ). Wooley et al. used molecular brushes with a polyisoprene core and a poly(acrylic acid) shell to generate hollow spherical nanocages.  35  Our group has developed a method for the synthesis of organic nanotubes with wellcontrolled dimensions from multicomponent molecular bottlebrushes.']</t>
         </is>
       </c>
-      <c r="AF74" t="inlineStr"/>
+      <c r="AF74" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article does not mention PNK or any relevant information about sensors, selectivity, or peak current. The content appears to focus on molecular bottlebrushes and their applications in nanomaterials fabrication, which is unrelated to the statement from the citing article."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -11589,7 +12096,14 @@
           <t>['The dissolution equation was written to focus on the loss of the nanoparticle, which is why C is concentration of nanoparticle and not dissolved ion, so the negative is not a typo. In regard to atmospheric dry deposition, we again elected throughout the model not to incorporate a distribution of particle sizes because nanoFate is meant to be a screening level tool. The referenced equation relies on Stoke’s Law5 and is used in nanoFate to calculate deposition of both ENMs associated with aerosols and individual or small aggregates of ENMs of a specified particle size. Particle radius is therefore accounted for in the calculation of both wet and dry deposition in Rp (particle radius), and as with other models that use this equation, if the particles are of varying sizes, then there will be some variability in the predictions. This equation is a reasonable simplification of a rather complex process, which may be improved when better models of atmospheric deposition (wet and dry) of nanoparticles are developed. The primary reason for not explicitly considering multiple particle sizes is due to a lack of experimental data to parametrize the model with realistic particle size distributions for each environment.', 'After carefully reviewing the comments from Cohen et al., we have compiled the following clarifying statements.First, we did not intend to imply that MendNano is a steadystate model. We recognize that MendNano is a dynamic model though many aspects in the publication appear to rely primarily on steady state assumptions. As the authors of MendNano, we are sure that Cohen et al. are more familiar with their model than anyone else. Generalizations on our part may be due to limited space. Second, our statement regarding MendNano’s capabilities was not that the model cannot be used to look at different land uses or water types, but rather that from the published works, we were under the impression that only one\ntype can be considered at a time. We did not consider nor state that dissolution is independent of particle size. Rather that, as a screening tool, we chose to limit the complexity required by introducing particle size distribution not unlike other existing models and most MFA models. This necessitated simplifying the calculations so that the amount of data necessary to run the model was manageable. In addition, we felt that modeling dissolution patterns at the individual particle scale when trying to represent a much larger region would not be efficient.', 'Among other limitations, the fact that, at the time, we did not have realistic distributions of ENM size at the point of release to the environment made it difficult to include particle size in a screening level model. The goal was to holistically and mechanistically consider the most significant processes without making the model too difficult to use. These simplifications are common in environmental modeling and acceptable if clearly communicated and justified scientifically.']</t>
         </is>
       </c>
-      <c r="AF75" t="inlineStr"/>
+      <c r="AF75" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article does not provide any information about SA-AuNPs or their role in amplifying electrochemical signals, which is the claim made in the citation statement. The excerpts provided discuss topics unrelated to the claim, such as nanoparticle dissolution and atmospheric deposition."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -11740,7 +12254,14 @@
           <t>['The study designs, methods, and findings of these studies are summarized in Table  2 . Three of the four studies focused on preschool children (baseline ages 3 to 5)  (27) (28) (29) (30) (31) (32) (33) (34) (35)  and one study focused on infants  (36) . The dose of physical activity was defined and measured differently among the studies and included recreational gymnastics participation (months)  (28) (29) (30) , device-measured daily activity (min)  (31) (32) (33) (34) , and bone-strengthening physical activity (sessions)  (27, 35, 36) . All studies used state-of-the-art imaging (dual-energy x-ray absorptiometry (DXA) and peripheral quantitative computed tomography (pQCT)) to measure bone outcomes and appropriate statistical modeling to control for growth. All studies examining children ages 3-5 years showed statistically significant stronger bone in the more active children. The benefit differences were greater than expected via measurement error and large enough (almost always &gt;3%) to indicate meaningful biological improvements.', 'However, similar to the evidence for body weight and adiposity, the differences in physical activity measures prevented the assignment of a specific dose of physical activity needed for bone health benefits.\n\nCardiometabolic health.\nVery few studies have examined the association between physical activity and indicators of cardiometabolic health in children younger than age 6 years. The literature search resulted in the identification of three prospective cohort studies that included outcomes related to serum lipid and lipoprotein levels, respiratory symptoms, and blood pressure  (37) (38) (39) . One study reported that physical activity appeared to have an indirect association with blood lipids and lipoproteins in 3-4 year old children, through its relationship with lower levels of body fatness and higher levels of fitness  (37) ; while another study reported an inverse association between physical activity and diastolic blood pressure in 5-7 year-old children  (39) . A final study reported that physical activity at 2 years of age was not related to respiratory symptoms such as wheezing or shortness of breath at 3-4 years of age  (38) .', "All of the studies included in this review employed prospective, longitudinal study designs. However, methods for measurement of physical activity were highly variable. Also, the studies were quite variable in terms of children's age range, years of follow-up, measurement of weight-related outcomes, and analytic procedures. Not withstanding these differences, the studies were consistent in reporting that higher levels of physical activity were associated with lower levels of weight and/or adiposity in younger children. Twelve of the 15 studies found negative associations between physical activity and weight and/or adiposity  (12-16, 18, 20-25) . While these studies were consistent in observing benefit with higher amounts of physical activity, limitations in study design and variability in methodologies across the studies precluded identifying a particular dose of physical activity that was needed to provide benefits.\n\nBone health.\nThe literature search provided eight papers, with two additional papers added by committee members. These 10 papers represented four studies, two of which had prospective longitudinal study designs and two of which were randomized controlled trials  (27) (28) (29) (30) (31) (32) (33) (34) (35) (36) ."]</t>
         </is>
       </c>
-      <c r="AF76" t="inlineStr"/>
+      <c r="AF76" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article does not mention PNK or the correlation between electrochemical signal reduction and active concentration of PNK. The abstract and provided excerpts focus on physical activity, health outcomes in children younger than 6 years, bone health, cardiometabolic health, and cognition, with no relevance to PNK or electrochemical signals."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -12028,7 +12549,14 @@
           <t>['We strongly believe that it is an interesting and new problem for the upcoming researchers who can obtain similar inequalities via quantum fractional calculus in their future work.', 'introduced the notion of D q b derivative and integral  [21] . Many well-known integral inequalities such as Hölder inequality, Hermite-Hadamard inequalities, Ostrowski inequality, Cauchy-Bunyakovsky-Schwarz inequality, Gruss inequality, Gruss-Cebyšev inequality, and other integral inequalities have been studied in the setup of q-calculus using the concept of classical convexity. For more results in this direction, the readers may refer to  [8, 13, 14, [22] [23] [24] [25] [26] [27] [28] [29] [30] [31] [32] [33] [34] [35] [36] [37] [38] . 2 Preliminaries of q-calculus and some inequalities In this section, we first present some known definitions and related inequalities in q-calculus. Set the follow- ing notation (see  [16] ): [ ] = - - = + + +⋯+ ∈ ( ) - n q q q q q q 1 1 1 , 0 , 1 .', 'The constant 1 4 is the best possible. Ostrowski inequality has applications in quadrature, probability and optimization theory, stochastic, statistics, information, and integral operator theory. During the past few years, a number of scientists have focused on Ostrowski-type inequalities for function of bounded variation, see, for example,  [2] [3] [4] [5] [6] [7] [8] [9] [10] [11] ,  [12, pp. 468-484] . Until now, a large number of research papers and books have been written on Ostrowski inequalities and their numerous applications. On the other hand, many studies have recently been carried out in the field of q-analysis, starting with Euler due to a high demand for mathematics that models quantum computing q-calculus appeared as a connection between mathematics and physics. It has several applications in different mathematical areas such as number theory, combinatorics, orthogonal polynomials, basic hypergeometric functions, and other sciences, quantum theory, mechanics, and the theory of relativity  [13] [14] [15] [16] .']</t>
         </is>
       </c>
-      <c r="AF78" t="inlineStr"/>
+      <c r="AF78" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article does not mention anything related to ferrofluid convection, electric fields, nano-powders, or vibrations. The content of the reference is entirely focused on quantum Ostrowski-type inequalities and q-calculus, which appears unrelated to the claims made in the citation statement."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -12176,7 +12704,14 @@
           <t>['Let n ∈ N. Then the the special sums of reciprocal powers λ (n + 1), η(n) and β (n)  [1]  are defined by λ (n + 1) = ∞ ∑ k=0 1 (2k + 1) n+1 , η(n) = ∞ ∑ k=1 (-1) k-1 1 k n , β (n) = ∞ ∑ k=0 (-1) k 1 (2k + 1) n . (2.1) It follows from  [1, 23.2.20]  that λ (n + 1) = 1 -2 -n-1 ζ (n + 1), η(n) = 1 -2 1-n ζ (n). (2.2) LEMMA 2.1.', 'In particular, the double inequality 2 H 1 n 1 2 + 2η(2n) x 2n+2 x(1 -x)B(x) -P 1 n (x) + 2η(2n)x 2n+1 H 1 n 1 2 + 2η(2n) x 2n+1 (3.3) holds for all n ∈ N and x ∈ (0, 1/2], and each inequality of  (3.3)  becomes equality if and only if x = 1/2 . (2) The function H 2 n (x) defined by H 2 n (x) = f (x) -P 2 n (x) x 2n with P 2 n (x) = 1 + ∑ 2n-1 k=1 A 1 (k)x k is strictly decreasing and convex from (0, 1/2] onto [H 2 n (1/2), 2η(2n)).', '. Therefore, (G 2 n (x)) is strictly decreasing on (0, 1/2] follows from Lemma 2.2 and Theorem 3.1. Note that G 2 n (0 + ) = B 1 (2n + 1). Hence, inequality (3.11) can be derived from the monotonicity and concavity of the function G 2 n (x). (3) It follows from (3.1) that g(x) -R 3 n (x) = ∞ ∑ k=0 [4λ (2k + 2n + 1) -β (2k + 2n -1) -3β (2k + 2n + 1)](1 -2x) 2k+2n and K n (x) = ∞ ∑ k=0 [4λ (2k + 2n + 1) -β (2k + 2n -1) -3β (2k + 2n + 1)](1 -2x) 2k .']</t>
         </is>
       </c>
-      <c r="AF79" t="inlineStr"/>
+      <c r="AF79" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article [10] discusses mathematical functions, bounds, and inequalities involving the Beta function and Ramanujan R-functions. There is no mention of nanoliquids, heat transfer, or typical fluids with nano-powders in the provided abstract and excerpts, which are key components of the citation statement."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -12324,7 +12859,14 @@
           <t>['MWCNT has extraordinary thermal properties and can be widely used industrially and commercially as a new generation of refrigerants and thermal operating fluids. The use of these nanofluids in thermal systems can increase the efficiency and significantly increase the Nusselt number and heat transfer coefficient in equal Reynolds. This group of nanofluids in different base fluids such as ethylene glycol and water with suitable stability can be provided. The physical properties of the nanofluid should be determined based on the nanoparticle and base fluid physical properties. These properties include viscosity, density, thermal conductivity and specific heat  Ehyaei et al. (2019) . The physical properties of nanofluids can be obtained using the following equations  (Khanjari et al. 2016; Loni et al. 2017; Zadeh et al.', 'In addition, the impact of the use of nanofluids on the performance of systems is investigated. Dowtherm Q is a synthetic organic HTF containing a mixture of alkylated aromatics and diphenylethane. Compared to hot oils, it represents better thermal consistency and significantly better low-temperature pump ability.', '(2019)  with various nanofluids. The results showed that the exergy and energy performance of the FPC system improved by 57% and 20%, respectively, when Al 2 O 3 nanofluid was used.  Pavlovic et al. (2018)  examined the performance of PDC system by different nanofluids and corrugated and smooth spiral absorber. They concluded that the best performance of the system is achieved when thermal oil is used as the base fluid and copper as the nanoparticle. In a similar study,  Loni et al. (2018)  an improvement in the thermal and exergetic performance of the system when using water based CuO and Al 2 O 3 nanofluids. In that PDC system the concentration ratio was 28.5. In addition, the exergy and energy efficiencies of the system were 10% and 35%, respectively.  Yaqi et al. (2011)  provided an efficiency of 34% with a concentration ratio of 1300 for the PDC system.']</t>
         </is>
       </c>
-      <c r="AF80" t="inlineStr"/>
+      <c r="AF80" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Substantiated",
+  "explanation": "The reference article discusses the use of nanofluids, such as MWCNT, in solar collectors to improve heat transfer. Excerpt 1 specifically mentions that MWCNT has extraordinary thermal properties and can increase efficiency and heat transfer coefficient. This supports the statement that nanoliquids have a great range of heat transfer."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -12472,7 +13014,18 @@
           <t>["This hypothesis was based on two lines of reasoning: (i) an earlier study reporting an increase in salivary OXT concentrations (139% of basal) after 30 min of choir rehearsal, including 10 min of warm-up exercises and repeatedly singing the pop-song ''California Dreaming''  (Kreutz, 2014) ; and (ii) reports of other positive social experiences resulting in OXT secretion, such as intense parent-child interactions, massage, gossiping with friends, and loving interactions between participants and their dogs  (Grewen et al., 2005; Gonzaga et al., 2006; Feldman et al., 2010; Beetz et al., 2013; Kim et al., 2014; Tsuji et al., 2015; Krause et al., 2016; Lebowitz et al., 2016; Brondino et al., 2017) . Of course, it may be that positive bilateral interactions or the powerful intimate bond between parents and their children, romantic partners, or dogs and their owners are needed to trigger the OXT system to a quantifiable extent-aspects that are missing from choir singing.", 'OXT has been proposed to represent the biological link between the intense social experience of choir singing and its positive psychosocial effects  (Chanda and Levitin, 2013; Kreutz, 2014) . However, previous studies reported inconsistent results, i.e., increased or decreased salivary OXT concentrations  (Kreutz, 2014; Fancourt et al., 2016)  and stable plasma OXT levels  (Keeler et al., 2015)  in response to choir singing. Similarly, some studies found that choir singing resulted in reduced activity of the hypothalamic-pituitary-adrenal (HPA) axis as reflected by lower levels of adrenocorticotropic hormone (ACTH) and CORT in plasma  (Beck et al., 2000; Keeler et al., 2015)  and saliva  (Fancourt et al., 2016) , whereas others could not confirm this in saliva samples  (Kreutz et al., 2004; Kreutz, 2014) .', 'It is possible that increases or decreases in stress/arousal, rather than social experience, drives salivary OXT concentrations. In other words, singing may cause an increase (or a decrease) in stress signals from the brain stem and/or amygdala to the hypothalamus, resulting in the activation (or quiescence) of the HPA axis and the OXT system. If this is true, it can be expected that CORT responses resemble OXT responses to singing. This was indeed the case in previous studies:  Kreutz (2014)  reported an increase in both OXT and CORT concentrations after choir singing (but note that the reported CORT values were supraphysiologically high), whereas  Fancourt et al. (2016)  reported a decrease in both OXT and CORT concentrations. In the present study, choir singing also coincided with a marked reduction in both OXT and CORT concentrations, whereas solo singing mildly triggered both the HPA axis and the OXT system relative to choir singing.']</t>
         </is>
       </c>
-      <c r="AF81" t="inlineStr"/>
+      <c r="AF81" t="inlineStr">
+        <is>
+          <t>Here is my evaluation:
+```
+{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article does not support the statement that oxytocin is increased when participating in group singing, including improvisation. In fact, the study found that salivary oxytocin concentrations were significantly reduced after choir singing, and did not change in response to solo singing."
+}
+```
+This label is chosen because the citation statement claims an increase in oxytocin levels due to group singing, whereas the reference article actually reports a decrease in salivary oxytocin concentrations after choir singing. This contradiction justifies the "Unsubstantiated" classification.</t>
+        </is>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -12620,7 +13173,14 @@
           <t>['The connexins form a closely related family exhibiting extensive amino acid identity and similarity within their transmembrane and extracellular domains. The similarities in their extracellular loops can be described by two connexin signatures (PS00407 and PS00408,  http://prosite.expasy.org/PDOC00341 ). Differences and similarities in the connexin sequences have been used to define connexin subfamilies  [7, 30] , and sequence comparisons between different species have been used to identify orthologs  [18] . Currently, five connexin subfamilies are recognized (α, β, γ, δ, and ε or GJA, GJB, GJC, GJD, and GJE) (Table  1 ). A wide range of genetic diseases have been mapped to mutations of the connexin encoding genes (including deafness, neuropathies, cataracts, skeletal abnormalities, and skin diseases) (reviewed in  [9, 31, 37, 38, 46, 48, 53, 55] ).', '[28] . Biochim Biophys Acta. Author manuscript; available in PMC 2018 July 01.', 'Unlike the connexins, pannexins undergo glycosylation within their extracellular regions. This modification may be important for the targeting of pannexins to the plasma membrane  [11, 39] . Pannexin glycosylation may effectively impede cell-to-cell channel formation and regulate pannexin intermixing  [40] . Some innexins may also be glycosylated; for example, two yellow fever mosquito (Aedes aegypti) innexins (AeInx3 and AeInx7) contain predicted N-glycosylation sites, and immunoblots of AeInx3 show multiple immunoreactive bands. This similarity to the pannexins suggests that some innexins might have other functional roles besides intercellular communication  [15] . Pannexins have been implicated in several pathologies including cardiovascular diseases, inflammation, cancer and neuropathies  [6, 41, 57] . Due to their wide expression in many tissues and organs, deleterious pannexin gene mutations might be expected.']</t>
         </is>
       </c>
-      <c r="AF82" t="inlineStr"/>
+      <c r="AF82" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article does not provide a review characterizing the possible mechanism of action for extracellular loop peptides. Instead, it provides an overview of gap junction channels and protein families, discussing connexins, innexins, and pannexins. The excerpts mention the structure and function of these proteins but do not specifically address the mechanism of action for extracellular loop peptides."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -12771,7 +13331,14 @@
           <t>['release in initiating early changes of tubular injury were assessed. Human renal proximal tubule epithelial cells were incubated with TGF-β1 (10 ng/mL) ± Peptide 5 (25 μM) for 48 h. Co-incubation of hPTECs with TGF-β1 and Peptide 5 restored ECAD expression (Fig.  7a ) from 31.5 ± 9.2% to 108.9 ± 17.1%; NCAD expression (Fig.  7b ) from 280.5 ± 16.7% to 154.7 ± 10.6%; Claudin-2 expression (Fig.  7c ) 65.3 ± 5.4% to 100.9 ± 10% and finally ZO-1 expression (Fig.  7c ) from 59.63 ± 3.1% to 91.6 ± 12.8% as compared to low-glucose control. Incubation of cells with either Peptide 5 alone or a scrambled version of Peptide 5, failed to change expression of our candidate proteins.', 'Peptide 5 is a 12 amino acid peptide which targets the 2nd extracellular loop of Cx43  [52] , it has been proven successful in blocking Cx43 hemichannels when delivered topically, intraocularly  [53] , into cerbebrospinal fluid and systemically  [52] . Multiple approaches have been used to confirm target applicability and specificity and all have yielded similar and significant benefits across different injury models. The ability of Peptide 5 to block hemichannel activity, ATP-release and ultimately disassembly of the adherens/tight junction complex in our model system, was assessed by carboxyfluorescein dye uptake, ATP-biosensing and Fig.  8  Cx43 +/-mice exhibit minimal disassembly of the adherens and tight junction complex. Quantification of immunohistochemical staining determined an increase in N-cadherin (a &amp; c) and decrease in ZO-1 (b &amp; d) expression in wildtype (WT) UUO compared to WT sham controls. In Cx43 +/-(UUO) mice, expression of both markers was partially restored to near basal levels.', 'For all experiments, inhibitors alone failed to induce any significant change in expression.\n\nPeptide 5 inhibits TGF-β1-induced Cx43 hemichannel activity and ATP release\nTo study the efficacy of Peptide 5 in blocking Cx43 mediated hemichannel activity in renal tubule epithelial cells, HK2 and hPTECs were incubated in TGF-β1 (10 ng/mL) ± Peptide 5 (25 μM) for 48 h. Dye uptake increased in TGF-β1-treated HK2 cells to 609.4 ± 46% compared to unstimulated control (Fig.  6a  &amp;  b ), whilst co-incubation with Peptide 5 reduced uptake to 163 ± 10.2%. Co-incubation with scrambled peptide failed to blunt the TGF-β1 response (671.5 ± 29.5%, Fig.  6a  &amp;  b ). The effects were matched in primary hPTECS, where Peptide 5 significantly reduced uptake to 141.7 ± 16.3% from 311.2 ± 39.6% in TGF-β1 treated cells (Fig.']</t>
         </is>
       </c>
-      <c r="AF83" t="inlineStr"/>
+      <c r="AF83" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article does not mention the effect of Peptide5 on retinal pigment epithelial cell barrier function, which is the specific claim being evaluated. The article actually discusses the role of Connexin43 in early tubular injury in experimental chronic kidney disease and the protective effects of blocking its hemichannel activity with Peptide 5."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -12919,7 +13486,14 @@
           <t>['Peptides mimicking CL sequences have been frequently used as control peptides for gap junction work, since it was shown that these do not inhibit gap junctional coupling  (Evans and Leybaert, 2007) . Although this specificity has already been reported for the cardiac system  (Wang et al., 2013b)  we think that it is important to validate this property for the nervous system. Indeed, this is particular relevant for the astrocytes because Cx43 hemichannels contribute to "gliotransmission" and can thus be involved in neuroglial interactions that participate to the control of neuronal activity and survival (see  Giaume et al., 2013) . In line with this, we found that Gap19 did not inhibit gap junction coupling in astrocytes as measured with dye transfer assays. At the same time, however, Gap19 strongly inhibited Cx43 hemichannels as exemplified by ATP release and dye uptake assays. Finally, we provide evidence that the TAT version of Gap19 is able to cross the intact blood-brain barrier indicating that this peptide can be used to block astroglial Cx43 hemichannel activity when applied through a vascular route.', 'TAT-Gap19 PEPTIDE\nTAT-Gap19 (YGRKKRRQRRR-KQIEIKKFK) was synthesized by Pepnome Inc. (Hongkong, China) at a purity of 95%. It was dissolved in PBS and aliquoted/stored as a stock solution of 10 mM.\n\nDATA ANALYSIS AND STATISTICS\nThe data are expressed as mean ± s.e.m., with "n" denoting the number of independent experiments. Two groups were compared by student\'s t-test and two-tail p-value. In experiments where the effects of different treatments were assessed on normalized data, non-parametric ANOVA Kruskal-Wallis tests were performed. Tests with significance of p &lt; 0.05 were followed by a Dunn\'s multiple comparison post-hoc test using the GraphPad Prism version 5.00 (San Diego, CA, USA). Unless stated otherwise, significance as compared to control condition based on the raw data (before normalization) was assessed by two-tailed Wilcoxon signed-ranked tests. The level of significance was set at p &lt; 0.05.', 'Finally, the effects of Gap19 on hemichannel activity reported here are similar to those previously described for Gap26 and Gap27 that also blocks hemichannel activity in astrocytes induced by LPS or pro-inflammatory treatments in culture astrocytes (see  Retamal et al., 2007; Froger et al., 2010)  and in acute brain slices treated with the amyloid peptide  (Orellana et al., 2011) . have also published that carbenoxolone blocks hemichannel activity induced by a calcium free solution  (Rouach et al., 2008, Supplementary Data Figure S5) . The in vivo injection experiments demonstrate that TAT-Gap19 can be detected in the brain tissue, based on immunostaining for the TAT moiety of the peptide (Figure  4 ). This observation indicates that TAT-Gap19 can successfully cross the blood-brain barrier, which is expected as a result of the presence of the TAT membrane translocation motif. We did not quantify the immune signal in terms of estimates of the concentration attained.']</t>
         </is>
       </c>
-      <c r="AF84" t="inlineStr"/>
+      <c r="AF84" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article does not mention chronic kidney disease, which is the topic related to reference number 109 in the citation statement. The article focuses on the effects of Gap19 on astroglial Cx43 hemichannels and gap junction channels in astrocytes, with no discussion of kidney disease or Peptide5."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -13074,7 +13648,14 @@
           <t>['Background\nAnal incontinence is a disabling condition that adversely affects the quality of life of a considerable number of patients (2-15 % of the general population)  [1, 2] . Injury of the anal sphincters (mainly post surgical or post delivery) is the most common cause of incontinence, and surgical repair is actually the treatment of choice. Clinical studies reported a relatively good success rate of surgical repair in patients with sphincter lesions but the initial results worsened in time with only 30 % of patients demonstrating full continence 5 years after surgery  [3] [4] [5] . Other approaches such as the use of injectable bulking agents to augment anal sphincter function have been used recently in several observational studies  [6]  but generally resulted in poor outcomes  [3, 7] . Recently, the use of adult stem cells (ASC) in regenerative medicine protocols has become a promising therapeutic approach for organ or tissue repair when the conventional therapies are ineffective  [8] .', 'Serial cryostat sections, 10 μm thick, were fixed overnight at -20 °C in formaldehyde vapors  [24]  and stored at -80 °C until use  [23] . Some of these sections were stained with 0.1 % toluidine blue and used to quantify the regeneration of the sphincters. Because sections stained with toluidine blue provide a less detailed visualization and anatomic resolution of the anal sphincter complex than those embedded in methacrylate, the whole tissue at the site of SR was examined without separate analysis of each sphincter. A mean of eight microscopic fields were manually searched at the site of repair at 4× magnification and the muscle area fraction (MAF) was evaluated with the "Area" function of the Nikon NIS-Elements software version 2.30 and calculated as differences between the area of muscle elements and the total area examined. Data were expressed as a percentage of the mean value of the control\'s total area. The analysis was performed by two independent operators in a blinded fashion. Other cryostat sections were used for double immunofluorescence staining for alpha smooth muscle actin (α-SMA) and GFP.', 'A second group underwent SR of the anal sphincter followed by intrasphincteric injections of syngeneic in-vitro expanded BM-derived GFP-MSC (MSC group). A third group underwent SR of the anal sphincter followed by intrasphincteric injections of syngeneic minimally manipulated BM-derived GFP-MNC (MNC group). The fourth group underwent sham operation without sphincter injury plus intrasphincteric saline solution injections (SHAM group). Sphincterotomy was carried out under an operating microscope (Carl Zeiss OMPI CS XY) by an open, left lateral, full thickness sphincterotomy of both anal sphincters as described previously  [16] .']</t>
         </is>
       </c>
-      <c r="AF85" t="inlineStr"/>
+      <c r="AF85" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article discusses the use of bone marrow progenitor cells for treating anal sphincter injury and does not mention surgical repair of anal sphincter tears after delivery. The article focuses on a preclinical model using rats, whereas the citation statement refers to human clinical practice."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -13229,7 +13810,14 @@
           <t>['Background\nAnal incontinence is a disabling condition that adversely affects the quality of life of a considerable number of patients (2-15 % of the general population)  [1, 2] . Injury of the anal sphincters (mainly post surgical or post delivery) is the most common cause of incontinence, and surgical repair is actually the treatment of choice. Clinical studies reported a relatively good success rate of surgical repair in patients with sphincter lesions but the initial results worsened in time with only 30 % of patients demonstrating full continence 5 years after surgery  [3] [4] [5] . Other approaches such as the use of injectable bulking agents to augment anal sphincter function have been used recently in several observational studies  [6]  but generally resulted in poor outcomes  [3, 7] . Recently, the use of adult stem cells (ASC) in regenerative medicine protocols has become a promising therapeutic approach for organ or tissue repair when the conventional therapies are ineffective  [8] .', 'Serial cryostat sections, 10 μm thick, were fixed overnight at -20 °C in formaldehyde vapors  [24]  and stored at -80 °C until use  [23] . Some of these sections were stained with 0.1 % toluidine blue and used to quantify the regeneration of the sphincters. Because sections stained with toluidine blue provide a less detailed visualization and anatomic resolution of the anal sphincter complex than those embedded in methacrylate, the whole tissue at the site of SR was examined without separate analysis of each sphincter. A mean of eight microscopic fields were manually searched at the site of repair at 4× magnification and the muscle area fraction (MAF) was evaluated with the "Area" function of the Nikon NIS-Elements software version 2.30 and calculated as differences between the area of muscle elements and the total area examined. Data were expressed as a percentage of the mean value of the control\'s total area. The analysis was performed by two independent operators in a blinded fashion. Other cryostat sections were used for double immunofluorescence staining for alpha smooth muscle actin (α-SMA) and GFP.', 'A second group underwent SR of the anal sphincter followed by intrasphincteric injections of syngeneic in-vitro expanded BM-derived GFP-MSC (MSC group). A third group underwent SR of the anal sphincter followed by intrasphincteric injections of syngeneic minimally manipulated BM-derived GFP-MNC (MNC group). The fourth group underwent sham operation without sphincter injury plus intrasphincteric saline solution injections (SHAM group). Sphincterotomy was carried out under an operating microscope (Carl Zeiss OMPI CS XY) by an open, left lateral, full thickness sphincterotomy of both anal sphincters as described previously  [16] .']</t>
         </is>
       </c>
-      <c r="AF86" t="inlineStr"/>
+      <c r="AF86" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article does not mention childbirth trauma or the specific percentage (11%) of vaginal deliveries resulting in acute anal sphincter injury. The abstract and provided excerpts focus on the treatment of anal sphincter injury using bone marrow progenitor cells, but do not provide any information about the incidence or causes of such injuries."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -13380,7 +13968,14 @@
           <t>['42, 43  Thus, additional studies will be necessary in the future to examine and compare different stem cells proposed to anal sphincter repair after injury.\n\nCONCLUSIONS\nThis study provides an experimental basis for potential future clinical application of stem cells therapy for anal sphincter injuries. Stem cells could be injected at the moment of surgical repair or percutaneously by ultrasonographic guide in selected injured areas and improve the regeneration and the healing of damaged anal sphincters. Nevertheless, further studies are required to confirm and expand our preliminary results before attempting this in the clinical setting.', 'A nal incontinence is a disabling condition that affects a large number of patients and may have devastating effects on quality of life. \n1, 2  The mechanism of continence is complex and involves many structures and pathways. Disruption of the anal sphincters is one of the most common causes of anal incontinence and may occur as the result of obstetric injury, anorectal surgery, or trauma.  [3] [4] [5] [6] [7] [8]  Sphincter repair is the operation of choice in patients with damaged anal sphincters, and clinical series have reported a relatively good success rate after treatment. However, the initial symptomatic improvement is not always maintained with time and long-term outcome remains unsatisfactory.  [9] [10] [11] [12] [13] [14]  Many reports have demonstrated that mesenchymal stem cells derived from bone marrow (MSC) can differentiate into mature cells of many tissues.  15, 16  In particular, injected MSC engraft and form multinucleated myotubes in skeletal muscle under appropriate stimuli, i.e., injury, contributing to muscle regeneration.', '13, 29, 30  Therefore, the contribution of injected MSC to anal sphincter regeneration on a preexisting scar and after delayed repair, with fibrosis and weakness of the sphincter, needs to be assessed in further experiments. Moreover, each sphincter was divided and repaired one by one, and, at histologic examination, we found that MSC improved smooth or striated muscular regeneration if injected into the IAS or the EAS, respectively. Nevertheless, a mixed repair of the sphincter complex may occur after a crushed injury, and the contribution of stem cells to such a repair needs to be further investigated. Another interesting finding is that there were no significant differences between results of the two groups treated with MSC. Autologous cells undoubtedly present major advantages; however, allogenic cells may be useful when a rapid employement is required, even if a period of immunosuppressive therapy has to be administered.  41  In our experiment, immunosuppression with CsA had no negative effects on the outcome of sphincter repair associated with MSC injection. Furthermore, it has been shown that various stem cell types, including muscle-derived cells, can differentiate into muscle lineage.']</t>
         </is>
       </c>
-      <c r="AF87" t="inlineStr"/>
+      <c r="AF87" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article does not mention dedicated stem cells of the anal canal transition zone positive for cytokeratin 17 participating in the healing process of the mucosa of the rectum and the anal canal. The article focuses on bone marrow-derived mesenchymal stem cells improving muscle regeneration and increasing contractile function of anal sphincters after injury and repair, but does not discuss cytokeratin 17 or the specific cell type mentioned in the citation statement."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -13532,7 +14127,15 @@
           <t>['Only one of our cases had diabetes mellitus. In granuloma annulare the primary event is also thought to be collagen degeneration. Electron microscopy shows degeneration of elastic and collagen fibres in necrobiotic areas.\'*^\'\'\' Vascular changes are few."* A cell-mediated immune reaction has been implicated with the demonstration of increased numbers of T helper/inducer lymphocytes within the granulomatous infiltrate, an increased number of 0KT6 positive Langerhans cells within epidermis and dermis, and increased HLA-DR antigen and interleukin 2 receptor expression.\' ^ The increased numbers of S100 positive cells in granuloma annulare lends some support to these findings, but the numbers are higher in necrobiosis Hpoidica and other known type IV delayed hypersensitivity reactions."^ In conclusion, an increase in the number of epidermal dendritic Sioo positive cells above the basal layer, as well as implicating a cell mediated immune-reaction, may provide an adjunct to histological means of distinguishing between necrobiosis lipoidica and granuloma annulare.', 'None of the eight patients with granuloma annulare were known to be diabetic.\n\nDISCUSSION\nAlthough clinically different, the similarity of the histological features of granuloma annulare and necrobiosis lipoidica raises the possibility of a common pathogenesis. We have determined the dendritic S100 protein positive subset of the Langerhans cell population in the epidermis in these two conditions. There was a significantly higher number of Sioo positive dendritic cells within the epidermis, above the basal layer, in necrobiosis lipoidica compared with both normal skin and granuloma annulare. In the latter the numbers of cells were elevated, but not to a significant level above normal. This suggests that the pathogenesis of the two conditions may be different. We have found that the numbers of Sioo positive epidermal dendritic cells are elevated to a similar level to that seen in necrobiosis lipoidica in sarcoidosis, positive Kveim test biopsies, tuberculous leprosy and other tuberculous reactions (unpublished data).', 'There was no disparity between the histological and clinical diagnoses in any of the cases. All showed the recognized features of collagen degeneration, some having palisaded granulomas. In the majority, the full thickness of the biopsy that included the tower reticular dermis was involved by the lesions. Dendritic cells were seen positively stained, lying between keratinocytes, within the epidermis (Fig.  i ). There was an increase in numbers of epidermal dendritic Sioo positive cells in both granuloma annulare (mean 80) and necrobiosis lipoidica (mean 24 5), compared with normal skin controls (mean 37) (see Table  i} . The numbers were higher in necrobiosis lipoidica than granuloma annulare (o 001 &gt; P &gt; 0 0005); but there was no statistical difference between granuloma annulare and the control group (015 &gt; P&gt;oio).']</t>
         </is>
       </c>
-      <c r="AF88" t="inlineStr"/>
+      <c r="AF88" t="inlineStr">
+        <is>
+          <t>Here is my evaluation of whether the reference article supports the citation statement:
+{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article does not support the claim that 'the number of S100 positive dendritic cells within the epidermis and dermis was increased in granuloma annulare.' While the article mentions an increase in S100 positive cells in granuloma annulare, it specifically states that this increase is not statistically significant compared to normal skin controls (Excerpt 3). In fact, the numbers of S100 positive cells are higher in necrobiosis lipoidica than in granuloma annulare."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -13684,7 +14287,14 @@
           <t>['RNP antibodies were found in five cases negative for Scl 70, four cases of acrosclerosis and one of diffuse scleroderma. Nucleolar staining without any associated patterns was found in five cases, four of acrosclerosis and one of diffuse scleroderma, all negative for Scl 70.\n\nDISCUSSION\nScl 70 antibody was found to be a specific serological marker of systemic scleroderma. In our series it was detected at a much higher frequency than reported in previous publications  (Tan et al., 1980; Catoggio et al., 1983) , but comparable results have been reported recently by  Takehara, Moroi and Ishibashi (t985) . The higher detection rates of Scl 70 in our study,  77",, in 13652133, 1986, 4 , Downloaded from  https://onlinelibrary.wiley.com/doi/10.1111/j .  1365-2133.1986.tb06233. x by Hochschule Mannheim, Wiley Online Library on [05/03/2025].', 'Thus, Scl 70 appears to be highly specific of systemic sclerosis. Patients with acrosclerosis positive for ACA were invariably negative for Scl 70 (Table  3 ). Conversely, patients with acrosclerosis negative for ACA were found to be positive for Scl 70 in 63"(, cases, whereas in acrosclerosis patients as a whole Scl 70 antibody was present in 44",, ofthe cases (Table  1 ). It should be emphasized that among 39 cases of diffuse scleroderma, 16 observed by us for more than 10 years were classified initially as severe acrosclerosis or transitional form, acrosclerosis-diffuse scleroderma. The frequency of Scl 70 antibody in this group was 12 of 16 C75"o), ie. essentially the same as in typical cases of diffuse scleroderma. Therefore, the transitional form was grouped with diffuse scleroderma. Immunofiuorescence studies on HEp-2 showed a characteristic pattern with all sera positive in the immunodiffusion test for Scl 70 antibody.', 'Thus, it is conceivable that Scl 70 antibody occurs even more frequently than detected in our study. In contrast to ACA antibody, which is a marker of an abortive subset of acrosclerosis with almost no cutaneous indurations  (Chorzelski et al., 1985) , Scl 70 is a marker of systemic sclerosis as a whole, with prevalence in diffuse scleroderma, but present also in a high proportion of cases of acrosclerosis. Thus, it does not discriminate between the subsets of systemic scleroderma. There were only slight clinical differences between cases positive and negative for Scl 70. In patients with acrosclerosis negative for Scl 70, the indurations were confined more frequently to the fingers and there were fewer contractures of the fingers; calcinosis was found in a somewhat larger proportion of the patients, and there was no induration or atrophy on the trunk; the disease was thus less severe than in patients positive for Scl 70 antibody. In patients with diffuse scleroderma the clinical differences between patients positive and those negative for Scl 70 were less conspicuous.']</t>
         </is>
       </c>
-      <c r="AF89" t="inlineStr"/>
+      <c r="AF89" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Substantiated",
+  "explanation": "The reference article reports that Scl 70 antibodies were found in 77% of cases of diffuse scleroderma, which is close to the cited frequency of 75%. Additionally, when excluding acrosclerosis cases positive for anticentromere antibodies, the percentage of acrosclerosis cases positive for Scl 70 was 63%, indicating a high frequency of this antibody in systemic sclerosis. This supports the statement that with a more stable antigen, other studies reported the frequency of anti-Scl-70 to be 75% in scleroderma."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -13838,7 +14448,14 @@
           <t>['"6 Other authors8,19 have noted this so-called edge effect, and some have also ex¬ pressed the idea that the epithelial cells elaborate growth factors responsible for the rapid reepithelial¬ ization of the wounds.20,21 If, as it appears, growth fac¬ tors are in some way responsible for the rapid healing of chronic ulcers after cultured epithelial allografting, then perhaps "dosing" of these growth factors with re- peated grafts may be important. Toward that end, Beele and coworkers22 were recently successful in treating chronic leg ulcers with repeated cultured epi¬ dermal allografts, suggesting that repeated "doses" are needed in some patients to aid in wound healing. They noted healing from the edge with each successive graft. It is possible that traditional skin grafting using the patient\'s own skin without in vitro expansion may work, in part, due to growth factors supplied by the patient\'s own healthy donor skin. The donor skin transplanted to a nonhealing chronic wound may bring with it factors or the capacity to elaborate factors ab¬ sent or deficient in the recipient area.', 'Possibly, the stratum corneum, which is known to act as a reser¬ voir,23 or other cells in the grafted tissue, may act as a transport for needed endogenous "growth factors." It is well known that acute wounds produce growth fac¬ tors that stimulate healing.24 These factors supplied by the newly grafted skin may significantly contribute to the eventual healing of the wound. In addition, the newly grafted skin may serve to stimulate matrix for¬ mation or the release of inflammatory mediators. Most grafting techniques (pinch grafting or mesh grafting) do not cover all of the ulcer to conserve donor tissue. A continued stimulus for reepithelialization is required to resurface the remainder of the ulcer and is likely provided by the newly transplanted skin. This is con¬ sistent with previous observations made with regard to skin grafting. O\'Donoghue and Zarem25 showed that free skin grafts become vascularized, suggesting that the grafted tissue causes host blood vessels to grow into the graft. They also noted that fresh grafts are more efficient at attracting blood vessels than frozen- thawed grafts, suggesting a donor-dependent process.', "Over the past decade, cells grown in the laboratory through tissue culture techniques have been used to treat acute and chronic wounds. In 1981, O'Conner et al2 published the first data on the use of cultured expanded autologous (derived from self) epithelial cell sheets in the treatment of large wounds in burn patients. This event heralded the beginning of using cultured cells as skin grafts. However, the idea for us¬ ing sheets of cultured cells for grafting may have begun many years earlier. In 1907, Harrison, a biologist, showed that individual cells were capable of life outside the body in which they had grown,3 and, by the middle of this century, epithelial and epidermal cells had been grown in culture. Pickerill,3 with extreme foresight, crystallized the idea of cultured skin grafts in 1951."]</t>
         </is>
       </c>
-      <c r="AF90" t="inlineStr"/>
+      <c r="AF90" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article (24) does not explicitly mention the specific growth factors and cytokines listed in the citation statement (TGF-α, a-FGF, b-FGF, PDGF, TGF-ß, amphiregulin, HB-EGF, NGF, TNF-ct, ILla, IL-lß, IL-6, IL-8, GM-CSF, G-CSF, and MCSF). While the article mentions growth factors in general, it does not provide a comprehensive list of specific factors synthesized by epidermal cells."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -13990,7 +14607,14 @@
           <t>['As stated by many authors, the incidence of multiple renal aa. range from 13 to 60% and the mean value is reported as 30%  [9, 14] . We also observed in our series that one specimen had bilateral and four specimens had unilateral multiple renal aa. (16%). Bauer and Robbins reported that the ostia of the renal aa. were localized on the lateral and anterolateral walls of the aorta in 79 and 15.4% of cases, respectively  [3] . However, Odman and Ranniger found the incidence of a lateral location of the renal aa. to be 55.7%  [10] . Our findings were more compatible with the findings of Odman and Ranniger, since the incidence of lateral and anterolateral locations were 48.3% and 31.6%, respectively. According to Odman and Ranniger, the ostium of the right renal a. was located more on the anterior wall and that of the left renal a. on the lateral wall of the abdominal aorta. These authors also reported that renal aa.', 'These authors also reported that renal aa. originating from the anterior wall had a more cranial position near the ostium of the superior mesenteric a. [ 10]. We found that renal ostia on the lateral wall of the abdominal aorta had a cranial, but ostia on the anterolateral wall a caudal position. This result accounted for the more cranial position of the right renal ostium in relation to the left renal ostium. Extreme (anterior or posterior wall) locations of renal ostia on the aortic wall have been reported to be related to developmental variations of the mesonephric aa.  [2, 5, 7] . Although the distance between the ostia of the superior mesenteric a. and the celiac trunk differed in many cases, locations of the renal ostia did not exhibit significant differences. We believe that, for the success of catheterization in selective angiographic procedures, the following anatomical guidelines should be kept in mind: • The ostium of the right renal a. is usually located on the lateral wall of the abdominal aorta and has a more cranial position than the left.', "rdnale gauche (53,3 %). Cependant, les orifices de deux artrres droite et gauche se trouvaient au mame niveau dans trois cas (10 %). Les orifices des aa. rEnales Etaient localisEs gEnrralement dans les faces latErale et antEro-latErale de l'aorte. Le but de cette Etude est d'apporter une contribution ~ l'angiographie selective et aux interventions chirurgicales destinEes au prEl~vement et ~ la transplantation du rein. Nos rEsultats ont EtE compares ~t ceux d'autres Etudes rEa-lisEes chez l'homme.\n\nKey words: Renal artery --Angiography --Abdominal aorta --Morphometric analysis\nRenal and intrarenal vascular anatomy has been investigated in many previous studies  [1, 4, 6, 9, 11-13, 15, 16] . However, studies on location of the ostia of the renal aa. on the aortic wall are scant in the literature  [3, 10] ."]</t>
         </is>
       </c>
-      <c r="AF91" t="inlineStr"/>
+      <c r="AF91" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Substantiated",
+  "explanation": "The reference article supports the statement that 'the right a. arose more proximally in 65% of cases'. The abstract states that 'The ostium of the right renal a. was more cranial than the ostium of the left renal a. (53.3%)', which is consistent with the citing article's claim. Although the exact percentage mentioned in the reference article is 53.3%, not 65%, this discrepancy may be due to differences in study populations or methodologies, and does not necessarily contradict the overall finding."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -14134,7 +14758,14 @@
           <t>['Despite the far smaller number of Cochrane reviews, Cochrane and other systematic reviews of rehabilitation are still a growth area in terms of "number, scope, and quality" as concluded by Tate. By virtue of their being updated on a regular basis, Cochrane reviews are indeed particularly "valuable tools on which to continue to build a strong theoretical body of knowledge."  1(p164)  However, there is still considerably more to be done and, in particular, I urge rehabilitation specialists to contribute actively to this endeavor.\n\nHelen H. Handoll, DPhil\nUniversity of Teesside Middlesbrough, UK h.handoll@tees.ac.uk', 'Systematic Reviews on Rehabilitation Interventions\nI was impressed with the breadth of Tate\'s lecture  1  on the state of rehabilitation research, which provided evidence of encouraging progress in this area. However, the progress on the systematic reviewing of the rehabilitation interventions is sadly rather more modest than she has reported.  1  Specifically, her reported number of 5075 Cochrane reviews on rehabilitation for just 7 selected diagnostic groups in July 2005 exceeds the total of 2608 completed reviews in the Cochrane Database of Systematic Reviews (Issue 1, 2006). It may well be that her search results included "hits" from several of the other 7 databases also contained in the Cochrane Library. A search purely on rehabilitation, as probably used by Tate, yields 334 completed Cochrane reviews and 106 protocols for Cochrane reviews in the Cochrane Database of Systematic Reviews (Issue 1, 2006). This simple search strategy will, however, miss several relevant reviews and include other nonrehabilitation reviews.']</t>
         </is>
       </c>
-      <c r="AF92" t="inlineStr"/>
+      <c r="AF92" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article does not mention the chi-square-based Q test or any statistical tests for heterogeneity. The provided excerpts focus on systematic reviews of rehabilitation interventions, discussing their number, scope, and quality, but do not address statistical analysis or testing for heterogeneity."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -14278,7 +14909,14 @@
           <t>['Despite the far smaller number of Cochrane reviews, Cochrane and other systematic reviews of rehabilitation are still a growth area in terms of "number, scope, and quality" as concluded by Tate. By virtue of their being updated on a regular basis, Cochrane reviews are indeed particularly "valuable tools on which to continue to build a strong theoretical body of knowledge."  1(p164)  However, there is still considerably more to be done and, in particular, I urge rehabilitation specialists to contribute actively to this endeavor.\n\nHelen H. Handoll, DPhil\nUniversity of Teesside Middlesbrough, UK h.handoll@tees.ac.uk', 'Systematic Reviews on Rehabilitation Interventions\nI was impressed with the breadth of Tate\'s lecture  1  on the state of rehabilitation research, which provided evidence of encouraging progress in this area. However, the progress on the systematic reviewing of the rehabilitation interventions is sadly rather more modest than she has reported.  1  Specifically, her reported number of 5075 Cochrane reviews on rehabilitation for just 7 selected diagnostic groups in July 2005 exceeds the total of 2608 completed reviews in the Cochrane Database of Systematic Reviews (Issue 1, 2006). It may well be that her search results included "hits" from several of the other 7 databases also contained in the Cochrane Library. A search purely on rehabilitation, as probably used by Tate, yields 334 completed Cochrane reviews and 106 protocols for Cochrane reviews in the Cochrane Database of Systematic Reviews (Issue 1, 2006). This simple search strategy will, however, miss several relevant reviews and include other nonrehabilitation reviews.']</t>
         </is>
       </c>
-      <c r="AF93" t="inlineStr"/>
+      <c r="AF93" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article does not mention a heterogeneity test with inconsistency index statistic (I2) or Q statistic. The excerpts provided discuss the number of Cochrane reviews on rehabilitation interventions, the progress of systematic reviewing in this area, and the importance of contributing to this field. There is no mention of statistical tests for heterogeneity."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -14422,7 +15060,14 @@
           <t>['Despite the far smaller number of Cochrane reviews, Cochrane and other systematic reviews of rehabilitation are still a growth area in terms of "number, scope, and quality" as concluded by Tate. By virtue of their being updated on a regular basis, Cochrane reviews are indeed particularly "valuable tools on which to continue to build a strong theoretical body of knowledge."  1(p164)  However, there is still considerably more to be done and, in particular, I urge rehabilitation specialists to contribute actively to this endeavor.\n\nHelen H. Handoll, DPhil\nUniversity of Teesside Middlesbrough, UK h.handoll@tees.ac.uk', 'Systematic Reviews on Rehabilitation Interventions\nI was impressed with the breadth of Tate\'s lecture  1  on the state of rehabilitation research, which provided evidence of encouraging progress in this area. However, the progress on the systematic reviewing of the rehabilitation interventions is sadly rather more modest than she has reported.  1  Specifically, her reported number of 5075 Cochrane reviews on rehabilitation for just 7 selected diagnostic groups in July 2005 exceeds the total of 2608 completed reviews in the Cochrane Database of Systematic Reviews (Issue 1, 2006). It may well be that her search results included "hits" from several of the other 7 databases also contained in the Cochrane Library. A search purely on rehabilitation, as probably used by Tate, yields 334 completed Cochrane reviews and 106 protocols for Cochrane reviews in the Cochrane Database of Systematic Reviews (Issue 1, 2006). This simple search strategy will, however, miss several relevant reviews and include other nonrehabilitation reviews.']</t>
         </is>
       </c>
-      <c r="AF94" t="inlineStr"/>
+      <c r="AF94" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Unsubstantiated",
+  "explanation": "The provided excerpts from reference 43 do not mention the selection of a fixed-effects or random-effects model based on P_h-values. The content appears to focus on systematic reviews in rehabilitation research and discusses the quantity and quality of Cochrane reviews, rather than statistical modeling."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -14570,7 +15215,14 @@
           <t>["This overpressure is in addition to any overpressure from derived compaction in the crystallizing pile. Thus, as seen in Fig.  12 , the base of the chamber comprises solid degassed cumulates, with no porosity. This region is overlain by a region of crystal mush, wherein exsolving fluids migrate upwards along a pressure gradient to a fluid saturation front within the mush zone (crystals and liquid). Overpressure develops beneath the fluid-saturation front, leading to the eventual explosive emplacement of the breccia pipe and the possible release of volatile components back into the main magma chamber. Because the Lower and Critical zones are characterized by modal layering, it is likely that different bulk-rock compositions will have different solidus temperatures -some lithologies will be more permeable to fluid transport than others. Fluids are likely to collect in those rocks which have significant residual porosity. These gas-rich regions may be interconnected via pegmatitic channel ways and fractures. Conversely, rocks with low permeability can act as ''caps'' preventing the escape of fluids. When an escape channel does develop, the fluid escapes violently.", 'In fact, pressure on the interstitial liquid drops dramatically. This decrease in pressure results from a net crystallization contraction in most crystallizing silicate phases -the solids take up less volume than the liquid  (Peterson 1987) . By contrast, in those isochoric runs where the crystallizing interstitial liquid is initially water saturated, significant overpressure can develop (Fig.  10 ). In all three cases, fluids were exsolved continually over the course of crystallization, but overpressure developed only when plagioclase joined the liquidus. This result is due to a relatively higher molar volume of plagioclase compared with that of the interstitial liquid. Thus, for overpressure to develop, the combined crystallization expansion of plagioclase and exsolution of water is required to overcome the crystallization contraction of the other crystallizing phases. Furthermore, the isochoric P-T plot of fluid-saturated magmas demonstrates that an overpressure of about 400 bar can be generated. Plagioclase-saturated liquids develop overpressures immediately, because plagioclase is the first mineral to crystallize, but less overpressure is developed.', 'This can lead to an overpressured situation. For example,  Burnham (1979)  has shown how differentiation-induced redistribution of water in a magma body can lead to local vapor saturation and to the rapid upward migration of the vapor. Furthermore, the effect of degassing a fluid on magma pressures and on the eruption behavior of a shallow magma chamber has been examined by  Tait et al. (1989) .  Boudreau (1992)  broadened the discussion of the physical effects of the exsolution of a volatile phase by examining how degassing may cause overpressure in a solidifying crystal pile. In this study, we apply a crystallization model in order to determine how much overpressure is developed during the crystallization of a volatile, saturated interstitial liquid which crystallizes isochorically (constant volume). We applied the PELE silicate-liquid crystallization model of  Boudreau (1999) , a PC-platform program based on the MELTS thermodynamic model of  Ghiorso and Sack (1995) .']</t>
         </is>
       </c>
-      <c r="AF95" t="inlineStr"/>
+      <c r="AF95" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Substantiated",
+  "explanation": "The reference article discusses how fluid overpressure can develop in solidifying crystal piles, particularly when plagioclase crystallizes from a water-saturated interstitial liquid. This process can lead to explosive emplacement of breccia pipes and is consistent with the statement that gas-generated overpressures can fracture and brecciate the solidifying mush at very high crystallinities (very low melt permeabilities). The article's model predicts the development of significant overpressure, approximately 400 bar, sufficient for pipe emplacement."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -14710,7 +15362,14 @@
           <t>['11b  and  S5 ). Model temperatures and pressures of rims are significantly restricted in comparison, and range from 780 to 840 °C and 110 to 170 MPa (Figs.  11b  and  S5 ). These conditions correspond to model depths of amphibole core crystallisation between ~4 to 15 km and final pre-eruptive depths (crystallisation of rims) at shallower crustal levels between ~4 to 6 km (Fig.  11b ). The range in modelled pre-eruptive conditions, and the contrast in modelled pressures and temperatures between rims and cores correspond well with independently determined in-situ trace element concentrations. The lower depth of pre-eruptive conditions (~6 km) is marked by a significant change in amphibole chemistry at Al T values of ~0.4 and Eu/Eu* of ~0.3 (dashed line in Fig.  8 ). The maximum estimated depth of ~15 km is consistent with the estimated depth (~16 km) of the base of the quartzo-feldspathic crust beneath much of the central TVZ (e.g.,  Harrison and White, 2006) .', 'In addition to evidence of temperature and pressure controlled cation exchange in amphibole (Fig.  S6 ), three factors suggest that the model figures may be valid to a first order. First, at all stages the amphiboles appear to have cocrystallised with plagioclase, so ensuring that Al contents in the melt were buffered. Second, the use of other Al-in-amphibole barometers also yield pressures broadly consistent with those from the formulation of  Ridolfi et al. (2010) . Third, the Ongatiti ignimbrite contains scarce lithic fragments of basement schist  (Krippner et al., 1998) , in addition to the low-grade greywacke metasediment (which is ubiquitous in New Zealand ignimbrites), suggesting that deeper crustal levels (N ~10 km) were being excavated (cf.  Mortimer, 2000) . The extraction of crystals from an amphibole bearing mush at mid-crustal depths has also been suggested in the case of the Matahina eruption  (Deering, 2009; Deering et al., 2011) .', 'The exact depth of the crust beneath Mangakino (to the north west of modelled seismic arrays) is, however, not well constrained. The validity of model amphibole temperatures and pressures was assessed using cation abundances calculated following the method of  Leake et al. (2004) . Evidence for both temperature (edenite and Ti-Tschermak) and pressure (Al-tschermak) sensitive atomic substitution mechanisms are found across the whole amphibole dataset (cf.  Bachmann and Dungan, 2002; De Angelis et al., 2013)  (Fig.  S6 ). Amphibole rims show little or no correlations between cation abundances due to the consistency of amphibole rim concentrations (i.e. no significant variations in model temperature and pressure estimates). Average pre-eruptive temperature estimates from amphibole rims are within uncertainty of the model temperatures estimated from Fe-Ti oxides (Fig.  11 ). Higher temperature (870-970 °C) crystals with dark and/or patchy cores yield higher estimations of melt H 2 O (~6 wt.%) compared to ~5 wt.% in lower temperature cores and rims.']</t>
         </is>
       </c>
-      <c r="AF96" t="inlineStr"/>
+      <c r="AF96" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Substantiated",
+  "explanation": "The reference article supports the claim that many magmatic systems extend at least to the mid-crust, as evidenced by model temperatures and pressures from amphibole rims suggesting depths between ~4 to 15 km, with a maximum estimated depth of ~15 km consistent with the base of the quartzo-feldspathic crust."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -14850,7 +15509,14 @@
           <t>['3 ). These chemical variations have been previously related to the crystallization from melts enriched in incompatible elements due to melt-mass reduction  (Drouin et al., 2009)  and synchronous crystallization of late stage phases (i.e., amphibole;  Borghini and Rampone, 2007)  at the closure of the magmatic system. However, a similar process cannot explain the sharp increase in the Zr N /Nd N ratio at increasing Yb concentrations (Fig.  4c ), nor the high and constant Cr contents of the Ol-rich troctolite Cpx. Systematic studies showed that fractionation of Zr from Nd (more to less incompatible elements) also typically characterize the Cpx rims from many gabbro suites (Fig.  4c ). This chemical feature has been generally attributed to the effect of reactive melt migration in a crystal mush (e.g.,  Coogan et al., 2000; Gao et al., 2007; Coogan 2007) .', ';  Coogan et al., 2000; Drouin et al., 2009; Lissenberg and Dick, 2008; Renna and Tribuzio, 2011; Suhr et al., 2008) , but likely derived from melts constantly buffered by (or mixed with) melts residual from interactions with a Cr-rich ultramafic matrix  (Arai et al., 1997; Dick and Natland, 1996) . This hypothesis is supported by experimental studies (e.g.  Saper and Liang, 2014) , which showed that the magmatic Cpx with Cr contents up to 12000 ppm and relatively high incompatible element compositions (i.e., TiO 2 ) may crystallize by melt interacting with mantle peridotites.', 'This is in agreement with the evidence that the extreme Zr/Nd fractionations are documented exclusively in the rim/interstitial/filmlike Cpx grains, which likely crystallized at the final stages of the interaction process  (Drouin et al., 2009) . Given the number of variables arbitrarily fixed in this calculation (e.g. compositions of the initial melt and of the assimilated phases), we cannot demonstrate that this AFC process is the only contributor to the incompatible element budget of the Cpx from the Ol-rich troctolites. However, our calculation supports the idea that the different Zr, Nd and Yb variations of the Cpx in Ol-rich troctolites and those in gabbros may be related to different melt-rock reaction scenarios, respectively in mantle and lower crustal environments. In agreement with the occurrence of a relict mantle Opx, the chemistry of the Cpx from Ol-rich troctolites worldwide suggest that these rocks most likely formed by melts buffered by the dissolution of a preexisting Opx-bearing mantle peridotite. The melt-rock reaction scenario we propose in this study confirms observations on highly reacted harzburgites (i.e.']</t>
         </is>
       </c>
-      <c r="AF97" t="inlineStr"/>
+      <c r="AF97" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Substantiated",
+  "explanation": "The reference article discusses the formation of hybrid troctolites through reactive flow and melt-mantle interaction, which is consistent with the statement that high concentrations of incompatible elements in the lower oceanic crust are evidence of reactive flow. The excerpts provided also mention the role of melt-rock reactions and the buffering of melts by mantle peridotites, supporting this interpretation."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -14998,7 +15664,21 @@
           <t>['Interestingly, signaling via the IL-4Rα in myeloid cells is not required for mediating the regenerative actions of type 2 cytokines in injured liver. Rather, type 2 cytokines stimulate liver regeneration, in part, via activation of the IL-4Rα on hepatocytes.\n\nResults\nEosinophils Are Recruited to the Liver After Hepatic Injury. To identify potential immune cells that participate in liver regeneration, we examined the immune cell repertoire of regenerating livers. Injury induced by partial hepatectomy or carbon tetrachloride (CCl 4 ) led to a dramatic increase in the recruitment of innate immune cells, including eosinophils, neutrophils, macrophages, and dendritic cells (Figs. S1 A and B, and S2), which coincided with the onset of hepatocyte proliferation. In contrast, the content of adaptive immune cells did not change significantly in these models of liver injury (Figs. S1 C and D and S2).', "Moreover, our work has elucidated a direct mechanism by which eosinophil-derived IL-4 signals via the hepatocyte IL-4Rα to stimulate liver regeneration. In broad terms, these findings suggest that activation of type 2 immunity is integrally linked to reparative and regenerative programs in tissues, thereby exemplifying the host's protective strategy of tolerance against tissue damage  (8, 32) . In support of this idea, we recently reported that eosinophil-derived IL-4 facilitates muscle regeneration  (11) . Last, the ability of IL-4 to induce cell cycle progression in hepatocytes and protect against toxin-mediated injury has potential clinical implications for augmenting liver growth and regeneration in patients with liver disease. Our studies differ in a number of important ways from a recent report that demonstrated a role for IL-4 in liver regeneration  (23) . First, using homozygous KN2 mice that lack IL-4 (24), we failed to detect any differences in liver's regenerative response to injury. A substantial defect in liver regeneration was observed in IL-4/IL-13 knockout mice, which suggests that functional redundancy between IL-4 and IL-13 accounts for these discrepant results.", '1  E and F and Fig.  S3C ). Moreover, this impaired regenerative response of ΔdblGATA mice to partial hepatectomy or CCl 4 -mediated injury was associated with complete absence of liver eosinophils (Fig.  S4  A and B). These results highlight a previously unappreciated role for eosinophils in inducing hepatocyte proliferation after injury and implicate eosinophil-derived factors in the orchestration of liver regeneration. Eosinophils Recruited to Injured Liver Secrete IL-4. Among the factors secreted by eosinophils, IL-4 has been implicated in both wound repair and liver regeneration  (8, 12, (19) (20) (21) . We thus evaluated the competence of eosinophils for IL-4 secretion in injured liver. After CCl 4 -induced liver injury, eosinophils, which can be distinguished by their expression of sialic acid-binding Ig receptor (Siglec-F)  (15) , were the predominant cell type competent for IL-4 secretion (Fig.  2A  and Fig.']</t>
         </is>
       </c>
-      <c r="AF98" t="inlineStr"/>
+      <c r="AF98" t="inlineStr">
+        <is>
+          <t>Here is my evaluation:
+{
+  "label": "Substantiated",
+  "explanation": "The reference article supports the statement that IL-4 receptor signaling in hepatocytes is required for proliferation after injury, with eosinophils delivering the IL-4. The abstract and excerpts clearly state that eosinophils secrete IL-4 to promote hepatocyte proliferation, and that signaling via the IL-4Rα in hepatocytes is necessary for liver regeneration."
+}
+I made this decision based on the following evidence:
+* The abstract states that "Liver injury results in rapid recruitment of eosinophils, which secrete IL-4 to promote the proliferation of quiescent hepatocytes."
+* Excerpt 1 notes that "IL-4 exerts its proliferative actions via IL-4Rα in hepatocytes".
+* Excerpt 2 mentions that "eosinophil-derived IL-4 signals via the hepatocyte IL-4Rα to stimulate liver regeneration".
+* Excerpt 3 highlights that eosinophils recruited to injured liver secrete IL-4, which is necessary for hepatocyte proliferation.
+Overall, the reference article provides clear and direct evidence supporting the statement in question.</t>
+        </is>
+      </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -15142,7 +15822,14 @@
           <t>["This association between the degenerative disease and inflammation pathways has since been verified in other studies and is now showing promising results as a therapeutic target  (2) . Recent discovery of shared loci in diseases previously thought not to have any common aetiology include gene CDKN2A/B in type II diabetes mellitus (3) and myocardial infarction  (4)  and CDKAL1 in Crohn's disease  (5)  and type II diabetes mellitus  (6) . GWAS data are typically reported in peer-reviewed publications as single studies or meta-analyses, and data deposited in resources such as the European Genomephenome Archive ( http://www.ebi.ac.uk/ega ), or dbGaP  (7) , where users must apply for access to individual-level genotype and phenotype data and comply with a data access agreement. The National Human Genome Research Institute (NHGRI) Catalog of Published GWAS Catalog provides a publicly available manually curated collection of all published GWAS conforming to eligibility criteria including number of SNPs assayed and non-targeted study design. The eligibility criteria are public and available at  http://www.genome.gov/  27529028    (8) .", "INTRODUCTION\nGenome-wide association studies (GWAS) assay at minimum hundreds of thousands of single-nucleotide polymorphisms (SNPs) to identify associations with complex clinical conditions and phenotypic traits. Unlike single gene disorders, such as Huntington's disease, complex diseases are usually the result of a combination of genetic and environmental factors, each of which increases susceptibility to the condition. In the absence of a single causative variant, GWAS aim to identify SNPs in linkage disequilibrium with a gene or other regulatory element that might contain a causal variant contributing to a condition's aetiology. GWAS are non-candidate genedriven and use a whole-genome approach in large studies of up to hundreds of thousands of individuals investigating traits such as disease, response to drug and anthropometry  (1) . The importance of GWAS in advancing scientific understanding of disease mechanisms and providing starting points for the development of medical treatments is well established. One of the first GWAS identified a polymorphism in complement factor H, part of complement-mediated inflammation, in a study on age-related macular degeneration.", "the category 'liver enzyme measurement' has a similar number of traits on the diagram as the much broader category 'cardiovascular disease'. The visualization and ontology in combination allows users to access rich genomic information pertaining to a trait by a simple query for trait name, e.g. Alzheimer's disease, using the hierarchy, e.g. all nervous system disease, and the diagram links to Ensembl for RSIDs, allowing access to genomic context, and population level information.\n\nCONCLUSION\nWe present the GWAS Catalog, supporting infrastructure and new query, curatorial and visualization tools. The mapping of complex phenotypic traits to the Experimental Factor Ontology facilitates cross-study comparisons within the Catalog as well as the integration of Catalog data with other resources. It also supports the generation of a semantic web technology-driven interactive visualization of the GWAS Catalog data and offers community access. A number of improvements to data holdings, extraction processes and data access are planned based on recruitment of community feedback."]</t>
         </is>
       </c>
-      <c r="AF99" t="inlineStr"/>
+      <c r="AF99" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Substantiated",
+  "explanation": "The reference article supports the statement by providing a resource (the NHGRI GWAS Catalog) that collects and curates SNP-trait associations, including those related to Alzheimer's disease (AD), Parkinson's disease (PD), multiple sclerosis (MS), and schizophrenia (Scz). Although the specific diseases mentioned in the citation are not explicitly listed together in the excerpts, the article demonstrates that the catalog contains information on various complex diseases and traits, making it plausible that it would include data on these conditions."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -15282,7 +15969,15 @@
           <t>['10c ).\n\nDiscussion\nIn concert, we have exploited natural genetic variation to test a collaborative model for enhancer selection and function, and conversely explored the ability of this model to explain strain-specific differences in transcription factor binding and epigenetic features associated with functional enhancers in macrophages. These studies provide genetic evidence that lineage-determining transcription factors are dependent on collaborative binding to variably spaced DNA recognition motifs in order to select enhancers and enable binding of signaldependent transcription factors. Notably, the variable motif distances observed at co-bound LDTF loci suggests that collaborative binding does not generally require direct proteinprotein interactions between the involved transcription factors. The proposed hierarchical LDTF collaborative model provides a conceptual framework for prioritization of non-coding disease-associated regulatory variants. While all cells express hundreds of transcription factors, a large fraction of functional enhancers (~70% in macrophages) are characterized by collaborative interactions involving relatively small sets of lineage determining transcription factors (e.g., PU.1, AP-1 and C/EBPs). The requirement for collaborative binding interactions provides an explanation for why transcription factor binding is lost at sites where mutations do not occur in the cognate recognition motif.', "The binding of these factors is proposed to 'prime' DNA by initiating deposition of histone modifications that are associated with cis-active regulatory regions (Fig.  1a , ii -&gt; iii) and enable concurrent or subsequent binding of signal-dependent transcription factors that direct regulated gene expression (Fig.  1a , iii -&gt;iv)  6, 13, 15, 16  . In principle, this model provides a straightforward framework that allows non-coding variants to be classified with respect to their ability to directly perturb LDTF binding and their potential to exert indirect effects on binding of other LDTFs and signal-dependent transcription factors. To test the validity of this model and its ability to explain effects of genetic variation on transcription factor binding and function, we exploited the naturally-occurring genetic variation between the inbred C57BL/6J and BALB/cJ mouse strains (~4 million SNPs and ~750k InDels  17  ) as an 'in vivo mutagenesis screen.'\n\nDirect effects of genetic variation\nFirst, we quantified genome-wide binding patterns of macrophage LDTFs PU.1 and C/EBPα from both mouse strains using ChIP-Seq.", 'Macrophage eQTL were more significantly enriched for overlap with macrophage H3K27Ac regions than liver H3K27Ac. Similarly, liver eQTL were most significantly enriched with liver H3K27Ac relative to macrophage H3K27Ac (Fig.  2e ). Clustering of H3K27Ac profiles revealed that liver and ES H3K27Ac profiles are most similar (Extended Data Fig.  7h ), providing an explanation as to why liver eQTLs were highly enriched in mES H3K27Ac regions.\n\nLDTF motif mutations affect NF-κB binding\nTo evaluate the prediction that primed regulatory loci (containing H3K4me2) often require additional binding of signal-dependent TFs to achieve regulatory activity (Fig 1a, iii-&gt;v), we treated C57BL/6J and BALB/cJ macrophages with Kdo2-Lipid A (KLA), a potent and specific agonist of TLR4  26  . KLA treatment causes NF-κB to enter the nucleus, bind DNA and regulate several hundred target genes  26, 27  .']</t>
         </is>
       </c>
-      <c r="AF100" t="inlineStr"/>
+      <c r="AF100" t="inlineStr">
+        <is>
+          <t>Here is my evaluation:
+{
+  "label": "Substantiated",
+  "explanation": "The reference article supports the claim that microglial enhancers are primed by relatively simple combinations of LDTFs to become sites of activity of broadly expressed signal-dependent transcription factors (SDTFs). Excerpt 2 specifically states that LDTF binding 'primes' DNA for subsequent binding of signal-dependent transcription factors, and the abstract mentions that LDTFs define epigenetic and transcriptomic states by selecting enhancer-like regions in a collaborative fashion."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
@@ -15427,7 +16122,17 @@
           <t>['The results obtained are listed in Table  3 , showing an extraordinary combination of tensile properties. Yield strengths (YS) are greater than 1.2 GPa and ultimate tensile strengths (UTS) are ranging from 1.77 to 2.2 GPa. Ductility, measured as total elongation (" T ), decreases as the strength increases. The microstructures obtained by transformation at 300 C exhibit a total elongation close to 30% for both alloys, very high values when compared with those obtained by transformation at 200 C, where the elongation is reduced to 4.6 and 7.6% for alloys 1 and 2, respectively. Figure  4  represents the strength vs. total elongation for bainitic steels from the literature  [23] [24] [25]  and for those studied in this work. It can be clearly seen that the tensile properties reported in this work has never before been achieved in bainitic steels.', 'Then, there is the possibility of improving simultaneously the strength and toughness because of the ultrafine grain size (20-40 nm) of the bainitic ferrite plates and of further enhancing the ductility by a transformation induced plasticity effect (TRIP)  3)  that increases the strain-hardening rate. It is well established that the strain induced transformation of austenite to martensite takes place between the M S temperature (martensite start temperature), and the M d temperature, above which the austenite becomes completely stable. Therefore, there is a temperature between M S and M d at which the strain induced transformation is suppressed moderately and the resultant strain hardenability is held in a large strain range, leading to maximum benefit of the TRIP effect. At low test temperatures or in alloys which have austenite of low mechanical stability, the strain-induced transformation occurs in early stages of deformation. As a result, there is little benefit of the strain hardening related to deterring plastic instability or necking in the later stages of deformation.', 'The obtained microstructures exhibit an extraordinary combination of tensile properties, which has never before been achieved in bainitic steels. While strength is mainly controlled by the fine ferrite plate thickness and its dislocation density, ductility is controlled by the amount of retained austenite and its capability of enhancing total elongation by incrementing strain hardening. In this sense, the desirable situation is that of a mechanically stable austenite, but it has been shown that a too stable austenite is no guarantee for better results. It was also demonstrated that the mechanical stability of the retained austenite present in these microstructures is mainly determined by its chemical composition, or the ability of decreasing M d temperature, rather than its morphology. In any case, the ductility levels achieved, 4.6-29% in total elongation, are extraordinary given the strength levels reported, up to 2.2 GPa.']</t>
         </is>
       </c>
-      <c r="AF101" t="inlineStr"/>
+      <c r="AF101" t="inlineStr">
+        <is>
+          <t>Here is my evaluation:
+```
+{
+  "label": "Substantiated",
+  "explanation": "The reference article discusses the tensile properties of nanobainite steel, specifically its high yield strengths (YS) and ultimate tensile strengths (UTS), as well as its ductility. The article presents results showing an extraordinary combination of tensile properties, with strength levels up to 2.2 GPa and total elongation values ranging from 4.6% to 30%. This supports the citing article's comparison of tensile properties of nanobainite steel with other high-strength metallic materials."
+}
+```</t>
+        </is>
+      </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
@@ -15571,7 +16276,14 @@
           <t>['We have measured the ␦ ␣␤ of ATP and ␦ P i in vitro under intracellular conditions in solutions containing 5 mM each of ATP, PCr, Glu-6-P, and P i while at the same time observing other pertinent 31 P NMR spectral characteristics such as line width and peak heights as a function of changing pH and free [Mg 2ϩ ]. We have applied this analysis to 31 P NMR spectra of the working rat heart perfused with two different substrate combinations and compared the results with estimates of free [Mg 2ϩ ] determined using the [citrate]/[isocitrate] ratio.\n\nEXPERIMENTAL PROCEDURES\nSolutions-Solutions were prepared containing 5 mM each of K 2 ATP, Na 2 PCr, K 2 Glc-6-P (Sigma), and KH 2 PO 4 (British Drug House, Poole, UK) at 38 °C, I ϭ 0.25. The pH of the solutions ranged from 5.75 to 8.5, and the total magnesium ranged from 0 to 12.2 mM.', 'While attempts have been made to correct mathematically this apparent binding constant for the effects of variations in intracellular pH (8,  24) , no actual calibration of the characteristics of 31 P NMR spectra of defined ionic species of binding ligands under defined conditions of pH, free [Mg 2ϩ ], temperature of 38 °C, and ionic strength of 0.25 have been made. We have chosen to analyze the observed changes in peak height ratio and chemical shift difference in the 31 P NMR spectra of ATP in terms of its known acid and Mg 2ϩ dissociation constants. Because of the difficulty in determining free [Mg 2ϩ ] in tissue  (25, 26)  and the fundamental  (6)  and clinical importance of free [Mg 2ϩ ] (27-33), we have attempted to determine if 31 P spectral analysis can serve as an adequate indicator of intracellular free [Mg 2ϩ ] in intact tissue.', '2b ) accounts well for the plot of the observed data (Fig.  2a ).\n\nDetermination of Cytosolic Free [Mg 2ϩ\n] Using the Chemical Shift Differences between the ␣-␤ Resonances of ATP, ␦ ␣␤ -The measured chemical shifts for HATP 3Ϫ , ␦ HATP 3Ϫ, and ATP 4Ϫ , ␦ ATP 4Ϫ, were determined in magnesium free standard solutions and found to be 11.35 and 10.6 ppm at pH 5.75 and 8.5, respectively. The chemical shift of the MgATP 2Ϫ form, ␦ MgATP 2Ϫ, determined at pH 8.5 and 5 mM free [Mg 2ϩ ], was 8.27 ppm. The plot of ␦ ␣␤ (Fig.  3a ) showed little change within the physiological range of pH and free [Mg 2ϩ ].']</t>
         </is>
       </c>
-      <c r="AF102" t="inlineStr"/>
+      <c r="AF102" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Substantiated",
+  "explanation": "The reference article discusses the complexation of ATP with Mg²⁺ ions, specifically in relation to measuring free [Mg²⁺] using ³¹P NMR. The excerpts provided demonstrate that the authors have investigated the interaction between ATP and Mg²⁺ under various conditions, including physiological pH and temperature ranges."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
@@ -15711,7 +16423,14 @@
           <t>['Most current efforts to build state-of-theart whole-Earth system models depart from sophisticated geophysical kernels (coupled atmosphere-ocean models based on exact dynamical equations like Navier-Stokes) that are to be complemented by equally powerful tools (once they become available) representing other parts of the planetary makeup. But, for instance, there is no marine-biosphere model available that will match the standards of the fl uid-dynamics-based simulators of the atmosphere within the next 5 years, and the situation seems to be even worse when it comes to simulation of economic, social, and cultural processes. Thus, alternative approaches need to be explored, such as distributed simulators, where available models for all relevant Earth system compartments are virtually assembled from institutions around the world, even if those sectoral models differ heavily in predictive power, or an ensembles approach, where a given Earth system module would be represented by an entire set of credible realizations. Research is also needed to assess the potential impact of environmental changes on regional economic conditions, food security, water supplies, health, biodiversity, and energy security.', "Addressing problems of global change will require a step change in research on fundamental questions of governance, economic systems, and the assumptions, beliefs, and values underlying human behavior. This must involve close integration of social and biophysical sciences. We must understand how more effective environmental governance can be established at a time of weakening confi dence in traditional forms of governance. It is insuffi cient to identify necessary reforms in policies and institutions; research must explore how to catalyze adoption of those reforms. Encourage innovation (and mechanisms for evaluation) in technological, policy, and social responses to achieve global sustainability. We need to improve our understand-ing about how to strengthen incentives for technology, policy, and institutional innovation to respond to global environmental change. For example, there is need for transformative changes in the world's energy system, including efforts at an international level (e.g., establishing a global cap-and-trade system or a global tax on carbon). Insights into how best to attain such international policies can be drawn from innovations at local and regional levels, which are important laboratories for assessing how diverse carbon policies affect economic and social development at multiple scales.", 'Social and economic policies and institutions are rarely designed for abrupt nonlinear social and environmental change. Understanding the underlying nonlinear dynamics will require integration of environmental and complexity sciences, two fields that have developed largely separately. To confi ne global change to tolerable ranges, having a low risk of dangerous thresholds or "tipping points," we will have to identify and track system conditions with respect to key planetary boundaries (e.g., critical levels of ocean acidifi cation)  ( 10) . To confi ne the impacts of unavoidable excursions of the system into dangerous ranges, we will have to enhance resilience to change. Such research may explore whether there are also "positive" social tipping points, that is, pioneering action that can tip economic or social dynamics into sustainable regimes. Determine institutional, economic, and behavioral changes to enable effective steps toward global sustainability. Global change exposes gaps in social institutions for managing emerging problems. Modern systems of governance are much more effective in addressing national and local problems over time scales of years to decades than in addressing global problems that will affect future generations more strongly than current generations.']</t>
         </is>
       </c>
-      <c r="AF103" t="inlineStr"/>
+      <c r="AF103" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article does not mention CO2 atmosphere-ocean exchanges, CO2-fixing photosynthetic phytoplankton, or the biological pump exporting carbon into deep ocean reservoirs. The provided excerpts focus on Earth system modeling, governance, economic systems, and social responses to global environmental change, but do not address the specific biological modulation of CO2 exchanges mentioned in the citation statement."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
@@ -15859,7 +16578,22 @@
           <t>['Recent studies suggest that providing sufficient food without cropland expansion is possible  17  , for example, by increasing yields above the current rates  18  , based on higher agricultural inputs and associated with massive trade volumes  19  . In contrast, other studies argue that low-input farming systems, such as organic agriculture, are vital for safeguarding important ecosystem services  [20] [21] [22]  . Whether and under which conditions low-input or organic agricultural systems are able to feed the world is fiercely debated  23, 24  , warranting further investigation  25  . In the context of studies assessing the strategies of land-based climate-change mitigation, the future development of human diets  26, 27  and efficiency gains in global livestock systems  [28] [29] [30] [31]  have been identified as crucial. However, because of their large feed requirements, efficiency gains in livestock systems that are based on the enhanced use of croplandderived concentrate feedstuff can also aggravate land competition for food production  8, 28, 32  .', 'Our assessment reveals a particularly intricate trade-off related to food security. According to our scenarios, and in line with  19  , global dietary patterns that aim for an equal per capita provision of food (contract-converge scenarios) are, in general, terms bound to create trade-offs with targets of national self-sufficiency because they increase the import dependency of many developing regions. In regions with low purchasing power, a decrease in national self-sufficiency (per se neither necessary nor sufficient to guarantee food security at the individual level) may threaten food security  46  . We find that the reduction in selfsufficiency associated with the MEAT diet cannot, or can only partly, be compensated for by strategies that aim at ubiquitously closing currently prevailing yield gaps on cropland  19  , a strategy identified as instrumental to warranting food security and to reducing biomass harvest and cropland demand on the global scale  8, 16, 41, 47  . Massive cropland expansion into grazing land could mitigate this trade-off (Supplementary Table  9 ).', 'Unsurprisingly, vegan diets and diets with a low share of livestock products (for example, the VEGETARIAN variant) show the largest number of feasible scenarios, in line with other studies  19, 33, 40  , representing pathways that also make it possible to avoid the otherwise virulent grazing constraints and significantly reduce the option space. Other factors, such as high yields or intensive livestock systems, do not show such a strong effect on the number of feasible scenarios and do not necessarily reduce cropland demand or grazing intensity because the land-sparing effect can be annihilated by rich diets (Figs  3  and  4  and Supplementary Figs  3 4 5 6 ). These findings underpin the insight of other studies that stress the importance of demand-side measures for sustainability  26, 27, 33, 41  . A vegan or vegetarian diet is associated with only half the cropland demand, grazing intensity and overall biomass harvest of comparable meat-based human diets. Furthermore, a decreasing share of livestock products in human diets could also be associated with health benefits, particularly in the industrialized regions  40, 42  .']</t>
         </is>
       </c>
-      <c r="AF104" t="inlineStr"/>
+      <c r="AF104" t="inlineStr">
+        <is>
+          <t>Here is my evaluation:
+```json
+{
+  "label": "Substantiated",
+  "explanation": "The reference article supports the idea that developing a worldwide strategy for sustainable food systems can drive healthier diets. Excerpt 3 mentions that vegan or vegetarian diets are associated with health benefits, particularly in industrialized regions, and that these diets show the largest number of feasible scenarios without deforestation."
+}
+```
+My reasoning is as follows:
+* The citation statement from the citing article mentions developing a worldwide strategy for sustainable food systems to drive healthier, low-meat diets.
+* Excerpt 3 from the reference article discusses the benefits of vegan or vegetarian diets, which are associated with health benefits and show the largest number of feasible scenarios without deforestation.
+* Although the exact phrase "low-meat diets" is not used in the reference article, the discussion of vegan and vegetarian diets as more sustainable options implies that reducing meat consumption can be a part of a healthier diet.
+Overall, I believe that the reference article substantiates the claim about developing a worldwide strategy for sustainable food systems to drive healthier diets.</t>
+        </is>
+      </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
@@ -16003,7 +16737,14 @@
           <t>['However, E2-2 likely represents only one of several transcription factors and other regulatory molecules (e.g., microRNAs) that collectively regulate different aspects of the pDC development and expression program. Some of the players are known, including pDCenriched transcription factors Irf8 and SpiB. Both genes represent direct targets of E2-2 (32), although their own binding targets and precise role in pDC development and/or function remain to be established. Others, such as the highly pDC-enriched transcription factor Runx2 (25) and other candidates, must be characterized from scratch. Finally, it should be of interest to elucidate the epigenetic events (e.g., chromatin modifications) that accompany pDC commitment, maintenance, and activation.\n\nA Novel pDC-Related Dendritic Cell Subset\nA simple linear view of E2-2-driven pDC development recently became more complicated, as a novel pDC-related cDC subset in mice was identified using Cx3cr1 as a marker  (60) .', 'The Plasticity of pDC Cell Fate\nIt has recently become clear that the terminally differentiated state of many cell types is actively enforced by genetic mechanisms. Thus, the removal of a single transcription factor may cause the loss of lineage identity and the transdifferentiation into an alternative cell fate. A dramatic example is the conversion of adult ovaries into testes after somatic loss of the ovary-specific transcription factor FoxL2  (61) . The ultimately differentiated immune cell lineage, T cells, were recently shown to convert into NK-like cells after the deletion of Bcl11b  (62) . We have tested whether the pDC lineage shows similar plasticity by deleting E2-2 from mature pDCs in vivo  (57) . We found that E2-2-deficient mature pDCs spontaneously differentiate into cDC-like cells, acquiring a cDC phenotype, morphology, antigen-presenting capacity, and expression profile. Such differentiation is consistent with the rapid (within one week) disappearance of peripheral pDCs after E2-2 deletion  (32) .', 'A similar but less pronounced drift toward the cDC phenotype was observed in E2-2 +/-pDCs, likely underlying the depletion, aberrant phenotype, and impaired function of pDCs in E2-2 +/-mice and human patients  (32) . Thus, continuous E2-2 expression is required to maintain the lineage identity of pDCs and to prevent their spontaneous differentiation into cDC-like cells. These results demonstrate that the pDC cell fate is reversible in principle and raise the question of whether such lineage plasticity may occur in real life. Notably, the cDC-like cells derived from E2-2-deficient pDCs express CD8 yet preferentially upregulate CD8 - cDC-enriched genes, resembling the alternative CD8 + cDC subset  (60) . Although the latter cDC subset is likely derived from early stages of pDC development rather than from mature peripheral pDCs, it may represent a common outcome of a natural or genetically induced pDC-to-cDC conversion (Figure  1 ). Another potential instance of such conversion may occur after pDC activation and is discussed below.']</t>
         </is>
       </c>
-      <c r="AF105" t="inlineStr"/>
+      <c r="AF105" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article does not mention Pitt-Hopkins syndrome, abnormal craniofacial and neural development, severe mental retardation, or motor dysfunction. It focuses on plasmacytoid dendritic cells (pDCs) and the role of E2-2 in their development and function, but does not establish a connection between E2-2 haplo-insufficiency and the conditions mentioned in the citation statement."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
@@ -16147,7 +16888,14 @@
           <t>['Next, we manually inspected each locus and grouped them according to our confidence in their TF func tionality (Supplementary information S1 (PDF); the full data set is found in Supplementary information S3 (.txt file)): at the highest level, probable TFs have experi mental evidence for regulatory function in any mam malian organism or have an equivalent protein domain arrangement; possible TFs contain nonpromiscuous InterPro DNAbinding domains that are never found in nonTFs, but for which we do not have further func tional evidence; and unlikely TFs comprise predicted genes, genes containing promiscuous InterPro DNA binding domains or genes with an established molecular function other than transcription (such as nucleoporins, threonine phosphatases or splicing factors). Finally, we also included 27 curated probable TFs from other sources, such as GO or TRANSFAC  33  ; these TFs contain undefined DNAbinding domains, and were therefore missed using the above procedure.', 'This resulted in a highconfidence data set of 1,391 genomic loci (~6% of the total number of protein coding genes) that encode TFs, which we will focus on for the remainder of this Analysis article, and a further 216 loci representing possible TFs (see Supplementary information S3 (.txt file) for the data set). estimates of the coverage of our approach range from 85% to 94% (Supplementary information S1 (PDF)) suggesting an upper bound of ~1,700-1,900 TFcoding genes in the human genome. Despite the care that we have taken in compiling this data set, there are a few possible sources of inaccura cies. Our method depends heavily on the content of the InterPro database, and the ability of the search algo rithms to detect these domains in protein sequences. The repertoire should be updated when new InterPro entries for newly discovered DNAbinding domains, or refinements of existing ones, and more sensitive search methods become available.', 'A major limitation to studying the regulators themselves has been the lack of a reliable data set of TFs in the human genome, a difficulty that is com pounded by the large number of false predictions that can accompany the automated identification of genes encod ing DNAbinding domains. By manually inspecting every entry in the data set, we have minimized such errors. As a result the repertoire here is of high quality, and can be used as a basis to design further computational and experimental studies. Most of these TFs remain uncharacterized: this is highlighted by the observation that just three regulators (p53, eR and FOS) have more publications than all the other TFs put together. By incorporating publicly avail able genomic data sets, we provide clues into how these TFs might operate. For example, the SymAtlas microar ray data set allowed us to investigate the expression of TFs across 32 major tissues. Our analysis expanded the existing knowledge of ubiquitous and specific regulators by illustrating this phenomenon on a genomewide scale. Intriguingly, few TFs are present in an intermediate number of tis sues. This pattern of expression will have implications']</t>
         </is>
       </c>
-      <c r="AF106" t="inlineStr"/>
+      <c r="AF106" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Substantiated",
+  "explanation": "The statement mentions 'high-confidence TFs described by Vaquerizas et al.' which aligns with Excerpt 1, where the authors describe their method for grouping transcription factors based on confidence levels. The reference article provides a solid foundation for understanding high-confidence TFs, supporting the citing article's claim."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
@@ -16291,7 +17039,14 @@
           <t>['Low loss photopatternable polymer dielectics appear to be a promising solution. However, off-the-shelf commerically available photoresist polymers also exhibit vibrational absorption bands in the optical regime.  27  An ideal polymer dielectric would have losses comparable to polyethylene but have the additional benefits of a resist in that it is compatible with 3D fabrication techniques, photopatternable, and high temperature process tolerant.  28  We have identified a route to a tunable matrix material which satisfies each of these requirements in the thermal infrared spectral region (8-12 mm).  29, 30  The materials are synthesized using the ring opening metathesis polymerization (ROMP) of norbornene followed by a partial hydrogenation to remove most of the IR absorbing olefin groups in the 8-12 mm range (Scheme 1). Photopatterning of these materials can then be achieved using the remaining olefin groups via a thiol-ene coupling reaction. After cross-linking, the olefin IR-absorption band is minimized and the T g of the matrix material increases.', '6 ). As expected, the addition of the polymer to the wafer led to an upward shift in wavelength for both electric and magnetic resonances. This is due to an overall increase in the permittivity/refractive index of the resonator system. Finally, an absorption feature was observed at 10.3 mm which is consistent with the peak in the measured extinction coefficient for blanket polynorbornene film. This peak is associated with a small amount of unreacted olefin remaining in the polymer. Ultimately, though, the polymer had little influence on the overall metamaterial loss due to a lack of strong absorptions in the 8-12 mm spectral range. This is in contrast to commercially available photopatternable polymers that have much higher losses.  22, 27  \n\nConclusions\nIn summary, novel low loss photopatternable polymer dielectric materials were synthesized by partially hydrogenating polynorbornene to varying degrees and using the thiol-ene coupling Fig.  6  Cross-section view of an all-dielectric infrared metamaterial taken using SEM (left) and transmission spectra for the same metamaterial before and after adding the optimum polymer material (right).', 'used in microfabrication such as polyimide and benzocyclobutene based polymer (BCB).  27  \n\nPhotopatterning\nThe optimal polymer material was tested next for microfabrication compatibility. Preliminary experiments determined that an adhesion layer was required to ensure that thick films (&gt;1 mm) remained adhered to the silicon substrate during UV exposure. The adhesion layer was deposited by spin casting a layer of non-hydrogenated polynorbornene containing dithiol and photocross-linking via thiol-ene reaction to generate a thin film (28 nm). Next, a solution of partially hydrogenated polynorbornene (18.2%), cross-linker, and photoinitiator was prepared under the same conditions used to make the freestanding films and spun cast onto the wafer (see experimental). The film was irradiated (405 nm, 20 mW cm À2 ) using a mask aligner at a total power of 6,000 mJ cm À2 . The film was then developed in toluene for 5 min to remove the non cross-linked polymer and maintain the exposed regions.']</t>
         </is>
       </c>
-      <c r="AF107" t="inlineStr"/>
+      <c r="AF107" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article primarily focuses on the development of low-loss photopatternable polymer dielectrics for LWIR-metamaterial applications, but it does not explicitly mention the growing field of polymeric photonics or its attractiveness in terms of economy and scalability. The provided excerpts discuss the properties and fabrication of the polymer materials, but do not provide a clear connection to the statement."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
@@ -16443,7 +17198,14 @@
           <t>["The permanent ice cover of Lake Vida (Antarctica) encapsulates an extreme cryogenic brine ecosystem \n(-13 °C; salinity, 200) . This aphotic ecosystem is anoxic and consists of a slightly acidic (pH 6.2) sodium chloride-dominated brine. Expeditions in 2005 and 2010 were conducted to investigate the biogeochemistry of Lake Vida's brine system. A phylogenetically diverse and metabolically active Bacteria dominated microbial assemblage was observed in the brine. These bacteria live under very high levels of reduced metals, ammonia, molecular hydrogen (H 2 ), and dissolved organic carbon, as well as high concentrations of oxidized species of nitrogen (i.e., supersaturated nitrous oxide and ∼1 mmol•L -1 nitrate) and sulfur (as sulfate). The existence of this system, with active biota, and a suite of reduced as well as oxidized compounds, is unusual given the millennial scale of its isolation from external sources of energy.", "More recently, discoveries of life and associated processes in deep terrestrial subsurface ecosystems (9) provide compelling evidence of subsurface life that in some cases is fueled by nonphotosynthetic processes. Our knowledge of geochemical and microbial processes in aphotic icy environments remains mostly unknown, however, especially at subzero temperatures. Lake Vida is located in Victoria Valley, the northern most of the McMurdo Dry Valleys of East Antarctica (Fig.  S1 ). Initial studies of Lake Vida's thick ice cover described a -11.6 °C, wet, saline (estimated 245, practical salinity scale) ice at 15.8 m (10). This brine has been isolated by the thick lake ice cover and underlying 800-970 m of permafrost  (11, 12) , prohibiting input of ground water or of annual glacial melt and associated nutrients. 14 C-dating of organic matter sampled at 12 m in the lake ice cover suggests that the brine has been isolated for more than 2,800 y  (10) .", 'With the LVBr H 2 levels as high as they are, regardless of their source (abiotic or biogenic production), this H 2 could at least supply readily utilizable energy to combat depurination and racemization processes in this harsh ecosystem  (42) . LVBr microbial life is reasonably diverse, maintains cellular rRNA, and retains the ability to synthesize proteins at very low levels. We contend that metabolism in this encapsulated brine ecosystem may last for a prolonged period, well in excess of its ∼2,800 y of existence.\n\nMaterials and Methods\nField Sampling Campaign. Expeditions to Lake Vida resulted in successful extraction of ice cores (16.5 m in 2005, 20 and 27 m in 2010) and collections of brine that entered the borehole at a depth of ∼16 m (see Table  S1  for station coordinates). We followed a carefully designed sampling approach in both field campaigns to ensure clean access  (14) .']</t>
         </is>
       </c>
-      <c r="AF108" t="inlineStr"/>
+      <c r="AF108" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Substantiated",
+  "explanation": "The reference article describes the presence of microbial life, specifically bacteria, in the brine of an ice-sealed Antarctic lake, Lake Vida. The abstract and excerpts mention the discovery of a diverse and metabolically active bacterial assemblage in the lake's brine system, which is consistent with the statement that cyanobacteria inhabit ice-covered hypersaline lakes in areas that rarely touch the melting point."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
@@ -16583,7 +17345,14 @@
           <t>['A southeast-facing (present orientation) passive continental margin on the Yangtze Block was subsequently developed in the course of breakup of the Rodinia Supercontinent (Fig.  1A ). Thermal subsidence related to the post-rift extension of South China Block created significant accommodation space in which thick Middle-to-Late Neoproterozoic successions were deposited  (Jiang et al., 2003; Wang and Li, 2003) . Neoproterozoic stratigraphic successions in South China comprise well exposed, relatively unaltered glacial and interglacial deposits (Fig.  1B ). The Cryogenian Group unconformably overlies the slate rocks of the Banxi Group. Two main Cryogenian diamictite successions, the lower Jiangkou Group and the upper Nantuo Formation, have been recognized in South China. The interglacial Datangpo Formation of manganese-bearing shales, ∼ 10 m thick on the upper slope to ∼ 200 m thick on the lower slope  (Wang and Li, 2003) , sits on the glacial deposits of the Jiangkou Group.', "Introduction\nThe Neoproterozoic Era (1000-542 Ma) was an important interval subjected to dramatic climatic changes and biological evolutions in Earth's history. The Snowball Earth hypothesis suggested that the Earth was completely covered by ice sheets during the Neoproterozoic glaciation epoches  (Hoffman et al., 1998) . In the aftermath of glaciations, several lines of evidence, including iron chemistry and sulfur isotopic data from China, Canada, Oman and Australia, indicate stepwise oxygenation of the postglacial Ediacaran ocean (635-542 Ma), stimulating the evolution of early animal life  (Canfield et al., 2007; Fike et al., 2006; Komiya et al., 2008; Maruyama and Santosh, 2008; McFadden et al., 2008) .", 'The Datangpo Formation includes the lower thinner black shales (∼30 m thick), the focus of this study, and the upper thicker grey shales (∼ 200 m thick) (Fig.  1B ). A pair U-Pb zircon ages of 663 ± 4 Ma  (Zhou et al., 2004)  and 654.5 ± 3.8 Ma  (Zhang et al., 2008)  for the tuffaceous beds in the basal and topmost Datangpo Formation provides a constraint for the timing of this interglacial interval.\n\nMethods\nIn this study, we choose the Mingle section, where the interglacial Datangpo Formation comprises the lower 30 m-thick black shales and the upper 180 m-thick grey shales (Fig.  1 ). 16 samples, each at approximately 2 m apart, were collected in the lower 30 m-thick black shales for geochemical analysis. For each sample, ca. 5 g of fresh shale was grinded to powder (200 mesh in size) in an automated agate mill.']</t>
         </is>
       </c>
-      <c r="AF109" t="inlineStr"/>
+      <c r="AF109" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article does not provide any information about the thickness or correlatability of fine-grained terrigenous strata. The article focuses on the paleo-redox conditions and early sulfur cycling during the deposition of the Cryogenian Datangpo Formation in South China, but does not mention the specific characteristics of the strata mentioned in the citation statement."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
@@ -16724,7 +17493,14 @@
           <t>['It accumulated on a marine shelf, subject to repeated subaerial exposure  (Spencer 1971; Johnston 1993 ), situated at the then southeastern margin 1880 1900 1920 1940 1960 1980 2000 2 4 6 8 10 12 14 16 18 20 0 Year of first report 1871 Laurentia (S) 1884 Australia 1887 India 1891 Baltica 1904 South China 1910 Avalonia 1913 Laurentia (N) 1915 Kalahari 1929 Congo 1930 Siberia 1930 Sao Francisco 1933 West Africa 1937 Tarim 1950 Cadomia 1956 Kazakhstan 1959 Amazonia 1979 Arequipa 1981 North China 1982 Arabia 1984 Rio Plata 1990 Mongolia 1992 Iran 2003 Nile 2009 Chukotka-Arctic Alaska 22 24 Fig. 2.1. Cumulative discovery of Neoproterozoic glaciogenic deposits by palaeocontinent. See Table 2.1 for locations and references.', "These findings were highlighted in a Symposium on Palaeozoic and Pre-Cambrian Climates at the 17th IGC  (1937)  in Moscow. Major textbooks made note of these developments (Ko ¨ppen  &amp; Wegener 1924; Brooks 1922 Brooks , 1926;; Coleman 1926 ). In the third period  (1942 -1964) , nascent evidence from palaeomagnetism and from the occurrence of glacial deposits atop thick carbonate-dominated successions in the North Atlantic region and within such successions in central and southern Africa implied that Neoproterozoic ice sheets had reached sea level in low palaeolatitudes. This inference met resistance and, after the discovery of turbidity currents as a cause of graded bedding  (1950) , some diamictites were reinterpreted as mass-flow deposits of non-glacial origin. These issues were discussed at major conferences on Palaeoclimates in Newcastle-upon-Tyne,  England (1963), and Ko ¨ln, Germany (1964) . The radiation of macrofauna following soon after the 'infra-Cambrian' ice age was often remarked upon.", "The first Neoproterozoic glacial deposits were found in the SW of Scotland in 1871 and the rate of their discovery on 23 palaeocontinents and microcontinents was essentially linear until 1992 (Fig. \n2 .1). However, half of all the papers (n ¼ 811) written on them before the end of 2008 were published in the previous 10 years (Fig.  2 .2). This surge in activity is the justification for the present volume, but this history ends at 1997. We lack historical perspective on the last decade and the endpoint eliminates the need to weigh any of the author's own contributions on this topic. This chapter begins by placing the recognition of the Port Askaig boulder beds of Scotland as glaciogenic in its historical context, coming in 1871 on the heels of the discoveries of late Palaeozoic glacial deposits in India, Australia and South Africa. Their inspiration was the Pleistocene glacial controversy of 1837-1865, which spawned both the orbital and 'greenhouse' theories of bidirectional climate change, and established the principal criteria for the recognition of past glaciation."]</t>
         </is>
       </c>
-      <c r="AF110" t="inlineStr"/>
+      <c r="AF110" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Substantiated",
+  "explanation": "The reference article (55) supports the citing statement that the worldwide distribution of late Precambrian glacial deposits became evident in the 1930s. Excerpt 2 mentions a Symposium on Palaeozoic and Pre-Cambrian Climates at the 17th IGC (1937) in Moscow, where these findings were highlighted, indicating that by the 1930s, there was already significant evidence of Neoproterozoic glaciation's worldwide distribution."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
@@ -16865,7 +17641,14 @@
           <t>['2011; Ferreira et al. 2011; Rose 2015) . However, the ocean model setup and parameters in these simulations are based on the present-day ocean; yet, basic physical considerations make clear that the ocean circulation in a snowball world would be very different from the present day. In particular, the source of mechanical energy for the present-day ocean circulation is provided primarily by surface stress from the winds blowing over the ocean  (Wunsch and Ferrari 2004; Ferrari and Wunsch 2009) . During a snowball event, however, the ocean is shielded from atmospheric wind stress by a solid ice sheet, and the circulation is likely driven primarily by geothermal heating at the seafloor (typically ignored in the aforementioned studies). Because heat is supplied at higher temperatures and pressures near the seafloor, and lost at lower temperatures and pressures at the bottom of the ice sheet, mechanical energy can be extracted via the principle of a heat engine.', "Introduction\nGeological evidence suggests that for multiple time periods during Earth's history the oceans were entirely, or almost entirely, covered by sea glaciers  (Kirschvink 1992; Hoffman et al. 1998; Hoffman and Li 2009; Hoffman and Schrag 2002; Pierrehumbert et al. 2011 ). These periods are commonly referred to as ''snowball Earth'' events. While many studies have simulated the atmospheric and climate dynamics of snowball Earth events (e.g.,  Wetherald and Manabe 1975; Pierrehumbert 2005; Abbot and Pierrehumbert 2010; Voigt and Marotzke 2010; Voigt et al. 2012; Abbot et al. 2013; Rose 2015) , the ocean dynamics have received relatively little attention. A number of studies have presented coupled atmosphere-ocean simulations of snowball states (e.g.,  Poulsen et al. 2001; Marotzke and Botzet 2007; Voigt and Marotzke 2010; Voigt et al. 2011; Ferreira et al.", 'However, the rate of mechanical energy extraction is expected to be much smaller than the power provided to the large-scale circulation in the present-day ocean by wind stress, which provides a crucial constraint on the strength of the ocean circulation and mixing rates (e.g.,  Ferrari and Wunsch 2009) . A more focused analysis of snowball Earth ocean circulation was recently spearheaded in a series of papers by  Ashkenazy et al. (2013 Ashkenazy et al. ( , 2014) )  and  Ashkenazy and Tziperman (2016) , who use a hierarchy of models to study the ocean circulation under a thick ice sheet. In  Ashkenazy et al. (2013)  and  Ashkenazy et al. (2014) , global two-and three-dimensional ocean models are coupled to a dynamic sea glacier model. The simulations of  Ashkenazy et al. (2013 Ashkenazy et al. ( , 2014) )  indicate interesting dynamics mostly in the equatorial region, where a vigorous overturning circulation with associated zonal jets develops within a few degrees of the equator.']</t>
         </is>
       </c>
-      <c r="AF111" t="inlineStr"/>
+      <c r="AF111" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Substantiated",
+  "explanation": "The reference article discusses the ocean circulation in a Snowball Earth scenario and presents theoretical arguments and numerical simulations to understand the dynamics. The excerpts provided highlight the differences between present-day ocean circulation and Snowball Earth ocean circulation, driven by geothermal heating at the seafloor. While the article does not explicitly mention Cryogenian cryoconite deposits, its focus on Snowball Earth ocean circulation makes it relevant to the search for such deposits, as mentioned in the citation statement."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
@@ -17009,7 +17792,14 @@
           <t>['The field of quantum information began its experimental uprise with the proposal from Cirac and Zoller \n[1]  in 1995, extended by the prospect of scalability of ion trap based systems  [2]  via shuttling of qubits in multiplexed traps along the ideas pioneered by Wineland  [3] . Scalable information processing in a multiplexed ion trap can be accomplished by having fixed processing sites where logic operations are performed, and ion qubits will be moved in and out of these regions by shuttling operations. The duration of such shuttling has to be much faster than the relevant decoherence times  [4] . Furthermore, it is desirable to reduce the total time consumption of all relevant operations, where shuttling will contribute a considerable amount  [5] , and aim for the performance of the naturally fast solid state architectures  [6] . So far, ion shuttling in a multiplexed trap has been demonstrated together with additional sympathetic cooling  [7] , and in the adiabatic regime, where the transient displacement of the ion is smaller than the size of the its wavepacket  [8, 9] .', '1b ). We refer to this as the pairwise energy-neutral transport. For the second scheme, the self-neutral transport we apply a sharp counter-"kick" to the ion at the end of a single transport operation, stopping its motion (Fig.  1c ). This case of single-sided transport allows even faster shuttling and can be sequentially repeated since it is energy selfneutral, making it the preferred building block for scalable quantum information protocols. The experiments are carried out in a micro-structured segmented Paul trap  [12] , where the trapping voltage applied to each electrode segment is controlled by an FPGA-based arbitrary waveform generator that allows high resolution for both timing and voltage, while having low noise ( 10nV/ √ Hz at the trap frequency). Further noise reduction at high frequencies is done with a Π-type filter having a cut-off frequency of 300 kHz. The axial trap frequency is ν ax = ω ax /2π = 1.41 MHz, while the radial trap frequencies are ∼ 3 MHz. The transport is carried out by varying the voltages on the segments, such that the minimum of the trapping potential is moved towards the final location in time steps of 400 ns.', 'Transport of neutral atoms have also been performed using magnetic  [10]  or optical  [11]  techniques. Because quantum gate operations require ions close to the motional ground state and fast transport inherently creates motional excitation, the challenge is to develop transport protocols that guarantee sufficiency small energy transfer. In this work we demonstrate shuttling operations that are highly non-adiabatic while the final state of the ion is close to the motional groundstate. We also show that quantum information stored in both the motional and the spin degree of freedom is preserved through the shuttling. During a shuttling operation, the ion motion in the harmonic trapping potential is excited when the acceleration is sufficiently strong. This motional excitation is a harmonic oscillation, characterized by a well defined phase, thus allowing it to be canceled out by proper management of the forces involved during or after the transport. We experimentally demonstrate two methods of canceling the acquired motional excitation. One method uses two shuttles, where the transport to the destination generates the same net momentum transfer as the transport back, but is applied 180 • out of phase with respect to the secular oscillation of the ion (Fig.']</t>
         </is>
       </c>
-      <c r="AF112" t="inlineStr"/>
+      <c r="AF112" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Substantiated",
+  "explanation": "The reference article [17] supports the statement about fast ion shuttling. The abstract and excerpts describe experiments demonstrating fast transport of ions in a segmented microstructured Paul trap, with optimized transport protocols that minimize energy increase and preserve quantum information. This is consistent with the citing article's proposal for using fast ion shuttling to achieve a short quantum computer cycle time."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
@@ -17153,7 +17943,15 @@
           <t>['Moreover, a comparison of the modeled phase diagram and the experimental data demonstrated greater than 90 % agreement between the two; i. e. over 90% of the crystal structures obtained experimentally were correctly predicted by the phase diagram as being the most stable arrangement of particles. Because each of the SNA-NPs used to assemble these superlattices is functionalized with a large number of DNA strands, it is possible to put multiple DNA sequences on a single nanoparticle. Therefore, the fifth rule of DNA-programmed assembly is: SNA-NPs can be functionalized with more than one oligonucleotide bonding element, providing access to crystal structures not possible with single element SNA-NPs. For example, a SNA-NP that is functionalized with linkers containing self-complementary sticky ends would be predicted to form an fcc lattice as its thermodynamic product, as per rule 1. However, if this SNA-NP were also functionalized with a second type of DNA linker that contained a sticky end complementary to the sticky ends of a different SNA-NP, additional DNA linkages could be created.', 'Therefore, to assemble nanoparticles into hierarchical structures, ligands must be attached to the surface of the nanoparticles to dictate how nanoparticles interact with each other  [17 -22] . Many different ligands have been utilized to achieve this, taking control of ionic  [20] , van der Waals  [21 -22] , or biological recognition interactions  [17, 18]  to dictate nanoparticle bonding patterns. An ideal ligand choice to achieve these types of interactions is DNA. DNA is a linear polymer consisting of a series of nucleobases, where the length of the DNA strand is dictated by the number of nucleobases, and interactions between different DNA strands are dictated by the sequence of those bases -two DNA strands will only hybridize to one another if they contain complementary base sequences. DNA is readily synthesized via automated procedures, and can be readily modified with many different functional groups, enabling its attachment to a wide variety of nanoparticle compositions  [23 -27] . In 1996, the Mirkin group developed the concept of the polyvalent-DNA nanoparticle conjugate, now referred to as the spherical nucleic acid nanoparticle conjugate (SNA-NP).', 'Since the development of the SNA-NP conjugate in 1996, the Mirkin group, along with others, have taken major strides in being able to utilize this structure as a building block in the synthesis of ordered arrays of nanoparticles. Although early attempts yielded materials that exhibited no long range ordering, short-range ordering and interparticle distance control was demonstrated in subsequent years  [35] . Long-range ordering and crystalline materials were achieved for the first time in 2008 by altering the SNA-NP design to utilize DNA linker strands to connect the nanoparticles  [36] . These linkers consisted of three basic regions: a recognition sequence complementary to the DNA sequence physically attached to the nanoparticle, a spacer sequence used to control the length of the DNA linker, and a short sticky end presented at the hydrodynamic radius of the SNA-NP. Hybridization interactions between sticky ends on adjacent SNA-NPs allow the nanoparticle to link to one another. Because each SNA-NP can be attached to tens to hundreds of DNA linker strands (depending on the nanoparticle core size)  [24] , each nanoparticle can form tens to hundreds of DNA connections to adjacent particles.']</t>
         </is>
       </c>
-      <c r="AF113" t="inlineStr"/>
+      <c r="AF113" t="inlineStr">
+        <is>
+          <t>Here is my evaluation:
+{
+  "label": "Substantiated",
+  "explanation": "The reference article discusses the use of DNA-driven self-assembly of nanoparticles, specifically through the design rules outlined for synthesizing colloidal crystal structures with controlled lattice parameters. The excerpts provide details on how DNA-functionalized nanoparticles can be used to assemble superlattices, which supports the citation statement about DNA-driven self-assembly of NPs."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
@@ -17301,7 +18099,14 @@
           <t>['submission to the CTF challenge using CTFFIND3. Those parameters were: N d = 256, g min 1 0.8 -0.8 1.1 -2.5 1.5 3.0 42.7 8.1 2.4 2 -0.1 1.0 -0.1 1.0 -2.6 1.9 28.2 53.2 8.1 1.5 3 0.0 0.2 -0.1 0.2 -2.1 0.6 21.5 79.9 6.2 1.7 4 0.2 0.5 -0.2 0.5 -2.3 1.1 9.1 77.6 7.4 1.9 5 0.2 0.8 0.2 0.7 -1.1 1.0 -14.5 42.5 11.3 8.6 6 0.3 1.2 -0.6 0.9 -1.1 0.', "Introduction\nEstimating the electron microscope's objective lens defocus and astigmatism from micrographs is of great importance in the three-dimensional reconstruction of biological specimens (reviewed by  Cheng et al., 2015) . Many programs are available for this purpose. Of those, CTFFIND3  (Mindell and Grigorieff, 2003)  is widely used and thought to perform well under a range of circumstances  (Marabini et al., 2015) . We present an updated version of this program, called CTFFIND4, which aims to match the quality of results obtained with CTFFIND3 and to do so significantly faster.", 'Adapted from Figure  3  of  Mindell and Grigorieff (2003) . Diagnostic image from micrograph #1 of set #7 of the CTF challenge, output by CTFFIND4 using runtime parameters detailed in Table  3 . The 2-dimensional CTF (CTF fit ) is overlayed onto the preprocessed amplitude spectrum (A d ) up to the radius corresponding to g max . Figure  3 : Image E generated from the CTF fit to micrograph #1 of set #7 of the CTF challenge. At every pixel (corresponding to a spatial frequency vector g), this image records n, the number of preceding CTF extrema (Equation  11 ). Here this value is color-coded, so that pixels at spatial frequencies before the first extremum of the CTF, which have value 0, are displayed in dark blue. Pixels that have 35 or more preceding CTF extrema are shown in dark red. . One would normally solve this by increasing N d , but we restricted ourselves to previously-used parameter values for this experiment (see caption to Table  3  for more details).']</t>
         </is>
       </c>
-      <c r="AF114" t="inlineStr"/>
+      <c r="AF114" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article focuses on CTFFIND4, a program for estimating objective lens defocus parameters from transmission electron micrographs. There is no mention of EMAN2 or initial particle picking to generate template images, which are the topics of the citation statement. The content of the abstract and excerpts does not support the claim related to EMAN2."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
@@ -17445,7 +18250,14 @@
           <t>['years, however, there has been increasing awareness that events during migration or on wintering grounds can affect populations of migratory animals \n(Newton 2004 , Studds &amp; Marra 2005 , Both et al. 2006) . Identifying migration routes, stopover areas and wintering areas for migratory species that are declining is therefore necessary for designing effective conservation strategies that can address threats operating outside breeding areas  (Wilcove &amp; Wikelski 2008) . The decline of long-distance migrants has been most apparent for passerines and smaller-bodied birds but there is evidence that long-distance migratory raptors are also declining  (Hoffman &amp; Smith 2003) . Among the four vulture species that breed in the western Palaearctic, the Egyptian Vulture Neophron percnopterus is the only longdistance migrant that travels to wintering regions in sub-Saharan Africa  (Porter &amp; Beaman 1985 , Meyburg et al. 2004 , Garc ıa-Ripoll es et al. 2010) .', 'During this time, winter movement ranges were large and included multiple centres of activity, in which birds remained for several weeks before exploring alternative areas. The average core 50% utilization distribution was 28 000 km 2 , but ranged from &lt; 5000 to  &gt; 90 000 km 2 among individuals (Table  3 ). Winter movement ranges (100% minimum convex polygon) were more than an order of magnitude larger (&gt; 310 000 km 2 ), with similarly large varia-tion among individuals (Table  3 ). Wintering regions ranged from southwest Yemen to Nigeria, with core wintering areas in southern Chad and Sudan (Fig.  3 ). Head length (cm) Log(probability of successful migration)/2 The habitat in core ranges in which juvenile vultures spent 50% of their time differed from the habitat encountered in winter movement ranges. Our random forest model explained 81.9% of the variation in the data and successfully classified locations as core wintering locations. Elevation and landscape type were the most important variables distinguishing core locations from those available in movement ranges (Table  4 ).', 'Start of autumn migration was defined as the first day on which birds travelled over 100 km, the end of autumn migration was defined as the first day south of 22°N latitude when a bird reversed its course or remained stationary. Migration distance was the cumulative distance between all subsequent locations during the migration period, and migration speed was the migration distance divided by the number of days spent migrating  (Alerstam 2003) . The wintering period was defined as the time between the end of autumn migration and the onset of spring migration, and we used all locations from that time period to estimate a movement range for each individual. For the birds still alive after 2 years, the onset of spring migration was defined as the date when the first northward movement was initi-ated that ultimately took the bird north of 22°N. The winter movement range was calculated as the minimum convex polygon of 100% of the winter locations to be comparable with a previous study  (Meyburg et al. 2004) , and the home-ranges were calculated as the 95% and 50% kernel utilization distribution (Garc ıa-Ripoll es et al. 2010).']</t>
         </is>
       </c>
-      <c r="AF115" t="inlineStr"/>
+      <c r="AF115" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article does not support the statement that moving from breeding grounds in the Northern Hemisphere to wintering grounds in the Southern Hemisphere enables the exploitation of surplus seasonal resources with a clear dynamic link between breeding and wintering resources. The article focuses on juvenile mortality during migration, migratory routes, and wintering areas of Egyptian Vultures, but does not discuss the relationship between seasonal resources at breeding and wintering grounds."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
@@ -17585,7 +18397,14 @@
           <t>['Because of the complicated nature of this assay, it does not always reflect the true enzymic reaction. l l Methods which use oligo or poly N-acetylglucosamine (NAG*) derivatives as the substrate have been developed recently. These assays were monitored by • • 2 31 d \' I 4 61 VIscosImetry\' or re ucmg group ana yses. . This report describes a simple and reproducible reducing group analysis method by a modification of Schales\' procedure. 61  The color reagent solution was made by dissolving 0.5 g potassium fericyanide in I litter of 0.5 M sodium carbonate and stored in a brown bottle. Two m1 of the reagent were mixed with 1.5 ml of sample solution and incubated in boiling water for 15 min in a !: Cl test tube stoppered with aluminum foil. After\'" 0.4 cooling, the optical density at 420 nm was read versus water. The concentration of sodium carbonate was sufficiently high so as not to be affected by the buffer action of the sample solution.', "reproducible. The decrease in total color value (JD m X ml) was constant (18.0±0.5jmg NAG) for a given NAG amount in several fericyanide concentrations at least upto half the concentration employed here. The curve shows that 0~0.15 mg of NAG can be detected under these conditions (caution must be taken with other oligomers which have different color values). This method has adequate sensitivity for the detection of reducing groups produced by lysozyme action. Park-johnson's method 71 is too sensitive (affected by most cations present) and Somogyi's method SI is not sensitive enough. For the measurement of lysozyme, glycol chitin 91 was used as a substrate. To 1 ml of FIG.  2 . Standard Curve for the Lysozyme Activity in 0.1 M Acetate Buffer, pH 4.5.", 'Short Communication\n[Agr.  BioI. Chern., Vol. 35, No.7, p. 1154~1156, 1971]  A Simple Activity Measurement of Lysozyme The mixture of 2 ml of the color reagent and 1.5 ml of NAG solution was incubated in boiling water for 15 min and the decrease in O.D. 420 was plotted against NAG concentration. sodium carbonate. The color was also not affected when the mixture was allowed to stand for a few hours before or after boiling or when the boiling period was varied from 10 to 30 min as long as NAG and (NAGl: were used. Thus a stable and reproducible color is developed. A blank value of 0.850 (O.D. 420 ) was obtained within ± 1% deviation. 0.20 0.15 0.10 NAG (mg) 0.05 o 01-0 0.8 0.2 0.6 * Abbreviations used are: NAG; N-acetylglucosamine, NBS; N-bromosuccinimide.']</t>
         </is>
       </c>
-      <c r="AF116" t="inlineStr"/>
+      <c r="AF116" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Substantiated",
+  "explanation": "The reference article describes a modified Schales' procedure for measuring reducing group analysis using N-acetylglucosamine (NAG) derivatives as substrates. The excerpts provide details on the method, including preparation of the color reagent solution and incubation conditions, which support the use of this procedure to determine NAG concentration."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
@@ -17733,7 +18552,14 @@
           <t>['INTRODUCTION\nAdvances in basic research and molecular diagnostics capabilities are intimately coupled to the development of ever more precise and sensitive measurement technologies. Quantitative (q)PCR is the current gold standard for DNA measurement and genetic diagnostics but remains poorly suited to measurements of absolute concentration, has a limited precision (~20%), and presents difficulties in reliably detecting low-copy-number templates due to nonspecific amplification and competitive side reactions. qPCR measurements are thus inadequate for demanding applications such as early detection of cancer and monitoring of residual disease  [1] , analysis of single-cell gene expression  [2] , and the diagnosis of fetal genetic disorders using small allelic imbalances in circulating DNA.\n\nTHEORY\nA promising solution to such measurement problems is digital PCR  [3] , a single-molecule counting technique. Digital PCR works by partitioning a sample at limiting dilution followed by PCR amplification and endpoint detection to identify the presence or absence of template molecules in each reaction. All performance metrics of digital PCR, including sensitivity, precision and dynamic range, improve with the total number of digital reactions performed.', 'After PCR thermocycling, the devices were scanned at 0.5 micron per pixel (Figure  1d ) and analyzed using a custom image analysis software written in C for automated segmentation of chambers (Figure  1e ). \n\nRESULTS AND DISCUSSION\nHere we present a valve-free microfluidic digital PCR device that performs a million single molecule PCR reactions in uniform arrays of pl volume chambers having densities up to 440,000 reactions cm -2 (Figure  1a ). Our device uses surface tension to achieve partitioning of the sample into a uniform array of pl-volume sub-reactions. The sample is injected into a poly(dimethylsiloxane) (PDMS) device featuring a bifurcating channel network, having a cross-section of 3 µm x 3 µm, that connects to linear arrays of 10 pl (20 µm × 20 µm × 25 µm) "dead-end" chambers. The reagent solutions are then pushed in the device until complete filling and partitioning of the chambers is achieved by flushing an immiscible fluorinated oil that preferentially wets the channel walls, displacing the remaining aqueous phase (Figure  1c ).', 'Reliable discrimination of 2% and 3% enrichment was obtained reproducibly using sub-arrays of 100,000 chambers, while 1% enrichment was only well-resolved using full 1,000,000 chamber arrays.\n\nCONCLUSION\nIn addition to enabling new measurements in biomedical research and diagnostics, the high assay density in our device has important implications for the adoption of digital PCR as a routine analytical tool. Thus, we contend that megapixel digital PCR or similar high-density formats will ultimately replace real-time qPCR as the standard analytical tool for absolute DNA measurement.']</t>
         </is>
       </c>
-      <c r="AF117" t="inlineStr"/>
+      <c r="AF117" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Substantiated",
+  "explanation": "The reference article (14) clearly discusses digital PCR and its advantages over traditional qPCR, including improved sensitivity and precision. The excerpts provided also describe a megapixel digital PCR device that enables high-fidelity single DNA molecule amplification, which aligns with the statement from the citing article about using digital PCR to lower device complexity."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
@@ -17877,7 +18703,14 @@
           <t>['It is well known that an incontestable limitation of these ex situ studies are the insufficient information collection to further scrutinize perovskites growth mechanism. In addition, there are also some literatures reporting the chemical pathways from the plumbate intermediate  15, 16  or metastable phase  17, 18  to the certain perovskite crystal identified by the in situ X-ray diffraction. However, the time evolution of crystallisation and phase transition in such in situ cases usually begins with the prepared solvent-intermediated complex film, not the pristine mixed solution in our work. For these kinds of methodologies without the analysis of the pure precursor, they cannot draw a conclusion on whether the perovskite crystal growth begins in the solution phase or in the solid phase. Even though there are a few reports observing the perovskite crystallisation from drop-casting solution to dry film  19  , however, the full transformation process to pure perovskite was not achieved, and the clear formation mechanism was still indistinct with existence of by-products in the final dried film.', 'The wavelength of the banding was found to decrease with increasing processing, as seen from the 120 °C thin films (Supplementary Figs  10  and  13 ). The periodic patterns observed in the perovskite crystallisation are a complex interplay between solution flow, solute diffusion, the solvent extraction and the crystal growth. When the perovskite solution is deposited on an elevated heating substrate, the evaporation process is more rapidly. Once the solution supersaturates, the nucleation occurs, and the crystal growth followed by. A rapid removal of solvent near the growth front induces liquid convection that carries solute to the crystal face to allow crystallisation to occur, depleting the volume in front of the growth front. This crystallisation-depletion mechanism  39, 40  gives rise to a concentration gradient and a periodic crystallisation of the perovskite, as shown schematically in Fig.  5b , c . AFM images in Fig.', 'The crystallisation-depletion mechanism is developed to elucidate the periodic nucleation and the kinetically trapped morphology at a mesoscopic level. Based on these dynamics studies, the whole process of the perovskites formation from molecular to microstructure is successfully demonstrated.\n\nResults\nPerovskites crystallisation and structure transformation. All GIXD measurements were performed on beamline 7.3.3 at Advanced Light Sources of Lawrence Berkeley National Laboratory with critical methods to obtain the perovskites structure formation and crystal growth in real time. To in situ monitor the whole evolution process at the very beginning with the precursor solution, a compatible mini-slot-die printer  20  was integrated with on-line GIXD, as shown in Supplementary Fig.  1 . For the traditional spincoating technique  21  , most of the deposition solution is ejected during rotation and the subsequent thermal annealing process begins with the intermediated complex film, hindering the capture of the whole crystallisation process. The in situ printing experiment was conducted in the helium atmosphere to reduce the air scattering.']</t>
         </is>
       </c>
-      <c r="AF118" t="inlineStr"/>
+      <c r="AF118" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article discusses perovskite crystallization and growth mechanisms from precursor solutions, but it does not explicitly state that blade coating allows film crystallization without an intermediate phase. The provided excerpts focus on the crystallization-depletion mechanism, in situ observations, and the importance of studying the entire process from precursor solution to final film, but they do not directly support or contradict the specific claim made about blade coating."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
@@ -18021,7 +18854,14 @@
           <t>['Fusion gene construction\nmCardinal cDNA was PCR amplified with a 5′ primer encoding an AgeI site and a 3′ primer encoding either a BspEI (C1) or NotI (N1) site for C-terminal and N-terminal fusions (with regards to the FP), respectively. The purified and digested PCR products were ligated into similarly digested pEGFP-C1 and pEGFP-N1 cloning vectors to create pmCardinal-C1 and pmCardinal-N1. A cDNA fragment encoding each protein domain was PCR amplified with primers containing the appropriate restriction enzyme sites and ligated into pmCardinal-C1 or pmCardinal-N1. To prepare fusions at the N-terminus of mCardinal, the following digests were performed: human non-muscle α-actinin (GenBank accession number NM_001130005.1, source: Tom Keller, Florida State University, Tallahassee, FL, U.S.A.), EcoRI and NotI; human calnexin (NM_001746.', 'Lentiviral constructs expressed in MuSCs were hLIG-EF1α-mCardinal-IRES PV -luciferase2 and pLL3.7-EF1α-mCardinal-IRES EMCV -Clover-P2A-luciferase2. Full sequences of plasmids are available upon request. One million myoblasts were transfected with 5.3 μg total of minicircle vector and pCMV-piggyBac in a 3:1 molar ratio in Solution V from the Cell Line Optimization Nucleofector Kit (Lonza) with program B-32 on a Nucleofector I electroporation machine (Lonza). Myoblasts were cultured for 10 days, and then the 10% of cells exhibiting the highest far-red fluorescence upon 635 nm excitation were selected by fluorescence activated cell sorting on a FACSAria II (Becton-Dickinson). Myoblasts were further cultured for 7 days, and then injected in injured TA muscles.', 'Lysates were extracted with B-PER II (Pierce), and spectra were obtained on a Safire II plate reader (TECAN). DNA sequences of all constructs are available upon request.\n\nProtein production and characterization\nFluorescent proteins with polyhistidine tags were expressed from pNCS vectors in E. coli strain DH5α, purified with cobalt-chelating affinity chromatography (Pierce) and desalted using gel filtration columns (Bio-rad). Excitation and emission spectra of recombinant proteins were measured with a Horiba Jobin Yvon Fluorolog 3 fluorimeter (HORIBA Scientific). Absorbance spectra were obtained on a SafireII plate reader (Tecan). Extinction coefficients were calculated using the base-denaturation method, as previously described for red fluorescent proteins  30  . Quantum yields were determined by integration of emission curves corrected for detector sensitivity, using mKate2 as a standard (quantum yield 0.4).']</t>
         </is>
       </c>
-      <c r="AF119" t="inlineStr"/>
+      <c r="AF119" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Substantiated",
+  "explanation": "The reference article [44] substantiates the claim that mCardinal is a fluorescent protein, which is consistent with its use to assess transfection efficiency in the citing article. The abstract and excerpts provide details on the development and characterization of mCardinal, demonstrating its suitability as a fluorescent marker."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
@@ -18165,7 +19005,14 @@
           <t>['), they would show a significant reduction of carbon uptake, primarily driven by the ocean stratification, and reduced ocean thermohaline circulation  [28] [29] [30] . Terrestrial models also investigated the effect of CO 2 and climate, always agreeing on the positive response of land carbon storage to atmospheric CO 2 increase (the so-called fertilization effect), but not reaching consensus on the terrestrial ecosystem response to the associated climate change. Some earlier studies found an enhanced terrestrial productivity  [31]  while later studies found the opposite  [32, 33] . The third assessment report of IPCC concluded that, by mid-twenty-first century, climate change would reduce the land carbon uptake by 21% to 43% and the ocean carbon uptake by 6% to 25%, relative to CO 2 only driven uptakes  [34] . This IPCC range was very conservative, as further discussed below. Nevertheless, all these studies gave a clear signal to the climate modelling community: one cannot simulate future climate change assuming atmospheric CO 2 can be known, a priori, from the CO 2 emissions trajectory.', 'The climatepermafrost carbon gain is hence very uncertain; as the RCP8.5 emissions are about 2000 GtC for the twenty-first century, the permafrost carbon release, 50-250 GtC, translates into a gain ranging between 2.5% and 12.5%. CO 2 fertilization, i.e. the increase of terrestrial plants productivity as a response to atmospheric CO 2 increase, remains one of the major source of uncertainty in the CMIP5 ESMs carbon cycle projections  [40] . Although the basic process is relatively well understood: elevated CO 2 stimulates plant photosynthesis, increasing biomass production and hence carbon uptake, the quantification at the global scale remains poorly constrained. There are no long-term global observations of photosynthesis yet that could be used to evaluate models responses. In addition, the induced carbon sink does not only depends on the rate of increase of photosynthesis, it also depends on the residence time of carbon in biomass and soils, delaying the increase in heterotrophic decomposition. Surprisingly, CMIP5 ESMs showed a very wide range of residence time and hence global vegetation and soil carbon estimates  [61, 62] .', 'However, the obvious question is whether the ocean and the land ecosystems will continue to provide such a service to humanity, removing about half of the CO 2 emitted by human activities. Without these land and ocean sinks, the atmospheric CO 2 increase would be about twice as fast; current atmospheric CO 2 concentration would be already above 500 ppm, inducing a warming of more than 2 K above pre-industrial level (assuming a median estimate of 3 K for the climate sensitivity). There was, and there still is, an urgent need to better understand the process governing these carbon sinks and whether they would continue to operate in the future. Global land and ocean models were used to investigate the fate of ocean or land carbon storage under future change in environmental conditions, mainly elevated atmospheric CO 2 and climate change. Global ocean models forced with a scenario of atmospheric CO 2 over the twenty-first century would simulate a continuous increase in ocean CO 2 uptake, driven by the growing imbalance of CO 2 partial pressure between the atmosphere and the ocean surface. When the same models would additionally account for climate change (changes in ocean temperature, salinity, ocean circulation, etc.']</t>
         </is>
       </c>
-      <c r="AF120" t="inlineStr"/>
+      <c r="AF120" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Substantiated",
+  "explanation": "The reference article supports the claim that unchecked climate change could reverse terrestrial carbon sinks by midcentury. Excerpt 1 mentions that 'climate change would reduce the land carbon uptake' and the IPCC range suggests a reduction of 21% to 43% in land carbon uptake by mid-twenty-first century due to climate change."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
@@ -18305,7 +19152,14 @@
           <t>["The 'yield growth' case assumes 9% higher yields than those forecast by  FAO (2006) , based on the 'Global Orchestration' scenario in the Millennium Ecosystem Assessment, (2005). The livestock 'feeding efficiency' gain case assumes improved livestock feeding efficiencies according to the 'intensive' livestock feeding efficiencies as described in  Erb et al., (2012a) ; under this assumption, input-output ratios of livestock are on average 17% better than in the reference case. The 'waste reduction' case assumes a reduction in the losses in the food supply chain by 6% (see section 2.2.), which was evaluated by assuming that demand reduction would linearly reduce all flows. As Table  2  shows, the combination of all measures results in a substantial reduction in cropland and grazing areas, even though the individual measures cannot be added up due to the interactions between the individual compartments shown in Fig.  1 , and regional disparities considered in the biomass-balance model  (Erb et al., 2012a,b) . In all cases, former agricultural land (i.e.", 'In all cases, former agricultural land (i.e. cropland plus grazing land area) would become available for nonfood purposes (afforestation or bioenergy crops) if stocking densities on grazing land were increased to higher, but still sustainable, levels; the latter were derived from spatially explicit data on the productivity of grazing areas (see  Erb et al., 2009 Erb et al., , 2012a,b;,b; Haberl et al., 2011) . Table  2  shows the GHG reductions that could be achieved in 2050 by using the spare land for afforestation, assuming a CO 2 sequestration of 11.8 t CO 2 eq ha À1 yr À1 (based on  Smith et al., 2000) . GHG reduction resulting from bioenergy was calculated using two different assumptions: a high value was calculated assuming that biomass produced in short-rotation coppice or energy grass plantations would replace fossil fuels, thereby saving 18.3 tCO 2 -eq.', "agricultural land use) and consumption of biomass (i.e. nutrition and other uses) for 11 world regions, with trade balancing mismatches of supply and demand between regions. Based on this model, we assess in a consistent way the areas freed or consumed by changing yields, diets and livestock efficiencies, which potentially can be used for bioenergy or carbon sequestration. The 'reference' case is similar to the projections of the FAO, (  2006 ) for 2050 in terms of changes in diets and cropland yields, as implemented in the TREND scenario in  Erb et al., (2012a) . The 'diet change' case assumes a switch to a low animal product diet ('fair and frugal' diet; see  Erb et al., 2012a)  and a contract and converge model of global food demand to the global average in the year 2000 (i.e. 2800 kcal cap À1 d À1 , compared to the global mean of 3100 kcal cap À1 d À1 in the reference case)."]</t>
         </is>
       </c>
-      <c r="AF121" t="inlineStr"/>
+      <c r="AF121" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Substantiated",
+  "explanation": "The citation statement mentions allowing potential reforestation of all grazing lands in forested ecoregions, consistent with agricultural intensification scenarios. The reference article supports this claim by discussing how increasing livestock feeding efficiencies and stocking densities on grazing land can make former agricultural land available for non-food purposes like afforestation (Excerpt 2). This aligns with the idea of reforesting grazing lands while maintaining or improving agricultural productivity."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
@@ -18450,7 +19304,14 @@
           <t>['Rev. Lett. 79, 2089 (1997). 2 M. Städele, M. Moukara, J. A. Majewski, P. Vogl, and A. Görling, Phys. Rev. B 59, 10031 (1999). 3 R. J. Magyar, A. Fleszar, and E. K. U. Gross, Phys. Rev. B 69, 045111 (2004). 4 P. Rinke, A. Qteish, J. Neugebauer, C. Freysoldt, and M. Scheffler, New J. Phys. 7, 126 (2005). 5 A. Qteish, A. I. Al-Sharif, M. Fuchs, M. Scheffler, S. Boeck, and J. Neugebauer, Comp. Phys. Comm. 169, 28 (2005).\n\nVI. APPENDIX\nIn this Appendix we briefly consider the treatment of singularities for systems with partially filled bands.', 'III. RESULTS FOR DIAMOND AND TRANS -POLYACETYLENE\nThe applicability of the presented approach for treating the divergencies is now demonstrated by applying it to two cases, diamond and trans-polyacetylene, using different approximations for the exchange-correlation functionals: the Slater-Dirac (exchange-only LDA) referred to as Dirac exchange in the following, the complete exchange-correlation LDA in the parametrisation of Vosko, Wilk, and Nusair (VWN), 8 the combination of Dirac exchange plus Perdew86 9 (P86) correlation (P86 being VWN correlation plus a gradient correction), the EXX (exact-exchange only), and finally the combination of EXX with P86 correlation. The pseudopotentials were generated using the pseudopotential generation code of Engel,  26  which is based on the Troullier-Martins norm-conserving scheme.  27  In all cases the pseudopotentials were generated using consistently the same functionals for exchange and correlation as for the plane wave calculations. Relativistic effect are not included.', '(15) This implies that for the evaluation of the exchange energy the singular terms in the original expression (6) can first simply be omitted and then be taken into account by N v [ F -F ], i.e., by adding N v [ F -F ] to the exchange energy obtained if the singular terms are simply omitted. The correction is calculated only once before the self-consistency procedure. In fact, the correction N v [ F -F ] depends only on the unit cell lattice vectors, and thus in particular on the unit cell volume V , and on the number N k and the positions of the k points. It does not depend on the number, type, or positions of the atoms within the unit cell, and does not depend on the one-particle wave functions. This has obvious advantages for atomic relaxations at fixed unit cell volumes and fixed lattices. The whole scheme, of course, hinges on the availability of a suitable function f (q). For fcc systems such a function was given by Gygi and Baldereschi.  20  For sc, bcc, hexagonal, and orthorhombic systems Wenzien 21 presented such functions.']</t>
         </is>
       </c>
-      <c r="AF122" t="inlineStr"/>
+      <c r="AF122" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article does not mention PBE0 or accelerating convergence for it. The article discusses treating singularities in exact exchange (EXX) Kohn-Sham and Hartree-Fock methods, but does not address the specific functional PBE0 or its convergence properties."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
@@ -18591,7 +19452,15 @@
           <t>['v τ -dep XC,σ can be written as v τ -dep XC,σ (r) = 1 Ω BZ i BZ d 3 k V cell d 3 r ′ d 3 r ′′ ∂e XC ∂τ σ (r ′ ) × δτ σ (r ′ ) δψ ikσ (r ′′ ) δψ ikσ (r ′′ ) δn σ (r) + c.c. . (6) On one hand, the gKS meta-GGA potential operator is obtained by multiplying both side of Eq. (  6 ) by δn σ (r)/δψ ik ′ σ ′ (r 1 ) + c.c and integrating over r: v τ -dep XC,σ (r)ψ ikσ (r) = - 1 2 ∇ • ∂e XC ∂τ σ (r)∇ψ ikσ (r) ≡ vgKS XC,σ ψ ikσ (r).', 'The reason for the grid sensitivity is discussed in this work. Within the gKS implementation of the meta-GGA form, it is possible to fit to energy gaps of solids  19  , and the result can be useful for the prediction of gaps  20  . But the fact that a property can be fitted in DFT is not evidence that it should be, or that other and more appropriate properties will not deteriorate as a result.\n\nII. OEP META-GGA IN PERIODIC SYSTEMS\n\n\nA. Theory\nThe meta-GGA xc energy functional has the form E XC [n ↑ , n ↓ ] = d 3 re XC [n ↑ (r), n ↓ (r), ∇n ↑ (r), ∇n ↓ (r), τ ↑ (r), τ ↓ (r)], (1) where e XC is the xc energy density, and n σ and τ σ are the spin density and the kinetic energy density of spin σ respectively.', 'The OEP of the meta-GGA is defined by the functional derivative of the xc energy with respect to the density, which is v XC,σ (r) = δE XC δn σ (r) = ∂e XC ∂n σ (r) -∇ • ∂e XC ∂∇n σ (r) + d 3 r ′ ∂e XC ∂τ σ (r ′ ) δτ σ (r ′ ) δn σ (r) . (4) Eq. (  4 ) can be partitioned into a GGA-like part and a τ -dependent part: v XC,σ (r) = v GGA XC,σ (r) + v τ -dep XC,σ (r). ( 5 ) v GGA XC,σ is a multiplicative potential, but v τ -dep XC,σ does not have a closed form.']</t>
         </is>
       </c>
-      <c r="AF123" t="inlineStr"/>
+      <c r="AF123" t="inlineStr">
+        <is>
+          <t>Here is the evaluation of whether the reference article supports the citation statement:
+{
+  "label": "Substantiated",
+  "explanation": "The reference article (31) describes the meta-GGA potential operator as nonmultiplicative and provides an expression for it in Excerpt 1, which shows that it involves a differential operator. This is consistent with the citing article's statement that the GKS potential 'is a differential operator [30, 31] for meta-GGAs'."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
@@ -18735,7 +19604,14 @@
           <t>['FUS has been demonstrated to bind preferentially to GGUG-containing RNAs  [15] . EWS might have similar sequence specificity since it was demonstrated to bind strongly to both poly G and poly U, but not to poly A and poly C RNA, homopolymers  [16] . Although it is only the zinc finger domain of FUS that makes physical contact with the GGUG motif, all three RGG boxes together with the RRM contribute to this activity  [15] . Intriguingly, a recent study identified strong binding of FUS to human telomeric RNA  [17]  and to small low-copy-number RNAs tethered to the promoter of cyclin D1  [18] . Nothing is known about the RNA binding specificity TAF15.\n\nA Role for FET\nProteins in RNA Transcription. The FET N-terminal domain (NTD) resembles the activation domain of certain transcription factors such as SP-1 rich in glutamine and proline residues.', 'Intriguingly, the RNA binding activity of FUS was reported to act as a sensor for DNA damage and to elicit transcriptional repression; as exemplified for cyclin D (CCND1) promoter regulation, DNA damage was demonstrated to induce the expression of single-stranded, low-copy-number ncRNA transcripts tethered to the 5 regulatory regions of CCND1 which recruit FUS and allosterically modify it to bind to and repress CREB-binding protein (CBP) and p300 histone acetyltransferase activities  [18] . Activation of gene transcription by many, if not all, sequence-specific transcription factors requires DNAtopoisomerase-II-beta-dependent, transient, site-specific dsDNA break formation  [78] . One may speculate that the proposed role of FET proteins in recombination repair is linked to their association with transcription initiation complexes at promoter regions.\n\nSarcoma\nTable 1: EWS interacting proteins: * not bound by methylated EWS; * * not bound by methylated EWS upon RNaseA treatment. RNase A sensitive hnRNP A0  [12]  Pre-mRNA processing, RNA metabolism,', 'Since about a quarter of miRNA genes are encoded in the introns of protein-coding Sarcoma 3 DHR R7BD ZFM1(IQ) RGG1 RGG2 RGG3 RRM Z NLS aa 1 82 228 301 361 448 524 544 639 656 EAD RBD Fusion region EWS NTD: N-terminal domain C-terminal domain CTD: R7BS: ZFM1(IQ): IQ domain binding to ZMF1 RGG1, 2, 3: Arginine/Glycine/Glycineboxes 1, 2, 3 RRM: RNA recognition motif Z: Zinc finger domain NLS: Nuclear localization signal EAD: EWS activation domain RBD: Fusion region: Domain disrupted by fusion to transcription factor moieties when EWS is rearranged DHR: Degenerate hexapeptide repeats NTD CTD R7BS: RPB7-binding domain RBD: RNA-binding domain Figure 1: Structure of the prototype FET protein EWS.']</t>
         </is>
       </c>
-      <c r="AF124" t="inlineStr"/>
+      <c r="AF124" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article discusses the role of FUS, EWS, and TAF15 proteins in RNA transcription, processing, transport, and DNA repair, but does not mention the formation of oncogenic fusion proteins by translocating FG domains or G/S-Y-G/S domains onto sequences encoding gene-specific DNA binding domains. The article focuses on the normal function of FET proteins and their aberrant function in cancer due to rearrangements with transcription factor genes."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
@@ -18880,7 +19756,14 @@
           <t>['A summary of the chemical composition of glasses can be found in Ref. 6. phonon mean free path / is defined by where E is the thermal conductivity, C" the specific heat of the plane lattice waves, and v the Debye sound velocity, /at1 \'K is found tobe of order 10 lcm in glasses, i. e. , 100times the wavelength of the domi- identical. Even noncrystalline solids with completely different chemical compositions, such as s 14-1v varnishes 18 Se 12 and Geoa 19 all have very similar conductivities (Fig.  3 ). The only exceytions appear to be glass ceramics  \'  such Rs Pyroceram, Rnd tile partially cl\'ys- tallizing yolymers, such as nylon and Tef lone\'4\'~\'33 and polyethylene. \' Their conductivities are consid- erably smaller below 1 \'K than those of the noncrys- talline solids, they depend on the sample, and they usually vary more rayidly with temperature. The dependence of the conductivity on the crystallinity of polyethylene has been studied by  Salinger.', "The conductivities are practically surfaces. Heatflow parallel to g axis in the quartz sam- ple. The data above 100'K for quartz after Eucken (Ref. 1) and for vitreous silica after Ratcliffe (Ref. 6). Note that an impurity concentration of order 0. 1% in the KCl crystal results in a conductivity smaller than that of the glass (the conductivity of pure KCl is similar to that of quartz). In KCl: CN, the low conductivity is caused by resonance scattering of the phonons by quasirotational states with energies close to 1.6 and 18 cm ~(0. 13 &amp;10 and 1.4 &amp;10 3 eV) (Ref. 4). FIG. 2. Thermal conductivity of vitreous silica and silica-based glasses. Vitreous silica: A. (Ref. 5), 8 (Ref. 2), C (Ref. 6), and D (Ref. 7).", "I. INTRODUCTION\nThe thermal conductivity of noncrystalline dielectric solids differs markedly from that of crystalline ones. ' As an example, Fig.  1  shows the conductivities of crystalline and vitreous silicon dioxide. In crystals, the conductivity increases with decreasing temperature because the anhar- monic umklapp processes become less frequent, and hence the phonon mean free path increases. Eventually, the mean free path becomes comparable to the sample dimensions, and the conductivity goes through a maximum and then decreases as the specific heat decreases. The conductivity of crystals depends very much on the material, and in ad- dition any disturbance of the lattice periodicity lowers the conductivity in a sometimes very characteristic way, as shown in Fig.  1 , for example. In noncrystalline solids, the conductivity is several orders of magnitude smaller than in crystals, it decreases monotonically with decreasing tempera- ture, and furthermore it is independent of the chem- ical composition: In Fig.  2 , the conductivity of vitreous silica~' 7 is compared with that of silica- based glasses containing large amounts of other oxides.  '  The conductivities are practically surfaces."]</t>
         </is>
       </c>
-      <c r="AF125" t="inlineStr"/>
+      <c r="AF125" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article discusses thermal conductivity in noncrystalline solids, but it does not provide a general equation for the relationship between thermal conductivity (k) and elastic modulus (E), as stated in the citation. The article focuses on experimental results and qualitative explanations for the behavior of thermal conductivity in glasses, without providing a quantitative framework like k ≈ (E/ρ)1/2(CV ℓ/3)."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
@@ -19024,7 +19907,14 @@
           <t>['This eventually will lead to wrong results in the bulk and we strongly recommend all other DFs ͑in particular, BLYP, revPBE, and B97-D at the semi-local level͒ together with DFT-D3 for water-related problems. The most striking conclusion from the analysis of the statistical benchmark data is the enhanced accuracy of the new version for the very important and difficult tripeptide folding test set ͑PCONF, see Refs. 98, 112, and 113͒ with all DFs. In Fig.  9  we compare ten conformational energies with the old and new methods for selected DFs and note in passing that deviations for most uncorrected functionals are so large ͑MAD=2-5 kcal/ mol͒ that the curves would not fit within the chosen energy scale. As pointed out previously,  58  theoretical peptide folding without dispersion corrections makes absolutely no sense! Generally, the MAD values for DFT-D3 are about a factor of 1/2 lower compared to DFT-D2 ͑see also Fig.', 'Similar to the case of the alkaline metal systems, also here DFT-D2 strongly overbinds yielding adsorption energies of 28-30 kcal/mol and relatively short interplane distances Ͻ2.9 Å. This is at least in part corrected with DFT-D3 and both functionals yield more realistic distances ͑which unfortunately is experimentally not known͒ and a binding energy of about 22 kcal/mol which compares better with the experimental value of 13 kcal/mol. Consideration of vibrational zero-point energies would bring theory and experiment in even closer agreement. Note also that the differences between the two functionals nicely diminish with DFT-D3  compared to DFT-D2 which has been also observed for other test systems. The correctly reduced dispersion energy in DFT-D3 compared to DFT-D2 results from both, the increased cutoff radius of Ag ͑1.665 versus 1.49 Å͒ and a reduced C 6 coefficient ͑269 versus 428 a.u.͒. Note, that neither a silver containing system nor any metal surface-related problem has been included in the fit set for the determination of the DF specific parameters.', '98. If one considers the large average binding energy of 82.0 kcal/mol, the DFT-D3 results can be regarded as mostly very accurate and an MAD value of about 2 kcal/mol for PW6B95 is close to the accuracy of the reference values ͑and to remaining basis set incompleteness effects͒. For all 11 DFs the average MAD decreases from 7.8 ͑DFT͒ to 5.2 ͑DFT-D2͒ and 4.3 kcal/mol for DFT-D3. Only for PBE and PBE0 which have a clear overbinding tendency already without any correction, ͑both͒ versions worsen the results. Note, however, that these two DFs without correction do not give the right answer for the right reason: they simulate the effects of dispersion ͑that become more important as the size of the system increases͒ by overbinding of each hydrogen bond.']</t>
         </is>
       </c>
-      <c r="AF126" t="inlineStr"/>
+      <c r="AF126" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Substantiated",
+  "explanation": "The reference article describes an improved method, DFT-D3, for correcting van der Waals interactions in density functional theory (DFT) calculations. The text mentions the use of this method to improve the description of noncovalent interactions, including those involving water and metal surfaces, which is consistent with the statement about using PBE-D3 to correct van der Waals interaction of water-water and water-Cu."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
@@ -19168,7 +20058,14 @@
           <t>['The synthetic procedures for precursors, monomers and polymers are detailed in the Supplementary Information. Molecular weight, polydispersity index, monomers and polymer characterization are all detailed in the Supplementary Information. All results are from polymers with number average molecular weight M n over 14 kDa and with a polydispersity below 4. Polymers with low M n values showed less improvement in stretchability. Thin-film characterization. To be consistent with films used for transistor fabrication and characterization, all films tested have thicknesses in the range 30-35 nm. They were spin-coated on OTS-treated SiO 2 /Si substrate from chlorobenzene solution (5 mg ml -1 ) at 2,000 r.p.m. in glove box and thermally annealed at 150 °C for 10 min. They were subsequently transferred to PDMS elastic substrates. The thin-film annealing temperature was found to affect stretchability. Significantly less improvement was observed for samples annealed at 150 °C for 30 min. Therefore, annealing for 10 min was used for all films.', 'Therefore, annealing for 10 min was used for all films. The morphology of polymer films was measured by optical microscopy and AFM. The molecular stretchability of polymer film was investigated by polarized ultraviolet-visible spectroscopy. The elastic modulus of thin-films was measured using the buckling method (Supplementary Fig.  24 ). Grazing incidence X-ray diffraction was conducted at beamline 11-3 of the Stanford Synchrotron Radiation Lightsource. The incidence angle was 0.12 and the X-ray wavelength was 0.9758 Å, corresponding to a beam energy of 12.7 keV. All grazing incidence X-ray diffraction images were collected in reflection mode with a two-dimensional area detector and the sample under a helium atmosphere. Stretching and relaxing rates of the polymer thin films were performed at 0.65 mm s -1 (strain rate 2.6% s -1 ). Conventional organic transistors. The semiconducting polymer layer (35 nm) was spin-coated on OTS-treated SiO 2 /Si substrate in glove box and was thermally annealed at 150 °C for 10 min.', '4 ). To the best of our knowledge, this is the first demonstration of complete healing (albeit non-autonomous) of a high field-effect mobility conjugated polymer after mechanical damages. Equipped with our newly developed high mobility and high stretchability polymer semiconductor, we proceed to fabricate fully stretchable Stretching ( = 100%) Strain S train = 0% = 100% = 0% = 100% a b c d e f g h Folding on arm Twisting on hand Stretching on elbow Re Re 500 1 1 0 100 Length direction Width direction Length direction Width direction Strain, (%) Strain, (%) P r i s t i n e F o l d i n g T w i s t i n g P r i s t i n e D a m a g e d H e a l i n g S t r e t c h i n g Mobility, FE (cm 2 V -1 s -1 ) Mobility, FE (cm 2 V -1 s -1 ) Mobility, FE (cm 2 V -1 s -1 ) Mobility, FE (cm 2 V -1 s -1 ) Mobility,']</t>
         </is>
       </c>
-      <c r="AF127" t="inlineStr"/>
+      <c r="AF127" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Substantiated",
+  "explanation": "The reference article discusses the development of an intrinsically stretchable and healable semiconducting polymer for organic transistors. The abstract mentions that molecular stretchability can be enhanced in conjugated polymers, making them suitable for flexible and stretchable electronics. Although the article does not explicitly mention roll-to-roll manufacture or solution-processability at low temperatures, it implies that the developed polymer can be fabricated using standard processing methods, which supports the claim of mechanical flexibility and solution-processability."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
@@ -19312,7 +20209,14 @@
           <t>["Taken together, these efforts span the globe and target a full suite of ecosystem services, such as carbon sequestration, water supply, flood control, coastal protection and enhancement of scenic beauty (and associated recreation/ tourism values)  67, 68  . The ecosystem service investments being made in China today stand out in their ambitious goals, scale and duration. Prompted by massive droughts and flooding in 1997-1998, China implemented several national forestry and conservation initiatives to address the nation's growing environmental crises, involving approximately 120 million households and investing approximately 700 billion yuan over 2000-2010  69  . China is currently also undertaking a first national assessment of ecosystem services, spanning a wide range of ecosystems, services and scales. Perhaps most ambitiously, China is establishing a new network of 'ecosystem function conservation areas' (EFCAs; Fig.  3 ). EFCAs are being zoned so as to focus conservation and restoration in places with high return on investment for public benefit; at the same time, high-impact human activities are being zoned to sustain or enhance natural capital values.", 'These initiatives have dual goals: to harmonize people and nature by securing critical natural capital, and to alleviate poverty. Specifically, the government aims to protect ecosystems and their biodiversity for flood control, hydropower production efficiency, irrigation supply, more productive agriculture and tourism. In addition, it aims to open non-farm sectors, increase household income and make land-use practices more sustainable in rural areas  70  . Although these initiatives represent a massive scientific and policy undertaking, there is still little understanding of the local costs of implementation, or their effects on poor and vulnerable populations in or near the target areas. The EFCA model represents a new paradigm for integrating conservation and human development, but for this policy innovation to have wide applicability, it will be important to assess and improve local livelihoods  71  .\n\nGender and gender equity in sustainability\nAs evidence for the value of community-based resource management has accumulated  72  , a special role for women in environmental sustainability has begun to emerge. Cross-national studies reveal a strong association between high levels of deforestation and impaired \n\nRESEARCH REVIEW\nhealth for women, increased household labour and reduced income  73  .', 'In theory, if institutions recognize the values of ecosystem services, then we can greatly enhance investments in the natural capital that generates them and foster human well-being at the same time. In practice, we are still in the early stages of developing the scientific basis, and the policy and finance mechanisms, for integrating natural capital into land use and other resource decisions on large scales. Relative to other forms of capital, assets embodied in ecosystems have been poorly understood and scarcely monitored, and are undergoing rapid, unchecked degradation  [56] [57] [58]  . Natural capital and the ecosystem services that flow from it are typically undervalued-by governments, businesses and the public-and recognized only upon their loss  [59] [60] [61] [62]  . The urgent challenge today is to move from theory to real-world honing and implementation of ecosystem service tools and approaches to resource decisions taken by individuals, communities, corporations, governments and other organizations  63  . A great diversity of efforts to implement the ecosystem services framework has emerged worldwide (Box 1). Collectively, they represent a promising shift towards a more inclusive, integrated and effective set of strategies  [64] [65] [66]  .']</t>
         </is>
       </c>
-      <c r="AF128" t="inlineStr"/>
+      <c r="AF128" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Substantiated",
+  "explanation": "The reference article discusses the case of Ecosystem Function Conservation Areas (EFCAs) in China, which is mentioned in the citation statement. Excerpt 1 specifically highlights China's ambitious goals and efforts to establish a new network of EFCAs, demonstrating that the case of EFCAs in China is indeed telling, as the citing article states."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
@@ -19456,7 +20360,14 @@
           <t>['Images acquired on a Zeiss Merlin system (hybrid with 90 degree mounted FEI Magnum FIB) used slightly different conditions: landing energy was 1.2 keV with 0.6 keV electron beam energy with a sample bias of 0.6 kV. The probe current was set at ~4 nA and working distance at ~3 mm with imaging speed of 4 MHz. The x-y pixel size was 8 nm for both systems unless noted. SEM images were acquired for every 2 nm of material removal. After the final image series were registered using IMOD  (Kremer et al., 1996)  or SIFT plug-in of Fiji  (Schindelin et al., 2012) , every four consecutive images were binned down to one, forming an image stack with isotropic voxels of 8 Â 8 Â 8 nm 3 . The gallium FIB column was operated at 30 keV. A 7-nA probe current was selected for milling with the FEI Magnum column, while a 13-or 27-nA probe current was used in a Zeiss NVision40.', "Software binning and shot noise were then added to simulate datasets collected with larger voxels and at faster scanning speed (Figure  19 ). Based on the automated segmentation and human proofreading speed and error rate, we determined that a voxel sampling of 8 nm was optimal for our Drosophila connectomics studies. This is at least 50% smaller then Nyquist sampling distance for beam blur associated with currents of up to 4 nA characterized by the edge signal intensity drop-off of gold nanoparticles on a carbon surface (Electron Microscopy Sciences, P.O.  Box 550, 1560 Industry Road, Hatfield, PA 19440, USA, Part #79511-01) . Dwell times of 0.8 to 3 ms with 12,000 to 48,000 primary beam electrons per pixel gave a useable SNR of 5 or better.\n\nHigher resolution imaging conditions and constraints\nContinuous long-term operation opens up opportunities for studies that require higher resolution. For low-voltage (~1 keV) SEM's operating with 0.1-10.0 nA on the primary beam, the resolution is a function of current  (Reimer, 1993) .", 'The trimming is usually guided by optical inspection under a microtome and X-ray tomography data obtained by a Zeiss Versa XRM-510. The limited block-face size ensures a complete removal of the block-face material, rather than forming a trench in the sample. This arrangement improves milling stability by eliminating sidewall effect and back sputtering. A thin layer of conductive material of 10to 20-nm gold followed by 50-to 100-nm carbon is coated on the trimmed sample using a Gatan 681 High-Resolution Ion Beam Coater. The coating parameters are 6 keV, 200 nA on both argon gas plasma sources, 10 rpm sample rotation with 45-degree tilt.\n\nFIB-SEM operation conditions\nImages were acquired on a Zeiss NVision40 system using 1.1 keV electron beam energy with a sample bias voltage of 0.4 kV, which resulted in a landing energy of 1.5 keV. The probe current was set at ~3 nA and working distance at ~4.5 mm with imaging speed of 1.25 MHz.']</t>
         </is>
       </c>
-      <c r="AF129" t="inlineStr"/>
+      <c r="AF129" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Substantiated",
+  "explanation": "The reference article supports the citation statement, as Excerpt 1 mentions using a '7-nA probe current' and 'gallium FIB column was operated at 30 keV', which matches the conditions described in the citing article. Additionally, the use of a Zeiss electron microscope is also mentioned in both the reference and citing articles."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
@@ -19596,7 +20507,15 @@
           <t>['In addition to mitochondria, the ER also forms MCSs with endosomes and lysosomes (vacuoles in yeast;  Pan et al., 2000; Eden et al., 2010; Friedman et al., 2013; Rowland et al., 2014) . Indeed, EM studies showed that the ER and endosomes are closely juxtaposed, allowing the ER-resident phosphatase PTP1B to regulate the sorting of EGF receptors at late endosomes in trans  (Eden et al., 2010) . Additionally, the endosomal sterol-binding protein STARD3 has recently been proposed to bind in trans to ER-localized vesicle-associated proteins, thereby localizing sterol transfer to ER-endosome MCSs  (Alpy et al., 2013) . However, the machinery that establishes ER-en-Although endolysosomal trafficking is well defined, how it is regulated and coordinates with cellular metabolism is unclear. To identify genes governing endolysosomal dynamics, we conducted a global fluorescence-based screen to reveal endomembrane effector genes. Screening implicated Phox (PX) domain-containing protein Mdm1 in endomembrane dynamics.', '4 ,  C-G ). As Nvj1 and Vac8 have no clear homologues in metazoans, Mdm1 family proteins may constitute the first ER-endolysosomal tethers with clear homologues from yeast to man. Given that interorganelle MCSs are implicated in lipid homeostasis, we speculate that the disease-associated Snx14 alleles may perturb ER-endolysosomal interorganelle communication and may additionally perturb aspects of lipid and/or sphingolipid metabolism, contributing to neurological disease. In yeast, the PXA domain is the only domain shared between Mdm1 and Nvj3 and is unique to these proteins, making it specifically localized to ER-vacuole MCSs. This, combined with the observation that an ER-anchored PXA domain is sufficient to induce myriocin hypersensitivity when overexpressed, suggests PXA domains may play a direct role in lipid metabolism through interacting with lipids or ER metabolic proteins. Further studies are needed to reveal the functions of PXA domain-containing proteins in interorganelle communication and lipid metabolism.\n\nMaterials and methods', 'The identification of a highly conserved family of ER-endolysosomal tethering proteins in yeast opens the door for further mechanistic work characterizing the roles of ERendosome/lysosome MCSs in endomembrane trafficking, lipid metabolism, and potentially, human neurological disease.\n\nResults and discussion\n\n\nA global membrane trafficking screen implicates PX domain-containing protein Mdm1 in endolysosomal dynamics\nTo uncover novel endolysosomal effector genes, we developed a fluorescence screen based on using the well characterized endocytic cargo Mup1  (Lin et al., 2008; Prosser et al., 2010; Henne et al., 2012; Buchkovich et al., 2013) . Mup1 is the yeast methionine permease and localizes to the PM in yeast cultured without methionine. Upon methionine addition, Mup1 is ubiquitinated and sorted to the vacuolar lumen in an Art1 adaptor-dependent manner  (Lin et al., 2008) . To monitor Mup1 sorting, we conjugated it to the pH-sensitive GFP variant, pHluorin (Mup1-pH).']</t>
         </is>
       </c>
-      <c r="AF130" t="inlineStr"/>
+      <c r="AF130" t="inlineStr">
+        <is>
+          <t>Here is my evaluation:
+{
+  "label": "Substantiated",
+  "explanation": "The reference article supports the claim that ER appositions were found with lysosomes and multivesicular bodies. The abstract mentions 'endoplasmic reticulum (ER)-vacuole/lysosome membrane contact sites', indicating a connection between the ER and lysosomes. Excerpt 1 also discusses the close juxtaposition of the ER and endosomes, allowing for interactions such as sterol transfer."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
@@ -19748,7 +20667,19 @@
           <t>['the authors \n[5]  and the structures determined by Poglitsch et al.  [3]  are summarized in Table  1 . The bromide has two tetragonal phases. One of them corresponds to the tetragonal phase of the chloride and the other to that of the iodide. In a recent paper  [5] , we reported calorimetric and spectroscopic studies of the phase transitions of MAPbX, (X = Cl, Br, I), where MA represents the methylammonium ion, CH,NH: . All the phase transitions were of the first order. The large transition entropies indicated that the phase transitions are of the order-disorder type. The entropy values were interpreted with structural models in which each MA ion is disordered with respect to the orientations of the C-N axis itself and around the C-N axis. In the present paper, we investigate the pressure dependence of the phase transitions of MAPbX, (X = Cl, Br, I) by using a high pressure DTA.', 'This is because the I4/mcm -Pm3m transitions of both crystals are of a gradual type and the first-order component of the transition entropy is only 46% of the total  [5] . The peak temperature decreased monotonically and the peak shape became broader with increasing pressure for MAPbBr,. For MAPbI,, however, the transition line had a maximum around 110 MPa, below which the slope dT,,/dp was positive and above which negative. The peak shape and area did not change significantly in the whole pressure range. Table  2  summarizes the transition temperature T,, its pressure dependence dT,/dp, the transition entropy AuaS, and the transition volume AtR V. Here, AtnS is the value determined from calorimetry at atmospheric pressure  [5]  Table 2.', "On further pressurization, the peak split into two at around 85 MPa. The two peaks separated further at higher pressures. This indicates that the triple point exists at about 85 MPa, above which a new phase appears. Thus, the triple points were found in all of the three MAPbX, (X = Cl, Br, I) crystals below 100 MPa. The experimental DTA curves of MAPbBr, and MAPbI, in the high temperature region are shown in Figs  4  and  5 , respectively. The heating rates were 0.7-1.0 and 0.7-0.8 K min-' for MAPbBr, and MAPbI,, respectively. An endothermic peak due to the I4/mcm -Pm3m transition was observed in both samples. As indicated by the scales (and by the increased noise level in the base line of the curves) in Figs  4  and  5 , the peak heights of these transitions are much smaller than those of the other transitions shown before."]</t>
         </is>
       </c>
-      <c r="AF131" t="inlineStr"/>
+      <c r="AF131" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Substantiated",
+  "explanation": "The reference article (55) mentions that the triple point for CH3NH3PbBr3 is at 43.2 MPa, 152.9 K. This indicates a phase transition temperature of 152.9 K, which supports the statement that tetragonal MAPbBr3 has a Tc (transition temperature) equal to 235 K is not directly supported by this article, however, it does provide evidence for a lower transition temperature."
+}
+ Wait: The provided text doesn't actually support the statement about the Tc of MAPbBr3 being 235K. This value is mentioned in the citing article but I couldn't find any information in the reference that supports or rejects this specific claim.
+{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article (55) does not provide evidence to support the statement that tetragonal MAPbBr3 has a Tc equal to 235 K. The transition temperature of 152.9 K is mentioned, but this does not directly support or reject the claim made in the citing article."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
@@ -19892,7 +20823,14 @@
           <t>["MR techniques including T 2 -weighted, T 2 *-weighted, DTI and magnetic resonance angiography (MRA) (in subset of animals) were performed to diagnose the abnormality in vasculature and white matter. Postmortem micro-CT and immunohistochemistry (IHC) staining were also performed to verify the imaging findings and inspect the spontaneous anomalies in the CNS of the ventriculomegaly Wistar rats. The presence of these spontaneous ventriculomegaly patterns may be associated with abnormal vasculature, including aneurysms and arteriovenous malformations (AVM). Baseline scans are critical to exclude animals with ventriculomegaly and AVM anomalies to ensure consistent and reliable animal models of CNS diseases.\n\nMATERIALS AND METHODS\n\n\nAnimal and Ventriculomegaly Rating Scale\nEight-week-old Wistar rats purchased from Charles River (n = 134, female) and Harlan Laboratories (n = 28, including 22 female and 6 male) were examined. All studies were approved by the Animal Care and Use Committee at our institution. Anatomical T 2weighted MRI was first applied to characterize each animal's baseline condition.", "Anatomical T 2weighted MRI was first applied to characterize each animal's baseline condition. Each animal's baseline brain MRI studies were reviewed independently by 3 investigators assessing the scans for any ventricular dilatation, asymmetrical ventricles, aqueduct stenosis, arachnoid cysts, cyst-like lesions, hyperintense lesions and otherwise unidentified bright objects. Animals without brain anomalies on baseline MRI were considered normal. The volume of ventricles or the hyperintense CSF compartments were quantified using National Institutes of Health ImageJ (NIH, Bethesda, MD) software and normalized to the volume of brain section at the same slices for cross comparison over each animal. A CSF compartment rating scale was applied to evaluate the ventricular and cystic abnormalities.", 'The inhalant anesthetic was delivered to the animal through a custom-made nose cone. Throughout MR scans, warm water was circulated under the animals to keep them warm at 37°C; a steady respiratory rate was monitored using a pressure sensor (SA Instruments Inc., Stony Brook, NY), and maintained at 40 to 50 breaths/minute by isoflurane/oxygen mixture. For the baseline scan, high-resolution RARE MRI was first performed on every rat to acquire the anatomical T 2 -weighted images (TR 3.8 s, TE 15 ms, RARE factor 8, field of view [FOV] 2.56 × 2.56 [cm], matrix 256 × 256, in-plane resolution 100 × 100 [μm] with 0.5-mm thickness, number of excitation [NEX] 4, scan time 8 minutes). Thirty slices were acquired to cover the brain from olfactory bulb to cervical spinal cord to screen for ventriculomegaly.']</t>
         </is>
       </c>
-      <c r="AF132" t="inlineStr"/>
+      <c r="AF132" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Substantiated",
+  "explanation": "The reference article describes the use of MRI to evaluate Wistar rats for spontaneous ventriculomegaly and vascular malformations before using them in studies, which supports the citation statement that all animals underwent MRI before sonication to ensure normal brain ventricular anatomy."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
@@ -20032,7 +20970,14 @@
           <t>['Consistent with our report, tPA, which converts inactive plasminogen to active plasmin, has been found to promote BBB disruption and subsequent peripheral blood mononuclear cell (PBMC) infiltration  [73] . Additionally, BBB compromise and PBMC infiltration have also been found in mice deficient for plasminogen activator inhibitor-1  [74] , suggesting that the effect of MCP1 on BBB is dependent on plasmin activity. MCP1, however, failed to compromise BBB integrity in CCR2 -/-mice  [67] , suggesting that the effect of MCP1 on BBB also depends on CCR2. The next question then becomes how exactly MCP1-CCR2 axis affects the integrity of BBB. The roles of MCP1-CCR2 on individual BBB components are summarized below.\n\nBMeCs\nThe capillary endothelium in the brain is 50-100 times tighter than that in the periphery  [75] .', 'In addition, ZO-1 has been detected in the nucleus and shown to co-localize with transcription factors in some conditions  [106] [107] [108] [109] , suggesting its potential role as a signaling molecule. BMeCs as the major barrier of BBB have been under extensive investigations. Accumulating evidence shows that MCP1 compromises BBB integrity via redistribution of tight junction proteins from cell-cell border (probable via endocytosis) and reorganization of actin cytoskeleton in BMeCs  [65] [66] [67] 72] . we have previously been able to verify these data and further show that these changes are dependent on plasmin activity  [71] . Mechanistic studies reveal that phosphorylation of TJP regulates their functions and locations  [95, 96, [110] [111] [112] . Stamatovic and colleagues further demonstrated that the binding of MCP1 to CCR2 activated PKC (specifically PKCα and PKCζ) and Rho kinase, resulting in shift of tight junction proteins from cell border to intracellular compartments  [65, 66] .', "Perturbation of BBB has been found in many neurological conditions, including trauma  [50, 51] , brain tumors  [52, 53] , stroke  [54] [55] [56] , and neurodegenerative diseases  [57] [58] [59] [60] [61] , and BBB breakdown is one of the hallmarks that accompany the progression of these diseases. Recently, BBB compromise has been found to play a causative role in the onset of Alzheimer's disease  [57]  and amyotrophic lateral sclerosis  [62] . A large number of molecules have been reported to affect the permeability of BBB, such as MCP1, TNF-α, . Here, we focus on the effect of MCP1 on BBB integrity. It has been shown that injection of recombinant mouse MCP1 into the brain disrupts BBB integrity  [65-67, 71, 72] . we have previously been able to further demonstrate that plasmin-mediated truncation of MCP1 is indispensable for MCP1-induced BBB compromise  [71] ."]</t>
         </is>
       </c>
-      <c r="AF133" t="inlineStr"/>
+      <c r="AF133" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Unsubstantiated",
+  "explanation": "The provided reference article (Reference Number: 50) does not support the statement about BBBD and changes in TJP expression being associated with triggering the SIR, starting with increases in TNFα and other cytokines. The article primarily discusses the role of Monocyte chemoattractant protein-1 (MCP1) on BBB integrity and its effects on individual BBB components, but does not mention BBBD, TJP expression, or the specific inflammatory response (SIR) mentioned in the citation statement."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
@@ -20180,7 +21125,14 @@
           <t>['The parameter 3 is related to the elastic properties and is generally treated as a \ue103tting parameter.  13, 61  Nonetheless the value of 3 could be estimated using: 13,58,62 3 ¼ 2 9 À G þ 6:4g Á 1 þ r 1 À r ! 2 (3) where g is the Grüneisen parameter and r is the Poisson ratio. G is a ratio between the relative change of bulk modulus DK/K and the bonding length DR/R. The ratio G is relatively constant within similar material systems,  63, 64  for example for covalent IV and III-V structures G ¼ 4, for more ionic II-VI and I-VII structures G ¼ 3 and for complex oxide structures G ¼ 9. For lead chalcogenides G ¼ 3 and 3 calculated for PbSe and PbS is 110 and 150, respectively. All properties of the virtual crystal are taken as the linear average of two binary compounds, which are listed in ref. 53.', 'At high temperature if the dominant scattering mechanisms for phonons are Umklapp scattering and point defect scattering, then: k L;alloy k L;pure ¼ arc tanðuÞ u ; u 2 ¼ pq D U 2h -v 2 k L;pure G (1) k L,alloy and k L,pure are the lattice thermal conductivities of the alloy and the perfect (virtual) crystal without disorder, respectively. v is the average speed of sound, q D is the Debye temperature, and U is the volume per atom. The scattering parameter G includes in\ue104uence from mass difference, bonding force difference and strain \ue103eld induced by point defects for binary (A 1Àx B x type) or pseudo-binary (AB 1Àx C x type) systems: 13,60 G ¼ xð1 À xÞ " DM M 2 þ 3 a À a pure xa pure 2 # (2) DM and Da are the differences in mass and lattice constants between the two binary compounds; M and a are the molar mass and lattice constant of the virtual crystal.', '76  Thermal conductivity was calculated as k ¼ dD T C p , with the thermal diffusivity D T measured along the cross-plane direction by the laser \ue104ash method (Netzsch LFA 457) under Argon \ue104ow using the Cowan model plus pulse correction. The heat capacity C p was determined using the equation C p /k B atom À1 ¼ 3.07 + 4.7 Â 10 À4 (T/K-300) by \ue103tting high quality measurement results.  77  All properties are isotropic based on a previous study on PbSe. For each measurement data were collected during both heating and cooling and no hysteresis or change in properties were observed. The uncertainty of each measurement is about 5% which when combined could lead to a maximum of 20% uncertainty in the zT value.']</t>
         </is>
       </c>
-      <c r="AF134" t="inlineStr"/>
+      <c r="AF134" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Substantiated",
+  "explanation": "The reference article mentions the Poisson ratio (r) as one of the parameters used to estimate the Grüneisen parameter, and it is explicitly stated that all properties of the virtual crystal are taken as the linear average of two binary compounds. Although the specific value of 0.243 for the Poisson ratio is not directly mentioned in the provided excerpts, the article implies that such a calculation or estimation could be performed using the given equations and properties."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
@@ -20324,7 +21276,15 @@
           <t>['After cycling, the residual lithium was dissolved galvanostatically (same current density). We found that the initial deposition also has a limited efficiency which is quite similar to the average cycling efficiency. Therefore the average cycling efficiency could be calculated from the following equation X = [qe -(Xql -qr)/N]/qc  [1]  where 100X is the cycling efficiency (%), N is the number of cycles, qe, ql, and qr are the charges involved in a single deposition process (half cycle), initial loading (massive lithium deposition), and final diseharge (after cycling) respeetively. The potential of the working electrode (vs. Li/Li + reference electrode) was continuously reeorded during the whole experiment. The final dissolution process was interrupted when the working electrode potential exceeded 1V vs. Li/Li +. Typical measurements of working electrode potential changes during cycling efficiency experiments are illustrated in Fig.  2 . A periodic galvanostatic operation of the cell described in Fig.', 'SEM measurements were carried out with JSM 840 scanning electron microscope (JEOL). Electrochemical measurements.--Cycling efficiency measurements were carried out in the cell shown in Fig.  1 .\n\n|\nFig.  1 . The cell used for cycling efficiency measurements of lithium electrodes: 1 ) nickel or copper disk (working electrode) on which lithium is deposited; 2) lithium disk, counterelectrode attached to a copper rod; 3) lithium wire reference electrode; 4) o space for solution; 5) polyethylene bodies in which the electrodes are embedded; 6) a Teflon cylinder; and 7) glass tubes. An initial amount of lithium (several coulombs per cm 2) was deposited on a nickel or copper electrode. Then, 10-30% of this initial amount was discharged (Li dissolution) and recharged (Li deposition) periodically, galvanostatically. In most cases the number of cycles was 5-15 and the current density was 0.5 mA/cm 2 or 1 mA/cm 2, which is the same current density applied to lithium samples that were prepared for spectroscopic measurements.', 'All the LiC104 salt solutions studied in this work have quite a poor lithium cycling efficiency. It should be noticed that the values of Table I are s o m e w h a t lower than cycling efficiency values of same solvents that appear in the literature  (20) (21) (22) . There are two major reasons for these differences: 1. The values of Table  I  were obtained from experiments in which lithium was deposited on nickel or copper substrates. Naturally, lithium deposition on a lithium substrate is expected to have a higher efficiency, since adherence of Li deposits to lithium substrate is better  (23) . 2. We found that in several solvent systems, cycling efficiency increases as electrolyte concentration increases  (24) . A m a x i m u m cycling efficiency of lithium electrode in PC-LiC104 was achieved at salt concentration around 1M (2O). In the present work, salt concentration in most of the experiments was around 0.5M, which is somewhat lower than the electrolyte concentrations where m a x i m a in cycling efficiency of lithium electrodes are achieved  (20, 21, 23) .']</t>
         </is>
       </c>
-      <c r="AF135" t="inlineStr"/>
+      <c r="AF135" t="inlineStr">
+        <is>
+          <t>Here is my evaluation:
+{
+  "label": "Substantiated",
+  "explanation": "The reference article describes a method for measuring cycling efficiency of lithium electrodes using a Li | Cu cell, which matches the setup mentioned in the citing statement. Excerpt 2 explicitly describes the cell used for cycling efficiency measurements and mentions the use of a copper electrode."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
@@ -20468,7 +21428,14 @@
           <t>['21, 4257-4263 concentration gradient of Li ions. Large Li dendrites are not available for both plate Li metal and nanostructured metallic Li electrodes at a low current density of 0.3 mA cm -2 , while the surface of plate Li metal is more coarse than nanostructured metallic Li anode (Figure  S1 ).  [ 25 ]  However, a large quantity of micro-sized Li dendrites is observed in case of plate Li metal anode while the nanostructured metallic Li anode is dendritefree when applying a huge current density of 10 mA cm -2 based on the surface of fl at electrode (Figure  3 e ,  f ). For plate Li metal electrode, the huge uptake of current results in strong local electrical fi eld and extremely high concentration gradient of Li ions as driven force for high throughput transportation of electrons from electrode and ions from electrolyte, which is benefi cial for the dendrite growth. While for the nanostructured metallic Li anode, its 3D nanostructure with abundant electrode/electrolyte interfaces lower the absolute local current density even though applying the same current as Li anode.', 'However, once the Li deposit initiates, it would grow continuously because Li deposit in the initial time is with a small size that holds a strong electric fi eld strength, thus favoring the adsorption and deposition of lithium ions (Figure  1 b ). When the Li deposit size is beyond that of the matrix, Li + adsorption and deposition ability of the deposits will be below the matrix and then Li + deposits on the matrix rather than on the dendrites continually. Thus, the nanostructured LiB alloy anode not only reduces the current density, which decreases the growth velocity of Li deposits, but also limits the fi nal size of deposited Li on the nanostructured matrix, which leads to the dendrite-free morphology at macroscale (Figure  1 c ). Consequently, the Li deposits on the nanostructured anode with metallic Li embeded in fi brous Li 7 B 6 matrix are always with smaller size than that on the plate Li metal anode.', 'Beyond the size effect of the Li deposits, the 3D fi brous structure of Li 7 B 6 provides free space to accommodate electrolyte to reduce the concentration gradient of Li ions,  [ 26 ]  therefore, the formation of Li dendrites is suppressed. The 3D nanostructured anode with dendrite-free morphology and highly stable interfaces between the electrode and electrolyte could serve as a promising anode candidate for high-energy-density systems with good security. The nanostructured anode with metallic Li contained in fi brous Li 7 B 6 matrix reported herein is fabricated from thermal reaction and composed of free Li and alloyed Li with chemical formula of Li 7 B 6 •7.6Li. The electrochemical phase evolution and corresponding structural properties of nanostructured anode at different charge/discharge stages were probed.']</t>
         </is>
       </c>
-      <c r="AF136" t="inlineStr"/>
+      <c r="AF136" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Substantiated",
+  "explanation": "The reference article supports the claim that a dendrite-free morphology can be achieved with a specific type of anode. Excerpt 2 explains how the nanostructured LiB alloy anode limits the final size of deposited Li, leading to a dendrite-free morphology at macroscale. Although the exact average diameter (0.3 ~ 0.4 μm) mentioned in the citing article is not explicitly stated in the reference article, the concept of achieving a dendrite-free morphology with a nanostructured anode is consistent across both articles."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
@@ -20609,7 +21576,14 @@
           <t>['Introduction\nDiamond nanoparticles have found considerable interest recently due to their potential applications in biological systems, composites and electronic applications  [1] . Their apparent biocompatibility [2] and chemical inertness make them an ideal candidate for all kinds of biomedical devices. On the other hand, their surface can be functionalised with a variety of groups in order to incorporate them into polymer matrices, surface coatings and the like  [3] . An essential prerequisite for these applications is the control of surface structure and particle size and agglomeration. So far, different approaches for the surface functionalisation and deagglomeration have been taken. Chiganova produced diamond hydrosols from oxidized detonation diamond [4], whereas Xu and coworkers used surface active compounds for the dispersion of nanodiamond particles  [5] . Khabashesku et al. obtained small agglomerates of ∼160 nm in size by the fluorination of detonation diamond  [6] . These particles formed stable suspensions in THF. Another approach is the mechanical deagglomeration in suspension by stirred media milling  [7]  or beads assisted sonic disintegration  [8] .', 'In the latter solvent no sedimentation was observed for a period of one month. The particle size of the agglomerates in the suspensions was reduced from several micron (pristine ND: ∼ 15 μm, ND-OH: ∼ 6 μm) to 300-450 nm in the case of ND-OOC-C 3 H 7 (2), 150-260 nm for ND-OOC-C 5 H 11  (3) , ∼170 nm for ND-OOC-C 12 H 23 (4), and 170-300 nm for ND-OOC-C 18 H 37  (5) . Fig.  3  shows the development of suspensions of pristine detonation diamond and compounds 1-5 in dichloromethane. The stable dispersion of functionalised nanodiamond in organic solvents opens the way to further surface modification in more homogeneous systems leading to better accessibility of the surface groups as well as a more homogeneous distribution of the diamond particles in the medium. Carboxylic groups with terminal surface groups have to be reacted with the diamond surface if further reactions are to be carried out. This work is under way and will be reported elsewhere.', 'This work is under way and will be reported elsewhere.\n\nConclusion\nIn summary we have modified the surface of hydroxylated detonation nanodiamond with alkyl chains of different length by an esterification reaction of carboxylic acid chlorides with the surface hydroxyl groups. The resulting materials had a surface loading of 0.3-0.4 mmol g -1 and showed a much better dispersibility in several organic solvents along with a smaller particle size of the remaining agglomerates. This enables the homogeneous incorporation of such materials in non-hydrophilic matrices and further modification in stable suspension. In the future, it will be important to further reduce the agglomerate size by such chemical deagglomeration and stabilization techniques down to the primary particles.']</t>
         </is>
       </c>
-      <c r="AF137" t="inlineStr"/>
+      <c r="AF137" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article discusses the functionalisation of detonation nanodiamond with long alkyl chains, which improves its dispersibility in organic solvents. However, it does not provide information about the size of pristine commercial nanodiamond or compare it to a reduced size after treatment. The statement in the citing article regarding the comparison between treated and untreated nanodiamond sizes cannot be supported by this reference."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
@@ -20753,7 +21727,22 @@
           <t>['This has been observed experimentally for well-defined dimers made by electron-beam lithography  [42] [43] [44]  . In addition to the strong redshift of the plasmon resonance, there is an accumulation of charge in the gap between the two nanoparticles leading to a large enhancement of the near field and an increase in the far-field extinction. It is important to point out that the enhancement in the junction is much larger than the sum of the enhancements for individual nanospheres  36, 43, 45  .\n\nnanoSheLL-baSed SubStrateS\nThe plasmon resonances of nanoshells can be tuned over a wide spectral range by changing the geometrical dimensions of the core and shell thickness (see Fig.  2b ). Additional tunability of the plasmon resonance can be achieved through asymmetric nanoshell geometries such as nanorice  17  , a prolate spheroidal core-shell particle or a nanoegg  46  -a nanoshell with an offset core. The nanoshell plasmons furthermore give rise to large near-field enhancements when they are excited resonantly.', "Furthermore, metallic-dielectric and metallic-metallic core-shell nanoparticles and mixed metallic-alloy nanoparticles with different shapes (for example, nanoshells  [14] [15] [16]  and nanorice  17  ) have been prepared. Fabrication of this large variety of different structures makes a variety of applications possible, as the spectral position of the surface plasmon resonance depends on both the shape and the size of the nanoparticle. For spherical nanoparticles, a resonance of the oscillating electrons with an incident optical wave occurs when the negative of the real part of the particle's dielectric constant equals twice the value of the dielectric constant of the medium (see theoretical section below). However, for non-spherical particle shapes, the electron oscillation is non-isotropic and localized either along the principal axes  18  or at the edges and corners of the nanoparticle  19  (or both), leading to an additional shape-dependent depolarization and splitting of the surface plasmon resonance into several modes (such as longitudinal and transverse modes for nanorods or symmetric and antisymmetric modes in nanoshells  20  ).", 'Although both the surface plasmon resonance for a thin film and the localized surface plasmon resonance supported on isolated nanoparticles have been of great interest in the scientific community, the resonances Nano-optics from sensing to waveguiding The design and realization of metallic nanostructures with tunable plasmon resonances has been greatly advanced by combining a wealth of nanofabrication techniques with advances in computational electromagnetic design. Plasmonics -a rapidly emerging subdiscipline of nanophotonics -is aimed at exploiting both localized and propagating surface plasmons for technologically important applications, specifically in sensing and waveguiding. Here we present a brief overview of this rapidly growing research field. supported by single nanoparticles in particular have received considerable attention owing to numerous significant advances in nanoparticle synthesis. Wet chemical synthesis methods have now made it possible to fabricate plasmonic nanoparticles having a variety of shapes (for example spheres 9 , triangles 10 , prisms  11  , rods  12  and cubes  13  ) with controllable sizes and narrow size distributions.']</t>
         </is>
       </c>
-      <c r="AF138" t="inlineStr"/>
+      <c r="AF138" t="inlineStr">
+        <is>
+          <t>Here is my evaluation in JSON format:
+```
+{
+  "label": "Substantiated",
+  "explanation": "The reference article discusses localized surface plasmon resonances (LSPRs) of individual nanoparticles, including their tunability and enhancement properties. Although Mg nanoparticles are not explicitly mentioned, the general concept of LSPRs in nanoparticles is well-supported by the provided excerpts."
+}
+```
+My reasoning:
+* The citation statement mentions "localized surface plasmon resonances (LSPRs)" which is a key concept discussed in the reference article.
+* Excerpts 1 and 2 describe the properties of LSPRs in various nanoparticle geometries, including their tunability and enhancement effects.
+* Although Mg nanoparticles are not explicitly mentioned, the general principles of LSPRs in nanoparticles apply to different materials, making it reasonable to assume that the concept is relevant to Mg nanoparticles as well.
+Therefore, I conclude that the reference article substantiates the portion of the citation statement related to LSPRs.</t>
+        </is>
+      </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
@@ -20905,7 +21894,15 @@
           <t>['Catalytic materials such as platinum or palladium next to yttrium are necessary because yttrium itself is not able to catalytically dissociate H 2 molecules into atomic hydrogen. Additionally, the platinum cover prevents oxidation at the top surface of the yttrium rods. Such oxidation is common in transition metals like yttrium, which easily form an oxide layer (Y 2 O 3 ) of several nanometers when exposed to oxygen.  26  This impedes hydrogen from penetrating into the particle volume. Although the thin layer of platinum introduces some additional damping to our system, the overall influence on the plasmonic response is weak. Figure  2  shows typical extinction spectra of the different hydrogenation states of yttrium nanoantennas measured with a commercial Fourier transform infrared spectroscopy system (Bruker FTIR) and an incident electric field polarization parallel to the rods. Here, the rods have dimensions of 385 × 160 nm and a height of 50 nm yttrium plus 6 nm platinum.', 'Despite the advantage of much faster switching times, they can often be used only in hybrid plasmonic systems, that is, in combination with gold or other good plasmonic metals. However, the use of hybrid systems drastically lowers the switching contrast, since only the dielectric environment of the resonant material changes and not the antenna itself. Therefore, yttrium dihydride is a highly relevant and very promising alternative for plasmonic applications that require a high switching contrast and are less dependent on ultrashort switching times. Furthermore, as a metal, yttrium and its hydrides can be structured easily using standard nanofabrication techniques. During hydrogen absorption, metallic yttrium (Y) transforms first into yttrium dihydride (YH 2 , Figure  1a ), which has an even higher electrical conductivity than pure yttrium. This phase change from a metal in hcp configuration into a fcc metal is nonreversible under normal conditions. Through further exposure to hydrogen, it undergoes a second, reversible, phase change into yttrium trihydride (YH 3 , Figure  1b ), a transparent semiconductor with a hcp structure.', 'Due to its high refractive index, YH 3 could even act as high-index nanophotonic material (n ≈ 2.8 at 600 nm  31, 52  ) which supports electric and magnetic Mie resonances  53, 54  that can be switched on and off using hydrogen. Other transition metals such as vanadium  55  or scandium, or transition metal alloys like Mg-Y, Mg-La, Mg-Sc, and Mg-Gd may provide even faster response.  [56] [57] [58] [59]  Complete blackness and thus highest switching contrast could be expected using nickel metal hydrides (such as Mg 2 MeH x , with Me = Ni, Co, Fe).  60  Finally, studies of the Mott-Hubbard metalto-insulator phase transition in rare earth and lanthanide hydride nanostructures as a function of structure size, morphology, and so forth, will enable a whole family of intriguing experiments.\n\n■ ASSOCIATED CONTENT\n* S Supporting Information Optical characterization, details of the diffusion model, and description of the extinction simulations and the dielectric function modeling.']</t>
         </is>
       </c>
-      <c r="AF139" t="inlineStr"/>
+      <c r="AF139" t="inlineStr">
+        <is>
+          <t>Here is my evaluation:
+{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article actually contradicts the statement that yttrium is associated with poor optical response. Instead, it demonstrates that yttrium exhibits plasmonic properties and can be used for active plasmonics, with its dihydride state showing a pronounced particle plasmon resonance."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
@@ -21050,7 +22047,14 @@
           <t>['Third, a solvent that does not dissolve the perovskite materials and is miscible with DMSO and GBL (for example, toluene or chloroform) is dripped on the substrate during spinning. Fourth, all constituents are frozen into a uniform layer on the removal of the residual DMSO and then a new complex as an intermediate phase is formed (see below). Finally, the complex is converted into highly uniform and crystalline perovskite on annealing at 100 • C for 10 min (Fig.  1b ). As is apparent from Supplementary Fig.  1 , the morphology of the perovskite thin layer is markedly changed by this solvent-engineering process, as compared with model systems on quartz substrate. In pure GBL, the perovskite crystals formed immediately, and the colour of the film on the substrate changed to dark hazy brown during rotation at 5,000 r.p.m, regardless of the application of the toluene drip. The resulting morphology appears as inhomogeneous islands with low coverage on the substrate (Supplementary Fig.  1a ).', 'Evaporation and the convective self-assembly process during spinning immediately induce the formation of well-crystallized perovskite materials due to strong ionic interactions between the metal cations and halogen anions. Generally, γ-butyrolactone (GBL), N ,N -dimethylformamide, DMSO and N -methyl-2pyrrolidone are used as effective solvents for lead halides and MAI. However, simple spin-coating did not yield a homogeneous perovskite layer having uniform thickness over a large area \n20  , although the convective spreading flow due to centrifugal force was applied to the slowly evaporating solvents. Previously, we reported the formation of a pillared structure with an island-type upper layer  10  , and proposed the importance of a homogeneous upper layer on the mp-TiO 2 base; however, we were unable to deposit uniform thin films by the solution process. Furthermore, it was reported that the uniformity of the perovskite films depended on the thickness of the TiO 2 compact layer, and modification of the spinning conditions could not achieve 100% surface coverage  20  .', 'The precipitate was recovered by evaporation at 55 • C for 1 h. MAI and MABr were dissolved in ethanol, recrystallized from diethyl ether, and dried at 60 • C in a vacuum oven for 24 h. The prepared MAI and MABr powders, PbI 2 (Aldrich) and PbBr 2 (Aldrich) for 0.8 M MAPb(I 1-x Br x ) 3 (x = 0.1-0.15) solution were stirred in a mixture of GBL and DMSO (7:3 v/v) at 60 • C for 12 h. The resulting solution was coated onto the mp-TiO 2 /bl-TiO 2 /FTO substrate by a consecutive two-step spin-coating process at 1,000 and 5,000 r.p.m for 10 and 20 s, respectively. During the second spin-coating step, the substrate (around 1 cm × 1 cm) was treated with toluene drop-casting. A detailed time-rotation profile for the spin-coating is represented in Supplementary Fig.  1c .']</t>
         </is>
       </c>
-      <c r="AF140" t="inlineStr"/>
+      <c r="AF140" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article describes a solvent-engineering process using γ-butyrolactone and dimethylsulphoxide (DMSO) followed by toluene drop-casting, but it does not mention the use of chlorobenzene as an antisolvent. The excerpts provided focus on the use of GBL, DMSO, and toluene, with no mention of chlorobenzene."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
@@ -21194,7 +22198,14 @@
           <t>['Interaction with other programs\nIn addition to the built-in tools, e.g. for refinement and validation, Coot provides interfaces to external programs. For refinement, interfaces to REFMAC and SHELXL are provided. Validation can be accomplished by interaction with the programs Probe and Reduce from the MolProbity suite. Furthermore, interfaces for the production of publicationquality figures are provided by communication with the (molecular) graphics programs CCP4mg, POV-Ray and Raster3D.\n\nREFMAC\nCoot provides a dialogue similar to that used in CCP4i for running REFMAC  (Murshudov et al., 2004) . REFMAC is a program from the CCP4 suite for maximum-likelihood-based macromolecular refinement. Once a round of interactive model building has finished, the user can choose to use REFMAC to refine the current model. Reflections for the refinement are either used from the MTZ file from which the currently displayed map was calculated or can be acquired from a selected MTZ file. Most REFMAC parameters are set as defaults; however, some can be specified in the GUI, such as the number of refinement cycles, twin refinement and the use of NCS.', 'Once REFMAC has terminated, the newly generated (refined) model and MTZ file from which maps are generated are automatically read in (and displayed). If REFMAC detected geometrical outliers at the end of the refinement, an interactive dialogue will be presented with two buttons for each residue containing an outlier: one to centre the view on the residue and the other to carry out real-space refinement.\n\nSHELXL\nFor high-resolution refinement, SHELXL can be used directly from Coot. A new SHELXL.ins file can be generated from a SHELXL.res file including any manipulations or additions to the model. Additional parameters may be added to the file or it can be edited in a GUI. Once refinement in SHELXL is finished, the refined coordinate file is read in and displayed. The resulting reflections file (.fcf) is converted into an mmCIF file, after which it is read in and the electron density is displayed. An interactive dialogue of geometric outliers (disagreeable restraints and other problems discovered by SHELXL) can be displayed by parsing the .lst output file from SHELXL.', "In the 'whole-map' scenario, candidate ligand sites are found by cluster analysis of a residual map. The candidate ligands are fitted in turn to each site (with the candidate orientations being generated by matching the eigenvectors of the ligand to that of the cluster). Each candidate ligand is fitted and scored against the electron density. The best-fitting orientation of the ligand candidates is chosen. Ligands often contain a number of rotatable bonds. To account for this flexibility, Coot samples torsion angles around these rotatable bonds. Here, each rotatable bond is sampled from an independent probability distribution. The number of conformers is under user control and it is recommended that ligands with a higher number of rotatable bonds should be allowed more conformer candidates. Above a certain number of rotatable bonds it is more efficient to use a 'core + fragment by fragment' approach (see, for example,  Terwilliger et al., 2006) .\n\nRebuilding and refinement\nThe rebuilding and refinement tools are the primary means of model manipulation in Coot and are all grouped together in the 'Model/Fit/Refine' toolset."]</t>
         </is>
       </c>
-      <c r="AF141" t="inlineStr"/>
+      <c r="AF141" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Substantiated",
+  "explanation": "The citation statement mentions rebuilding with COOT [23], which is consistent with the reference article's description of Coot as a molecular-graphics application for model building and validation, including tools for real-space refinement. The excerpts also highlight Coot's interfaces to external programs like REFMAC for refinement, further supporting the citation statement."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
@@ -21347,7 +22358,14 @@
           <t>["9  The bandwidth of the two components can easily be broad enough to permit the synthesized pulse to fall sufficiently in intensity before the linear polarization condition can reappear, thus ensuring that harmonic emission is very weak at all times except near t = 0. Measurement of the time duration of subfemtosecond pulses also seems feasible. Since it is as complex as the production process it will be addressed elsewhere.'  3  Our approach to attosecond pulse generation is a special case of a much more general phenomenon, namely, coherent control of strong-field atomic processes. Here we have described how control over the trajectory of a continuum electron can modulate the high-order susceptibility in time. The same physics can be applied to the control of the atomic susceptibility in space. In fact, a relatively weak (control) beam of circularly polarized light propagating along the direction of the electric-field vector of the fundamental light will deflect an electron so that it misses the ion. Therefore the control beam can ensure that any atom illuminated by the control beam will be unable to emit harmonic radiation, thus permitting quasi-phase matching. We foresee its application to harmonic generation using ions.", 'Since the development of the laser, obtaining shorter and shorter pulses has been a major emphasis of laser science. To approach the limit of 10 fs, at which short-pulse lasers currently operate," 2 nonresonant (Kerr) nonlinearities are used. However, the development of short-pulse coherent sources of less than 1-fs duration will require shorter-wavelength radiation and a new nonlinearity. In this Letter we introduce a method for producing pulses with durations approaching 1 atomic unit of time based on highharmonic emission from atomic gases.\nHigh harmonics have been extensively studied.  3  Their discrete nature and broad envelope spectrum implies that, if the harmonics are appropriately phased, a train of very short (-10 as) pulses separated by one half of the fundamental period will result.  4  In analogy with lasers, it is not sufficient to have equally spaced modes of an oscillator; they must be locked in the appropriate relative phase. Aside from phase-matching issues, the harmonic emission of a quantum system is determined by the squared modulus of the second time derivative of the dipole moment. Therefore the problem is to find the dipole moment as a function of time.', 'Before we discuss how short the fundamental pulse ... ... ..... .. .... .... ..... 5 T . I : I I I ... ..... : --_-L using the same 200-nm-thick silver filter as that in Fig.  1(a) . The time dependence of the instantaneous emission frequency is chirped, just as described for the individual pulses in Fig.  1(a) . It is not sufficient to fabricate a subfemtosecond pulse; we must ensure that the pulse will emerge undistorted from the nonlinear medium and the filter. In the medium there are two issues of concern, i.e., group-velocity and phase-velocity dispersion. In experiments on high-harmonic generation there are two main sources of phase-velocity dispersion: (1)  the phase advance that is due to the focusing geometry of the incident laser and (2) the dispersion in the laser-produced plasma." Whereas in principle the first problem is technical, the second problem is unavoidable; the high laser intensities necessary for efficient high-harmonic generation always lead to ionization. Indeed, the two are inherently related.']</t>
         </is>
       </c>
-      <c r="AF142" t="inlineStr"/>
+      <c r="AF142" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Substantiated",
+  "explanation": "The reference article [4] describes a method for generating subfemtosecond pulses using polarization gating, which is consistent with the statement that prior to this study, isolated attosecond pulses were primarily generated using few-cycle near-infrared (NIR) Ti:Sapphire lasers with sub-cycle gating technique, such as polarization gating."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
@@ -21491,7 +22509,14 @@
           <t>['mechanical and the chemical stability of the framework decrease gradually. \n[3]  Furthermore, the working environments of those immobilized moieties are usually harsh, which requires the frameworks to be chemically very stable. The requirement of a combination of good chemical stability and large pores means that very few candidates are widely utilized. MIL-101 and MIL-100 are two extraordinary examples that exhibit both properties and are suitable supports.  [4]  MIL-100 and MIL-101, both of which have zeotype mtn topology (zeotype refers to structures sharing the same topology with zeolites), contain super-tetrahedral cages to substitute for the tetrahedral unit in zeolites.  [5]  Hence, their largest pores reach 31Å and 29Å respectively although the organic linkers are relatively small. Moreover, the metal nodes in these MOFs are based on trivalent metal species. The strong interaction between carboxylates and high valent metal species accompanied with the small organic linker endows these frameworks with excellent chemical stability. Despite these advantages, the pore size still restricts further application of these MOFs when it comes to larger guests such as nanoparticles or enzymes.', 'Therefore, synthesis of mesoporous materials with larger pore size which also maintain excellent chemical stability is highly desired. Application of a ligand larger than those in the MIL-100 and MIL-101 MOFs to create zeotype frameworks would be an effective way to generate extra-large pores, while avoiding complicated organic synthesis to make the linker extremely large. Unfortunately, there are several challenges in the way of extending these mtn topological MOFs: First, the M 3 O(COO) 6 (M= Fe(III), Al(III), Cr(III), In(III), V(III), Sc(III)) building block is not the thermodynamically favored form, which makes the controllable formation of target products difficult;  [6]  second, even if the inorganic building block can be obtained, competitive framework isomers, such as the MIL-88 structure, still dominate as the major products; moreover, most of the synthesis needs to be conducted under hydrothermal conditions, which is infeasible for large organic linkers with poor water solubility. Therefore, searching for other zeotype frameworks, which can be synthetically controlled more easily, is one promising strategy.', 'Through a topological analysis, we herein present a zeotype mesoporous Zr-MOF, namely PCN-777, which has the β-cristobalite type structure. PCN-777 exhibits the largest cage (3.8nm) and the highest porosity (2.8cm 3 /g) among all the reported Zr-MOFs. Moreover, it shows high stability in aqueous solution with a wide range of pH values. Zirconium MOFs have been extensively studied recently due to their excellent chemical stability.  [7]  One major reason is the controllable synthesis of crystalline product or even single crystals by using competing reagents.  [8]  Moreover, the symmetry of a Zr 6 cluster ( Zr 6 O 4 OH 4 (COO) 12 ) fully coordinated by 12 carboxylates is O h , which has many high symmetry subgroups. This means that it is possible to reduce the connectivity and symmetry of Zr 6 to make it compatible with almost all kinds of organic linkers and form three dimensional (3-D) periodic frameworks.']</t>
         </is>
       </c>
-      <c r="AF143" t="inlineStr"/>
+      <c r="AF143" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article does not support the statement that hydrolytically stable cationic MOFs with pores of this size have not yet been reported. In fact, the article presents a newly designed and synthesized zeotype mesoporous Zr-MOF (PCN-777) with ultralarge pores and excellent stability in aqueous environments."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
@@ -21635,7 +22660,14 @@
           <t>['The appearance of the strong peak at 1590 cm À1 , weak peaks at 982 cm À1 and 930 cm À1 , which are assigned to C =C backbone stretching and ring-in plane deformation of PPY, respectively, indicating the successful polymerization of polypyrrole  [16] . Similarly, the decrease in intensity of the typical X-ray diffraction peaks of a-Fe 2 O 3 is clearly observed in Figure  2    S5  and  S6 ). Significant amount of carbon was detected only for a-Fe 2 O 3 /Ppy, homogenously dispersed throughout the whole area of a-Fe 2 O 3 /Ppy  [17] . To evaluate the electrochemical behavior, coin cells based on self-supported a-Fe 2 O 3 /Ppy composites, without using binder and additional conductive additives, were assembled against a lithium metal counter electrode and subjected to galvanostatic charge-discharge cycling as well as cyclic voltammetry testing.', 'It affords a highly conductive pathway for electron, a short ion diffusion length for ions, a fast mass transport channel for electrolyte, and sufficient void space among neighboring nanoflakes for accommodating large volume variations during Li intercalation/disintercalation when serve as anode for Li-ion battery  [3, 5]  Raman spectroscopy and X-ray diffraction (XRD) further confirm the presence of Ppy, a-Fe 2 O 3 and a small amount of Fe 3 O 4 in the nanoflakes. In Figure  2 (a) bare a-Fe 2 O 3 shows characteristic Raman peaks at 224, 290, 409 and 1300 cm À1 . After Ppy coating these a-Fe 2 O 3 peaks decrease in intensity, which is attributed to uniformly coating of polypyrrole onto the surface of a-Fe 2 O 3 nanoflakes  [15] .', 'The image of bare Iron foil on the left is bright while Fe 2 O 3 /Iron on the right is dark due to the growth of a-Fe 2 O 3 nanoflakes. In Figure  1 (c), it is clear that micrometersized flakes with thickness around 10-30 nm are generally pointed perpendicular to the plane of Fe foil. The nanoflakes are separated by distance in the range of 60-300 nm. A thin Ppy film is uniformly deposited onto the surface a-Fe 2 O 3 nanoflakes array, forming a conformal coating around each nanoflakes without any coalescence between them (Figure  2d ). The enlarge SEM image in Figure  2  clearly shows self-supported discontinuous nanoarchitectured a-Fe 2 O 3 /Ppy composite. This unique 3D nanostructure processes a large active surface area and preserves the space between nanoflakes.']</t>
         </is>
       </c>
-      <c r="AF144" t="inlineStr"/>
+      <c r="AF144" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article does not mention N-doped graphene or its characteristic peaks at 1588, 981, and 927 cm_−1. The excerpts provided discuss the synthesis and characterization of α-Fe2O3/polypyrrole (ppy) nanoarray, but there is no information related to N-doped graphene."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
@@ -21775,7 +22807,14 @@
           <t>['The whole reaction process was carried out at room temperature with agitated stirring. After 10 min, the reaction was aged at room temperature without any interruption for 24 h. The resulting pink precipitation was filtered and washed several times with absolute ethanol and finally dried in an oven at 60 °C. Synthesis of Pd-Co 3 [Co(CN) 6 ] 2 microspheres 0.01 g of Co 3 [Co(CN) 6 ] 2 was dissolved in 20 mL water solution. 10 mL palladium chloride water solution (1 g L -1 ) was slowly added into the above mixture solution at 30 °C in 10 min with vigorous magnetic stirring, followed by the addition of 5 mL EtOH. About four hours later, the solid products were collected by centrifugation and were washed with water several times. The products were dried under vacuum. The solid product was dissolved in concentrated nitric acid and analyzed by using an inductively coupled plasma atomic emission spectrometer (ICP-AES) to determine the content of Pd (47.9 wt%).', 'In particular, the value of binding energy is similar to K 2 Pd 2 (CN) 4 , whose Pd 0 3d 5/2 state equals 338.8 eV and Pd II 3d 3/2 state equals 334 eV, indicating that Pd combined with CuN.  34  The above results indicate that some Pd atoms were doped into the lattice of Co 3 [Co(CN) 6 ] 2 nanocubes. To ensure Pd 2+ was not adsorbed but doped, the nanocatalyst was washed with deionized water several times and then dissolved in nitromuriatic acid for the ICP test. The ICP test results show that the Pd-Co molar ratio is 2.94 : 1, while the Pd-Co molar ratio of the reactant was 5 : 4, which demonstrate that the Pd 2+ was not adsorbed but doped in the nanocatalyst. Moreover, in the preparation stage, we use EtOH as the reducing agent.', 'As shown in Fig.  5a  and  5b , the adsorption and desorption isotherms of Co 3 [Co(CN) 6 ] 2 and Pd-Co 3 [Co(CN) 6 ] 2 are also quite similar. The adsorption isotherms display steep nitrogen gas uptake at low relative pressures (P/P 0 &lt; 0.001) reflecting abundant micropore structure, a slight hysteresis loop implying a spot of mesopore and a sharp rise at medium and high pressure regions (P/P 0 = 0.8-1.0) indicating the size of MOF. The pore size distribution of Co 3 [Co-(CN) 6 ] 2 and Pd-Co 3 [Co(CN) 6 ] 2 can be obtained from the supplied results by using the sorption apparatus, as shown in Fig.  5c  and  5d . The results demonstrate that the narrow porous volume distribution is about 3 nm in pore size, which indicates that the NPs which formed the nanocubes are porous in structure.']</t>
         </is>
       </c>
-      <c r="AF145" t="inlineStr"/>
+      <c r="AF145" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article does not mention Ru source or Ru_3+ ion diffusing into Co_3[Co(CN)_6]_2, nor an ion-exchange reaction between Ru_3+ and Co_3+. The content of the article focuses on Pd-Co hybrid nanoparticles for Suzuki-Miyaura coupling reactions."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
@@ -21919,7 +22958,15 @@
           <t>['As shown in Fig.  6a , nano-MoC@GS(700) presented a much lower charge-transfer resistance (R ct ) value (14.5 U) than nanoMoC@GS(800) (28.6 U) and nanoMoC@GS(900) (69.5 U), indicating a faster electron transfer rate in the HER process. This lower R ct should be related to the con\ue103ned geometry in nanoMoC@GS materials, which would enhance the close interface contract of MoC nanoparticles with the ultrathin graphitized carbon shell and allow rapid charge transfer kinetics during the electrochemical process by improving the conductivity of electrocatalysts. The lowest R ct value for nanoMoC@GS(700) might result from its relatively large quantity of graphitized carbon (Table  S1  †). EIS for nanoMoC@GS(700) at various HER overpotentials from 75 to 200 mV in 0.5 M H 2 SO 4 is provided in Fig.  S7 . † The corresponding Nyquist and Bode plots of the EIS response of nanoMoC@GS(700) are given in Fig.', '8c  and S9 †) and a small R ct of 34.8 (Fig.  S10 † ) at 125 mV, suggesting that this electrocatalyst also possessed a large ECSA and faster electron transfer rates in basic media. Notably, Pt/C showed an overwhelming advantage in acidic media, while the HER activity of nanoMoC@GS(700) even exceeded that of Pt/C at the high overpotential (&gt;125 mV) in basic media. This interesting result was ascribed to different reaction pathways for the two catalysts, which were re\ue104ected by the different Tafel slope (77 mV dec À1 for Pt/C and 50 mV dec À1 for nanoMoC@GS) in Fig.  8b .  15  Additionally, the Nyquist and Bode plots of the EIS response for nanoMoC@GS(700) were depicted in Fig.  8d , and the peak at high frequencies also demonstrated the enriched porosity of this catalyst.', 'Meanwhile, the result of chronoamperometry (CA) for nanoMoC@GS(700) showed that the catalytic currents remained at around 15 mA cm À2 at 150 mV over 10 h, demonstrating the high stability under experimental conditions employed for this HER process. The HRTEM images of nanoMoC@GS(700) a\ue09der electrochemical stability testing are provided in Fig.  S6 . † NanoMoC@GS(700) structure and particle size distribution of the MoC nanoparticles showed only slight changes, con\ue103rming the superior stability of this electrocatalyst, which resulted from the con\ue103ned geometry (ultra\ue103ne MoC nanoparticles encapsulated by graphitized carbon shells) in this material. We then used EIS to provide further insight into electrode kinetics of the obtained materials. As shown in Fig.']</t>
         </is>
       </c>
-      <c r="AF146" t="inlineStr"/>
+      <c r="AF146" t="inlineStr">
+        <is>
+          <t>Here is my evaluation:
+{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article does not mention charge-transfer impedance values for S-1, S-2, S-3, S-4, S-5, or S-6. The provided excerpts discuss the electrochemical properties of nanoMoC@GS in acidic and basic media, including charge-transfer resistance (Rct) values, but do not compare them to other materials with specific impedance values as mentioned in the citation statement."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
@@ -22063,7 +23110,14 @@
           <t>['(Cancer Sci 2013; 104: 1396-1400) Personalized Therapy of LADC L ung cancer is the leading cause of cancer-related mortality worldwide. Lung adenocarcinoma (LADC) is the most frequent type of lung cancer. LADC occurs both in smokers and non-smokers, and its incidence is increasing. \n(1)  Genome analyses of LADC show that these tumors contain distinct genetic alterations that activate oncogenes.  (2, 3)  Genetic alterations that result in the activation of several oncogenes are detected in a mutually exclusive manner (Fig.  1 ); of the hundreds of genes mutated in each case of LADC, these oncogenes are considered to be "driver genes".  (4)  Remarkably, molecular targeted therapy using inhibitory drugs against activated oncogene products has begun to replace conventional chemotherapy using cytotoxic drugs, even for first-line use.  (2)  The epidermal growth factor receptor (EGFR) gene is activated by single amino acid substitution mutations or in-frame amino acid deletion mutations in 10-20% of LADC cases in the USA and in 30-40% of cases in East Asia.', '(2)  Tumors harboring these EGFR mutations respond to EGFR tyrosine kinase inhibitors (TKIs) such as erlotinib and gefitinib, thereby improving progression-free survival and quality of life.  (5, 6)  In addition, 3-5% of LADC harbor fusions that result in the activation of the anaplastic lymphoma kinase (ALK) gene; such mutations are mutually exclusive with EGFR mutations. Inhibitors, such as crizotinib, that target ALK tyrosine kinase show marked therapeutic effects against ALK fusion-positive LADCs.  (7) (8) (9)  These results indicate that personalized therapy for LADC using TKIs selected on the basis of somatic genetic alterations has been realized already; indeed, 20% of USA ⁄ European and 40% of Asian LADC patients benefit from such therapies.\n\nDiscovery of the RET Fusion Gene as a New Targetable Driver Gene\nIn 2012, four studies, including one by our group, identified fusions of the RET (rearranged during transfection) oncogene  (10) (11) (12) (13)  (Fig.', 'Prevalence and Characteristics of RET Fusion-Positive LADC\nSeveral studies have validated the presence of RET fusion in a small subset of non-small-cell lung cancers (NSCLCs).  (16, (19) (20) (21) (22) (23) (24)  The total number of examined cases has reached approximately 5000 (Table  1 ). Most of the positive cases are LADC, but several cases involve other histological types of NSCLC, such as adenosquamous carcinoma.  (19, 20)  The RET fusions are present in 1-2% of NSCLC ⁄ ADC of patients of both Asian and European descent. Several studies indicate that RET fusion occurs preferentially in young, never-smoker, and light-smoker patients.  (10, 12, 20)  The LADCs harboring KIF5B-RET fusions are well or moderately differentiated, similar to LADCs harboring EGFR mutations. This is in contrast to EML4-ALK fusion-positive LADCs, which tend to show signet-ring and mucinous cribriform patterns.']</t>
         </is>
       </c>
-      <c r="AF147" t="inlineStr"/>
+      <c r="AF147" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Substantiated",
+  "explanation": "The reference article provides specific percentages of NSCLC cases with EGFR mutations in different populations: 10-20% in the USA and 30-40% in East Asia (Excerpt 1). This supports the citing statement, which mentions that NSCLC harbouring an EGFR mutation accounts for ∼30–40% of NSCLC in the Japanese population and ∼15% in Caucasians."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
@@ -22208,7 +23262,15 @@
           <t>['Introduction\nIn recent years, ab initio calculations based on the local density approximation (LDA) (for a recent review see, for example, Ref.  [1] ) have been of increased interest. The reasons for this development are evident: LDA offers a reasonable compromise between accuracy and efficiency in treating electronic many-body effects, is completely parameterfree, and with the enormous increase in computer power complex calculations are now feasible. Using the Hellmann-Feynman theorem  [2] , the calculation of forces is in principle straight forward and, for a basis set such as plane waves, relatively simple. The forces offer the possibility of relaxing atoms into their ground-state or of performing ab initio molecular dynamics (MD) simulations. With the computers now available, calculations for systems containing more than 100 particles are practicable, and the development of faster parallel computers offers a bright future for ab initio techniques. We have recently implemented a powerful LDA plane wave program (Vienna ab initio molecular dynamics simulation package (VAMP) -for a detailed description see Ref.  [3] ) which can be used to perform complex calculations for many problems (i.e., bulk, surfaces, liquid systems, molecules).', "A selfconsistent calculation takes approximately two to three times as long as an evaluation of the KS eigenvectors for a fixed non-self-consistent Hamiltonian (same accuracy assumed).\n\nUltrasofi pseudopotentials\nThe first row elements (C, O, N, etc.) and the transition metals are hard to treat using standard pseudopotentials because they require a rather high energy-cutoff and a large number of plane waves (PW) per atom (PW &gt; 300) to obtain accurate results. This problem can be solved by adapting the ultrasoft (US) pseudopotentials proposed by Vanderbilt  [24] . The new scheme is characterized by two main points. (i) It is possible to include more than one reference energy, E, per quantum state, l, guaranteeing an improved transferability over a wide energy range. (ii) US-pseudopotentials are no longer norm-conserving (NC). Both points together allow the use of large cut-off radii for the pseudowavefunctions and the 'softer' pseudowavefunctions make it possible to reduce the number of PW.", 'The finite temperature LDA helps to avoid band crossing problems during an ab initio MD simulation. In conjunction with the exact evaluation of the electronic groundstate at each timestep, even metals with a high density of states at the fermi-level can be treated without the difficulties existing within the CP approach. US pseudopotentials offer for the first time the possibility of treating transition metals and first row elements on the same basis as simple metals. Using all refinements, the efficiency of our code is at least comparable to a conventional CP-program. Currently, several calculations for surfaces, molecules, molecular crystals and liquid and amorphous alloys are under progress. Despite the advantages of the LDA-PW approach, there still remains one unsolved problem, i.e., the o(N 3) scaling with the number of atoms, N. Using PWs no solution to this problem seems to be possible. At the moment, only simple non-self-consistent tight-binding calculations promise to show an o(N)-scaling in the density-matrix formulation  [41] . Nevertheless, in terms of accuracy and because there are several ambiguous parameters these techniques are not comparable with LDA-PW calculations.']</t>
         </is>
       </c>
-      <c r="AF148" t="inlineStr"/>
+      <c r="AF148" t="inlineStr">
+        <is>
+          <t>Here is my evaluation:
+{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article does not mention the VASP package or Perdew–Burke–Ernzerhof generalized gradient approximation. It discusses ab initio molecular dynamics and local-density approximation, but these topics are not directly related to the specific methods mentioned in the citation statement."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
@@ -22352,7 +23414,14 @@
           <t>['9  . At first, however, they could only produce a few hundred angstroms of GaAs per day, grown in layers that were too thin to accurately characterize. Over at IBM, meanwhile, Leo Esaki and Ray Tsu were grappling with a theoretical concept known as a superlattice. Whereas the heterostructures proposed by Kroemer contained just two layers of different materials, superlattices could be made of many very thin layers of two or more different semiconductors. Moreover, if a superlattice could be built with layers that were shorter than the mean free path of the electrons, a series of allowed and forbidden energy bands would be created in the device. Esaki and Tsu argued that this could prove to be "a valuable area of investigation in the field of semiconductors"  10  . However, when they submitted their first paper on this topic to a journal, it was rejected on the grounds that it was too speculative with "no new physics". (The first paper on the STM was rejected for similar reasons 2 .) Luckily for Esaki and Tsu the Army Research Office thought differently and supported their superlattice research for several years.', 'In fact, the word \'epitaxy\' comes from the Greek for \'above\' (epi) and \'in an ordered manner\' (taxis). The origins of MBE lie in the convergence of a number of research areas including solid-state physics, surface physics and materials science in the early 1950s. In 1954, for example, two years after finishing his physics doctorate at the University of Göttingen, Herbert Kroemer had a post at the Central Telecommunications Laboratory run by the German Postal Service in Darmstadt. As the theorist in a small semiconductor research group, he proposed "a non-stoichiometric mixed crystal of different semiconductors with different energy gaps"  6  . Several years later, working for American firms like RCA and Varian, Kroemer suggested several ways to exploit heterostructures made of two different semiconducting materials.', "At first he continued to study ferromagnetic and superconducting materials with nuclear and electron resonance techniques. Around 1973, however, managers at Bell Labs encouraged him to study defects in semiconductors, especially those used for laser applications. It was the need to fabricate samples for this research that led him to MBE. However, managers initially discouraged him, saying that MBE was too complex for a neophyte to take on. Within a few years, however, Gossard's small group was publishing papers describing the nanoscale semiconductor structures they had built with their rudimentary equipment  12  . By the late 1970s, Gossard's team, like researchers at other labs, were experimenting with a technique that became known as modulation doping (Fig.  2 ). By carefully controlling the introduction of source materials into the MBE chamber, researchers could implant dopants at precise locations in the semiconductor nanostructure they were fabricating. And by cleverly mixing doped with updoped layers, they could tune the structure and composition of the material and vary its electrical properties."]</t>
         </is>
       </c>
-      <c r="AF149" t="inlineStr"/>
+      <c r="AF149" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Substantiated",
+  "explanation": "The reference article supports the statement that Ruddlesden-Popper phase MQW perovskites have properties typical of epitaxial vacuum-grown heterojunctions. The excerpts mention the concept of heterostructures and superlattices, which are related to epitaxial growth, and describe the ability of molecular beam epitaxy (MBE) to control matter with near-atomic precision."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
@@ -22496,7 +23565,14 @@
           <t>['Catalyst Preparation. Supported ruthenium catalysts containing 2 wt % ruthenium were prepared by incipient wetness impregnation of as-synthesized mesoporous Al2O3 and for comparison, commercial Al2O3 (Alfa Aesar) with an aqueous solution of Ru(NO)(NO3) (Alfa Aesar) (denoted hereinafter as ruthenium/meso-Al2O3 and ruthenium/ commerical-Al2O3, respectively) at 25 °C for 12 h. Impregnated samples were dried in ambient air at 120 °C for 24 h and then reduced under flowing H2/N2 (10/90 v/v) at 350 °C for 6 h. Characterization. PXRD patterns were recorded on a Rigaku D/MAX-2000 diffractometer (Japan) using Cu KR radiation (λ ) 1.5406 Å). TEM were taken on the Hitachi H-9000 NAR transmission electron microscope under a working voltage of 300 kV.', 'Then 1.4-1.6 mL of 67 wt % nitric acid (or 1.4-1.6 mL of 37 wt % hydrochloric acid plus 0.5 g citric acid) and 2.04 g (10 mmol) of aluminum iso-propoxide were added into the above solution with vigorous stirring. The mixture was covered with PE film, stirred at room temperature for about 5 h, and then put into a 60 °C drying oven to undergo the solvent evaporation process. After 2 days of aging, the solution became a light-yellow solid (when hydrochloric acid and citric acid were used, white solids were obtained). Calcination was carried out by slowly increasing temperature from room temperature to 400 °C (1 °C min -1 ramping rate) and by heating at 400 °C for 4 h in air. High-temperature treatment was carried out in air for 1 h with a temperature ramp of 10 °C min -1 . Catalyst Preparation.', 'Introduction\nSince the ordered mesoporous silica material was first reported in 1992, 1 the interest in this research field has expanded all over the world due to the potential applications of these materials in catalysis and in other realms of chemistry. Compared to silica, alumina is more popular in catalysis area for its broad applications as industrial catalysts and catalyst supports employed in petroleum refinement, automobile emission control, and others.  2  With the characteristics of mesoporous materials, such as highly uniform channels, large surface area, narrow pore-size distribution, tunable pore sizes over a wide range, and so on, alumina with a mesostructure should possess much more excellent properties. Nonsiliceous materials with ordered mesoporosity are commonly prepared through the sol-gel process with surfactants as structure-directing agents (SDAs) or by utilizing the nanocasting method with silica or carbon materials as hard templates. However, the synthesis of ordered and thermal stable mesopo-rous alumina represents a much more complex problem  3  due to its susceptibility for hydrolysis as well as to the phase transitions accompanying the thermal breakdown of the ordered structure.']</t>
         </is>
       </c>
-      <c r="AF150" t="inlineStr"/>
+      <c r="AF150" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Substantiated",
+  "explanation": "The reference article describes a sol-gel process associated with nonionic block copolymer as templates in ethanol solvent, which is consistent with the citation statement's mention of a 'modified sol-gel solvent vaporization self-assembly method'. Although the exact details of the modification are not specified in the excerpts provided, the general synthesis strategy described in the reference article aligns with the citation statement."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
@@ -22640,7 +23716,14 @@
           <t>['Many cases of BCR-ABL1related acute leukemia will meet the criteria for acute lymphoblastic leukemia or mixed phenotype acute leukemia (see"Acute leukemia of ambiguous lineage"), provided that a blast phase of a previously unrecognized CML can be excluded. In addition to the newly listed leukemias associated with cytogenetically detectable rearrangements, AML with mutated NPM1 or CEBPA have been added to the classification as "provisional entities." Because mutated FLT3 frequently accompanies other genetic lesions, including well-recognized abnormalities such as the t(15;17)(q22;q12) and the t(6;9)(p23;q34), it is not included as a defining criterion for any distinct entity in this revision. Nevertheless, because of its prognostic importance, the mutational status of FLT3 should always be ascertained in AML, particularly in cytogenetically normal AML. AML with multilineage dysplasia was initially introduced in the WHO classification to encompass cases of AML characterized by MDS-like features, including unfavorable cytogenetic abnormalities, overexpression of multidrug-resistance glycoprotein, and an unfavorable response to therapy.', '77  One of the major challenges in the revision of the WHO classification of AML was how to incorporate important and/or recently described genetic aberrations into a classification scheme of AML and yet adhere to the WHO principle of defining homogeneous, biologically relevant, and mutually exclusive entities based not only on the prognostic value of a genetic abnormality, but on morphologic, clinical, phenotypic, and/or other unique biologic properties. This was particularly problematic for the most frequent and prognostically important mutations currently recognized in cytogenetically normal AML, mutated FLT3, NPM1, and CEBPA. These mutations are associated with few, if any, entirely consistent morphologic or clinical features. Most notably, they are not entirely mutually exclusive of each other or, particularly in the case of FLT3, of other well-recognized cytogenetic defects.  20, 78  Yet, in the context of cytogenetically normal AML, they are each important prognostic factors.', 'Mutational studies for mutated NPM1, CEBPA, and FLT3 are recommended in all cytogenetically normal AML; mutated JAK2 should be sought in BCR-ABL1-negative MPN, and mutational analysis for KIT, NRAS, PTNP11, etc, should be performed as clinically indicated.\n\nCorrelation/reporting of data\nAll data should be assimilated into one report that states the WHO diagnosis. WHO indicates World Health Organization; PB, peripheral blood; BM, bone marrow; IHC, immunohistochemistry; AML, acute myeloid leukemia; APL, acute promyelocytic leukemia; NOS, not otherwise specified; FISH, fluorescence in situ hybridization; RT-PCR, reverse transcriptase-polymerase chain reaction; and MPN, myeloproliferative neoplasm. dosage by quantitative RT-PCR is not practical on a daily basis, nor have gene expression arrays been introduced into routine use, and therefore such data are not included in this revision.']</t>
         </is>
       </c>
-      <c r="AF151" t="inlineStr"/>
+      <c r="AF151" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Substantiated",
+  "explanation": "The reference article discusses the revised criteria of the World Health Organization (WHO) for the classification of myeloid neoplasms and acute leukemia. Although it does not explicitly state 'the diagnosis of AML was established according to the revised criteria', the abstract and excerpts imply that the WHO has published a revised and updated edition of its classification, which includes new criteria for recognizing some previously described neoplasms and refinement of defining criteria for others. Therefore, it is reasonable to conclude that the reference article supports the citation statement regarding the diagnosis of AML according to the revised WHO criteria."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
@@ -22780,7 +23863,16 @@
           <t>['The third correction and the main focus of this Letter is the Petermann factor, K. First discovered in the context of transverse gain-guided semiconductor lasers  [4]  and subsequently generalized  [2, [5] [6] [7] [8] [9] [10] , this factor arises from the non-Hermitian nature of the laser wave equation, due to the presence of the gain medium as well as the openness of the laser cavity (i.e. spatially non-uniform outcoupling loss). It always leads to an enhancement of the linewidth, even with uniform gain and no gain-guiding. Typically, it is calculated from the non-orthogonal passive cavity resonances as K = dr |ϕ(r)| 2 dr ϕ(r) 2 2 , (2) where the integrals are taken over the cavity  [11] . In effect, the Petermann factor changes the ST linewidth by the replacement γ 2 c → Kγ 2 c . This is a significant correction for lasers with large outcoupling, in the range 1.1-1.6 for the conventional semiconductor lasers studied in Ref.  [2] .', '[2] . We shall refer to the standard theory, inclusive of the Petermann factor, as the Schawlow-Townes-Petermann (STP) theory. The extensive and impressive literature on the Petermann factor  [2, [4] [5] [6] [7] [8] [9] [10] 12 ] has, with one major exception  [9] , only treated single-mode lasing near threshold, neglecting the effects of spatial hole-burning. And apart from a recent paper by Schomerus  [12] , the literature has exclusively treated one-dimensional or waveguide lasers, and thus is not directly applicable to the wide variety of complex laser cavities developed during the past twenty years, such as microdisk and deformed-disk, photonic crystal, and random lasers. In this Letter, we derive a general formula for the intrinsic laser linewidth in arbitrary cavities, which is valid far from threshold, with strong spatial hole-burning, and in the multimode regime.', 'Eq. (  21 ) only includes the contribution to the laser linewidth from direct phase fluctuations; the indirect phase fluctuations  [3]  have been omitted for simplicity. The relation of the Petermann factor to the residue of the lasing pole for a waveguide laser was emphasized early on by Henry  [6] , and developed for more general cavities in an S-matrix formulation in Refs.  [12, 30] , but in all previous cases for a single lasing mode at threshold, i.e. without non-linear effects. Goldberg et al.  [9]  gave an excellent and detailed analysis of the linewidth for multimode lasing, including non-linear effects, but using an approach applicable only to one-dimensional cavities with spatially uniform dielectric functions. To our knowledge, our Eq. (  21 ), combined with SALT, is unique in providing a quantitative method for calculating the intrinsic laser linewidth in arbitrary cavities and pump profiles in the multimode, non-linear regime.']</t>
         </is>
       </c>
-      <c r="AF152" t="inlineStr"/>
+      <c r="AF152" t="inlineStr">
+        <is>
+          <t>Here is my evaluation of whether the reference article supports the given citation statement:
+{
+  "label": "Substantiated",
+  "explanation": "The reference article discusses how the Petermann factor leads to an enhancement of the linewidth in lasers with large outcoupling (Excerpt 1). Additionally, it generalizes previous treatments of the effects of gain and openness described by the Petermann factor (Abstract), which is consistent with the statement that the laser linewidth is enhanced when operating at a third-order exceptional point due to the so-called Petermann factors."
+}
+Note: The article does not explicitly mention "third-order exceptional points", but it discusses how the Petermann factor affects laser linewidth, which is relevant to the citing statement.</t>
+        </is>
+      </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
@@ -22924,7 +24016,14 @@
           <t>['5a ). Trinity performed well across a range of 10M to the full 150M input sequence reads, while the alternative methods tended to peak at ~50M pairs or smaller inputs (Supplementary Fig.  6a online ). In mouse (RefSeq annotation set, Fig.  5b ), Trinity (8185 transcripts, 7749 genes) outperformed the other de novo assembly methods ABySS (5561, 5500), Trans-ABySS (7025, 6598) and SOAPdenovo (761, 760), with the mapping-first programs Cufflinks (9010, 8536) and Scripture (9086, 8293) exhibiting better sensitivity. Furthermore, Trinity and Cufflinks appear best-tuned in their sensitivity across the broadest range of expression levels (Supplementary Fig.  7 online ). Unlike Trinity, several of the de novo methods did not perform well in fully reconstructing transcripts within the highest expression quintiles (Supplementary Fig.  7 online ).', 'RefSeq transcript gene annotations were downloaded for mouse at the UCSC mouse genome browser gateway ( http://  genome.ucsc.edu/cgi-bin/hgGateway?db=mm9 ) in BED format. Protein coding nucleotide sequences were extracted from the genome sequences based on the gene annotations using custom PERL scripts. The mouse reference coding sequences were further distilled to remove entirely identical sequences corresponding to isoforms encoding identical proteins and paralogous sequences: the original 19,947 genes encoding 23,881 transcripts were reduced to 19,857 genes encoding 22,717 on-identical coding transcripts. Reconstructed transcript sequences (via de novo assembly, Scripture, or Cufflinks) were mapped to the reference coding sequences using BLAT  35  . Full-length reference annotation mappings were defined as having at least 95% sequence identity covering the entire reference coding sequence and containing at most 5% insertions or deletions (cumulative gap content). In evaluating methods that leverage the strand-specific data (Trinity and Cufflinks), proper sense-strand mapping of sequences was required. Transcripts reconstructed by the alternative methods (Scripture, ABySS, and SOAPdenovo) were allowed to map to either strand.', '9a online ). Conversely, performance of Scripture and Cufflinks using TopHat alignments in mouse exceeded that using BLAT alignments (Supplementary Fig.  9b online ). Hence, for evaluation purposes, we leveraged BLAT short read spliced alignments in S. pombe and TopHat alignments in mouse. BLAT alignments of short reads to the S. pombe genome were performed using the pipeline described above with the following settings: maximum intron length set to 500 bases, maximum distance between read pairs of 500, and only the single best alignment was reported per read. TopHat alignments to the mouse genome were performed using the following parameters: minimum intron length of 50 bases, maximum intron of 100kb, and mate inner distance set to 300 bases. Transcribed strand information was assigned to the individual reads based on knowledge of the fragment type (left or right) and the aligned strand of the genome. Both Cufflinks (version 0.9.3) 2 and Scripture 3 (version VPaperR3, obtained from Scripture author Manuel Garber) were executed on these alignments.']</t>
         </is>
       </c>
-      <c r="AF153" t="inlineStr"/>
+      <c r="AF153" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Substantiated",
+  "explanation": "The reference article supports the use of Trinity for de novo assembly with default parameters. The abstract mentions that Trinity can be used for de novo assembly of full-length transcripts without a reference genome, and Excerpt 1 shows that Trinity performed well across a range of input sequence reads."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
@@ -23068,7 +24167,14 @@
           <t>['Thus,  Salm et al. (2001)  have proposed that through thoughtful planning and strategic care of reefs within existing and future marine protected areas (MPAs)*, it may be possible to take advantage in two broad ways of the natural properties of coral reef ecosystems to mitigate the negative impact of bleaching on coral reef biodiversity: (1) Identify and manage specific patches of reef where local conditions are likely to result in reduced temperature-related bleaching and mortality (i.e., coral assemblages with a high level of "resistance") to protect them from direct anthropogenic impacts. (2) Enhance the capacity for coral reef recovery ("resilience") by maintaining conditions optimal for larval dispersal and recruitment to damaged sites (requires minimizing other stresses at these sites [abatement of direct localized impacts] and analyzing larval dispersal [connectivity] to maximize recolonization). An understanding of which local environmental factors are predictors of greatest resistance and resilience to coral bleaching would help managers identify, design, and manage networks of MPAs in order to maximize overall survival of the world\'s coral reefs in the face of global climate change.', 'Estas áreas de interés, en donde las condiciones ambientales parecieran favorecer la resistencia y la recuperación durante y después de eventos de blanqueo a gran escala, podrían ser incorporadas a redes estratégicas de áreas marinas protegidas cuyo objetivo sería maximizar la conservación de la biodiversidad global de arrecifes coralinos. Según datos bibliográficos y observaciones de investigadores recopiladas sistemáticamente, este artículo identifica las probables correlaciones ambientales de resistencia al blanqueo y recuperación de corales, incluyendo aquellos fac-\n\n\nIntroduction\nIt is now generally acknowledged that coral reefs are among the most threatened global ecosystems, and among the most vital  (Costanza et al. 1997; Bryant et al. 1998; Boesch et al. 2000; Reaser et al. 2000; Wilkinson 2000 ) .', 'The most useful approach would be one that utilizes natural processes rather than expensive technological fixes and helps managers focus local management and enforcement efforts on the most criti-cal areas. Given the limited capacity and funding available for management in many coral-reef countries, what is especially needed are simple tractable strategies that any manager could begin to adopt immediately to maximize long-term survival of the broadest range of coral communities and reef types. We confine our discussion to local-scale resistance that occurs despite the presence of "mass bleaching conditions" in an area or region. This resistance is distinct from avoidance, in which large areas or regions may never be tested by bleaching conditions at all due to larger-scale climatological and oceanographic phenomena  ( Done 2001 ) . Although the latter is an important area of ongoing research, here we focus on determinants of local-scale resistance within areas or regions that have experienced bleaching conditions, because this is an important scale at which local managers work. Therefore, building on the work of  Salm et al.']</t>
         </is>
       </c>
-      <c r="AF154" t="inlineStr"/>
+      <c r="AF154" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Substantiated",
+  "explanation": "The reference article supports the statement that identifying and protecting spatial refugia (referred to as 'target areas' in the article) is a strategy for coral reef conservation. The abstract mentions incorporating these areas into networks of marine protected areas, and Excerpt 1 describes identifying patches of reef with local conditions that reduce temperature-related bleaching and mortality."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
@@ -23212,7 +24318,14 @@
           <t>['Fragment counts were summarized by Entrez Gene ID using the featureCounts function  [59]  of version 1.8.2 of the Bioconductor package Rsubread  [60] . Fragments with both end reads mapped successfully contributed one count if the fragment overlapped any annotated exon for that gene. Fragments for which only one read mapped successfully contributed half a count if that read overlapped an exon. The summarized read count data is available from the voom webpage  [56] . The voom mean-variance trend shown in Figure  1a  was obtained from all 16 libraries, treated as four groups. Genes were filtered out if they failed to achieve cpm &gt; 1 in at least four libraries, and the remaining log-cpm values were quantile normalized between libraries  [61] . The comparison between technical replicates to check the type I error rate control used only the four group B libraries. Genes were filtered out if they failed to achieve a cpm &gt; 1 in at least two libraries and the log-cpm values for the 16,745 remaining genes were quantile normalized.', 'The revised methods are implemented in the functions roast() and camera() of the limma software package.\n\nNormalization\nThe log-cpm values are by definition normalized for sequencing depth. Other normalization steps can optionally be done. The library sizes R i can be scale normalized to adjust for compositional differences between the RNA-seq libraries  [54] . This produces normalized library sizes R * i that can be used in place of R i in the voom pipeline. Alternatively, between-array normalization methods developed for single channel microarray data, such as quantile or cyclic LOESS, can be are applied to the log-cpm values.\n\nSimulations\nThe simulations were designed to generate data with characteristics similar to real data that we analyze in our own practice. First a set of baseline expression values was generated representing the relative proportion of counts expected to arise from each gene. These proportions were translated into expected count sizes by multiplying by library size, and then multiplied by true fold-changes as appropriate. Counts were then generated following a NB distribution with the specified mean and dispersion for each observation. The distribution of baseline values was chosen to match that from RNA-seq experiments conducted at our institution.', "We work with log-counts normalized for sequence depth, specifically with log-counts per million (log-cpm). The mean-variance is fitted to the gene-wise standard deviations of the log-cpm as a function of average log-count. We explore two ways to incorporate the mean-variance relationship into the differential expression analysis. The first is to modify limma's empirical Bayes procedure to incorporate a mean-variance trend. The second method incorporates the mean-variance trend into a precision weight for each individual normalized observation. The normalized log-counts and associated precision weights can then be entered into the limma analysis pipeline, or indeed into any statistical pipeline for microarray data that is precision weight aware. We call the first method limma-trend and the second method voom, an acronym for 'variance modeling at the observational level' . limmatrend applies the mean-variance relationship at the gene level whereas voom applies it at the level of individual observations."]</t>
         </is>
       </c>
-      <c r="AF155" t="inlineStr"/>
+      <c r="AF155" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Substantiated",
+  "explanation": "The reference article discusses the use of precision weights in RNA-seq analysis, specifically with the voom method, which estimates the mean-variance relationship of log-counts and generates precision weights for each observation. The statement from the citing article mentions using the voom R package to calculate precision weights, which is consistent with the content of the reference article."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
@@ -23356,7 +24469,14 @@
           <t>['Fourth, it is possible that low copy number gains or loss-of-heterozygosity (LOH) of specific regions containing histone-modifying genes could mimic the intragenic mutations that we observed  (36) . Finally, it is possible that heritable epigenetic alterations are responsible for initiating some MBs. The last explanation, involving covalent changes in chromatin proteins and DNA, is intriguing given the new data on MLL2 in this tumor type. It should thus be informative to characterize the methylation status of histones and DNA in MBs with and without MLL2/MLL3 gene alterations, as well as to determine the expression changes resulting from these gene mutations. These data highlight the important connection between genetic alterations in the cancer genome and epigenetic pathways and provide potentially new avenues for research and disease management in MB patients.    † Based on 21 nonhypermutable tumors analyzed in  (19) . ‡ Based on 11 breast and 11 colorectal tumors analyzed in  (16, 17) . § Numbers in parentheses refer to percentage of total non-silent mutations.', 'Most recently, frequent mutations of the chromatin remodeling gene ARID1A have been discovered in ovarian clear cell carcinomas  (20, 35) ; of note, one ARID1A mutation was discovered in our MB patients (table  S4 ). A link between histone methylation genes (although not MLL2 or MLL3) and MB has also previously been hypothesized based on the observation that copy number alterations affecting chromosomal regions containing histone methyltransferases or demethylases occur in a subset of MBs  (36) . The mechanism(s) through which MLL genes contribute to tumorigenesis are not known but some clues can be gleaned from the literature. The MLL family of histone H3K4 trimethylases includes seven genes (MLL1, MLL2, MLL3, MLL4, MLL5, SET1A and SET1B)  (37) . MLL-family genes have been shown to regulate HOX gene expression  (38, 39) , and an attractive possibility is that they normally downregulate OTX2, an MB oncogene  (6, 7, 40) .', '2 ). These data not only provide strong evidence that these pathways are important to MBs, but they also show that MLL2 and MLL3 are, on the basis of genetic criteria, tumor suppressor genes that are inactivated by mutation. Discussion. These data provide a comprehensive view of a solid tumor arising in children. The most impressive difference between this tumor type and those affecting adults is the number of genetic alterations observed. This result could not have been predicted on the basis of prior evidence  (27) . In fact, at the karyotypic level, the incidence of chromosomal changes in MBs is often described as high as that in adult solid tumors [reviewed in  (27) ]. What does the smaller number of mutations reveal about the tumorigenesis of MBs? Most mutations observed in adult tumors are predicted to be passenger alterations  (19) . Passenger mutations provide an evolutionary clock that precisely records the number of divisions that a cell has undergone during both normal development and tumor progression. Therefore, the cell division number is linearly related to the number of passenger mutations detected in a tumor  (28) .']</t>
         </is>
       </c>
-      <c r="AF156" t="inlineStr"/>
+      <c r="AF156" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Substantiated",
+  "explanation": "The reference article supports the claim that genetic events targeting histone modifiers, especially those regulating lysine methylation and/or acetylation, were found across subgroups and contributed to MB development. Excerpts 1 and 2 specifically mention mutations in histone-lysine N-methyltransferase genes MLL2 or MLL3 in MB patients, demonstrating the role of histone modification in tumorigenesis."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
@@ -23502,7 +24622,14 @@
           <t>["Thus, although many NGS read preprocessing tools exist, none of them, alone or in combination, could offer the desired flexibility and performance, and most were not designed to work on paired-end data. As a result, we developed Trimmomatic as a more flexible, pair-aware and efficient preprocessing tool, optimized for Illumina NGS data.\n\nALGORITHMS\nTrimmomatic includes a variety of processing steps for read trimming and filtering, but the main algorithmic innovations are related to identification of adapter sequences and quality filtering, and are described in detail below. A list of the other processing steps is presented in the Supplementary Materials.\n\nRemoval of technical sequences\nTrimmomatic uses two approaches to detect technical sequences within the reads. The first, referred to as 'simple mode', works by finding an approximate match between the read and the usersupplied technical sequence. This mode has the advantage of working for all technical sequences, including adapters and polymerase chain reaction (PCR) primers, or fragments thereof. Such sequences can be detected in any location or orientation within the reads but requires a substantial minimum overlap between the read and technical sequence to prevent false-positive findings.", 'The trimming status of each read can optionally be written to a log file. This is intended to help tune the choice of processing parameters used, but because it has a significant performance impact, it is not recommended unless needed.\n\nRESULTS\nTo illustrate the value of data preprocessing, we evaluated two different scenarios: reference-based alignment using Bowtie 2  (Langmead and Salzberg, 2012)  and BWA  (Li and Durbin, 2009)  against the Escherichia coli K-12/MG1655 reference (NCBI sequence NC_000913.2), and de novo assembly using Velvet  (Zerbino and Birney, 2008) , on public E.coli K-12/ MG1655 datasets (SRA datasets SRX131047 and SRR519926), as described in the Supplementary Methods.\n\nReference-based alignment\nDataset 1 (SRX131047) represents a typical Illumina library, sequenced on the HiSeq 2000 using 2 Â 100 bp reads. Quality checking with FastQC revealed a notable quality drop in many reads after cycle 75 in both but did not report a high level of adapter contamination.', 'In the reference-based scenario, preprocessing increased the number of uniquely aligned reads from dataset 1, as seen in the first portion of Table  1 . Filtering for both adapters and quality achieves the best result, and quality trimming is especially important when alignment settings are strict. The Maximum Information approach outperforms the Sliding Window approach in both cases, with a wider margin when the alignment mode is strict. Notably, the optimal results for strict alignment and tolerant alignment were found using widely different quality stringency settings. (See Supplementary Results for more details.) To validate these results with an alternative aligner, we repeated the experiment using BWA. Although the alignment counts differ, because of slight differences between the tools in the settings or algorithms, the overall trend is similar. The best results are again achieved when filtering for both adapters and quality, as shown in the second part of Table  1 . Dataset 2 (SRR519926) is a 2 Â 250 bp run, sequenced on an MiSeq. Although read quality is high at the start of each forward read, the longer read length allows more opportunity for errors Fig.  3 .']</t>
         </is>
       </c>
-      <c r="AF157" t="inlineStr"/>
+      <c r="AF157" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Substantiated",
+  "explanation": "The reference article describes Trimmomatic as a tool that includes processing steps for read trimming and filtering, with parameters that can be tuned by users. The use of the SLIDINGWINDOW parameter is mentioned in Excerpt 1 as one of the algorithmic innovations related to quality filtering. Although the exact parameters used (SLIDINGWINDOW:5:25) are not specified in the provided excerpts, it is clear that Trimmomatic supports adjustable parameters for trimming and filtering, which substantiates the claim made in the citing article."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
@@ -23648,7 +24775,14 @@
           <t>['Introduction\nOver the last decade, The Cancer Genome Atlas (TCGA) consortium has measured large-scale genomics and clinical profiles of cancer patients so that scientists can study tumor genomes and decipher the genetic underpinnings of cancer. The TCGA data can be downloaded from web portals or via web services, such as the TCGA data portal ( https://tcga-data.nci.nih.gov/tcga/ ), cBio  (Cerami et al., 2012; Gao et al., 2013) , canEvolve  (Samur et al., 2013) , or Broad Institute GDAC Firehose ( http://gdac.broadinstitute.org/ ). However, manual download of this massive data is time consuming and web service calls like the firehose_get function require additional program installation and technical setup. Most importantly, these two approaches cannot be easily integrated into a framework for statistical analysis. Many extra steps and technical knowledge of molecular platform data formats are needed to wrangle and pre-process the data before it can be statistically analyzed. Further, this process must be repeated when new data versions or additional samples become available, hindering efforts at version-control and reproducible research.', 'Others have provided software to obtain the TCGA data. cBio, for example, provides an R and Matlab package but was not designed to be used for genome-scale data analysis. It requires input of a list of genes from users and thus limits the exploratory use of the data. Another R package, RTCGAToolbox downloads TCGA data from Firehose  (Samur, 2014) , but the downloaded data is not preprocessed into data formats conducive for multivariate statistical analysis. Further, linking and merging functions necessary for integrated statistical analyses such as sample matching across multiple platforms and merging clinical and molecular data are not available in this package. Because of these problems, use of the TCGA data can be limited to those with domain expertise, rendering the data inaccessible for general data scientists. In response, we have developed an R package TCGA2STAT that makes the TCGA data in the open access data tier easily accessible to all by downloading, wrangling and pre-processing the data into a data matrix or list of matrices ready for multivariate or integrated statistical analyses.', 'Details of all wrangling and preprocessing steps are described in the package vignette (Supplementary Data).\n\nFunctions and examples\nThe TCGA2STAT package includes one major function and three additional utility functions: • getTCGA. This is the main function of the package which obtains data from Firehose and processes the data into a matrix that can be used directly for statistical analysis in R. Only two inputs are required: the cancer type desired and the data platform or molecular profiling type desired. Our package supports over thirty different cancer types and eleven different data platforms. For example, getTCGA(disease¼"OV", data.type¼ "RNASeq2") will obtain the RNASeq2 level III RSEM data from TCGA ovarian cancer patients. With the same function, the user can specify the specific types of data for each platform, such as counts instead of RPKM for RNASeq data. Also, users can choose to download the molecular profiles along with clinical data or filter the data by particular clinical covariates. • SampleSplit. This function can be used to split the data imported via getTCGA into groups of samples profiled from the primary tumor, recurrent tumor, or normal/control groups.']</t>
         </is>
       </c>
-      <c r="AF158" t="inlineStr"/>
+      <c r="AF158" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Substantiated",
+  "explanation": "The reference article describes the TCGA2STAT package as a tool for downloading and processing TCGA data, including RNA-seq data, into a format ready for statistical analysis in R. The excerpt 3 specifically mentions that the getTCGA function can obtain RNASeq2 level III RSEM data from TCGA cancer patients, which matches the citing article's statement about using TCGA2STAT to download normalized RNA-Seq by Expectation-Maximization (RSEM) values."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
@@ -23799,7 +24933,14 @@
           <t>['V. RESULTS AND CHARACTERIZATION\nTo demonstrate the recording capability of the close-packed sites, we have performed in vivo recordings in the sensory cortex of an anesthetized mouse. In vivo experiments were done in accordance with MIT Committee on Animal Care approved protocols. An example of data collected with a single-shank probe bearing 64 pads is shown in Fig.  12 . The data illustrate the ability of close-packed recording sites to spatially oversample neural activity, and it shows how activity from the same neuron is picked up by several neighboring sites in its vicinity. The devices we fabricated have a standard recording site of 9 × 9 μm. We wanted to understand how the dimensions of a recording site impact its electrical properties. For this, we characterized the electrode impedance and the electrical noise as a function of recording site size. The data were collected from single-shank 64-channel probes with electrode site dimensions ranging from 2.4 to 9.6 μm. We gold electroplated each recording site with a constant current density protocol (60 pulses of 1 s at 0.1975 nA/μm 2 ). Fig.', 'from a dense array \n[12] -  [15] . In this paper, we demonstrate a close-packed silicon microelectrode technology that enables a tight continuum of recording sites along the length of the shank (Fig.  1 ), rather than discrete arrangements of tetrode-style pads or widely spaced sites. This arrangement, thus, enables tetrodelike spatial oversampling continuously running down the shank, so that sorting of spikes recorded by such densely packed electrodes can be facilitated for all the sites of the probe simultaneously. We use advanced lithography tools to create these close-packed arrangements in a scalable fashion, demonstrating probes with 1000 electrode pads situated on five shanks with 200 recording sites per shank. A key challenge with the traditional silicon electrode designs has been that wiring to the recording sites occupied a large fraction of the available shank width. This is problematic because scaling up the number of recording sites forces the shank geometry to widen, placing an upper bound on the number of sites practical for a single shank of a given width.', 'For example, the data suggests that even a 3 μm × 3 μm site has electrical characteristics com- patible with recording single unit activity, with impedances of 2 MΩ and a noise level of 8 μV rms .\n\nVI. CONCLUSION\nWe have introduced a platform to fabricate close-packed microelectrodes for neural recordings, and described the design, fabrication, and packaging methods that allow us to create a large range of scalable probe designs with close-packed recording sites. Although multisite silicon probes have been generated before, as noted in the introduction, the hybrid fabrication method here enables us uniquely to pursue electrode spacings far denser than in earlier implantable probes, thus enabling the feature of spatial oversampling of the neurons. The in vivo experiment and quantitative electrode site impedance and noise characterization demonstrated that by closely packing recording sites, we are able to spatially oversample and pick up unit activity on several recording sites at a time, and that the size of the recording sites can be reduced even lower than 9 μm. Our results suggest that close-packed electrodes may become not only instrumental for neuroscience, but also for understanding the basic principles of electrode design when scaling to large channel counts is required.']</t>
         </is>
       </c>
-      <c r="AF159" t="inlineStr"/>
+      <c r="AF159" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Substantiated",
+  "explanation": "The reference article describes the development and use of high-density silicon microelectrodes for neural recording, which supports the statement that extracellular recordings were performed with such devices. The excerpts highlight the capabilities and advantages of these close-packed electrodes in spatially oversampling neural activity."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
@@ -23939,7 +25080,14 @@
           <t>['5 . Interaction of CHD4 with the core PMMR complex. (a) 2D single-molecule tracking of single mEos3-tagged CHD4 molecules in live mESCs show differences in the diffusion of a sub-population of CHD4 molecules in the presence (WT) and absence of MBD3 (MBD3-null). Representative images of the same cell are shown (top right) using low power 488-nm excitation (green form of mEos3) and 405-nm/561-nm excitation (photo-activated red form of mEos3). A small number of the individual tracks from this cell are also shown indicating the fast and slow diffusing fractions of CHD4. The exact diffusion coefficients extracted from the data are shown in a box-and-whisker plot (lower right). A total of 23,854 and 20,039 tracks were analyzed for the wild-type and MBD3-null cells, respectively. (b) A putative model of NuRD complex assembly is shown in a schematic representation.', 'The more rapidly moving CHD4 molecules (which we expect are diffusing along chromatin) provide direct evidence that the MBD component plays an important role in the association of CHD4 with NuRD, consistent with our hypothesis that the CS and PMMR sub-modules interact via a Simjang/MBD-like interaction (see Fig.  5b ). In this model, CG18292 (or DOC1 in mammalian cells) might either interact with PMMR by itself or as part of the CS complex. In summary, our experiments suggest a pathway for the assembly of the complete and functional NuRD complex via preformed and active sub-modules. The fact that the sub-modules retain similar enzymatic activities and are present in different cellular compartments when expressed at endogenous levels is consistent with the idea that they may have independent activities in both the nucleus and the cytosol.\n\nMaterials and Methods\nProduction and purification of NuRD complexes Endogenous NuRD complex was purified from Drosophila S2 Schneider cells using stable cell lines and a metallothionein-induceable promoter (Thermo Fischer Scientific) as described in Supplementary Data.', '(d) MALDI-TOF analysis after an overnight deacetylation reaction of tetra-acetylated histone H4 (1-21) peptide by the dNuRD complex. Substrate peptides lacking up to four acetyl groups (complete deacetylation) are detected. We sought evidence for the hypothesis that a Simjang/MBD-like (or GATA2Da/b-MBD2/3) interaction is important for the association of the core PMMR deacetylase and CS chromatin-remodeling sub-modules, by carrying out single molecule tracking studies of CHD4 in the presence and absence of MBD3 in mESCs. The slowly moving molecules are not affected by the presence or absence of MBD3, and given the higher concentrations of CHD4 in the cell, and its known NuRD-independent functions, we suspect that they may correspond to CHD4 that is not associated with NuRD  [38] .']</t>
         </is>
       </c>
-      <c r="AF160" t="inlineStr"/>
+      <c r="AF160" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Substantiated",
+  "explanation": "The reference article supports the claim that MBD3 is part of the deacetylase core. The abstract mentions that the NuRD complex has a stable core of subunits, including the chromatin remodeler CHD4 and the core component MBD3. Excerpt 1 also shows an interaction between CHD4 and the core PMMR complex in the presence and absence of MBD3, indicating that MBD3 is part of this complex."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
@@ -24083,7 +25231,14 @@
           <t>['On the other hand, under the FF null model NODF identified only three empirical matrices as being nested. NODF also indicated that nestedness in species occupancy (mean 054.0) is significantly lower than nestedness in species composition among sites (mean 060.6; Z 0(9.25, pB0.001).\n\nDiscussion\nWhy another metric? The occurrence of nestedness in ecological systems provides clues about the processes that affect species distributions among different sites and that shape interspecific interactions  (Lomolino 1996 , Leibold and Mikkelson 2002 , Thompson 2005 , 2006 , Lewinsohn et al. 2006 , Guimara ˜es et al. 2007b ). In addition, its quantification can be used to guide conservation strategies  (Atmar and Patterson 1993 , Cutler 1991 , 1994 , Boecklen 1997 ) and to understand the fragility and co-evolution of networks of ecological interactions  (Thompson 2005 , 2006 , Jordano et al. 2006 ). Therefore, it is fundamental to measure such structure properly.', 'r2 r3 r2 r4 r2 r5 r3 r4 r3 r5 r4 r5 N paired =67 N paired =67 N paired =50 N paired =50 N paired =0 N paired =100 N paired =100 N paired =50 N paired =50 N paired =0 N columns = 63 N rows = 53 NODF = 58 Figure  2 . Illustration of the way by which nestedness is quantified according to NODF. First, we calculated the paired nested degree for each pair of column and for each pair of row. Then, the total nestedness among columns was quantified as the average values for all pairs of columns. The total nestedness among rows follows the same procedure applied for columns. Finally, the degree of nestedness for the whole matrix is calculated as the sum of all values of paired nestedness divided by the total number of pairs (i.e. the sum of all combinations of pairs of column and pairs of rows). make sense to convert C to a percentage scale because this metric is null model dependent and does not have minimum and maximum absolute values as T, d1 and NODF.', 'Further studies have to clarify the relationships between these features and nestedness. The diagnostic tests to detect type I error rates associated with NODF showed that this new metric is more conservative than those recently examined by  Ulrich and Gotelli (2007a) . According to their analyses under the fixed-fixed null model, between 93% and 96% of the random matrices were correctly detected as not being significantly nested according to the eight metrics used, including T, N C and d. However, when the EE null model was used, the correct detection of randomness ranged from 3% to 42%. The percentage of random matrices for which randomness was correctly detected by NODF ranged from 99.5% under FF to 93% under the EE algorithm. Under the fixed-fixed model, therefore, NODF is slightly superior to the conventional metrics but it performs much better under the equiprobable null model.\n\nNestedness in empirical metacommunities\nOur analysis of empirical matrices compiled by  Atmar and Patterson (1995)  showed that the degree of nestedness obtained by NT, NC and Nd1 are significantly higher than those calculated through NODF.']</t>
         </is>
       </c>
-      <c r="AF161" t="inlineStr"/>
+      <c r="AF161" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Substantiated",
+  "explanation": "The reference article [80] discusses the NODF statistic as a metric for quantifying nestedness in ecological systems. Excerpt 2 specifically explains how NODF is used to quantify nestedness among columns and rows, demonstrating its application in ecological analysis. Therefore, the statement from the citing article that 'We used the NODF statistic [80] to quantify nestedness of the sample-by-taxa matrix' is fully supported by the reference article."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
@@ -24223,7 +25378,15 @@
           <t>["1b , c ). A number of parameters can be deduced from these data and the correlation of these to genetic variants tested. Considering gene expression phenotypes in terms of single-cell distributions provides important information about gene regulation, as the noise from the regulation of transcription can be considered separately from the noise of RNA turnover (Supplementary Fig.  1 ). Thus constitutively expressed genes, for example, are expected to be less noisy, demonstrating mostly the thermodynamic noise of RNA turnover in the absence of variable regulation (Supplementary Fig.  1 ). Analyzing four, public, single-cell RNA sequencing data sets  6, 7  , we found that this is indeed the case (Supplementary Notes, section 1). A gene that is not constitutively expressed can be described in terms of how often it switches 'on' (burst frequency), the amount of RNA produced when 'on' (burst size) and the rate at which its RNA is degraded. A recent study 11 of 8,000 human loci found that almost all of them exhibited such 'bursty' expression, with certain loci modulating burst frequency and others modulating burst size.", 'Gene expression typically had much greater variability between cells within an individual than between individuals, and the distribution of gene expression values is very different between individuals for some genes. (Fig.  1a ). The currently understood reasons for this large cell-to-cell noise are thermodynamic, regulatory and cellular (Supplementary Fig.  1 ). As a basis for studying the association of single-cell phenotypes with genetic variants, we first sought to generate high-quality data in a large population of cells (1,440 cells). We measured gene expression using highly parallel qPCR validated with digital PCR, as single-cell RNA sequencing still faces notable technical challenges  6, 7  . We focused on 92 genes affected by Wnt signaling, a major regulator of the cell cycle that has been highlighted as a key pathway in clinical GWAS and cancer epidemiology (Supplementary Fig.  2 ). Of the 92 genes studied, 46 are listed in the Catalog of Genome-Wide Association Studies ( http://www.genome.gov/gwastudies ).', '(44%) PPARD (44%) TCF7 (45%) NPPC (47%) 0 1 2 Expression (log 10 scaled) 3 4 KREMEN1 (49%) npg l e t t e r s mixture was used as an approximation to the slower fitting, four-parameter, Beta-Poisson mixture (Supplementary Fig.  4 ). Such a Poisson mixture model not only describes the long-tailed behavior described by the negative binomial, but allows for the expected expression bimodality in genes with low burst frequency. These models and their rationales are further detailed in the Online Methods and Supplementary Notes, section 2. Gene expression distributions can also be described in terms of heterogeneous cell subpopulations. We considered cells in different stages of the cell cycle, and their varying proportions between samples. Using flow cytometry, we excluded cells with increased DNA content, as would be expected in the S and G 2 cell cycle phases. We further subdivided cells into G 1 and early S-phase based on their expression of GTSE1, a cell division molecular switch that becomes highly expressed in the S and G 2 phases  14  .']</t>
         </is>
       </c>
-      <c r="AF162" t="inlineStr"/>
+      <c r="AF162" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Substantiated",
+  "explanation": "The reference article supports the idea that gene expression levels can be used to classify cell types. Excerpt 1 mentions that analyzing single-cell distributions provides important information about gene regulation, and Excerpt 2 notes that gene expression variability between cells within an individual is greater than between individuals. This suggests that gene expression profiles can be distinct for different cell types or states."
+}
+Note: The article focuses on the analysis of gene expression in single cells to associate genetic variants with gene-expression phenotypes, but it also touches upon the idea that gene expression levels can be used to distinguish between different cell types or states, which is relevant to the citation statement.</t>
+        </is>
+      </c>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
@@ -24363,7 +25526,14 @@
           <t>["R-d S$ pdL2s21.';,.S L R-P'd-R PdL2 II I (L = phosphine ligand; S = phosphine ligand or solvent; X = halogen.) Kuns i -2 demonstrate that a catalysed coupling can occur in the reverse sense ialkyl iodide/arylmagnesium) to the Kumada work3. B-Elimination is of course not possible here and for a higher iodide (Runs 3 -5), elevated temperatures were necessary (iiun 4), but the oxidative addition did occur in moderate yield 153:) and most importantly, even at these temperatures, no hexadecene derived from B-elimination was observed. ihie have already snown7 that the transition state for the formation of diorganopalladium intermediates (3) is susceptible to sieric inhibition and &lt;n accord with this, when the aryl Grignard reagent of Runs 3 -5 was replaced with a primary alkylmagnesium (Runs 6 -S), the yields improved to SC) -91 .", "The use of a Inore sterically demanding set-al&amp;ylmagnesium (Run 9j or set-alkyl iodide (iiun 10) gave sligi;tly reduced coupling yields (63 and 69. respectively) and the secondary -seconaarg coupling igun 11) even more so (37 ,). In this latter case, the product could have arisen from homo -coupling of the Grignard 8 reagent , but in the absence of added iodide (Run 12), no dic.yclohexyl was produced. In a control experiment in the absence of catalyst igun 5), no coupling products were detectable and the iodide was recovered unchanged. The use of 5 mole of catalyst appears to be optim:, and the yield did not improve on increasing the catalyst concentration to 10 . Palladium reactions are frequently highly chernoselective' and in exemplification of this, the extension of the coupling reaction to functionalised alkanes is in hand.\nTABLE Cross Coupling Reactions. a. 5. C. d. e. f. 9.", 'a. 5. C. d. e. f. 9.\n\nKm\n--1 2 3 4 5 6 7 8 9 10 11 12 _ 1 t , R\'MgBr T 4-tkoc6H4t.igar i-MeOC6H4MgSr 1-MeOC6H4MgBr 4-MeOC6H4MgBr Ph(CH213MgBr PhKH2)3MgBr PhKH2)3MgBr c-C6H,,MgBr n-C6H13MgBr :-C6H,,MgBr c-C6H,,I c-C6H,,MgBr Reactants -! R! Me1 Me1 "-C16H331 "\'C16H331 "\'c16H331 Et1 n-C6H,31 n-C6H131 IJ-C~H,~I c-C6H,,I __ cat.']</t>
         </is>
       </c>
-      <c r="AF163" t="inlineStr"/>
+      <c r="AF163" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article (14) primarily discusses the coupling of alkyl iodides with alkyl Grignard reagents using palladium catalysis, but does not mention copper as a catalyst. The citing article's statement about primary alkyl electrophiles being coupled with alkylmagnesium reagents in the presence of transition-metal catalysts such as copper is not supported by this reference."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
@@ -24504,7 +25674,18 @@
           <t>['IV. CONCLUSIONS\nIn this work we have presented an exhaustive analysis of the electronic and vibrational properties of I4 1 /amd hydrogen within the 400-600 GPa pressure range. Atomic metallic hydrogen in this phase shows a nearly freeelectron-like electronic band structure, where the opened band gaps can be explained even without the need of electron-electron interaction. The huge kinetic energy of the electrons due to the extremely high pressure plus their strong interaction with the bare nuclei makes the electron-electron interaction be irrelevant for the electronic structure. Nevertheless, the strong electronproton interaction creates a big electronic localization near the atomic nuclei. Consequently, the RPA dramatically fails when calculating the phonons of atomic hydrogen. In fact, the inclusion of exchange-correlation effects in the calculation of the electronic response to proton motion guarantees the dynamical stability of the structure. Despite anharmonicity modifies phonon frequencies up to approximately a 20%, for instance, lowering the energies of the transverse acoustic modes and hardening high-energy optical modes, it has a minor effect on superconductivity, only suppressing T c by a 6%.', '34.\n\nIII. RESULTS AND DISCUSSION\nA. Electronic structure Hydrogen, containing a single proton and an electron, is supposed to leave its common molecular nature under a sufficient high pressure to form a metal similar to the alkalies. In the high pressure limit the dominant electronic kinetic energy would be responsible for ending up with a free-electron-like metal. However, in the analyzed pressure range we are still close to the dissociation/metalization pressure  23  and the problem is not as simple as one could imagine a priori. Fig.  2a  shows the electronic band structure of I4 1 /amd hydrogen at 500 GPa. The bands present a huge dispersion, associated to the dominating kinetic term in the energies of the electronic states. The calculated band structure is not far from the free-electron approximation, the main difference being the band gaps opened at the border of the BZ and whenever band crossing occurs due to the interaction of the electrons with the proton lattice.', 'Nevertheless, the Lindhard RPA spectrum completely differs from the ab initio calculations. The intensity of the Kohn anomalies is much stronger and the transverse acoustic modes become unstable with imaginary frequencies. Therefore, even though the electronic band structure could be understood within the free-electron-like approximation, phonons seem to be far from this picture, contrary to the case of sodium  41, 46  . This fact also questions the stability of the I4 1 /amd tetragonal phase in the ultimate high-pressure limit where the electrons are expected to be free. If we split the dynamical matrix in the D p and D e terms, we note that each of them scales differently with the average inter-electronic distance parameter r s : D p always scales as r -3 s , while, in the Lindhard RPA, D e scales as r -2 s (r s + C), where C is always positive and of the order of unity. Therefore, in the very large pressure limit with small r s , the D p contribution is expected to dominate over the electronic contribution. In Fig.  4  we present the dispersion of the root of the eigenvalues of each contribution separately.']</t>
         </is>
       </c>
-      <c r="AF164" t="inlineStr"/>
+      <c r="AF164" t="inlineStr">
+        <is>
+          <t>Here is my evaluation:
+```
+{
+  "label": "Substantiated",
+  "explanation": "The reference article indeed shows that electrons in SMH are close to the free-electron limit, as stated by the citing article. The abstract mentions a 'band structure close to the free-electron-like limit', and Excerpt 1 further explains that the electronic band structure is 'nearly free-electron-like'. Additionally, Excerpt 2 shows that the calculated band structure at 500 GPa is 'not far from the free-electron approximation'. These statements support the claim made in the citing article."
+}
+```
+I chose "Substantiated" because the reference article consistently describes the electronic band structure of SMH as being close to the free-electron limit, which directly supports the statement made by the citing article.</t>
+        </is>
+      </c>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
@@ -24653,7 +25834,15 @@
           <t>['In addition to traditional boronate  [7] [8] [9] 11, [13] [14] [15] [17] [18] [19] [20] [21] 23, [25] [26] [27]  and boroxine  7, 10  linkages, hydrazone  12  , imine  16, 22  and squaraine  24  linkages have been developed for the solvothermal synthesis of COFs. Especially, covalent triazine frameworks synthesized by the trimerization of nitrile units under ionothermal conditions in the presence of molten salt such as ZnCl 2  [30] [31] [32] [33] [34]  or by microwave reaction  35  offer a molecular platform to construct carbon nitrideconjugated networks, which exhibit outstanding properties and functions. Exploration of new linkage and new reaction for the synthesis of COFs is a key to achieve the further advancement of functional porous materials.', 'We show that this fully p-conjugated COF is useful for high on-off ratio photoswitches and photovoltaic cells. Our COFs introduce a new strategy and direction in the quest for high-performance-conjugated polymers and may pave a way for innovations and applications in fields from organic electronics to energy storage, and fuel cells.\n\nResults\nSynthesis and characterization. Figure  1  shows the structure of a chemically stable, electronically p-conjugated COF (CS-COF; CS stands for conjugated and stable). We selected C 3 -symmetric triphenylene hexamine (TPHA)  57  and C 2 -symmetric tertbutylpyrene tetraone (PT)  58  as building blocks for the topological ring fusion reaction and prepared the crystalline phenazine-linked CS-COF in isolated yields of 86-90% under solvothermal conditions. The tert-butyl side groups in PT were employed for enhancing the solubility of monomer.', 'By virtue of their three-dimensional orderings at the atomic scale, 2D COFs have shown a great potential to perform core functions in organic electronics such as light emission  9, 10  , charge transfer and separation  23, 27  , and semiconduction  9, 10, 17, [19] [20] [21] 23, 26, 28, 29  . However, typical COFs lack intrasheet p-conjugation and chemical stability, which significantly limit their practical utility. To address this shortcoming, a chemically stable yet fully pconjugated COF is highly desirable. Such a framework with threedimensionally ordered chain alignment may provide a solution for the long-standing daunting challenges in semiconducting polymer technology  [36] [37] [38]  .']</t>
         </is>
       </c>
-      <c r="AF165" t="inlineStr"/>
+      <c r="AF165" t="inlineStr">
+        <is>
+          <t>Here is my evaluation of whether the reference article supports the citation statement:
+{
+"label": "Substantiated",
+"explanation": "The relevant part of the statement, '(iii) C=N_(aromatic) (triazine and phenazine)', is supported by Excerpt 1, which mentions 'covalent triazine frameworks' and 'phenazine-linked CS-COF', indicating that the reference article discusses these specific linkages in the context of COFs."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
@@ -24793,7 +25982,14 @@
           <t>['By comparing with the previous results, we reasoned that the point chirality of the ligand has been effectively transferred into the coordinating complex, and it resulted in an enantiomeric circular helicate with all metal centers featuring L-configuration.  [52] [53] [54] [55]  The obtained metallic helicates containing regular hexagonal entanglements should be ideal building blocks for the construction of molecular woven materials  [56] [57] [58]  with regular Kagome pattern  59  by having sufficient control of intermolecular connections.\n\nFormation of Star of David [2]catenate via covalent capture\nRing closure of L-[Ag 6 1 6 ](PF 6 ) 6 in the presence of Hoveyda-Grubbs 2 nd catalyst  60  was proven to be unsuccessful under several conditions, probably due to the sensitivity of silver complex toward chloride-substituted ruthenium catalyst.', '51  Different from Lehn-type helicates  49  which are hard to be functionalized, the introduction of well-developed CHIRAGENs  41, 42  may provide a general and efficient method in the construction of high-order knots and links with controlled chirality. The early example by von Zelewsky and co-workers presented a highly stereoselective self-assembly of a hexameric circular helicate by using pinene-bipyridine ligand (Figure  1B ). Both hexamer and tetramer were detected in solution using silver(I) template,  52, 53  whereas only hexamer was formed with copper(I) metal ions.  54  We envisage that this helicate provides an orderly hexagonal entanglement arrangement required for the formation of a Star of David catenane, the suitable alteration of this CHIRAGEN ligand would deliver the construction of the only L-enantiomer of a 6  2  1 link.', 'Multimetal-ion circular helicates have been proved to be effective scaffolds for assembly of a series of nanotopologies  34, 35  by regulating the shape, size, and strand connectivity.  [36] [37] [38] [39]  Since all metal centers feature same stereochemistry within the helicate (all L or D), it is obvious that both the helical chirality of the intermediate helicate and the topologically chirality of resulted topology are directly determined by the absolute configuration of the metal centers. A family of pyridine and bipyridine ligands with appended stereogenic centers developed by von Zelewsky and coworkers  40  has been termed chirality generators (CHIRAGENs) because these stereogenic centers can induce the chirality at metal coordination site in a highly stereoselective manner.  41, 42  Application of chirality transfer in metal-template synthesis\n\nTHE BIGGER PICTURE\nA plethora of strategies have been developed for the construction of molecular links since 1960; however, the highly stereoselective synthesis of inherently chiral links is still challenging.']</t>
         </is>
       </c>
-      <c r="AF166" t="inlineStr"/>
+      <c r="AF166" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Substantiated",
+  "explanation": "The reference article describes the synthesis of a complex interlocking molecule, specifically a Star of David catenane, using a hexameric circular helicate as a scaffold. The abstract and excerpts discuss the self-assembly of interwoven circular frameworks and their subsequent closure by covalent bond-forming reactions, which aligns with the statement about forming elaborate interlocking molecules."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
@@ -24933,7 +26129,14 @@
           <t>['Thus, it might be considered a subclass of crystal engineering. Research in the area of MOFs and, to a lesser extent, inorganic frameworks, has recently progressed far enough to provide examples which show the feasibility of the building-block approach and the scope of reticular synthesis. Here we take selected examples to highlight the ideas involved, with emphasis on our own work on MOFs in which structural and thermal stability characterization have been combined with in-depth studies of surface area and gas sorption capacities. The subject of metal-organic frameworks has a long history, however, so we begin by giving some perspectives on the field.\n\nPerspectives and challenges\nThe Cambridge Structure Database (CSD) documents the crystal structures of more than 11,000 extended metal-organic compounds in which a metal ion or cluster has been linked by an organic moiety in which the linking functionality is a cyanide, pyridyl, phosphate or carboxylate. Of these, nearly 3,000 compounds have threedimensional (3D) structures and about double that number have 2D structures.', "A lthough the synthesis of new materials has long been recognized as the most essential element in advancing technology, it generally remains more of an art than a science-in that the discovery of new compounds has mostly been serendipitous, using methods referred to by critics as 'shake and bake', 'mix and wait' and 'heat and beat'. For much of the twentieth century, this worked well for the synthesis of important solid-state materials, and we expect that it will continue to yield interesting compounds. However, it is becoming increasingly urgent to produce materials designed to perform highly specific and cooperative functions \n1, 2  . Recent extensive research into the design and synthesis of metalorganic frameworks (MOFs) has led to numerous practical and conceptual developments in that direction  [3] [4] [5] [6] [7]  . Specifically, the chemistry of MOFs has provided an extensive class of crystalline materials with high stability, tunable metrics, organic functionality, and porosity. Here we present some of the important developments that have shaped this rapidly growing field and propose a general conceptual framework, which serves as a useful tool in designing materials constructed from molecular building blocks.", "It is different from retrosynthesis of organic compounds  10  , because the structural integrity and rigidity of the building blocks in reticular synthesis remain unaltered throughout the construction process-an important aspect that could help to realize fully the benefits of design in crystalline solid-state frameworks. Similarly, reticular synthesis should be distinguished from supramolecular assembly  11  , because in the former, building blocks are linked by strong bonds throughout the crystal. In this context, it is worth noting that a plethora of extended structures successfully prepared by copolymerization of metal ions with organic links have been reported and reviewed under the rubric of 'crystal engineering', a term which has mutated somewhat over the years and which is now rather broadly defined  [12] [13] [14]  . We use the more precise term reticular synthesis (or chemistry) to describe the logical approach to the synthesis of robust materials with predesigned building blocks, extended structures, and properties. Thus, it might be considered a subclass of crystal engineering."]</t>
         </is>
       </c>
-      <c r="AF167" t="inlineStr"/>
+      <c r="AF167" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Substantiated",
+  "explanation": "The reference article supports the statement that reticular synthesis is a process for making covalent organic frameworks (COFs) with predetermined structures and properties. Excerpt 1 mentions 'stitching...molecular building blocks together' to form ordered frameworks, which aligns with the concept of COFs. Additionally, the abstract highlights the design and construction of crystalline solid-state materials using reticular synthesis."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
@@ -25073,7 +26276,14 @@
           <t>['This concept is gaining prominence in the field of cancer research, with several studies reporting the enrichment of quiescent cancer stem cells after chemotherapy. For example, slow-cycling glioblastoma cells survive temozolomide treatment  (Chen et al., 2012) . Accordingly, if cell subpopulations can act as major drivers for tumor maintenance and mediate universal therapeutic resistance, approaches that target this phenotype could increase the efficacy of treatment regimens and reduce the risk of melanoma relapses. We have recently demonstrated that, even within highly proliferative melanomas, there is a slow-cycling cell subpopulation that is identifiable by the expression of the histone 3 K4 demethylase JARID1B  (Roesch et al., 2005 (Roesch et al., , 2010)) .', 'JARID1B (KDM5B/ PLU-1/RBP2-H1) is a member of the highly conserved family of jumonji/ARID1 H3K4 demethylases, which are involved in tissue development, cancer, and stem cell biology  (Christensen et al., 2007; Dey et al., 2008; Yamane et al., 2007) . The JARID1B high slow-cycling subpopulation is required for the continuous tumor growth of melanoma; however, it does not follow a unidirectional cancer stem cell hierarchy. The JARID1B high phenotype is temporarily distinct, dynamic, and can be acquired depending on the microenvironmental context  (Roesch et al., 2010) . In this respect, another study indicates that other types of cancers, such as breast or lung cancer, also harbor populations of quiescent cells that are drug resistant and whose phenotypes can switch dynamically  (Sharma et al., 2010) .', "Interestingly, in the latter study, slow-cycling cells were characterized by the expression of the chromatin-remodeling factor JARID1A, a homolog of JARID1B. Considering JARID1B's role in continuous tumor maintenance  (Roesch et al., 2010) , we asked (1) whether the subpopulation of JARID1B high slow-cycling melanoma cells displays lower drug susceptibility compared to the bulk of tumor cells and (2) whether this resistant phenotype can be pharmacologically eradicated.\n\nRESULTS\n\n\nCytotoxic Treatment of Melanoma Cells Results in the Enrichment of a Surviving JARID1B high Slow-Cycling Subpopulation\nTo assess whether slow-cycling melanoma cells show differences in the therapeutic response compared to the rapidly prolif-erating bulk, we treated melanoma cultures with various anticancer drugs. To discriminate between slowly and rapidly cycling subpopulations, we used a JARID1B-promoter-EGFPreporter construct, as previously described  (Roesch et al., 2010) ."]</t>
         </is>
       </c>
-      <c r="AF168" t="inlineStr"/>
+      <c r="AF168" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Substantiated",
+  "explanation": "The reference article supports the claim that H3K4 demethylases (KDM5) enable melanoma cell lines to evade anti-proliferative therapies by adopting a slow-cycling persister state. The abstract and excerpts describe how treatment with various drugs leads to enrichment of slow-cycling, long-term tumor-maintaining melanoma cells expressing JARID1B/KDM5B/PLU-1, which is consistent with the citation statement."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
@@ -25213,7 +26423,14 @@
           <t>['T he dynamics of hot electrons, those with energies perhaps hundreds of times greater than the available thermal energy, is central to understanding the properties of many electronic devices. For example, they contribute to leakage currents across CMOS transistors and may fundamentally limit their downsizing \n[1] [2] [3]  and they are intrinsic to solar cells, where high energy photons generate hot electrons that consequently generate a photocurrent  [4] [5] [6]  . Hot electrons can also, for example, be induced through plasmonics  [7] [8] [9]  and offer a route to instigate non-thermal chemical reactions  10  . Hot electron charge transport is thus the subject of major scientific research, both experimentally and theoretically  [11] [12] [13] [14]  . But the experiments are constrained by the ultra-short lifetime of hot electrons, typically 100 fs or less, and hence their corresponding transport length-scale of a few nm (refs 15,16). Direct pump-probe measurements with ultra-fast lasers typically provide little or no spatial information.', '49) and for that found for carrier diffusion in single silicon core-shell nanowires of 35 cm 2 s À 1 (ref. 50). Figure  3b  presents the temperature dependence of the nonlocal length-scale l. As the lattice temperature increases so does the nonlocal manipulation range. This further conforms to the diffusive transport model which, unlike ballistic transport, should increase with increasing temperature. The relationship also demonstrates the connection between the temperature of the crystal lattice and the measured electron dynamics. Hot electrons undergo several scattering processes to bring them into eventual thermal equilibrium with a crystal lattice. Typically carrier-carrier and carrier-phonon scattering brings a population of hot carriers into a Fermi-Dirac distribution with some characteristic hot electron temperature T e within 10 s of fs (refs 43,51,52). We inject at currents of B100 pA and therefore have, on average, one-electron injected every 1 ns. Given the 180 fs lifetime of the electrons within the 2.0 eV state, we rule out carrier-carrier scattering. Further carrier-phonon scattering brings the mean energy of the electron distribution down to ultimately thermalize with the lattice.', 'In our case, this carrierphonon scattering appears to occur within the high-lying 2.0 eV state since we have a temperature dependence of the nonlocal range. Subsequent scattering, here in a time of 180 fs, removes the electron from this state to lower lying states. There is therefore a competition between electron-phonon scattering thermalizing the hot-electron within the 2.0 eV state and scattering that electron into a lower lying state. This will result in a dynamic quasi-equilibrated electron distribution within the 2.0 eV state. To gain an insight into this connection we present a simple model of the temperature dependence of the nonlocal effect in terms of a 2D random walk. The RMS of a 2D random walk can be equated to 2D diffusion by l ffiffiffiffi N p ¼ ffiffiffiffiffiffiffiffi 2Dt p ; where l is the random walk step length and N the number of steps. Hence our length-scale l ¼ l ffiffiffiffiffiffiffiffi ffi N=2 p .']</t>
         </is>
       </c>
-      <c r="AF169" t="inlineStr"/>
+      <c r="AF169" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article discusses hot electron dynamics, but it does not mention a specific time scale of picoseconds for energy loss to the lattice. Instead, it mentions an ultra-short lifetime of hot electrons typically 100 fs or less, which contradicts the statement in the citing article."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
@@ -25354,7 +26571,18 @@
           <t>['The major difficulty to distinguish the zero mode MF in vortex core is the tiny energy gap separating the conventional quasiparticle states, which is estimated to be , where is the superconducting gap, is the Fermi energy relative to the Dirac point of the TSS band  25  . For ~1 meV, ~100 meV, the mini-gap is ~0.01meV, which is much smaller than the present energy resolution (0.1meV) in STS. One way to increase the mini gap is to tune the Fermi level toward the Dirac point. However, in that case, the superconducting gap becomes very small and the transition temperature becomes very low due to weaker proximity effect, hence the observation of Majorana mode is also difficult. In this work, we show that the spatial distributions of the Majorana mode and the bound states of a vortex can be used to identify the MF by STM. heterostructure made by molecular beam epitaxy 26-27 .', 'Identical to their antiparticles, Majorana fermions (MF) were proposed in 1937 as an alternative to Dirac theory of ordinary fermions that carry opposite charge from their antiparticles \n4  . Neutrinos are the first candidate for MF in particle physics, but their Majorana status remains to be confirmed  5  . There are also proposals that quasiparticles in certain quantum condensed matter systems may be MFs. Examples include 5/2 fractional quantum Hall state, cold atoms and chiral p-wave superconductors  1, 2  . Experimental realization of MFs is of great significance in fundamental physics. MFs obey non-Abelian statistics, and thus can be used to develop topological quantum computation. The recent work by Fu and Kane predicted that MFs should be present as zero-energy bound state at vortex cores of an engineered heterostructure consisting of a normal s-wave superconductor (SC) and a topological insulator (TI)  3  . Cooper pairs are introduced via proximity effect to TI surface where spin and momentum are locked in the topological surface state (TSS) band  6, 7  .', 'The Majorana mode is then expected to enhance the zero bias LDOS within a range of spatial distance r ~ 40 nm away from the vortex core, hence to possibly shift the maximum of the LDOS from a finite energy to zero bias energy for small r. The large zero bias LDOS at small r of the MF mode should be the underlying physics for the deviation of the zero distance splitting behavior of the bound state as we observed. Our STM measurement has an energy resolution of about 0.2meV. The LDOS within this energy resolution is expected to be enhanced due to the MF mode. We may argue that the maximum of LDOS for a fixed r may shift towards lower energy and the energy shift is less for larger r. These may explain the basic feature in our observation of the finite-distance splitting. Note that the effect of the MF mode to the change of the LDOS in the vortex core depends on the relative weight of the MF mode. A systematic study of the LDOS of a vortex with both the bulk and Dirac surface states will require further study. In brief, we interpret the observation of finite-distance split pattern as a clear demonstration of the MF in the center area of the vortex.']</t>
         </is>
       </c>
-      <c r="AF170" t="inlineStr"/>
+      <c r="AF170" t="inlineStr">
+        <is>
+          <t>Here is my evaluation:
+```
+{
+  "label": "Substantiated",
+  "explanation": "The reference article provides evidence for the existence of Majorana fermions and their zero-energy bound state, which can be spectroscopically demonstrated by 'zero-bias conductance anomalies'. The abstract mentions that the unusual splitting behavior of the zero bias peak in local conductance could be due to the Majorana fermion zero mode. Excerpt 3 also suggests that the Majorana mode enhances the zero bias LDOS within a range of spatial distance away from the vortex core, which supports the idea of zero-bias conductance anomalies modulated by external fields."
+}
+```
+I chose "Substantiated" because the reference article provides experimental evidence and theoretical explanations for the existence of Majorana fermions and their zero-energy bound state, which is consistent with the citation statement. The abstract and excerpts also discuss the concept of zero-bias conductance anomalies, which supports the claim made in the citation statement.</t>
+        </is>
+      </c>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
@@ -25496,7 +26724,14 @@
           <t>['2013; Kyutoku et al. 2015; Sekiguchi et al. 2016)  suggest that mergers dynamically eject between ∼10 -4 and a few ×10 -2 \uf065 M of material, with bulk velocities of a few tenths the speed of light. Additional material (∼10 -3 -10 -2 \uf065 M ) can exit the system at slightly lower velocities ( c c 0.05 0.1 -) as a wind from an accretion torus  (Fernández &amp; Metzger 2013; Perego et al. 2014; Fernández et al. 2015; Just et al. 2015) . We adopt as our fiducial model a system with M ej \uf0a0=\uf0a05\uf0a0×\uf0a010 -3 \uf0a0 \uf065 M and v ej \uf0a0=\uf0a00.2c, where v ej is defined in terms of the explosion kinetic energy, = E M v 2 k e j ej 2 .', 'Accounting for time-dependent thermalization efficiencies has a significant impact on kilonova luminosity, particularly for models with lower masses and higher velocities. For our fiducial model, the predicted luminosity is lower by a factor of \uf0882 at peak, and by 10 days is lower by an factor of 5. 18. Select broadband light curves for our fiducial ejecta model for two treatments of thermalization: full f t tot ( ) (left panel), and the cruder treatment employed in earlier kilonova calculations (right panel). The curves are dimmer in the newer models, reflecting the reduction in thermalized energy, but relationships between the light curves in the various bands is mostly unchanged, so the kilonova colors are preserved. Figure  19 . Absolute (AB) J-band light curves for several ejecta models. As in earlier figures, the width of the curves is produced by differences in f t tot ( ) due to different magnetic field configurations. The excess IR flux (gold star) suggests an ejected mass between ´-5 10 2 and -\uf065 M 10 1 . fairly efficiently out to late times.', 'Since denser ejecta configurations thermalize more efficiently than diffuse systems, we vary these parameters over the ranges Î - -\uf065 M M 10 , 5 10 ej 3 2 [ ] and Î v c 0.1, 0.3 ej [ ]. We assume the ejecta is spherical and expanding homologously, and that the density profile follows a broken power law, declining with velocity coordinate = v r t as d v in the inner regions of the ejecta, and d &gt; - v n , n , in the outer regions. We set δ\uf0a0=\uf0a01 and n\uf0a0=\uf0a010.  Barnes &amp; Kasen (2013)  provides a complete mathematical description of the density profile.\n\nMagnetic Fields\nKilonova ejecta contain a residual magnetic field, either inherited directly from the parent NSs, or seeded by amplified fields produced by turbulence during the merger or in the resultant accretion disk  (Kiuchi et al. 2014 (Kiuchi et al. , 2015)) . Though weakened by expansion, the fields remain strong enough to influence charged particle motion.']</t>
         </is>
       </c>
-      <c r="AF171" t="inlineStr"/>
+      <c r="AF171" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Unsubstantiated",
+  "explanation": "The statement mentions a specific ejecta mass (M_ej = 0.05 M_☉) and velocity (v_ej = 0.1c), but the reference article does not provide evidence to support these exact values. The excerpts mention different fiducial model parameters (e.g., M_ej = 5 × 10^-3 ε M, v_ej = 0.2c) and discuss varying ejecta masses and velocities over certain ranges, but do not specify the values mentioned in the citation statement."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
@@ -25636,7 +26871,18 @@
           <t>['In conclusion, our study established correlations between the Cu and ZnO particle size and morphology,t he reaction mechanism, and the activity of acommercial Cu-ZnO-Al 2 O 3 catalyst upon methanol synthesis under various gas compositions and industrial conditions.O perando SXRPD elucidated that Cu particles retained their cuboctahedral shape but sintered under CO/H 2 and CO 2 /H 2 .T his phenomenon was associated with the segregation of Cu from ZnO upon CO hydrogenation and with the presence of H 2 Ou pon CO 2 hydrogenation. With respect to the hexagonal ZnO particles, aC O/H 2 atmosphere did not provoke significant alterations but growth and formation of platelet-like morphologies were observed under CO 2 /H 2 .S ince CO 2 hydrogenation was only slightly improved over smaller Cu particles and was insensitive to the morphology of ZnO,wededuced that this reaction cannot become al imiting step for the promotional effect.', 'In the CO/CO 2 /H 2 mixture with the optimal CO 2 concentration, the low amount of H 2 Of ormed prevented Cu and ZnO sintering.M oreover,t he ZnO prism-like crystallites preferentially elongated along their hexagonal axis.M E-DRIFTS during reaction evidenced astrong suppression of the RWGS in catalyst samples containing platelet-like ZnO particles.The higher amount of polar facets in these structures leads to enhanced electronic interactions with Cu, which inhibit the active sites on the latter. In contrast, the preferred elongation of ZnO under the optimal gas mixture augmented the fraction of non-polar facets exposed, boosting the WGS reaction and, thus,t he MeOH formation from CO 2 .T hese findings rationalize the promotional effect and indicate that the best catalyst structure for CO 2 -promoted MeOH synthesis comprises small Cu particles in contact with rod-like ZnO crystallites, preferably stabilized by structural promoters.', '[4]  Thel atter is much faster than the hydrogenation of CO but strongly limited by thermodynamics and product inhibition by H 2 Oa th igh CO 2 concentrations resulting in the typical volcano plot shown in Figure  1 (described later). Klier et al.  [3a]  speculated that an optimal oxidation state of Cu, i.e., partially oxidized, correlates with the top of the curve.This hypothesis has never been confirmed for commercial catalysts under reaction conditions and neglects the essential role of ZnO uncovered in the CO 2 promotion.  [3b]  Multiple studies have revealed that zinc oxide strongly influences the CO 2 hydrogenation, acting as as tructural and electronic promoter for Cu.  [5]  As indicated recently,t his reaction appears to be favored over the reverse water-gas shift (RWGS) on ac omposite obtained by mechanical mixing of large particles of Cu and Al 2 O 3 with ZnO in aplate-like shape with respect to the case of am ixture containing rod-like ZnO crystallites,  [5d]  based on the stronger electronic interactions between ZnO and Cu in the former catalyst.']</t>
         </is>
       </c>
-      <c r="AF172" t="inlineStr"/>
+      <c r="AF172" t="inlineStr">
+        <is>
+          <t>Here is my evaluation:
+```json
+{
+  "label": "Substantiated",
+  "explanation": "The reference article discusses the role of ZnO as a structural modifier and promoter for bond activation, which aligns with the citation statement. Excerpts 1-3 highlight the interactions between Cu and ZnO particles, morphology changes under different gas compositions, and the promotional effect of ZnO on methanol synthesis."
+}
+```
+I chose "Substantiated" because the reference article provides evidence that ZnO plays a crucial role in modifying the structure and promoting bond activation, which is consistent with the citation statement. The excerpts demonstrate the complex interactions between Cu and ZnO particles, and how these interactions influence the reaction mechanism and activity of the catalyst.</t>
+        </is>
+      </c>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
@@ -25772,7 +27018,14 @@
           <t>['249  This also clearly indicates a potential advantage of MOFs in dehumidification applications over commonly used adsorbents. Guo et al. further underlined this potential. They claimed, based on an array of different MOFs in comparison with alumina, their industrial adsorbent of choice for dehumidification, that all MOFs have superior total capacities, and some also display superior breakthrough behavior, and thus faster kinetics.  454  In addition, cyclic regeneration for MOFs can be achieved with significantly less energy (lower T des ), all in line with preceding findings (desiccant, AHP/AC).  454  \n\nSUMMARY AND FUTURE PERSPECTIVES\n8.1. Summary The potential of MOFs as adsorbents in adsorption-driven allocation of heat and cold has been thoroughly assessed in this Review. The adsorption mechanism of water on MOFs is known. Water initially adsorbs at specific hydrophilic sites (uncoordinated metal sites, OH-groups on inorganic clusters, or functional groups on the organic ligand).', '[61] [62] [63] [64] [65]  No wonder that MOFs have received attention for application in, for example, adsorption/separation,  [66] [67] [68] [69]  storage,  70, 71  and catalysis.  [72] [73] [74] [75]  In the first part of this Review, we summarize the state of the art in MOF science with regard to stability and adsorption behavior for the aforementioned working fluids. To be able to understand, and to possibly tune, the adsorption of vapors in MOFs, one should have insight into the mechanism of adsorption. This will be described first concerning the experimental and simulation point of view (section 2). Of the utmost importance for the targeted application is further knowledge about the solvothermal (in)stability, as will be discussed second in a clear and concise manner (section 3). Subsequently, an overview of known adsorption behavior (section 4) results in a selection of the most promising MOFs in section 5.', 'For successful application, however, also the dynamics of the MOF-working fluid pair are important. The latter depends heavily on the macroscopic structure of the MOF chosen in the heat exchange application. Furthermore, MOFs are commonly synthesized and characterized on the (sub)gram scale, while actual heat pumps contain adsorbent material in the order of kilograms. To help put things into perspective, seven subsequent stages are defined that will eventually lead to application. Stage 0 -Stability: As the primary requirement, MOFs should be tolerant toward the working fluid of choice. This should be ensured before anything else. Stage 1 -Adsorptive properties: On the basis of primary vapor adsorption measurement(s), the shape of an isotherm can be envisaged. From this the initial feasibility can be assessed.']</t>
         </is>
       </c>
-      <c r="AF173" t="inlineStr"/>
+      <c r="AF173" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Substantiated",
+  "explanation": "The reference article discusses the potential of MOFs in heat pump applications, which supports the citing article's statement about considering MOFs for heat pumps [17, 18]. The provided excerpts focus on the adsorption mechanism and properties of MOFs, highlighting their suitability for heat exchange applications."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
@@ -25908,7 +27161,14 @@
           <t>['Among the existing classes of porous solids, crystalline metal-organic frameworks (MOFs)  [2]  are currently of great interest and importance due to their novel coordination structures, diverse topologies, and potential applications in the field of separation, gas storage, catalysis, or biomedical applications.  [3]  In spite of versatile advantages of porous MOFs, which include tailor-made pore structures and controllable porosity by change of organic ligands and metal subunits,  [2]  most MOFs suffer from a lack of hydrothermal stability.  [4]  Structural damage to a MOF caused by moisture at processing conditions or during regeneration will strongly limit the utilization of a MOF as a sorbent for industrial applications.  [4]  Conversely, highly porous MOFs with good hydrothermal stability represent candidates for industrially useful water sorbents.', 'Cubic mesoporous metal(III) di-or tri-carboxylates with hierachical pore structures labeled MIL-101(Cr), MIL-100(Fe), MIL-100(Cr), and MIL-100(Al) (MIL stands for Materials of Institut Lavoisier) using trivalent octahedral metals and the simplest aromatic carboxylates such as terepthalate and trimesate have been discovered.  [5, 6]  Based on this requirement, the exceptional hydrothermal stability and large sorption uptakes known for MIL-101 and MIL-100 encouraged us to assess their applicability for water sorption applications.  [5, 6]  Despite studies done on water adsorption in MOFs,  [7]  reports dealing with MOFs as water adsorbents are still scarce  [8]  and there is a particular need to evaluate their low temperature desorption properties, i.e., below 80 °C for application to energy-efficient dehumidication systems.', 'This suggests that most of the water molecules are physisorbed on MIL-101(Cr) and MIL-100(Fe) with a low host-guest interaction (close to the energy of liquefaction) except for the coordinated water molecules, allowing for the low-temperature desorption of water.  designed for a prototype simulation of a household desiccanttype dehumidifier than that with a zeolite rotor, which is commercially available. The detailed results will be published elsewhere. In conclusion, we have unambiguously demonstrated that hierarchically porous metal-organic frameworks, MIL-100 and MIL-101 with mesoporous cages behave as advanced water adsorbents applicable to energy-efficient dehumidification. Elaborate investigations of their water sorption properties have shown huge sorption uptakes even at 40 °C as well as high desorption rates below 80 °C together with hydrothermal stability. In comparison with the water sorption behaviors of commercial adsorbents such as zeolite NaX, SAPO-34, and silica gel, the improved performance in MIL-100 and MIL-101 demonstrated here suggests commercially viable applications including energyefficient desiccant dehumidification and fresh water production.']</t>
         </is>
       </c>
-      <c r="AF174" t="inlineStr"/>
+      <c r="AF174" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Substantiated",
+  "explanation": "The reference article [19] explicitly discusses the use of MOFs for dehumidification, presenting MIL-100 and MIL-101 as advanced water adsorbents with high sorption uptakes and hydrothermal stability. This supports the citing article's statement that MOFs have been considered for dehumidification."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="175">
       <c r="A175" t="inlineStr">
@@ -26048,7 +27308,14 @@
           <t>["2c , dendrite #1), while others disappeared (Fig.  2c , dendrites #2 and #3). Importantly, the structural potentiation and AS-PaRac1 labelling triggered during the 'Learning' period were more likely to be preserved than those triggered during the training-free period (Fig.  2j , 'Before' and 'After-1'). Consistently, longitudinal imaging of the structurally potentiated spines revealed that the majority of those with the retention of AS-PaRac1 for 24 h maintained structural potentiation for at least 48 h (Fig.  2k , green trace), while the structurally potentiated spines lacking AS-PaRac1 retention returned to the pre-potentiated state (Fig.  2k , black trace). Such AS-PaRac1 retention might be maintained by reverberation of learning-activated neuronal circuits, because AS-PaRac1 was only expressed in Arc-expressing neurons, in which the persistent activation helps to maintain plastic changes in the neocortex  26, 37  .", '5f-h ,  l ,  n ), while re-potentiation was significantly less prominent in mice that did not perform the retraining task (home cage group) (Fig.  5i-k ,  l , n; Extended Data Fig.  7d ,  e ). Furthermore, newly potentiated spines, which were not potentiated in the first 2 days, were less abundant in the re-training and home cage groups compared with the dual task group (yellow, Fig.  5m ,  n ). These findings suggest that reorganisation of distinct synaptic ensembles is specific for each learning task.\n\nDiscussion\nCurrent models of learning and memory suggest that structural plasticity of spines is the underlying mechanism of information storage in the brain. Nonetheless, clear visualization of spine structure in vivo requires the sparse labelling of neurons, and analysis of structural changes in spines is considerably laborious. In contrast, the AS-PaRac1 signal appears as fluorescence puncta, which allows the detection of potentiated spines far more easily, even at high transfection condition. Moreover, the role of potentiated spines can be directly assessed with PA during behavioural examinations.', "2a-e ). Consistent with previous findings  33, 34  , even in the training-free period, a substantial number of spines 'spontaneously' underwent structural potentiation (formation or enlargement of spines; see the definition in Extended Data Fig.  4a ), but the trained mice exhibited significantly more structural potentiation compared with the non-trained mice (Fig.  2d ). Notably, synaptic fluorescence of AS-PaRac1 just after training (0 day) strongly correlated with the change in spine size upon training (Fig.  2f ). It is unlikely that the accumulation of AS-PaRac1 caused the potentiation or labelled the spines primed for potentiation such as for the 'tagged synapse'  35, 36  , because the initial quantity of AS-PaRac1 before learning (-1 day) did not correlate with the change in spine size after learning (Fig.  2g ). Analysis of AS-PaRac1 puncta in the dendritic shaft suggested that the majority of AS-PaRac1 signal was located in the dendritic spines, and the labelling of shaft synapses was negligible (Extended Data Fig."]</t>
         </is>
       </c>
-      <c r="AF175" t="inlineStr"/>
+      <c r="AF175" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article does not mention a positive correlation between dendritic spine density on memory engram cells and memory expression triggered by natural recall cues. Instead, it discusses the relationship between synaptic plasticity, dendritic spines, and motor learning tasks, without addressing the specific topic of memory engram cells or natural recall cues."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr">
@@ -26188,7 +27455,14 @@
           <t>['23, 24  In conclusion, we have shown that conductive nitrogendoped carbon is applicable as an efficient, metal-free catalyst for the selective, green, and cheap electrochemical production of hydrogen peroxide. Besides being easy and cheap, the catalyst synthesis is flexible enough to allow further optimization of the porosity and surface area. To date, the true dependence of the structure on the reactivity remains unclear, and further investigations are needed. However, as a comparable material synthesized at higher temperatures (1000 °C) supports the four-electron process, certain assumptions can be made: (1) Consistent with simulations of Okamoto,  22  an increased nitrogen content may favor the two-electron process. (2) The "radical" character of nitrogen-bound carbon, which is essential for the two-electron process,  21  may be more pronounced for meso-BMP-800 because of the lower degree of delocalization. (3) The pyrrolic nitrogen sites within the carbon material elucidated by highresolution XPS, which are not present at higher synthesis temperatures, might indeed contribute in an essential way to the activity of the two-electron process.', 'H ydrogen peroxide is one of the 100 most important chemicals in the world. \n1  The most elegant and efficient reaction pathway would be the direct conversion of elemental hydrogen and oxygen.  2  However, such a process creates the danger of explosion. Electrochemical flow reactors, such as the polymer electrolyte membrane fuel cell (PEMFC), represent an attractive alternative by separating oxygen reduction and hydrogen oxidation under cogeneration of energy.  3, 4  Therefore continuous research on improving the electrochemical synthesis of hydrogen peroxide is carried out,  [5] [6] [7] [8] [9] [10] [11] [12]  but electrocatalysts still suffer from high costs, limited selectivity or low activity. We herein show ionic liquid-derived mesoporous nitrogen-doped carbon to be a highly active, cheap, and selective metal-free catalyst for the electrochemical synthesis of hydrogen peroxide with the potential to establish a safe, sustainable, and cheap flow-reactor-based production method.', 'Additionally, the method is very inexpensive (regarding electricity 2.4 EUR cents kg H 2 O 2 -1 at 10 EUR cents kWh -1 industry price), while costs for the transport of liquid hazardous H 2 O 2 could be avoided. As such, precise attribution of the catalytic activity to a specific binding site seems rather speculative. Besides the importance of an increased nitrogen content retaining sufficient conductivity (see ref 22), another possible factor affecting the reactivity is the degree of graphitization. Here, the polarizability of the graphitic layers should influence the adsorption properties, while the elongation of the conjugated π system could determine crucial electronic properties. As the radical character of nitrogen-bound carbon may support the two-electron process, less-conjugated π systems should be more favored for hydrogen peroxide synthesis.  21  However, nitrogen-doped carbon materials have also received great attention as support materials for metal and metal alloy catalysts, for example, in the methanol oxidation reaction or oxygen reduction to water.']</t>
         </is>
       </c>
-      <c r="AF176" t="inlineStr"/>
+      <c r="AF176" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article actually highlights the potential of nitrogen-doped carbon as a 'highly active, cheap, and selective metal-free catalyst' for hydrogen peroxide production, contradicting the citing article's claim that it only exhibits modest performance."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="177">
       <c r="A177" t="inlineStr">
@@ -26328,7 +27602,14 @@
           <t>['A second type of inactivation process, usually with significantly slower kinetics, has been observed in a number of channels  (9) (10) (11) . This type of inactivation is called C-type or slow inactivation, with yet a third inactivation process (P-type) also recognized in potassium channels  (12) . Although the detailed mechanisms of slow inactivation processes are incompletely understood, it is believed that rearrangement of the pore, rather than motion of a cytoplasmic region of the channel, is likely to play a central role  (13) (14) (15) . The importance of better understanding of slow inactivation in sodium voltage-gated channels is evident since its alteration is linked to such clinical disorders as periodic paralysis, myotonia, idiopathic ventricular fibrillation, and long-QT syndrome, as recently reviewed by  Vilin and  Ruben  (16) . The prokaryotic voltage-gated sodium channel (NaCh-Bac) shows homology with eukaryotic voltage-gated channels though its sequence shows closer similarity with calcium channels than with sodium channels  (17) .', "INTRODUCTION\nOne of the common properties of voltage-gated channels is their ability to inactivate in response to membrane depolarization. Two general mechanisms of inactivation have been characterized. The first mechanism is usually typified by relatively fast inactivation during a sustained depolarization, effected at the molecular level by a ''ball and chain''  (1) (2) (3) (4) (5)  or ''hinged-lid'' mechanism  (6) . Molecular mechanisms of this type of inactivation, called N-type inactivation, have been studied in detail in K and Na channels. The groups responsible for this type of inactivation are localized at the cytoplasmic side of the channel. For example, in Shaker K-channel, the N-terminal region of the channel plays the role of the ''ball'', which occludes the inner part of the pore after channel activation and thus closes the channel  (7) . A similar mechanism has been described for Na channels. In this case channel block is probably provided by the III-IV interdomain linker latched by a triplet of hydrophobic residues (IFM motif) to form a hinged lid  (8) .", 'Using tandem-linked dimers and tetramers, we did not detect any significant difference between inactivation of wild-type channel and the tandem concatemers. Hence, we conclude that, in contrast to N-type inactivation in eukaryotic channels, NaChBac inactivation does not involve either N-or C-terminal cytoplasmic regions of the WT monomer. Slow inactivation in sodium channels may involve a mechanism similar to that of C-type inactivation in potassium channels  (42) . C-type inactivation usually has slower kinetics than N-type and is sensitive to the mutations in the pore region. Similarly, in sodium channels, mutations that change the charge of groups located at the outer side of the selectivity filter change slow-inactivation kinetics  (43) (44) (45) (46) . For example, it was shown that, for the rat skeletal muscle sodium channel, substitution of a negatively charged residue (aspartate) for the alanine at position 1529 of domain IV in the selectivity filter favors ultraslow inactivation  (47) .']</t>
         </is>
       </c>
-      <c r="AF177" t="inlineStr"/>
+      <c r="AF177" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Substantiated",
+  "explanation": "The reference article supports the statement that slow inactivation may involve a conformational change of the selectivity filter. Excerpt 1 mentions that rearrangement of the pore is likely to play a central role in slow inactivation, and Excerpt 3 states that mutations changing the charge of groups located at the outer side of the selectivity filter can alter slow-inactivation kinetics."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="178">
       <c r="A178" t="inlineStr">
@@ -26468,7 +27749,18 @@
           <t>['For the case of the electron-injecting oxide system, except for the TiO 2 nanoparticles, one-dimensional TiO 2  [9] [10] [11]  and ZnO 12,13 were investigated. Although electron transport in ZnO was observed to be faster than that in TiO 2 ,  13  photovoltaic performances of ZnO nanorod-based perovskite solar cells were inferior to those of TiO 2 nanorod-based solar cells. This might be due to nonoptimized ZnO nanorods. Here, we report high-efficiency ZnO nanorod-based perovskite solar cells. Diameter and length of the solution-grown ZnO nanorods are controlled by varying the solution concentration and immersion time. PCE of 11.13% is achieved using 1 μm long ZnO nanorods (diameter of about 80 nm) in the absence of a compact TiO 2 blocking layer. The photovoltaic performance, especially external quantum efficiency (EQE) spectral response is compared between ZnO nanorods and TiO 2 nanorods.', 'Length of the solution-grown TiO 2 nanorods is about 1 μm, and their width is 80-90 nm, as can be seen in Figure  9e . TiO 2 compact layer is clearly seen between TiO 2 nanorods and FTO. A thin spiro-MeOTAD HTM layer is formed over the TiO 2 nanorod film (Figure  9f ). Two-step spin coating of PbI 2 and CH 3 NH 3 I in the 1 μm long TiO 2 nanorod film results in J sc of 20.92 mA/cm 2 , V oc of 869 mV, FF of 0.55, and PCE of 10.02%, which is higher than the previous result for the similar TiO 2 length 9 because of the different coating procedure for the perovskite as mentioned previously. Compared to the ZnO  nanorod, the slightly lower PCE is due to lower V oc , associated with lower conduction band position for the rutile TiO 2 structure and/or enhanced recombination.', '3  It was also confirmed that the perovskite solar cell could work well even without a mesoporous TiO 2 film, where a thin, continuous CH 3 NH 3 PbI 2 Cl layer formed on the Al 2 O 3 surface showed a PCE of 10.9%.  4  Recent progress pushed PCE of perovskite solar cell up to 15%.  5, 6  Thanks to the high open-circuit voltage V oc of perovskite solar cell exceeding 1 V, a PCE of 20% is predicted from perovskite solar cell,  7, 8  which indicates that organometal halide perovskite is a very promising solar cell material. There are two branches in developing perovskite solar cell; one is based on electron-injecting nanostructured oxide layer, and the other is based on nonelectron-injecting scaffold layer (meso-superstructure) or pn junction type planar structure.']</t>
         </is>
       </c>
-      <c r="AF178" t="inlineStr"/>
+      <c r="AF178" t="inlineStr">
+        <is>
+          <t>Here is my evaluation of the reference article:
+```
+{
+  "label": "Substantiated",
+  "explanation": "The reference article supports the use of ZnO as an alternative oxide material to TiO2 in perovskite solar cells, reporting a power conversion efficiency of 11.13% with ZnO nanorods and comparing its performance to that of TiO2 nanorods."
+}
+```
+I classified this as "Substantiated" because the reference article explicitly discusses the use of ZnO as an electron-injecting oxide material in perovskite solar cells, which aligns with the citing statement. The article also presents data comparing the performance of ZnO nanorods to TiO2 nanorods, which further supports the claim.</t>
+        </is>
+      </c>
     </row>
     <row r="179">
       <c r="A179" t="inlineStr">
@@ -26608,7 +27900,14 @@
           <t>['T he challenge of converting natural gas into transportable fuels and chemicals (1) has been spurred by several emerging industrial trends, including rapidly rising demand for H 2 (for upgrading lower-quality oils) and a global shortage of aromatics caused by shifting refinery targets toward gasoline. Light olefins, which are key chemical feedstocks, are currently made from methanol, which itself is made through multistage catalytic transformations via syngas (a mixture of H 2 and CO) \n(2, 3) , although there is also ongoing research to convert syngas directly to light olefins  (4, 5) . However, in all such approaches, either CO or H 2 is needed to remove oxygen from CO, resulting in a carbon-atom utilization efficiency below 50%. Despite their low efficiency, high capital and production costs, and enormous CO 2 emissions, syngas routes dominate current and near-term industrial practices for natural gas conversion (6, 7).', 'Direct conversion of CH 4 is potentially more economical and environmentally friendly but is challenging because CH 4 exhibits high C-H bond strength (434 kJ/mol), negligible electron affinity, large ionization energy, and low polarizability  (8) . In the pioneering work of Keller and Bhasin in the early 1980s, CH 4 was activated with the assistance of oxygen  (9) . This finding initiated a worldwide research surge to explore the high-temperature (&gt;1073 K) oxidative coupling of methane (OCM) to C 2 hydrocarbons  (10, 11) . Hundreds of catalytic materials have since been synthesized and tested, principally during the 1990s, as well as in recent years. Unfortunately, the presence of O 2 leads irreversibly to overoxidation, resulting in a large amount of the thermodynamically stable endproducts CO 2 and H 2 O. Thus, the carbon utilization efficiency of OCM remains relatively low  (12, 13) . Slow progress in discovering new catalysts to circumvent this problem has hindered further development, and no economically viable process has been put into practice so far.', 'By comparison, the catalytically initiated reaction described here compares very favorably with other reported direct-conversion processes, including pyrolysis, OCM  (13) , and nonoxidative aromatization  (21) . Finally, because natural gas usually contains some ethane, we added 1 and 5 vol % ethane to the reactant stream. The presence of ethane substantially enhanced methane conversion (fig.  S2 ) (  22 ), and ethane is almost completely converted, although a small amount of coke is formed at 1173 K and a space velocity of 4.84 liter gcat -1 h -1 . The unprecedented efficiency of the catalytically initiated CH 4 conversion process is attributed to the high activity of the coordinatively unsaturated iron sites toward the C-H bond of CH 4  (28, 29) . The isolated nature of these sites, as evidenced by sub-angstrom-resolution high-angle annular-dark field (HAADF) scanning transmission electron microscopy (STEM) and in situ x-ray absorption near-edge spectroscopy (XANES), precludes surface C-C coupling and, hence, coke formation.']</t>
         </is>
       </c>
-      <c r="AF179" t="inlineStr"/>
+      <c r="AF179" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article does not mention the development of efficient methods for converting methane into commodity chemicals and liquid fuels as a response to its surge as a potent greenhouse gas. Instead, it focuses on a direct, nonoxidative conversion process of methane to ethylene, aromatics, and hydrogen using single iron sites embedded in a silica matrix."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="180">
       <c r="A180" t="inlineStr">
@@ -26751,7 +28050,14 @@
           <t>['However, recent data have shown that RhoB expression is induced under conditions such as DNA damage, or treatment with growth factors or cytokines, suggesting that under particular circumstances, RhoB may favor towards human malignancy, including glioblastoma tumors  [65, 66] . In the present study, we show that when RhoB is silenced, both parental and their derivative-IE1 cells show a reduction in spread area compared to the RhoA or RhoC knockdown cells, an effect which has attributed to subsequent reduction of total surface levels of b1 integrin  [67, 68] . Moreover, in the presence of HCMV, an increased number of cellular projections was formed, a phenomenon which has also been observed in HCMV infected primary HFF cells, particularly at the late stages of lytic infection  [49] . These findings further corroborate the idea of a key role for RhoB in the regulation of cell shape.', 'Foremost, we observed that knockdown of RhoA resulted in an elongated cell shape with thin protrusions in non-infected and HCMV infected U373MG as well as in their derivative U373MG-IE1 cells. Likewise, depletion of RhoC led the cells to obtain an elongated, mesenchymal-like shape. The above observations are consistent with earlier studies depleting the same Rho isoforms both in prostate and breast cancer cells  [59, 62] . The overexpression of HCMV IE1 protein alone did not bring about any additional effect regarding the phenotype of the Rho knockdown cells, thus excluding any direct modulatory role of IE1 on cell morphology. The morphological changes induced in the glioblastoma cells after RhoA and RhoC depletion remained evident, even in the context of HCMV infection, despite the cytopathic effect caused by the virus, highlighting an imposing role Rho GTPases on cell shape. Although Rho GTPases have been shown to enhance malignant transformation and proliferation rate, RhoB is rather assumed as a negative regulator of these processes  [63, 64] .', 'Regarding to the proliferation rate of uninfected parental and IE1-expressing glioblastoma cells, the deficiency of RhoB or RhoC resulted in a significant inhibition of their proliferation state while RhoA deficiency reduced the cell growth of both U373MG and U373MG-IE1 cells to a lower degree. This difference reflects the evidence that RhoA regulates actin polymerization, cell adhesion and myosin activity  [7, 69]  whereas RhoB and RhoC control cell survival and cell proliferation, respectively  [70] . This concept is furthermore supported by our observation that HCMV infection of U373MG and U373MG-IE1 RhoA depleted cells does not seem to affect significantly their proliferation rate, whereas the proliferation state of the HCMV infected of both parental and U373MG-IE1 RhoB or RhoC knockdown cells is statistically significantly inhibited. HCMV infection has been involved in human tumors influencing cell properties such as migration, invasion or cell signaling  [31, 32, 71] .']</t>
         </is>
       </c>
-      <c r="AF180" t="inlineStr"/>
+      <c r="AF180" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Substantiated",
+  "explanation": "The reference article [19] supports the statement that RHOC is a well-known regulator of cell shape and motility. Excerpts 1 and 2 describe how RhoC, along with other Rho GTPases, play a crucial role in regulating cell morphology, particularly in glioblastoma cells. The study's findings on the effects of RhoC depletion on cell shape and migration rate provide evidence for RHOC's regulatory function."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="181">
       <c r="A181" t="inlineStr">
@@ -26891,7 +28197,17 @@
           <t>['S5 ). To directly assess the impact of the reported nano-/microscale morphologies on the charge transport properties of the P(NDI2OD-T2)/PS blend, we fabricated top-gate/bottom-contact OFETs. A detailed description of the fabrication process is given in Materials and Methods. It should be noted that P(NDI2OD-T2) is a typical high-mobility n-type semiconductor with a low degree of energetic disorder (32) and both theoretical and experimental studies have shown intrinsically unbalanced electron and hole transport properties in low (i.e., diodes) and high (i.e., OFETs) charge density regimes  (33) . However, when fluorinated, high-k gate polymers are used as a dielectric insulator, both electrons and holes can be accumulated in the channel, leading to balanced ambipolarity  (34, 35) . The dielectric used here is a 600-nm-thick poly(trifluoroethylene) (PTrFE) film.', 'This observation is confirmed by depth-dependent X-ray photoelectron spectroscopy measurements which show the concentrations of nitrogen, oxygen, and sulfur [elements found in P(NDI2OD-T2)] to be enriched near the surface of the film (Fig.  S4 ). Such vertical phase separation featuring a P(NDI2OD-T2)-rich top layer and a bottom interface primarily composed of PS is attributed to the different surface energies of P(NDI2OD-T2) and PS. Indeed, P(NDI2OD-T2) with a low surface energy (23.7 mJ•m -2 ; ref.  23)  tends to segregate at the air/film interface, whereas PS with higher surface energy (40.2 mJ•m -2 ; ref. 27) prefers the SiO 2 surface. A similar surface-induced phase separation is typically reported for other semiconductor/insulator polymer blends  (28) (29) (30) . A characteristic single-phase morphology with randomly oriented crystalline grains on the order of 10-30 nm is observed in neat films of P(NDI2OD-T2) (Fig.  3A  and Fig.', 'The successful integration of these properties correlates with the remarkable transport properties of the polymer and serves as a guideline for the rational design of next-generation polymers. Research should be shifted to the molecular level with a focus on the interchain coupling in the aggregates and/or the design of molecules that afford delocalization and minimize trapping  (38) .\n\nMaterials and Methods\nOFET Device Fabrication. Corning Eagle 2000 glass substrates were cleaned sequentially in water, acetone, and isopropanol for 10 min each, following by drying with nitrogen. Source-drain electrodes patterns were fabricated using a conventional evaporation procedure through metal shadow mask (channel length 30 μm, channel width 500 μm). Five-nanometer-thick Ti was used as adhesion layer of the Au electrodes on glass. The semiconducting polymer P(NDI2OD-T2) (ActivInk N2200; Polyera Inc.) and PS (molecular weight 100 kDa; Aldrich) were separately dissolved in 1,2dichlorobenzene, both at the concentration of 8 mg/mL.']</t>
         </is>
       </c>
-      <c r="AF181" t="inlineStr"/>
+      <c r="AF181" t="inlineStr">
+        <is>
+          <t>Here is my evaluation:
+```
+{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article does not mention fabrication techniques for stretchable polymer semiconductor films, nor does it discuss scalability and cost. The excerpts provided focus on charge transport properties of conjugated polymers and phase separation in a specific blend, but do not relate to the statement about fabrication methods."
+}
+```</t>
+        </is>
+      </c>
     </row>
     <row r="182">
       <c r="A182" t="inlineStr">
@@ -27031,7 +28347,16 @@
           <t>['It therefore follows that if the incoming photon has the polarization given by the linear combination a It) + f31-)-for example, it could be linearly polarized in a direction 45 0 from the vertical, so that a = f3 = 2-t !2-the result of its interaction with the apparatus will be the superposition of equations (  2 ) and (3): IAo)(al t )+f3I-» -+ aIAvert)ltt)+f3IAhor)I~) (4) If the apparatus states IA v .. t ) and IA hor ) are not identical, then the two photons emerging from the apparatus are in a mixed state of polarization. If these apparatus states are identical, then the two photons are in the pure state a Itt) + f31~) (5) In neither of these cases is the final state the same as the state with two photons both having the polarization al t )+f3I-). That state, the one which would be required if the apparatus were to be a perfect amplifier, can be written as which is a pure state different from the one obtained above by superposition [equation (  5 )].', 'Note that if photons could be cloned, a plausible argument could be made for the possibility of faster-than-light communication 2 • It is well known that for certain non-separably correlated Einstein-Podolsky-Rosen pairs of photons, once an observer has made a polarization measurement (say, vertical versus horizontal) on one member of the pair, the other one, which may be far away, can be for all purposes of prediction regarded as having the same polarization 3 • If this second photon could be replicated and its precise polarization measured as above, it would be possible to ascertain whether, for example, the first photon had been subjected to a measurement of linear or circular polarization. In this way the first observer would be able to transmit information faster than light by encoding his message into his choice of measurement. The actual impossibility of cloning photons, shown below, thus prohibits superluminal communication by this scheme. That such a scheme must fail for some reason despite the well-established existence of long-range quantum correlations 6 on an incoming photon with polarization state Is): IAo)ls)-+ IA.', 'W. H. Zurek\nTheoretical Astrophysics 130-33, California Institute of Technology, Pasadena, California 91125, USA If a photon of definite polarization encounters an excited atom, there is typically some non vanishing probability that the atom wiD emit a second photon by stimulated emission. Such a photon is guaranteed to have the same polarization as the original photon. But is it possible by this or any other process to amplify a quantum state, that is, to produce several copies of a quantum system (the polarized photon In the present case) each having the same state as the original? If it were, the amplifying process could be used to ascertain the exact state of a quantum system: in the case of a photon, one could determine Its polarization by first producing a beam of identically polarized copies and then measuring the Stokes parameters•. We show here that the linearity of quantum mechanics forbids such replication and that this conclusion holds for all quantum systems.']</t>
         </is>
       </c>
-      <c r="AF182" t="inlineStr"/>
+      <c r="AF182" t="inlineStr">
+        <is>
+          <t>Here is my evaluation:
+{
+  "label": "Substantiated",
+  "explanation": "The reference article explicitly states that it is impossible to amplify a quantum state, specifically mentioning photons, due to the linearity of quantum mechanics. This directly supports the claim in the citing article that entangled photons cannot be amplified because of the quantum noncloning theorem."
+}
+I based my decision on the abstract and excerpts 1 and 3, which all discuss the impossibility of amplifying a quantum state, including photons, due to the principles of quantum mechanics. This directly addresses the claim in the citing article that entangled photons cannot be amplified because of the quantum noncloning theorem.</t>
+        </is>
+      </c>
     </row>
     <row r="183">
       <c r="A183" t="inlineStr">
@@ -27171,7 +28496,17 @@
           <t>['A particularly interesting case is piezoresponse force microscopy (PFM), which is unique in that it probes a tensorial property, the coupling between electric field and mechanical strain. While the first and most obvious application of this technique is to straightforwardly map domains in ferroelectric materials, PFM does much more both in terms of the information content and of applications. Coupling between electric fields and mechanical strain underpins a broader range of phenomena in ferroelectrics and other polar materials. This article highlights recent examples in which PFM directly probes electromechanical interactions in systems ranging from complex ferroelectric materials and piezoelectric compounds to biological tissues. These examples also illustrate that creative variants of PFM or a quantitative approach to data analysis contribute to a fundamental understanding of complex phenomena in solids.\n\nImaging of Ferroelectric Domains: Statics and Dynamics\nPFM utilizes a basic experimental setup of atomic force microscopy in which a conducting tip at the end of a cantilever is brought in contact with a piezoelectric sample. When a voltage is applied to the tip, the resulting deformation of the sample is monitored through the mechanical displacement of the cantilever-piezoresponse.', '11  Further experiments in a wide variety of relaxor systems  [31] [32] [33] [34] [35]  established PFM as a unique method that allows  access to many otherwise unreachable phenomena, including the grain size effect,  33, 34  local variability of the correlation length (Figure  6 ),  33  the role of nanodomains in the macroscopic piezoresponse,  31  bias-induced phase transitions,  32, 36  and domain nucleation. 37\n\nPFM Imaging of Functional Materials\nCoupling between electrical and mechanical phenomena is common in a wide range of inorganic and organic materials, including piezoelectrics, semiconductors, polymers, biomolecules, and biological systems. The ability of PFM to probe electromechanical coupling on the nanometer scale opens a new approach to the delineation of local structure and functionality of these materials. Recently, PFM has been extensively used to study domain structures in polar III-V nitrides and biopolymers, as summarized in the text that follows.', 'In comparison, both vertical PFM (VPFM) and lateral PFM (LPFM) images show a very strong electromechanical response attributed to the presence of protein (presumably ameliogenin) fibrils embedded within a nonpiezoelectric hydroxyapatite matrix (Figure  8d  and  8e ). The spatial resolution of PFM, determined as a halfwidth of the boundary between different piezoelectric regions, is ~5 nm. Note that the resolution achieved is comparable to the best results to date achieved for thin films of ferroelectric perovskites. Comparison of the VPFM and LPFM images shows a different pattern of piezoelectric domains, suggesting a complicated structure of the fibrils, consisting of several protein molecules. The color encoded vector piezoresponse map (vector PFM), shown in Figure  8f , clearly delineates the helical structure, visualizing the electromechanically active protein fibril conformation in real space.\n\nPFM Manipulation and Lithography\nPatterning ferroelectric domains to engineer devices is a relatively recent phenomenon.']</t>
         </is>
       </c>
-      <c r="AF183" t="inlineStr"/>
+      <c r="AF183" t="inlineStr">
+        <is>
+          <t>Here is my evaluation of whether the reference article supports the given citation statement:
+```
+{
+  "label": "Substantiated",
+  "explanation": "The reference article (28) discusses the use of piezoresponse force microscopy (PFM) for studying electromechanical behavior at the nanoscale, including its ability to probe piezoelectric domains in ferroelectric materials. The excerpts provided demonstrate that PFM has submicrometer spatial resolution, allowing it to image domain structures and functionality in various materials. This supports the citing article's statement about using PFM to confirm large d_33 values within a single domain."
+}
+```</t>
+        </is>
+      </c>
     </row>
     <row r="184">
       <c r="A184" t="inlineStr">
@@ -27311,7 +28646,14 @@
           <t>['Ferroelectricity was originally discovered in Rochelle salt  (8)  in 1921 and later in a few other molecular systems  (9) , but the rapid development of ferroelectrics took place only after the discovery of ferroelectricity in perovskite barium titanate (BTO)  (10)  and lead zirconate titanate (PZT)  (11) . Relative to BTO and PZT, most  molecular ferroelectrics suffer from low spontaneous polarization (P s ), low melting temperature and phase transition temperature (Curie temperature, T c ), small dielectric constant, and weak piezoelectricity; their advantages include light weight, mechanical flexibility, and environmentally friendly processing as they are lead-free. Ferroelectric polymers such as poly(vinylidene fluoride) (PVDF) and its copolymers  (12)  share some of the drawbacks of molecular ferroelectrics, which limits their applications.', 'The recently reported croconic acid (6) has a high spontaneous polarization of around 23 mC cm -2 ; however, evidence for a ferroelectric phase transition, piezoelectric response, or ferroelectric domains has not been reported. By searching among organic compounds with a polar point group at room temperature and relatively high melting point, we found that diisopropylammonium chloride (DIPAC) is a ferroelectric with spontaneous polarization of 8.2 mC cm -2 (13). Here, we show that diisopropylammonium bromide (DIPAB), a molecular crystal processed from aqueous solution, possesses ferroelectric properties comparable to those of BTO. A crystalline sample of DIPAB was grown by slow evaporation of the aqueous solution; the recrystallization of DIPAB yields two different polymorphs  (14) . One (1-F), obtained from methanol, is needle-shaped, whereas the other (1-P), obtained from water or a methanol-water solu-tion, has a block shape (fig.  S1 ).', 'P s is measured to be 23 mC cm -2 , compared to 8 mC cm -2 for PVDF (4), 26 mC cm -2 for BTO (4), 30 to 55 mC cm -2 for PZT  (21) , and 8 mC cm -2 for DIPAC  (13) . We also observed that the variation of P s with respect to temperature is very similar to that of c (2) , which can be explained from the relationship c (2) = 6e 0 bP s deduced from Landau theory, where b is the high-order dielectric coefficient  (1, 19) . To verify our measurement of spontaneous polarization, we performed first-principles density functional theory  (22, 23)  calculations within the generalized gradient approximation to the exchange correlation potential according to the Perdew-Burke-Ernzerhof (PBE) method  (24)  and the Heyd-Scuseria-Ernzerhof hybrid (HSE) functional  (25) . The spontaneous polarization (Fig.']</t>
         </is>
       </c>
-      <c r="AF184" t="inlineStr"/>
+      <c r="AF184" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Substantiated",
+  "explanation": "The reference article supports the claim that researchers focus on improving the spontaneous polarization (P_s) and the phase-transition temperature (T_c) of organic ferroelectrics. The abstract mentions that molecular ferroelectrics, including diisopropylammonium bromide (DIPAB), have been found to have high spontaneous polarization and Curie temperature, making them a promising alternative to perovskite ferroelectrics."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="185">
       <c r="A185" t="inlineStr">
@@ -27453,7 +28795,14 @@
           <t>["d2-2 then self-assembled into the two-dimensional RNA scaffold D2 with PP7 and MS2 binding domains (step iv). In vitro transcribed RNA modules d1 and d2'/d2'' were characterized using atomic force microscopy (AFM). d1 formed one-dimensional RNA fibers D1, while d2'/d2'' assembled into two-dimensional extended RNA fibers D2 (Fig.  2A ). The width of D1 (~5 nm, a few tiles wide) is smaller than that of its DNA analog  (14) , and might thus also correspond to one-dimensional ribbons D1 2 constructed from a continuous line of single-tiles (Fig.  1E , step ii). Given that D2 preferentially grows in a single direction when compared to its DNA analog  (13) , it might also correspond to RNA nanotubes D2 2 that are relatively wider than D1 (Fig.  1D , step iii). To confirm the validity of our assemblies, we used analogs of d1 and d2' with a poly-T stretch in place of the DD incapable of assembling; d1 T and d2' T did not generate extended assemblies (Fig.", 'Here, we engineered synthetic RNA modules that assemble into functional discrete, one-, and two-dimensional scaffolds in vivo, and used them to control the spatial organization of bound proteins (Fig.  1A ). Scaffold D0 was constructed from a single RNA module d0, which folded into a duplex with PP7 and MS2 aptamer domains that bind PP7 and MS2 fusion proteins (Fig.  1B )  (13) . We developed an approach for the in vivo isothermal assembly of extended RNA scaffolds by constructing sequence-symmetric RNA building blocks (Fig.  1 ,  C  and  D ) inspired by two-dimensional DNA analogs  (13, 14) . These RNA strands possess dimerization (DD) and polymerization domains (PD). To prevent the formation of ill-defined networks, it was necessary to disfavor the collapse of the palindromic regions  (15)  and control assembly-order by insuring tile formation before polymerization. We achieved this by designing PDs that fold intramolecularly into kinetically protected hairpin structures (Fig.  1D , step i).', '1D , step i). The stem of these hairpins is an overlapping shared domain with DD that discourages collapse (Fig.  1D , red segments), allowing DD to "activate" PD upon self-binding (Fig.  1D , step iii). We further destabilized the collapsed-state by incorporating wobble-pairs and mispairs (figs. S1 to S4). The one-dimensional RNA assembly D1 was derived from a single RNA d1 with PP7 and MS2 binding domains (Fig.  1E ). d1 assembled into d1-1 (step i), which self-assembled into d1-2 (step iii). The torsion in d1-2 induced folding into an RNA nanotube capable of growing into the onedimensional scaffold D1 (step iv). The two-dimensional RNA assembly D2 was formed from d2\' and d2\'\', each carrying a distinct PP7 and MS2 aptamer (Fig.  1F ). The dormant tile d2\' spontaneously generated the pro-tile d2-1 (step i), which interacted with d2\'\' to generate tile d2-2 (step ii).']</t>
         </is>
       </c>
-      <c r="AF185" t="inlineStr"/>
+      <c r="AF185" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Substantiated",
+  "explanation": "The reference article describes the design and assembly of multidimensional RNA structures, including one-dimensional and two-dimensional scaffolds. Excerpt 1 specifically mentions 'RNA nanotubes D2 2' and Excerpt 3 explains how a single RNA module assembles into a one-dimensional scaffold D1 capable of growing into an RNA nanotube. This directly supports the claim that molecular assemblies from synthetic nucleic acids, such as tubes, have been generated."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="186">
       <c r="A186" t="inlineStr">
@@ -27595,7 +28944,18 @@
           <t>["d2-2 then self-assembled into the two-dimensional RNA scaffold D2 with PP7 and MS2 binding domains (step iv). In vitro transcribed RNA modules d1 and d2'/d2'' were characterized using atomic force microscopy (AFM). d1 formed one-dimensional RNA fibers D1, while d2'/d2'' assembled into two-dimensional extended RNA fibers D2 (Fig.  2A ). The width of D1 (~5 nm, a few tiles wide) is smaller than that of its DNA analog  (14) , and might thus also correspond to one-dimensional ribbons D1 2 constructed from a continuous line of single-tiles (Fig.  1E , step ii). Given that D2 preferentially grows in a single direction when compared to its DNA analog  (13) , it might also correspond to RNA nanotubes D2 2 that are relatively wider than D1 (Fig.  1D , step iii). To confirm the validity of our assemblies, we used analogs of d1 and d2' with a poly-T stretch in place of the DD incapable of assembling; d1 T and d2' T did not generate extended assemblies (Fig.", 'Here, we engineered synthetic RNA modules that assemble into functional discrete, one-, and two-dimensional scaffolds in vivo, and used them to control the spatial organization of bound proteins (Fig.  1A ). Scaffold D0 was constructed from a single RNA module d0, which folded into a duplex with PP7 and MS2 aptamer domains that bind PP7 and MS2 fusion proteins (Fig.  1B )  (13) . We developed an approach for the in vivo isothermal assembly of extended RNA scaffolds by constructing sequence-symmetric RNA building blocks (Fig.  1 ,  C  and  D ) inspired by two-dimensional DNA analogs  (13, 14) . These RNA strands possess dimerization (DD) and polymerization domains (PD). To prevent the formation of ill-defined networks, it was necessary to disfavor the collapse of the palindromic regions  (15)  and control assembly-order by insuring tile formation before polymerization. We achieved this by designing PDs that fold intramolecularly into kinetically protected hairpin structures (Fig.  1D , step i).', '1D , step i). The stem of these hairpins is an overlapping shared domain with DD that discourages collapse (Fig.  1D , red segments), allowing DD to "activate" PD upon self-binding (Fig.  1D , step iii). We further destabilized the collapsed-state by incorporating wobble-pairs and mispairs (figs. S1 to S4). The one-dimensional RNA assembly D1 was derived from a single RNA d1 with PP7 and MS2 binding domains (Fig.  1E ). d1 assembled into d1-1 (step i), which self-assembled into d1-2 (step iii). The torsion in d1-2 induced folding into an RNA nanotube capable of growing into the onedimensional scaffold D1 (step iv). The two-dimensional RNA assembly D2 was formed from d2\' and d2\'\', each carrying a distinct PP7 and MS2 aptamer (Fig.  1F ). The dormant tile d2\' spontaneously generated the pro-tile d2-1 (step i), which interacted with d2\'\' to generate tile d2-2 (step ii).']</t>
         </is>
       </c>
-      <c r="AF186" t="inlineStr"/>
+      <c r="AF186" t="inlineStr">
+        <is>
+          <t>Here is my evaluation:
+```
+{
+  "label": "Substantiated",
+  "explanation": "The reference article describes the design and assembly of multidimensional RNA structures, including two-dimensional scaffolds. Excerpt 1 specifically mentions the formation of two-dimensional extended RNA fibers D2, which corresponds to the mention of 'lattices' in the citation statement."
+}
+```
+I chose "Substantiated" because the reference article clearly describes the creation of two-dimensional RNA scaffolds, which matches the claim made in the citation statement about generating lattices. The specific details provided in Excerpt 1 further support this connection.</t>
+        </is>
+      </c>
     </row>
     <row r="187">
       <c r="A187" t="inlineStr">
@@ -27735,7 +29095,14 @@
           <t>['Design of hydrogels with hybrid crosslinking based on unstructured proteins. A) Schematic representation of designer unstructured proteins capable of covalent (CCP) and metal coordination (MCP 1 and 2) crosslinking. Elastin-like polypeptide domains (green) of varying length are interspersed with metal crosslinkable (blue) or covalently crosslinkable (red) domains. B) Force-extension profiles of individual molecules show similar elasticity. Each molecule follows the worm-like chain model for an unfolded polypeptide with a persistence of 0.365 nm, which is indicative of an unstructured polypeptide. C) Schematic illustrations of the covalently crosslinked networks, metal crosslinked networks, and interpenetrating networks (water molecules not to scale). Tough hydrogels are formed, depending on the concentration of ZnSO 4 present in the system. D) When the interpenetrating network hydrogel is stretched and relaxed, the phase transitioned ELP can be disrupted and reformed, respectively. Reversible decrosslinking/ crosslinking also occurs within the MCP network while the CCP network maintains elasticity throughout.', 'It is notable that the level of adhesion strength achieved here is much higher than recently developed nanoparticle adhesives for gels and biological tissues,  [34]  although it is lower than the adhesion of tough hydrogels on various nonporous solid surfaces recently achieved.  [35, 36]  Further investigation into the relative contributions of the metal coordination and hydrophobic interactions to enhance adhesion will be considered in future studies. In summary, we have demonstrated that genetically engineered unstructured proteins with covalent and reversible crosslinking (due to metal coordination and hydrophobic interactions) yield hydrogels with extremely high strength (&gt;2.5 MPa), toughness (&gt;1300 J m -2 ), stretchability (&gt;500%), and self-adhesion in Zn 2+ solutions. A number of future research directions now become possible in both the fundamental understanding of the physical properties of protein-based materials and their practical applications. While we have used reversible metal coordination and hydrophobic interactions for mechanical-energy dissipation to toughen our networks, other reversible crosslinking mechanisms such as hydrogen bonding and ionic crosslinking can also be precisely designed through genetic encoding of recombinant proteins.', 'DOI: 10.1002/adma.201604743\nstretchability, insensitivity to structural defects, and the capacity for self-healing.  [4] [5] [6] [7] [8] [9]  The strategies employed thus far to achieve these properties are primarily focused on incorporating structured protein domains, such as coiled coils, titin-like motifs, and folded fibrin.  [6, [10] [11] [12]  The interactions between, and/or unfolding of, these structured domains dissipate mechanical energy and maintain high elasticity of protein networks to enhance the strength and toughness of the resultant material.  [13]  Despite these successes, the synthesis of hydrogels containing highly structured proteins is limited by the often relatively low and variable production yield. Additionally, many of these proteins can elicit unwanted biological responses due to their tertiary structure, ultimately limiting material functionality, and use in target applications.']</t>
         </is>
       </c>
-      <c r="AF187" t="inlineStr"/>
+      <c r="AF187" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Substantiated",
+  "explanation": "The reference article describes designing hydrogels with hybrid cross-linking mechanisms using unstructured proteins, which results in materials with superior toughness and high fracture energy. Excerpt 1 shows the combination of covalent and metal coordination crosslinking, enabling toughening mechanisms that maintain high elasticity. This supports the claim of combining multiple cross-linking mechanisms to achieve hydrogels with superior toughness."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="188">
       <c r="A188" t="inlineStr">
@@ -27875,7 +29242,14 @@
           <t>['ζ-potential, measured at 25°C in 10mM NaCl, of pre-and post-XL NPs are approximately the same, while deposition of materials post-XL results in surface charge characteristics consistent with the material deposited (see Supplemental Figure  4 ). A range of polyelectrolyte multilayers were explored, including poly-L-lysine (PLL)/hyaluronic acid (HA) [PLL/HA 500K ], PLL/dextran sulfate (DXS) [PLL/DXS], PLL/poly(acrylic acid) [PLL/PAA], chitosan/HA [Chit/HA 500K ], and chitosan/PAA [Chit/PAA] (see Supplemental Figure  4 ), further illustrating a primary advantage of LbL as a means of tailoring the surface properties of these NP systems. These films, while diverse in the range of materials incorporated, behaved similarly in coating the NP systems without compromising the particle shape or significantly increasing the size beyond a few tens of nanometers. Recovered and purified particles visualized by electron microscopy, including SEM and TEM, are displayed in Figures  3  and  4 .', 'As a result, the cross-linked films can be placed in water without particle detachment. Following crosslinking, it was observed that particles could be readily functionalized, as evidenced by maintenance of iridescence from the NP array following each processing step (Figure  1E ,  1F ). This step therefore allowed for the deposition of water-based polyelectrolytes using Spray-LbL. As shown in Scheme 1, Spray-LbL on PRINT® nanoparticles, following vapor-phase crosslinking of the PVA support films, is achieved by spraying an aqueous solution of cationic polyelectrolyte is sprayed onto the NP containing films for 3 seconds and, after briefly rinsing with water (3 seconds), an anionic polyelectrolyte is subsequently sprayed onto the films (3 seconds). This cycle can then be repeated indefinitely to control the thickness of the polyelectrolyte coating. In the final step, the particles are harvested by sonicating the films in water, which causes the particles to detach from the PVA substrate.', 'For both particle types, uniformity of the particle population is maintained as evidenced by the PDI of functionalized particles (see Table  1 : PRINT® PLGA 200×200nm particles -original 0.01, 0.06 following deposition of three bilayers of PLL/HA 500K ; PRINT® PLGA80×320nm particles -original 0.05). A slight decrease in size following crosslinking is observed for both particle types, consistent with the amount of material exposure to the crosslinking contraction forces on the PVA adhesive layer. The change in size for functionalized particles is indicative of a very thin LbL film, approximately 15-20nm for 3 bilayers of PLL/HA 500K , based on dynamic light scattering (Table  1 ) and confirmed with electron microscopy (Figures  3 ,  4 ). Histogram overlays also illustrate the thin coatings applied to the particle surface (Supplemental Figure  4 ). Characteristic surface charge reversal of the LbL deposition is also observed, as evidenced by samples taken at different steps in the functionalization process.']</t>
         </is>
       </c>
-      <c r="AF188" t="inlineStr"/>
+      <c r="AF188" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Substantiated",
+  "explanation": "The reference article discusses the use of poly(L-lysine) (PLL)/poly(acrylic acid) [PLL/PAA] as an example of a polyelectrolyte multilayer, demonstrating control over surface properties. Although it doesn't directly state that PLL offers better control over electrostatic properties than other materials, the mention of PLL/PAA as one of several explored combinations in Excerpt 1 supports the idea that synthetic polyelectrolytes like PLL can be used to tailor surface properties."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="189">
       <c r="A189" t="inlineStr">
@@ -28015,7 +29389,16 @@
           <t>['We focus the following discussions on 532 nm resonance. Details of results obtained with 633 nm excitation are presented in the Supporting Information. A modes. Detailed assignments of multiphonon bands according to recently calculated phonon dispersion curves  43, 59  are summarized in Table  S1  of the Supporting Information. The most prominent resonance feature emerges near the 1 2g E peak for both WS 2 and WSe 2 . This peak, labeled as 2LA(M), is a second-order Raman mode due to LA phonons at the M point in the Brillouin zone  43, 54  . We found that the 2LA(M) mode shows distinct downshift of 5 cm -1 with increasing flake thickness from monolayer to trilayer for WSe 2 (See Supporting Information for details). In contrast, the same mode in WS 2 showed no obvious trend. The first-order phonon LA(M) in both WS 2 and WSe 2 is widely involved in the overtone and combination mode of other zone edge phonons, similar to the case of MoS 2 44, 60 .', 'The 1g E mode, which is an in-plane vibration of only the chalcogen atoms, is forbidden in the back-scattering Raman configuration  50, 51  . Monolayer WX 2 belongs to 3h D point group and has 9 modes at the Brillouin zone center.  43  The rigid layer shear mode 2 2g E is absent in monolayers 26, 45, 55, 58 . Unpolarized Raman spectrum of bulk WS 2 obtained with 473 nm excitation shows characteristic 1g A and 1 2g E peaks that are clearly separated and of similar intensity (Figure  1c ). In contrast, only one prominent peak can be clearly seen in bulk WSe 2 spectrum in the frequency region where we expect 1g A and 1 2 g E peaks  57  (See Supporting Information). In 633 nm excitation condition, however, multiple peaks are evident in this region (Figure  1d ). There have been inconsistent reports on the assignment of these peaks  7, 31, 32, 47  .', "The 532 nm excitation is in resonance with the B exciton peak of WS 2 and A' exciton peak of WSe 2 . On the other hand, 473 nm excitation is roughly in resonance with the interband transition peak C for WS 2 and interband absorption continuum for WSe 2 . The 633 nm excitation is in resonance with the A excitonic absorption for WS 2 and interband absorption but close to the B excitonic absorption for WSe 2 . Raman features of both WS 2 and WSe 2 strongly depend on the excitation conditions due to energy dependent Raman cross section of the phonons (See Supporting Information for details). The absorption peaks shift slightly with flake thickness  21  but the resonance conditions remain largely unaltered. The crystal structure of 2H-WX 2 belongs to 4 6h D point group. There are 18 lattice dynamical modes at the center of the Brillouin zone ( \uf047 point)  [50] [51] [52] [53] [54]  ."]</t>
         </is>
       </c>
-      <c r="AF189" t="inlineStr"/>
+      <c r="AF189" t="inlineStr">
+        <is>
+          <t>After evaluating the reference article, I conclude that:
+{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article does not provide specific information about the Raman spectrum of WS2 and WSe2 exhibiting peaks at 350 cm−1 and 419 cm−1 for WS2, or a peak at 250 cm−1 for WSe2. While the article discusses the Raman spectra of WS2 and WSe2, it does not mention these specific peak values or their correspondence to the E’ and A_1’ resonance modes."
+}
+Note that the reference article provides general information about the Raman spectra of WS2 and WSe2, including the dependence on thickness and excitation conditions. However, it does not provide specific details about the peak values mentioned in the citation statement. Therefore, I conclude that the reference article does not substantiate the claim made in the citing article.</t>
+        </is>
+      </c>
     </row>
     <row r="190">
       <c r="A190" t="inlineStr">
@@ -28155,7 +29538,18 @@
           <t>['1998; Garza &amp; Williamson 2001) . Additional research at other isolated systems that have not undergone recently a major disturbance will help evaluate further whether these populations at Scott Reef experienced bottlenecks in 1998. Nevertheless, despite these differences between the two studies, our results not only support the finding of high levels of genetic differentiation by  Ayre &amp; Dufty (1994) , but also extend our understanding of the processes underlying these patterns, by providing direct evidence that populations are subdivided on a scale of tens of metres. Consequently, the conclusion that the majority of brooded larvae produced by S. hystrix settle very close to their natal colony is now well supported in two very different ecological systems, irrespective of local environmental conditions and history. Disturbance, broader scale dispersal, and source/sink dynamics Despite this preponderance of local recruitment over scales of tens of metres, we have also presented evidence that S. hystrix larvae periodically disperse over much greater distances. The pairwise F-and R-statistics indicated that some sites separated by relatively large distances were more closely related than those that were nearer to each other.', 'In particular, several tests are now available that can assign individuals to their population of origin, from which present day migration patterns can be inferred  (Waser &amp; Strobeck 1998) . Although the development of high resolution DNA markers in scleractinian corals has been difficult  (Marquez et al . 2002) , recent progress has been made  (Magalon et al . 2003; Miller &amp; Howard 2004; Baums et al . 2005a; Underwood et al . 2006 ). Here, we present biological data utilizing the microsatellites developed by  Underwood et al . (2006)  to investigate the pattern of genetic connectivity among populations of the brooding pocilloporid Seriatopora hystrix within the Scott Reef system in northern Western Australia. The life history characteristics and genetic structure of S. hystrix suggest that the majority of dispersal is local. Larvae are produced sexually through internal fertilization of the eggs, are brooded within the polyp, and then released into the water column at an advanced developmental stage.', '2002; Palumbi 2003; Cowen et al . 2006) . Investigations have been limited by the considerable difficulties involved in tracking small propagules through the expansive oceans. Because of the resultant lack of direct, empirical data detailing patterns of larval dispersal or retention, researchers have had to draw on a wide range of indirect, interpretative and aggregative studies  (Thorrold et al . 2002; Largier 2003) . Analysis of the spatial distribution of genetic variation is one such method. Because gene flow reduces genetic divergence, population models are used to partition the genetic variation of a species among different geographical locations, and consequently assess the spatial scales over which they are reproductively closed. However, estimating recent patterns of migration from these models requires several simplified and often unrealistic assumptions  (Whitlock &amp; McCauley 1999) . Alternatively, when highly variable DNA markers such as microsatellites are utilized, the units of analysis can be shifted from populations to individuals, allowing more detailed and direct estimates of gene flow at ecologically relevant scales  (Estoup &amp; Angers 1998) .']</t>
         </is>
       </c>
-      <c r="AF190" t="inlineStr"/>
+      <c r="AF190" t="inlineStr">
+        <is>
+          <t>Here is my evaluation in JSON format:
+```
+{
+  "label": "Substantiated",
+  "explanation": "The reference article supports the statement that a pattern of local-scale genetic differentiation is commonly observed among brooding species. The abstract and excerpts describe findings of high levels of genetic differentiation at small spatial scales, with larvae recruiting to within 100 m of their natal colony, indicating localized dispersal."
+}
+```
+I chose "Substantiated" because the reference article provides evidence for local-scale genetic differentiation in a brooding coral species (Seriatopora hystrix), which aligns with the citation statement. The abstract and excerpts highlight the findings of localized larval recruitment and genetic subdivision at small spatial scales, supporting the claim made in the citing article.</t>
+        </is>
+      </c>
     </row>
     <row r="191">
       <c r="A191" t="inlineStr">
@@ -28295,7 +29689,18 @@
           <t>['High-resolution STEM imaging (Fig.  1b  and Supplementary Fig.  1 ) and the corresponding chemical mapping (Fig.  1d ) showed that the NiO shell was not uniform, containing small NiO grains with different orientations and might contain small gaps in the shell to expose some NiO/Ni nano-interfaces (Fig.  1c ). X-ray photoelectron spectroscopy (XPS) confirmed the NiO-Ni structure (Supplementary Fig.  2a ). The as-made material exhibited mostly Ni 2 þ species on the surface with a weak shoulder peak at B853 eV from Ni 0 . On Ar ion sputtering of the surface, the detected Ni species were mostly Ni 0 with decreased amount of Ni 2 þ , consistent with NiO-decorated Ni nanoparticles. The Ni K edge spectrum of the sample recorded by X-ray absorption near edge spectroscopy (XANES) further corroborated the co-existence of NiO and Ni (Supplementary Fig.  2b ). Since Ni K edge probed deeper into the material, we could estimate the Ni/NiO ratio B73/27 by linear fitting of standard patterns.', 'Synergistic effects of NiO and Ni on HER catalysis. When annealed at 300 °C at a higher Ar pressure of 1 atm (in contrast toB1.5 torr for producing NiO/Ni-CNT), the same Ni(OH) 2 precursors on CNTs was transformed to pure 3-4 nm NiO nanoparticles (NiO/CNT; Fig.  2b  and Supplementary Fig.  4 ), suggesting no Ni 2 þ reduction under a high annealing pressure with the release of oxygen gas. On the other hand, Ni 2 þ reduction was accelerated by raising the annealing temperature to 500 °C in B1.5 torr Ar, generating Ni nanoparticles (mostly410 nm particles) nearly free of NiO on CNTs (Ni/CNT; Fig.  2c  and Supplementary Fig.  4 ). The Ni surface oxidation state on NiO/CNT and Ni/CNT were confirmed to be þ 2 and 0, respectively, by XPS and XANES spectra (Fig.  2g , h ) and by EELS chemical mapping (Fig.', '2g , h ) and by EELS chemical mapping (Fig.  2e ,f and Supplementary Figs  5  and  6 ). The NiO/CNT material afforded a much larger overpotential of B400 mV, despite a smaller Tafel slope and CNT alone showed negligible HER current density before À 0.5 V versus RHE (Supplementary Fig.  7 ). The Ni/CNT hybrid gave similar Tafel slope in HER but a larger overpotential of B130 mV than the B0 mV overpotential for NiO/Ni-CNT. This advantage was partially attributed to the higher surface area of NiO/Ni-CNT (152.2 m 2 g À 1 ) compared with that of Ni/CNT (86.5 m 2 g À 1 ; Supplementary Fig.  8a ). With current density normalized to the surface area instead of the geometric area, NiO/Ni-CNT still outperformed Ni/CNT by B100 mV (Supplementary Fig.  8b ).']</t>
         </is>
       </c>
-      <c r="AF191" t="inlineStr"/>
+      <c r="AF191" t="inlineStr">
+        <is>
+          <t>Here is my evaluation:
+```
+{
+  "label": "Substantiated",
+  "explanation": "The reference article [26] supports the statement that the spectra for the Ni substrate contained peaks corresponding to metallic Ni (Ni_0) at 852.1 eV and Ni_2+ at 853.5 eV, as shown in Excerpt 1. Although it does not explicitly mention a peak at 855.3 eV corresponding to Ni_3+, the article discusses the co-existence of NiO and Ni species on the surface, which may imply the presence of other nickel oxidation states."
+}
+```
+Note that while the reference article does not explicitly mention the peak at 855.3 eV corresponding to Ni_3+, it provides strong evidence for the presence of metallic Ni (Ni_0) and Ni_2+ species, which substantiates part of the statement.</t>
+        </is>
+      </c>
     </row>
     <row r="192">
       <c r="A192" t="inlineStr">
@@ -28435,7 +29840,18 @@
           <t>['Reports\nThe Intergovernmental Panel on Climate Change (IPCC) Fifth Assessment Report  (1)  concluded that the global surface temperature "has shown a much smaller increasing linear trend over the past  15 years [1998-2012]  than over the past 30 to 60 years." The more recent trend was "estimated to be around one-third to one-half of the trend over 1951-2012." The apparent slowdown was termed a "hiatus," and inspired a suite of physical explanations for its cause, including changes in radiative forcing, deep ocean heat uptake, and atmospheric circulation changes  (2) (3) (4) (5) (6) (7) (8) (9) (10) (11) (12) . While these analyses and theories have considerable merit in helping to understand the global climate system, other important aspects of the "hiatus" related to observational biases in global surface temperature data have not received similar attention. In particular, residual data biases in the modern era could well have muted recent warming, and as stated by IPCC, the trend period itself was short and commenced with a strong El Niño in 1998.', 'Given recent improvements in the observed record  (13, 14)  and additional years of global data (including a record-warm 2014), we reexamine the observational evidence related to a "hiatus" in recent global surface warming. The data used in our long-term global temperature analysis primarily involve surface air temperature observations taken at thousands of weather observing stations over land, and for coverage across oceans, the data are sea surface temperature (SST) observations taken primarily by thousands of commercial ships and drifting surface buoys. These networks of observations are always undergoing change. Changes of particular importance include: (i) an increasing amount of ocean data from buoys, which are slightly differ-ent than data from ships; (ii) an increasing amount of ship data from engine intake thermometers, which are slightly different than data from bucket sea-water temperatures; and (iii) a large increase in land-station data that enables better analysis of key regions that may be warming faster or slower than the global average. We address all three of these, none of which were included in our previous analysis used in the IPCC report  (1) .', 'It is evident that in most latitude bands, the global trends in the past 15 years are comparable to trends in the preceding 50 years. Finally, we consider the impact of larger warming rates in high latitudes  (24)  on the overall global trend. To estimate the magnitude of the additional warming, we applied large-area interpolation over the poles using the limited observational data available. Results (Fig.  1 ) indicate that, indeed, additional global warming of a few hundredths of a degree Celsius per decade over the 21st century is evident, providing further evidence against the notion of a recent warming "hiatus." See supplemental materials for details. In summary, newly corrected and updated global surface temperature data from NOAA\'s NCEI do not support the notion of a global warming "hiatus." As shown in Fig.  1 , there is no discernable (statistical or otherwise) decrease in the rate of warming between the second half of the 20th century and the first 15 years of the 21st century.']</t>
         </is>
       </c>
-      <c r="AF192" t="inlineStr"/>
+      <c r="AF192" t="inlineStr">
+        <is>
+          <t>Here is my evaluation:
+```
+{
+  "label": "Substantiated",
+  "explanation": "The reference article [20] discusses the 'global warming hiatus' and presents updated global surface temperature analysis that contradicts the notion of a slowdown in global surface temperature increase. The abstract and excerpts clearly state that newly corrected and updated data do not support the idea of a recent warming 'hiatus', thereby substantiating the claim that tracking Earth's heat and ocean heat is related to the 'global warming hiatus' research surge."
+}
+```
+I chose "Substantiated" because the reference article [20] explicitly addresses the topic of the "global warming hiatus", which is part of the citing statement. The abstract, Excerpt 1, and Excerpt 3 all provide evidence that contradicts the notion of a slowdown in global surface temperature increase, thereby supporting the claim made in the citing article.</t>
+        </is>
+      </c>
     </row>
     <row r="193">
       <c r="A193" t="inlineStr">
@@ -28575,7 +29991,14 @@
           <t>['In summary, the choice of the descriptors is of vital importance because it is the set of descriptors to which the energy is assigned. The number of descriptors has an immediate impact on the feasibility of any ML potential, as it does not only restrict the efficiency of the energy evaluation but also determines the dimensionality of the coordinate space to be mapped by the training sets. On the other hand, the number of descriptors must be sufficiently large to enable an unambiguous distinction of different structures. In Secs. II B 1-II B 4 several descriptors which have been developed for ML potentials are discussed. This list is by far not complete, and there are plenty of new interesting approaches, which have been proposed recently, like moment tensors,  30  scattering transforms,  31  and many others.\n\nB. Descriptors for machine learning potentials\n\n\nAtom centered symmetry functions\nA ML approach applicable to high-dimensional systems containing large numbers of atoms has been proposed by Behler and Parrinello in 2007 employing NNs.', 'GAPs belong to the class of kernel methods, which have the general form E i (d i ) = N basis \ued70 j=1 α j χ j (d i ), (20) i.e., they are linear combination of some basis functions χ j depending on descriptor d i for the environment of i. The coefficient vector α is independent of the specific environment. The energy is expanded in terms of the known data points using a nonlinear kernel function K(d, d i ) providing a measure for the similarity of any two structures or environments, 54 E i = N train \ued70 j=1 α j K(d, d j ). (21) GAPs use the squared exponential kernel K SE (d, d ′ ) = exp - \ued70 j (d -d ′ ) 2 θ j . (22) Kernel methods are very frequently used. Another example is the combination with a Coulomb matrix descriptor for representing the atomization energies of organic molecules by Rupp et al.', 'The set of descriptors plays a central role, not only in the construction of PESs,  21  but also beyond in applications like structure-property relationships for property prediction in materials science  22  and also in the strongly related older field of QSAR.  23  Further applications with similar requirements regarding the structural description are the analysis of MD trajectories, the screening of large numbers of atomic configurations for certain features, and structure identification in general.  24  Even the collective variables used in simulation techniques like metadynamics have similar requirements.  25  The substantial challenge of finding suitable descriptors for ML potentials has been recognized in the advent of the first NN potentials about 20 years ago,  26  which initially have been developed for rather low-dimensional systems like small molecules and diatomic molecules interacting with frozen surfaces. As NNs, like all other ML methods, process ordered vectors of numbers, the output is not invariant with respect to any permutation of the position of equivalent atoms in the structure. Further, directly available descriptors of the atomic positions like Cartesian coordinates are not invariant with respect to translation and rotation of the system, while the resulting ML potential must possess these properties.']</t>
         </is>
       </c>
-      <c r="AF193" t="inlineStr"/>
+      <c r="AF193" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Substantiated",
+  "explanation": "The reference article discusses the importance of suitable kernels and descriptors for machine learning potentials in atomistic simulations. Excerpts 1-3 all touch on the topic of descriptors, highlighting their significance in machine learning approaches and discussing various types of descriptors that have been developed. This content directly supports the statement that there is an extensive body of research on suitable kernels and descriptors for energy prediction tasks."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="194">
       <c r="A194" t="inlineStr">
@@ -28715,7 +30138,14 @@
           <t>['This recognition has dramatic implications. For instance, when the GSTCs for passive lossless HMSs are rigorously examined, it turns out that plane-wave refraction cannot in general be realized with zero reflection, as the metasurface symmetric structure can only be matched to a single wave impedance value  [7, 19] . Indeed, the formulation in  [18]  showed that sufficient conditions to ensure passive and lossless design in this case include local power conservation and local wave-impedance equalization, requiring at least one additional diffraction mode, e.g. specular reflection. Although this reflection is minor for small-tomoderate angle refraction, it becomes significant when wide-angle refraction is considered. These observations raised serious questions regarding previously-reported achievements. Primarily, could passive lossless metasurfaces achieve truly-reflectionless engineered refraction? In a recent paper, Wong et al.  [20]  provided a positive answer to that question.', '[20]  provided a positive answer to that question. Relying on generalized scattering matrix theory, the authors showed that an asymmetric stacking of three reactance sheets could be designed to simultaneously match the wave impedance of both the incident and refracted plane waves, leading to zero reflections even in the case of wide-angle refraction. This approach was generalized in  [21] , showing that this structure corresponds to an omega-type bianisotropic metasurface (O-BMS). In O-BMSs, meta-atoms exhibit electric and magnetic polarizabilities as in HMSs, but also feature magnetoelectric coupling  [2, 22] . This additional degree of freedom allows passive and lossless implementation of metasurfaces which are matched to different wave impedances on their top and bottom facets; similarly, O-BMSs can be used for achieving asymmetric reflection properties  [23] . The wave impedance perspective, thus, can be used to find a passive and lossless solution for transforming a given incident plane wave to a desirable transmitted plane wave. But what happens when more than one mode exists below or above the metasurface?', "Thin planar arrangements of polarizable subwavelength particles (metasurfaces) have been attracting significant attention lately due to their demonstrated ability to efficiently implement a variety of electromagnetic functionalities \n[1] [2] [3] [4] [5] . Many innovative low-profile devices manipulating the phase, magnitude, and polarization of aperture fields have been reported in recent years  [6] [7] [8] [9] [10] [11] [12] [13] [14] [15] [16] , pointing out the immense potential of these surfaces in optics and microwave physics and engineering. While the first demonstrations used a single layer of electrically polarizable particles (meta-atoms)  [6] , it was soon found that these suffer from a limited transmission efficiency. To achieve a unity transmission magnitude with arbitrary transmission phase, both electrically and magnetically polarizable meta-atoms must be used  [8, 9, 17] . When illuminated by an incident field, such metasurfaces induce orthogonal electric and (equivalent) magnetic currents on the surface, forming Huygens' sources, capable of unidirectional radiation (i.e., full transmission)  [9] ."]</t>
         </is>
       </c>
-      <c r="AF194" t="inlineStr"/>
+      <c r="AF194" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article does not support the claim that it is possible to realize anomalously reflecting metasurfaces that operate perfectly without any parasitic reflections, scattering, and absorption. The excerpts provided focus on reflectionless beam splitting, perfect reflection, and the challenges of achieving zero reflection in passive lossless metasurfaces, but do not directly address anomalously reflecting metasurfaces or their perfect operation."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="195">
       <c r="A195" t="inlineStr">
@@ -28855,7 +30285,15 @@
           <t>['MANY TROPICAL FORESTS MAY HAVE BEEN SHAPED BY FIRES THAT OC-CURRED ONCE OR TWICE PER MILLENNIUM\n  (Turcq et al. 1998 , Bush et al. 2008 , McMichael et al. 2012) . However, in recent decades, especially in Brazil and Indonesia, fire-return intervals have become decadal or even shorter in some forests  (Cochrane 2003 , Langner &amp; Siegert 2009) . This increase in fire prevalence is primarily caused by an increase in ignition sources from agricultural activities that use fire as a tool for land management  (Laurance 2004 , Cardoso et al. 2008 , Morton et al. 2013 ) and an increase in forest flammability from other human activities, such as logging and fragmentation  (Cochrane 2001 , Siegert et al. 2001) . In addition, fires are often associated with severe droughts  (Chen et al. 2011) .', '2011) . For example, around 2.6 million hectares and 3.9 million hectares of forest were burned during El Niño Southern Oscillation (ENSO) in Indonesia and Brazilian Amazon  (Siegert et al. 2001 , Alencar et al. 2006, respectively) . Most of the predictions of fires associated to climate changes and human land uses in general, state that such events may occur more often in the coming years (e.g.,  Cochrane &amp; Barber 2009 , Fu et al. 2013) , affecting not only Amazon forest, but also the hyper-fragmented Brazilian Atlantic Forest. Thus, the interactions between human economic activities, climate change, and fire pose a serious threat for tropical forests. One of the consequences of this increase in fire-return intervals is an increase in the area of forests being subjected to repeated burns, which can alter forest structure and composition when compared to single burns  (Barlow &amp; Peres 2008) .', "2005) . Recurrent fires may reach into the forest canopy, killing many mid-sized, and large trees and most of the remaining aboveground biomass  (Kinnaird &amp; O'Brien 1998 , Cochrane et al. 1999 , Peres 1999 , Cochrane 2003) . While the effects of single fires on tropical forests are relatively well described, much less is known about recurrent fires. For example, single fires change the plant, bird and leaf litter ant species composition  (Barlow et al. 2002 , Barlow &amp; Peres 2008 , Silveira et al. 2013, respectively) , reduce sapling, seedling and tree densities  (Clearly et al. 2006) , and cause substantial reptile mortality  (Kinnaird &amp; O'Brien 1998) . Existing studies on the impacts of recurrent fires are primarily focused on plants (e.g.,  Cochrane &amp; Schulze 1999 , Barlow et al. 2003a ,b, Haugaasen et al. 2003a , Slik &amp; Eichhorn 2003 , Toma et al."]</t>
         </is>
       </c>
-      <c r="AF195" t="inlineStr"/>
+      <c r="AF195" t="inlineStr">
+        <is>
+          <t>Here is my evaluation:
+{
+  "label": "Substantiated",
+  "explanation": "The reference article (46) supports the claim that human-induced forest fires devastate large areas in primate range regions yearly, resulting in increased tree mortality and losses of up to one-third of canopy cover. The abstract mentions that recurrent fires reduce live tree biomass and increase canopy openness, while Excerpt 3 states that recurrent fires may kill many mid-sized and large trees, reducing aboveground biomass."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="196">
       <c r="A196" t="inlineStr">
@@ -28995,7 +30433,14 @@
           <t>['On one hand, the use of solid electrolytes to suppress dendrite propagation remains premature in the current stage  [15] [16] [17]  , for they often fall short of meeting the high-power requirement at ambient temperature due to limited ionic conductivity  18, 19  , together with issues such as large interfacial impedance  20, 21  . On the other hand, the most common approaches to dendrite mitigation in liquid electrolyte focus on the stabilization of SEI via adjusting the electrolyte composition and additives  [22] [23] [24] [25] [26]  . Though proven to be effective, most additives will be continuously consumed during battery cycling so that the suppression effect is not fully sustainable  [27] [28] [29]  . Alternatively, the application of a mechanically stable artificial SEI coating such as polymer or solid-state blocking layers has been proposed  [30] [31] [32] [33]  .', 'For example, a promising nanoscale interfacial engineering approach has been demonstrated recently based on interconnected hollow carbon nanospheres, ultrathin two-dimensional boron nitride or oxidized polyacrylonitrile fibres to control the dendrite growth and improve the cycling CE  [34] [35] [36]  . Nevertheless, all these studies adopted the galvanostatic Li plating/stripping approach on a current collector, which is still unable to address the issue of infinite volume change since the electrodes expand during Li plating and shrink during stripping. In addition, contrary to Li-ion batteries where Li ions are stored in prelithiated cathodes, many of the intensively studied high-energy-density battery chemistries (e.g., Li-air and Li-S) involve cathodes in the nonlithiated form. Therefore, it is apparent that a metallic Li anode design with no volume change at the whole-electrode scale and long-term cycling stability in liquid electrolyte is of paramount research importance  3  . Herein, we demonstrate a rational design of metallic Li anode that successfully achieves minimum volume change at the wholeelectrode level and stable, dendrite-free Li cycling.', 'T he ever-increasing demand for high-energy-density storage systems for transportation (electric vehicles), portable electronics and other applications has stimulated intensive research on rechargeable batteries that go beyond the conventional lithium (Li) ion chemistry \n1  . Among all the possible options 2,3 , Li metal is the most ideal anode material due to its high theoretical capacity (3,860 mAh g À 1 ) as well as its low electrochemical potential ( À 3.040 V versus standard hydrogen electrode)  4, 5  . Despite the appealing properties, Li metal electrode has been plagued for decades with the problem of ramified growth during repeated stripping/plating and the associated electrolyte decomposition, which lead to serious safety concerns and poor battery cycling efficiency  6, 7  . It is well known that Li is highly reactive such that in liquid electrolyte it reacts spontaneously with solvent molecules and salt anions to form an insoluble layer of solid-electrolyte interphase (SEI)  8  . When SEI becomes stabilized to block electron transfer, this passivating film can slow down or, ideally, prevent the electrolyte from further decomposition.']</t>
         </is>
       </c>
-      <c r="AF196" t="inlineStr"/>
+      <c r="AF196" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Substantiated",
+  "explanation": "The reference article discusses a design for a metallic lithium anode that suppresses dendrite growth and achieves minimum volume change through the use of a polymeric matrix. This aligns with the statement's mention of 'Li-hosted matrices' as a method to reduce Li dendrites in liquid electrolyte systems."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="197">
       <c r="A197" t="inlineStr">
@@ -29135,7 +30580,14 @@
           <t>['Several years earlier, it was reported by Henderson (one of the coauthors in this work), as well as other researchers, that highly concentrated liquid electrolytes prepared with glyme solvents and lithium salts have both a relatively high ionic conductivity and high oxidative stability  [17] [18] [19] [20] [21] [22]  . More recently, a number of publications have shown the striking differences between the properties and cell performances for dilute and highly concentrated electrolytes with glyme solvents, as well as other aprotic solvents  [23] [24] [25] [26] [27] [28] [29]  . One study, in particular, found that highly concentrated LiTFSI-1,3-dioxolane (DOL)/DME electrolytes inhibited Li metal dendritic growth, but the Li plating/stripping CE was reported to be rather low (B71%)  24  . Lu et al.  11  reported that stable Li depositions can be obtained in the liquid electrolytes reinforced with halogenated salt blends with no signs of deposition instabilities over hundreds of cycles of charging and discharging. Zheng et al.', 'Zheng et al.  8  used interconnected hollow carbon nanospheres to stabilize Li surface with a CE of B99% for 4150 cycles. However, no electrolytes have been reported to date that simultaneously overcome all of the challenges-dendritic metal deposition, low CE during Li deposition/stripping processes and poor rate performance-of Li metal electrodes. Most of the approaches reported to date mainly worked at relatively low current densities (o1 mA cm À 2 ), which are insufficient to meet the requirements for many practical applications (43 mA cm À 2 )  2, 8, 10, 11  . Therefore, new electrolytes that can lead to the high rate and stable cycling of the Li metal anode are urgently needed for the further development of rechargeable Li metal batteries. Here we demonstrate that the use of highly concentrated electrolytes composed of ether solvents and the salt lithium bis(fluorosulfonyl)imide (LiFSI or LiN(SO 2 F) 2 )  30  results in the dendrite-free plating of Li metal at high rates and with high CE.', 'The use of additives (for example, vinylene carbonate (VC), fluoroethylene carbonate (FEC) and so on) and/or replacement of the LiPF 6 electrolyte salt with other salts-such as LiAsF 6 , LiBF 4 , LiClO 4 , LiCF 3 SO 3 or LiTFSI (that is, LiN(SO 2 CF 3 ) 2 )-does not ameliorate this poor performance to any significant extent  12  . The search for other solvents for this application has also been problematic. Electrolytes based on ether solvents generally result in a less-dendritic Li morphology and improved CE for Li plating/stripping owing to their lower reactivity with Li metal  10  , but these features are not retained on prolonged cycling  5  .']</t>
         </is>
       </c>
-      <c r="AF197" t="inlineStr"/>
+      <c r="AF197" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article does not mention the use of electrolyte additives to mitigate Li dendrites in liquid electrolyte systems. Instead, it focuses on the development of highly concentrated electrolytes composed of ether solvents and lithium bis(fluorosulfonyl)imide salt for high-rate cycling of lithium metal anode."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="198">
       <c r="A198" t="inlineStr">
@@ -29275,7 +30727,14 @@
           <t>['No characteristic peak of the metals was detected, which indicated that metal catalysts were completely removed by the etching process. Electrical properties of graphene and graphite can be modulated by controlling the number of graphene layers (n). First, we show that conductivity or sheet resistance can be controlled by more than an order of magnitude, dependent on n. Films of graphene and graphite with differing n were synthesized using different metal catalyst films as previously described (also see Methods and Supplementary Information). Fig.  2a  shows the sheet resistance values of graphene and graphite measured using a four-point probe, as a function of n. The sheet resistance was reduced about 25 times (from 2,463±1,037 Ω/sq down to 98±46 Ω/sq), as n increased from ~2-4 to ~850 layers. The local variation of n influences the deviation of the sheet resistance. We also characterized the field-effect response of both 2-4 layer graphene and ~850 layer graphite (Supplementary Fig.  S5 ).', 'S5 ). Current versus backgate characteristics showed much stronger modulation in 2-4 layer graphene, compared to negligible change in the thick graphite (~850 layers) due to stronger screening effect as the number of layers increases  26  . The low sheet resistance and field-effect response of graphite are advantageous for applications in conductive films or electrodes, in contrast to superior transconductance level of the 2-4 layer graphene which is appropriate for active channels of field-effect transistors (FETs). The capability to modulate electronic properties through synthetic control of the graphite thickness provides a route to rationally designing and synthesizing large-scale electronics based entirely on carbon. The metal catalyst, Cu/Ni (700 nm/5 nm), was used to synthesize 2-4 layer graphene channels and the same combination with an additional Co (400 nm) was used to produce graphite electrodes which serve as the source (S) and drain (D) (Fig.  2b ). This method enabled the fabrication of all-carbon based transistor arrays which were then transferred onto a 285 nm-thick SiO 2 on Si wafer for measurement of backgate response.', 'In addition to contact properties of graphite electrode to graphene channel, advantages of the graphite, compared to metals, lie in its superb mechanical flexibility. We observed that even when graphite electrodes were distorted up to strain of ~2 %, I-V characteristics remained the same (Fig.  2f ). The synthetic method facilitated the creation of a large-scale field-effect sensor arrays composed of monolithic graphene-graphite, which were transferred onto 285-nm SiO 2 / Si wafer. One block of the array contained nine of 2-4 layer graphene field-effect sensors with graphite single common source and independent drains. The sensor chip had four of these blocks composed of 36 sensor devices total, as illustrated in Fig.  3a . The graphite electrode parts were covered with a 2 μm-thick SU8 passivation layer with openings around the 2-4 layer graphene channels. The current change measured while sweeping Ag/AgCl water-gate voltage at different pH solution is presented in Fig.  3b . The charge neutrality point shifted positively with increasing pH, and the pH sensitivity was ~17 mV/pH.']</t>
         </is>
       </c>
-      <c r="AF198" t="inlineStr"/>
+      <c r="AF198" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article (22) discusses the synthesis of monolithic graphene-graphite integrated electronics and explores their electronic properties. While it mentions the modulation of electrical properties in graphene, it does not demonstrate electrochemical or electrocatalytic properties, which are the focus of the citation statement."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="199">
       <c r="A199" t="inlineStr">
@@ -29415,7 +30874,17 @@
           <t>['As expected for AMP-PNP binding, a cluster of residues within the small lobe of the enzyme is highly sensitive to the addition of nucleotide. The most pronounced changes (⌬␦ Ͼ 0.05 ppm) are observed in residues of the ␤3-strand and the highly conserved glycine-rich loop (␤1-and ␤2-strands), which actively participate in positioning the nucleotide. Crystal structures have shown that the ␤3-strand flanks the nucleotide-binding site and contains K72, which coordinates the ␣and ␤-phosphates of ATP  (13, 14) . Gradual decreases of ⌬␦ toward the C-and N-terminal regions from the glycine-rich loop suggest that nucleotide binding affects distal sites within the small lobe of the enzyme. This is evident by the large ⌬␦ values for residues that in the crystal structure are Ͼ35 Å away from helices A and B (Fig.  3 ). A second region is centered at A188 and at the surface of the large lobe where substrate docking would take place (Figs.', "Reverse Order of Ligand Binding. The titrations were repeated by inverting the order of ligand additions, adding Kemptide first (i.e., intermediate-S) and then saturating the enzyme with AMP-PNP to form the Michaelis complex [the histograms with residue vs. ⌬␦ number are provided in supporting information (SI) Fig.  5 ]. Unlike AMP-PNP addition to the apo-enzyme, saturation with Kemptide caused relatively modest changes to the enzyme fingerprint. Only the phosphorylated S10 located in the A helix shows a drastic chemical-shift change. However, smaller changes are detected throughout the entire enzyme's backbone, which indicates that Kemptide binding radiates its effects to both lobes. Subsequent addition of AMP-PNP to the Kemptide-bound enzyme caused changes in three regions that are similar to the direct titration: around the glycine-rich loop, between the catalytic and peptide-positioning loops, and the unstructured C-terminal portion of the enzyme (SI Fig.  5 ).", 'The low on-rates support the hypothesis of a rather complex binding mechanism for the nucleotide, which requires conformational changes in the small lobe  (18) . These changes within segments of the small lobe are thought to be responsible for binding, aligning, and positioning the nucleotide for the formation of a catalytically competent complex. In addition to this, changes in both lobes occur to properly position the substrate and shield the active site from bulk water  (26) .\n\nDiscussion\nNMR spectroscopy is becoming the method of choice to analyze allostery  (27) (28) (29) (30) (31) (32) (33) (34) (35) , cooperativity  (27, 32, (36) (37) (38) , energy landscapes  (11, 32, (36) (37) (38) , and coordination of reactions for small and large enzymes  (11, 38, 40) . The first vivid picture of the complex changes occurring during the transitions from apo to intermediate and from intermediate to closed conformations in the backbone of PKA-C emerges from our NMR titrations.']</t>
         </is>
       </c>
-      <c r="AF199" t="inlineStr"/>
+      <c r="AF199" t="inlineStr">
+        <is>
+          <t>Here is my evaluation:
+```
+{
+  "label": "Substantiated",
+  "explanation": "The reference article supports cooperative substrate binding, as evidenced by NMR spectroscopy showing changes throughout the enzyme's backbone upon Kemptide (substrate) binding. Additionally, the article highlights positive allosteric cooperativity generated by nucleotide and substrate binding during conformational state transitions."
+}
+```</t>
+        </is>
+      </c>
     </row>
     <row r="200">
       <c r="A200" t="inlineStr">
@@ -29555,7 +31024,14 @@
           <t>['In this section we discuss these three possibilities in turn.\n\nSaturation in demand for raw lumens\nAs has been discussed, at current levels of per-capita consumption of light, there is no evidence that we have reached a saturation in the demand for light. It is nevertheless an open question whether we will approach such a saturation in the future or whether per-capita consumption of light will continue to scale linearly with gdp/CoL. To understand this question more quantitatively, we decompose per-capita consumption of light into the product of three factors: I N , the average illuminance foot_11  (or light per unit area, in units of lm m -2 ) that a person is surrounded by during his or her waking hours; τ on /(τ on + τ off ), a dimensionless illumination duty factor that accounts for how many hours per year the area around a person is actually illuminated and a N /(1 + a N ρ N ), the average unshared illuminated area (in units of m 2 ) that a person is surrounded by  24  . In other words, ϕ = I N • τ on τ on + τ off • a N 1 + a N ρ N .', 'Moreover, even if the enclosed indoor areas in which we work and live might ultimately saturate, the unenclosed outdoor areas which we either occupy for short periods during the day or evening, or which are visible from enclosed indoor areas, may be less prone to saturation. Such unenclosed outdoor areas (e.g. streets, parks and other recreation and public spaces) could all be rendered more useful if better illuminated in the evening hours (albeit at the cost of reducing the contrast of the night sky due to light pollution (Boyce 2003)). And there is a natural human tendency to gaze out (we value windows, not just because they are a portal for incoming light, but because of the view they afford (Boyce 2003)) into faraway spaces, even if we do not directly occupy those spaces. We conclude that it is possible that the average unshared illuminated area is nearing a saturation point, but plausible arguments can be made that the saturation point may yet be a factor 10× or greater away.\n\nDemand for features beyond lumens\nAlthough the primary demand for light is to illuminate our environment, there are many other features of light that are important to the consumer.', 'However, reasonable arguments can also be made that as a human society we are not near a saturation in consumption of light. As discussed in section 5.1, the average illuminance that a person is surrounded by during his or her waking hours and the average unshared illuminated area that a person is surrounded by may each yet be 10× or more from saturation. As discussed in section 5.2, new performance attributes associated with SSL have the potential to unleash new and unforeseen ways of consuming light. As discussed in section 5.3, guidelines and regulations may also have limited influence on light consumption.']</t>
         </is>
       </c>
-      <c r="AF200" t="inlineStr"/>
+      <c r="AF200" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Substantiated",
+  "explanation": "The reference article discusses the possibility of saturation in demand for light, specifically addressing whether per-capita consumption of light will continue to grow or if developed countries are nearing a saturation point. Excerpts 1 and 3 explicitly mention that it is an open question whether we will approach saturation in the future, and argue that plausible arguments can be made that the saturation point may yet be far away."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="201">
       <c r="A201" t="inlineStr">
@@ -29695,7 +31171,14 @@
           <t>['Because the spectra of the SD calibration and lunar calibration are different, the on-orbit change of the DNB RSR is expected to introduce deviation between the detector gain changes tracked by SD calibration and lunar calibration. In this paper, the deviation is estimated and verified by the measurement.    [Mills, 2010] . Journal of Geophysical Research: Atmospheres\n\nDNB LGS Calibration and Calibration Methodology\nThe DNB gain stages are automatically selected for EV images depending on the radiance level of each pixel. The gain stage information is recorded on a pixel level. For a given pixel, which can be operated at any of the three gain stages, the equation that yields DNB top-of-atmosphere radiance is L DNB ¼ F LGS;LUT Á P 2 i¼0 c i;LUT Ádn i DNB RVS DNB;LUT ; (1) where the LGS F factor F LGS,LUT , the background DN offset,LUT , and the adjustment coefficients c i,LUT are regularly updated as look-up tables (LUT). Here dn DNB is background-subtracted detector response DN DNB À DN offset,LUT .', 'The calibration of the DNB LGS uses the solar diffuser (SD) view, and the procedure is similar to the one used for the other RSBs  [Lei et al., 2015a; Lei et al., 2015b] . As has been demonstrated for other RSBs as well, the Moon can be used as a source to independently perform the calibration and track the stability of the SD calibration  [Xiong et al., 2015] . In our study, the RSB lunar calibration algorithm is extended to DNB with the DNB LGS F factor calculated from the lunar images captured during VIIRS scheduled lunar calibrations. The VIIRS design incorporates a rotating telescope assembly (RTA) that can protect the main optical elements from on-orbit contamination  [Weiss, 2011] . Due to tungsten contamination on the coating of the RTA mirrors, the S-NPP VIIRS has experienced strong wavelength-dependent throughput degradation since launch  [Barrie et al., 2012] . In addition to causing the decrease of the signal level and then SNR, the relative spectral response function (RSR) of VIIRS bands is altered by the degradation.', 'The change of the detector gain coefficient F factor can be tracked through lunar calibration, and the results are consistent with the SD calibration within ±0.5% for all calibration events since 2 April 2012 when the first lunar DNB F factor can be calculated. Unlike other narrow-band RSBs, the analysis shows that the change of the modulated RSR has much more significant impact to the calibration of the DNB. Also, the impact to the lunar calibration and solar calibration are different due to different source spectra. Taking into account this effect, the difference between the SD and lunar calibration is about 0.3% since 2 April 2012, in terms of the long-term deviation. The seasonal variation observed in lunar calibration result has been attributed to the ROLO lunar irradiance model instead of VIIRS measurement, as is demonstrated by the lunar calibration results of other RSBs as well.']</t>
         </is>
       </c>
-      <c r="AF201" t="inlineStr"/>
+      <c r="AF201" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Substantiated",
+  "explanation": "The reference article (43) discusses the radiometric calibration stability monitoring of the DNB using lunar data and solar diffuser measurements. The abstract and excerpts indicate that long-term changes in the DNB's radiometric calibration are well understood and accounted for, with a deviation of less than 0.3% between the solar diffuser and lunar trends since April 2012. This suggests that corrections can be made to ensure accurate calibration."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="202">
       <c r="A202" t="inlineStr">
@@ -29835,7 +31318,14 @@
           <t>['These ideas are fully compatible with existing chemistries and materials approaches in tissue engineering, in the sense that embedded lattice structures can provide the necessary mechanical response without altering the physicochemical and biochemical properties of the matrix, as shown for the example in Fig. 1 (ref. 42). Substrates for bio-integrated electronics. These types of bioinspired soft composites represent ideal platforms for stretchable electronic systems that intimately integrate with the human body  [43] [44] [45] [46] [47]  . Figure  6a-c  and Supplementary Fig.  14  shows an example that consist of a thin (2 mm), filamentary metal mesh that rests on a layer of silicone (B60 mm) with an embedded network structure (described in Methods section) designed to match the mechanical properties of the epidermis. The result is a skin-mounted sensor for electrocardiography (ECG) that has sufficiently small thickness and low modulus (at low strain) to maintain conformal contact with the skin, but with skin-like physical toughness (Fig.  6b ) to allow multiple cycles of application and removal without damage to the device or the skin (Fig.  6c ).', '(b) Stress-strain measurements on this device and schematic cross-sectional illustration. The wavy polyimide network used in the composite substrate adopts a triangular lattice of horseshoe building blocks, with y ¼ 120°, w ¼ 40 mm, t ¼ 55 mm. (c) ECG signals measured using devices without (I, blue) and with (II, purple) the soft composite substrate. The result (III, red) corresponds to a measurement performed after applying and removing the device with composite substrate 20 times. All signals show expected PQRST features in the waveforms. (d) Optical and infrared (IR) images of a wirelessly controlled responsive hydrogel delivery system. All scale bars are 1 mm. This system consists of three functional layers: a thermally responsive hydrogel membrane, a stretchable radio frequency antenna with Joule heating element and a composite substrate. As shown in inset IR image, the wirelessly activated heater locally increases the temperature of the hydrogel.', 'The net effect is a compliant artificial structure with non-linear properties, that is, B30-fold increase in the tangent modulus (that is, local slope of stress-strain curve) with strain, of potential value in active or passive devices that integrate intimately with the human body, as illustrated in conformal wrapping on flat and curved regions of the skin (Fig.  1a , b  and Supplementary Fig.  4 )  32, 33  . Deterministically defined non-linear mechanical responses. The mechanical properties can be adjusted to match, precisely, the properties of the skin or other organs. This tunability follows from the ability, via a simple lithographic process, to render the networks into nearly any 2D configuration  29, [34] [35] [36]  . Here theoretical descriptions of the mechanics represent essential tools for optimized selection of key design parameters, including the material type, the network topology, the filament dimensions and the microstructure geometry, to meet requirements of interest. Spatially homogeneous or heterogeneous mechanical properties are possible, with isotropic or anisotropic responses. In all cases, the design is inherently scalable in terms of a limited set of nondimensional parameters that define the microstructure geometry.']</t>
         </is>
       </c>
-      <c r="AF202" t="inlineStr"/>
+      <c r="AF202" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Substantiated",
+  "explanation": "The reference article supports the claim about stretchable design. Excerpts 1 and 3 describe skin-mounted electrophysiological sensors with mechanics precisely matched to the human epidermis, demonstrating the potential of soft composite materials for stretchable biomedical devices."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="203">
       <c r="A203" t="inlineStr">
@@ -29975,7 +31465,14 @@
           <t>['Carbon-supported multiarmed star-like platinum nanowires made in aqueous solution displayed high activity and durability  [9] . A similar enhancement in oxygen reduction reaction (ORR) activity was observed for Pd nanorods prepared by electrodeposition  [10] . Other 1D platinum group metal (PGM) catalysts including PtFe nanowires  [11] , Pd-Pt dendrites  [12] , and Pd-Pt core-shell nanowires  [13]  also showed outstanding performance. However, the synthesis of high quality ultrathin (sub 5 nm) Pt nanowires with high aspect ratio and uniform diameter is still challenging  [14, 15] . Here we report the synthesis of Pt nanowires assisted by [Cr(CO) 6 ] and a study of their electrocatalytic properties in ORR. Such Pt nanowires can be readily tuned to nanocubes by decreasing the concentration of [Cr(CO) 6 ].\n\nExperimental', 'According to the study by Wang et al.  [21] , for faceted particles, ligands favorably passivate on facets rather than at edges or corners. As shown schematically in Fig.  4 (c), the joint of a dumbbell then acts as a catalytic site and favors the addition of more Pt atoms due to the non-uniform distribution of the ligands on the surface, as well as interfacial strain. Subsequently this joint becomes autocatalytically elongated to form a nanowire. The exact role of the Cr species in the formation of nanowires needs to be further explored in order to completely understand the mechanism. The catalytic activity of the synthesized nanocubes and nanowires was investigated by electrochemical measurements using Pt/C (45 wt%, Vulcan, Tanaka) and Pt black (fuel cell grade, Sigma) as benchmarks. The catalysts (Pt nanocubes, nanowires, Pt black, and Pt/C) were deposited onto glassy carbon with a geometric area of 0.196 cm 2 as the working electrode.', 'Improved stability of the Pt nanowires can be expected because no additional carbon support is required. \n\nConclusions\nWe have successfully synthesized Pt ultrathin nanowires with a uniform diameter of 2-3 nm and high aspect ratio by symmetric growth from dumbbell nuclei. [Cr(CO) 6 ] plays a pivotal role in the formation of these dumbbell nuclei. These nanowires exhibit superior catalytic properties compared with Pt nanocubes and commercial catalysts. Considering that [Cr(CO) 6 ] acts as both reducing and shape directing agents, we believe that this method opens the door to synthesize Pt-based alloy ultrathin nanowires with controllable composition.']</t>
         </is>
       </c>
-      <c r="AF203" t="inlineStr"/>
+      <c r="AF203" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Substantiated",
+  "explanation": "The reference article [14] describes a method for synthesizing Pt ultrathin nanowires, which is relevant to the statement that 'Pt-based NW electrocatalysts have been achieved through several approaches'. Excerpt 1 specifically mentions previous work on platinum group metal catalysts and the challenge of synthesizing high-quality ultrathin Pt nanowires, while the article as a whole reports a successful synthesis method for such nanowires."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="204">
       <c r="A204" t="inlineStr">
@@ -30116,7 +31613,14 @@
           <t>['The PPy film was cut into a 10 mm × 2 mm strip and set in a one-compartment three-electrode cell described elsewhere  [8]  to measure change in length of the PPy strip by using a laser displacement meter (KEYENCE LE-4000) at typically 0.1 MPa load (under isotonic conditions) on applying potential. The definition of electrochemical strain of PPy actuators was change in length of the strip divided by the original length ( l/l 0 ). When the maximum strain was measured, potential was swept between -0.9 and +0.7 V versus Ag/Ag + by using a potentio-galvanostat (Princeton Applied Research 263A) at 2 mV s -1 in H 2 O/PC solutions of LiTFSI. Electrochemical contraction and expansion were conducted by applying a constant potential of -0.7 and +0.7 V versus Ag/Ag + , respectively, for 100 s except the second expansion (30 s) at room temperature.', 'Introduction\nConducting polymers (CPs) such as PPy are promising soft actuator materials potentially applicable to artificial muscle devices because of their large electrochemical stresses  (3) (4) (5)    [1] [2] [3] [4] , 10 times as large as that (0.35 MPa)  [5]  of mammalian skeletal muscles. The applications of CP linear actuators have been, however, quite limited due to their moderate electrochemical strains (1-3%)  [1, 2, 6] . Recently, some PPy actuators with more than 10% electrochemical strains appeared  [7] [8] [9] [10] [11] [12] , and some of which achieved up to 40% strain  [11, 12] , almost same level as that of skeletal muscles. Such extremely large electrochemical strains were measured when potential was swept at very slow scan rates of 2 or 0.2 mV s -1 . Obviously, most applications of CP actuators require much faster response rates, so CP actuators with large strains and fast response rates are highly expected.', 'The peak response rate was much larger than that (ca. 0.1% s -1 ) of other conventional PPy actuators  [2] , and that (3.2% s -1 ) of a PF 6 --doped PPy by using resistance compensation techniques  [14] . Ding et al.  [15]  prepared a tubular PF 6 --doped PPy with a Pt helical wire, exhibiting up to 13% s -1 strain rate and 5% strain, and we reported a PPy film with a compliant Au electrode at one side, prepared from an MB solution of TBACF 3 SO 3 , showed a peak strain rate of 8.8% s -1 and the maximum strain of 12.1%  [16] . Additional metal electrodes such as the Pt helical wire and the compliant Au thin layer decreased the voltage drop along the PPy actuators, giving fast response rates.']</t>
         </is>
       </c>
-      <c r="AF204" t="inlineStr"/>
+      <c r="AF204" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Substantiated",
+  "explanation": "The reference article discusses the electrochemical strain of a free-standing polypyrrole (PPy) film actuator, which exhibited up to 29% electrochemical strain. This value is significantly higher than the 'typically observed' strains mentioned in the citation statement, thus supporting the claim that the resulting strain in the citing article is lower than typically observed for pure PPy films."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="205">
       <c r="A205" t="inlineStr">
@@ -30256,7 +31760,18 @@
           <t>['We also note that AIHP NWs have far smaller thermal conductivity compared with traditional inorganic oxide perovskites whose values are 2-10 W•m -1 •K -1 (30). To elucidate the fundamental mechanisms responsible for the observed ultralow thermal conductivity, we apply a combination of density-functional theory (DFT) and the Boltzmann transport equation (BTE) (details in SI Appendix)  (31) . Considering the intrinsic uncertainty associated with perturbation theory and DFT-based simulations, the calculated k lattice values without fitting parameters are in reasonable agreement with the experimental values at high temperature (Fig.  2 A-C ). At low temperature, an empirical model is adopted to describe defect and boundary scatterings, and the computed data qualitatively agree with the trend observed in experimental data (Fig.  2 A-C ). Our simulations show that the extremely low k lattice can be attributed to low group velocities (v g ) and more importantly to extremely short phonon mean-free paths (l). The calculated v g in all cases is quite small (v g &lt; 2,000 m•s -1 ) due to constituent heavy atoms in AIHP (SI Appendix, Fig.', 'Both of these halide perovskites have been investigated for potential applications in solution-processed optoelectronic devices such as photovoltaics  (12, 13) , light-emitting diodes  (14, 15) , and lasers  (16, 17) . However, fundamental study of thermal transport in halide perovskites has been significantly lacking despite its practical and fundamental importance. For HHP, very few experimental studies have been performed for thermal conductivity  (18, 19)  and an ultralow thermal conductivity value of 0.5 W•m -1 •K -1 has been reported for single-crystalline CH 3 NH 3 PbI 3 . Computational study revealed that the main reason for the ultralow thermal conductivity of HHP is rotational motions of organic CH 3 NH 3 + ions  (20) (21) (22) . For instance, Hata et al.', 'For instance, Hata et al. computationally demonstrated the critical role of CH 3 NH 3 + rotations by comparing results with A-site cations possessing different degrees of freedom, where the elimination of the rotational degree of freedom results in greater thermal conductivity by a factor of ∼2  (20) . While limited investigations of thermal transport in HHP have been reported and some aspects of thermal transport in HHP are understood, fundamental understanding of thermal transport in AIHP remains largely elusive. The thermal transport mechanism in AIHP is expected to be fundamentally different from that in HHP, since vibrational density of states in organic and inorganic ions are largely mismatched for HHP, and monoatomic Cs + in AIHP does not contain rotational modes in contrast to the CH 3 NH 3 + ion in HHP  (20, 21) .']</t>
         </is>
       </c>
-      <c r="AF205" t="inlineStr"/>
+      <c r="AF205" t="inlineStr">
+        <is>
+          <t>Here is my evaluation:
+```
+{
+  "label": "Substantiated",
+  "explanation": "The reference article reports an ultralow thermal conductivity of around 0.4 W⋅m−1⋅K−1 in all-inorganic halide perovskites, which falls within the range mentioned in the citation statement (10−1 to 10^0 W m−1 K−1). The article also compares this value to traditional inorganic oxide perovskites with higher thermal conductivity values (2-10 W•m -1 •K -1), supporting the claim that the thermal conductivities of these materials are one to two orders of magnitude lower than those in conventional inorganic semiconductors."
+}
+```
+I determined that the reference article substantiates the citation statement because it provides a specific example of an all-inorganic halide perovskite with ultralow thermal conductivity, and also compares this value to other materials, which supports the claim made in the citation statement.</t>
+        </is>
+      </c>
     </row>
     <row r="206">
       <c r="A206" t="inlineStr">
@@ -30397,7 +31912,14 @@
           <t>["In many networks, ranging from online communities to food webs, metabolic networks, and genetic regulatory networks, there are communities or modules that play distinct functional roles. A fundamental problem is to detect these communities and understand what role they play in the network's structure and dynamics. In social networks, these communities are often assortative, meaning that there is a higher density of connections within communities than between them, and many approaches to detecting these communities have been proposed (see e.g. \n[1] ). In other networks, however, these modules may consist of nodes with few connections to each other, but which connect to the rest of the network in similar ways. In this Letter we analyze a random generative model for sparse modular networks, known as the stochastic block model. It provides a useful playground for theoretical ideas and the analysis of algorithms, and is a popular model for functional modules in real networks. Using the cavity method developed in the physics of disordered systems  [2, 3]  we exactly analyze the detectability of these modules in the limit of large sparse networks. As a function of the parameters, we compute the phase diagram and locate the associated phase transitions.", 'Only when the paramagnetic phase is no longer locally stable does inference become easy. We can compute the location of the transition to this easily-detectable phase analytically by analyzing how a small random perturbation to the paramagnetic fixed point propagates as the BP equations are iterated  [11, 19] . It follows that for |c in -c out | &gt; q √ c , (5) the original group assignment is dynamically attractive and hence many algorithms, e.g. MC or BP, will converge to it. Note that it is typically still hard to compute the ground state of (  2 ), even though we can compute the marginals, and therefore the optimal estimate of the group assignment, asymptotically exactly. On the other hand, if  (5)  is not satisfied then community detection is either impossible, or at best as hard as solving the hardest known optimization problems. When c out &lt; c in the phase transition is of first-order for q &gt; 4, as can be retrieved from data presented in  [19] . However, the detectable but hard region is so narrow that is is quite unlikely to appear in realistic situations. Real-world networks.', 'As a function of the parameters, we compute the phase diagram and locate the associated phase transitions. We distinguish between a detectable phase where it is possible to learn the model\'s parameters and the group assignments of the nodes, and a non-intuitive undetectable phase where learning is impossible because the network\'s topology does not retain enough information about the original group memberships. The existence of a phase where a certain class of algorithms is unable to detect communities was previously predicted  [4] , but its location was only found approximately (and its size overestimated). In addition, unlike previous works based on finding a ground state, i.e., minimizing a cost function associated with a group assignment  [4, 5] , our analysis is more general as it relies on the properties of the entire Boltzmann distribution of group assignments. We also unveil a transition from an algorithmically "hard" phase, where, we believe, no polynomial algorithm for learning the groups and parameters exists, to an "easy" phase where polynomial algorithms do exist. In the latter phase, we show that Belief Propagation (BP)  [6]  works on large networks in essentially linear time as a function of their size.']</t>
         </is>
       </c>
-      <c r="AF206" t="inlineStr"/>
+      <c r="AF206" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Substantiated",
+  "explanation": "The reference article supports the statement that communities may be undetectable in sparse networks. The abstract mentions a phase transition from a detectable to an undetectable regime, and Excerpt 2 explains that when a certain condition is not met, community detection is either impossible or extremely hard."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="207">
       <c r="A207" t="inlineStr">
@@ -30538,7 +32060,17 @@
           <t>["Introduction\nA common goal in the analysis of network data is to characterize the dependence between network relations and a set of node-specific attributes. For example in recent years many studies in the social sciences have examined the relationship between individuals' friendship networks and their health measures, such as happiness, smoking and drinking behavior, and obesity (e.g.  Veenstra et al. (2013)  and references therein). Similarly in the biological sciences, scientists are interested in the relationship between how proteins interact and their biological importance (see  Butland et al. (2005)  for example). In each of these applications, parameter vector. The covariate vector x i,j typically includes terms for each attribute of the sender node i and receiver node j, as well as interaction terms measuring the similarity between the sender and receiver attributes. These interaction terms are frequently specified as the absolute difference between the attributes, an indicator of whether an attribute is the same for both the sender and receiver node (in the case of discrete attributes), or the product of the nodes' attributes.", "The improvement was greatest for male drinking frequency and female GPA where prediction mean squared error was reduced by about 15%. This illustrates that when dependence exists between the network and attributes, improvements in the predictions of missing values can be obtained by using both the network and attribute information.\n\nDiscussion\nIn this article we introduced an original approach to testing whether dependencies exist between a network and attribute data, and a joint modeling framework for the network and attributes, which relies on a simplified representation of the network in terms of latent nodespecific factors. As discussed in the Introduction, many others have proposed methodology for investigating the relationship between network and attribute data. The most common methods involve regressing either the network on functions of the nodal attributes or each node's attributes on functions of the attributes of the node's neighbors in the network. Frequently final models are settled upon after some, often undocumented, model selection procedure which not only alters the interpretation of the results, but also adds an additional element of subjectively to the analysis. The key distinction between the previous methods and those presented here is that our method does not involve any model selection procedures and simultaneously tests and estimates first and second order dependencies between the network and attributes.", "(see  Cohen-Cole and Fletcher (2008)  and  Lyons (2011)  for additional discussion of these methods). Other similar models include the auto-regressive network effects models of  Erbring and Young (1979)  and  Marsden and Friedkin (1993)  and the p * social influence models of  Robins et al. (2001) . All of these models are univariate, focusing a single attribute of interest that is possibly subject to social influence. While modeling the network and attributes as functions of one another is able to provide some insight into their dependence structure, there are two primary drawbacks to utilizing these methods for analysis. First, neither modeling framework allows for simultaneous inference about the dependencies between and among the network relations and attributes. For example, when analyzing data on an adolescent friendship network and individuals' health behaviors there may be interest in whether smoking habits and obesity status are conditionally independent given the network. Addressing this question of dependence between attributes conditional on the network is impossible using either of the conditional modeling frameworks. A second limitation of these methods is that they are unable to accommodate, and provide predictions for, datasets that have both missing network and attribute information."]</t>
         </is>
       </c>
-      <c r="AF207" t="inlineStr"/>
+      <c r="AF207" t="inlineStr">
+        <is>
+          <t>Here is my evaluation:
+```
+{
+  "label": "Substantiated",
+  "explanation": "The reference article discusses the relationship between network structure and nodal attributes, including methods to test and model dependencies between them. The provided excerpts describe how dependencies exist between a network and attribute data, and how joint modeling frameworks can capture these dependencies. This supports the citation statement that correspondence between metadata and communities suggests a relationship between how nodes interact and the properties of the nodes themselves."
+}
+```</t>
+        </is>
+      </c>
     </row>
     <row r="208">
       <c r="A208" t="inlineStr">
@@ -30678,7 +32210,16 @@
           <t>['Designing over orders of magnitude\nEngineering the nanoscale interaction between cells and electrodes may be the fundamental challenge to massively parallel intracellular recordings, but a complete in vivo recording system presents additional technical obstacles. For instance, each recording site must transmit information out of the brain (&gt;millimeters) to downstream electronics, which can become logistically challenging as the number and density of the electrodes increases. While up to 512 electrodes have been accommodated by flexible connectors  [19] , dramatically larger numbers of electrodes are probably to require multiplexing and/or wireless transmission. Electrode arrays of up to 26,400 electrodes have been achieved in vitro with multiplexing  [96] , but such a demonstration has yet to be achieved in vivo. Finally, electrode micromotions within the brain can disrupt the recording if the electrode moves relative to the cell  [97] . Ideally the recording site could move independently from the rest of the electronics, such as a wireless device on the brain surface  [98]  or a soft physical tether to the outside world  [19] .', 'Active mechanical stabilization has been used to correct the micromotion of rigid glass microelectrodes in vivo  [97] , but high density recordings will more probably rely on the compliance of flexible micro-wires or nanowires arrays  [99, 100]  to passively decouple recordings sites from recording electronics. Such a design will be particularly important for awake recordings, where animal movement requires special attention to electrode stabilization  [101] . Indeed, motivated by the difficulty of interfacing rigid structures with brain, there is much ongoing work adapting flexible electronic materials for use in neuroscience  [102, 103] . Flexibly tethered recordings present a different problem, however, as they cannot be delivered deep within the brain without the aid of a rigid shuttle  [102, 103]  or other means of providing reversible rigidity during insertion  [104, 105] .', 'Whole-cell patch recording  [15] , sharp microelectrode recording  [16, 17] , and silicon-based extracellular electrodes  [18, 19]  remain the state-of-the-art in neural recordings despite their well-known limitations: whole-cell patch recording causes dialysis over periods of minutes  [20] [21] [22] , sharp microelectrodes change input resistance and resting membrane potential  [23] [24] [25] [26] [27] , and extracellular recording cannot measure subthreshold changes in neuronal transmembrane potential  [28] . The motivation for developing nanoscale tools for neurophysiology is to record intracellular electrical activity from thousands of neurons simultaneously without perturbing their physiological properties. Furthermore, to make these tools impactful to neuroscience, they should be robust, easy to use, and their performance reproducible across labs. Several groups have now demonstrated that solid-state nanoscale devices can record electrical activity in neurons and cardiomyocytes, which signals an important step toward parallelizable, non-dialyzing intracellular recording. The remaining challenge is to demonstrate that these devices can be used over timescales relevant to neurophysiological experiments while preserving native cellular function.']</t>
         </is>
       </c>
-      <c r="AF208" t="inlineStr"/>
+      <c r="AF208" t="inlineStr">
+        <is>
+          <t>Here is the evaluation result:
+{
+  "label": "Substantiated",
+  "explanation": "The reference article discusses challenges in implementing nanoscale electrical probes for neural recordings, including electrode micromotion and wiring of individual nanowires to external systems. Excerpt 1 specifically mentions the logistical challenges of transmitting information from a large number of electrodes, as well as electrode micromotions disrupting recordings."
+}
+I chose "Substantiated" because the reference article directly addresses the challenges mentioned in the citation statement, particularly in Excerpt 1. The article discusses the difficulties of transmitting information from a large number of electrodes and the issue of electrode micromotion, which aligns with the concerns raised in the citation statement about placement, micromotion, and wiring of individual nanowires.</t>
+        </is>
+      </c>
     </row>
     <row r="209">
       <c r="A209" t="inlineStr">
@@ -30818,7 +32359,14 @@
           <t>['In the stretched states, the currents also showed similar negative linear correlations with the interval of the electrode and the touch points. A 2D hydrogel panel was tested in order to detect the position of the touch point. As shown in Fig.  2 ,  A  and  C , a thin hydrogel film, rectangular in shape, was connected to the Pt electrodes at each corner. Four current meters were also installed between the voltage source and each corner. Two normalized distances, a and b, were used to indicate the position of the touch on the panel. The bottom left corner of the panel corresponded to (a, b) = (0, 0), and the top right corner corresponded to (a, b) = (1, 1). When the panel is touched by a finger, it can be virtually divided into four resistive sections by the touch point (Fig.  2B ). In the circuit, four virtual resistors are connected together in parallel, and this parallel circuit of resistors is connected to the capacitor by the finger in series. In Fig.  2C , the test positions of the touches are displayed.', 'As shown in Fig.  4D , we subsequently touched from TP#1 to TP#4 on the epidermal touch panel, and the current was measured with the A1 current meter. The correlation between the measured currents and the touched position was not influenced by the attachment. The epidermal touch panel could successfully perceive various motions, such as tapping, holding, dragging, and swiping. Thus, various applications can be easily managed by integrating the panel. As shown in Fig.  4 , E to G, writing words (Fig.  4E ), playing music (Fig.  4F ), and playing chess (Fig.  4G ) were accomplished via adequate motions on the epidermal touch panel (movies S3 to S6). We have demonstrated a highly stretchable and transparent ionic touch panel. We used a PAAm hydrogel containing 2 M LiCl salts as an ionic conductor. We investigated the mechanism of position-sensing in an ionic touch panel with a 1D strip. The ionic touch strip showed precise and fast touch-sensing, even in a highly stretched state. We expanded the positionsensing mechanism to a 2D panel.', 'A schematic design of an epidermal touch panel is shown in Fig.  4A . The epidermal touch panel was built on a 1-mm-thick VHB film (3M, Maplewood, MN) so as to insulate the panel from the body. Because VHB film was originally developed as an adhesive, the panel could be attached to an arm without using extra glues (Fig.  4B ). The epidermal touch panel was fully transparent so that it could convey visual content behind the touch panel. Moreover, the panel was mechanically soft and stretchable so that a user is comfortable with movement while wearing it. The currents measured before and after attachment are plotted in Fig.  4C . The baseline currents increased after the attachment owing to a leakage of charges through the VHB substrate. The thicker insulating layer generated a smaller baseline current. The effect of thickness of the insulating layers on the baseline currents is shown in fig.  S8 . The sensitivity to touch decreased after the attachment; however, the touching current was still sufficient to be detected. As shown in Fig.']</t>
         </is>
       </c>
-      <c r="AF209" t="inlineStr"/>
+      <c r="AF209" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Substantiated",
+  "explanation": "The reference article (26) describes a highly stretchable and transparent ionic touch panel that can detect touch and sustain large deformations. Excerpt 1 specifically mentions the use of four electrodes attached to a hydrogel film, which is consistent with the citing article's statement about detecting touch and stretch with four electrodes on a transparent sheet of conductive gel."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="210">
       <c r="A210" t="inlineStr">
@@ -30958,7 +32506,14 @@
           <t>["At low frequencies, the value of 𝜀𝜀 𝑟𝑟 ′ increases with temperature, whereas at high frequencies the trend is opposite but at a much smaller rate. This low-/high-frequency boundary is at ~10 3 Hz for our MAPbI3 thin film. The dielectric loss 𝜀𝜀 𝑟𝑟 ′′ shows a 1/f behavior for frequencies below a few kHz, following the so-called Jonscher's law, which accurately reveals the ionic conductivity of the material.  39, 40  As temperature increases, a small and wide shoulder (indicated by the arrow in Fig.  4b ) begins to appear and shifts toward higher frequency with temperature. Such a behavior is typical for relaxation processes, found in the generic Debye expression of permitivity.  37  Considering the low frequency and broad peak feature, this relaxation process could be a Maxwell-Wagner type interfacial polarization relaxation, possibly attributed to grain boundary effects or blocking at the contacts. The dielectric loss tangent of the material was found to be high at lower frequencies, especially at lower temperature.", 'It is known that a peak in dielectric constant and loss tangent is a characteristic of a ferroelectric material when crossing its ferroelectric-paraelectric phase transition (Tc).  21, 35, 36  However, no such peaks, either sharp or broad, were found in the temperature suggesting the phase change across the regions. The temperature dependence of dielectric loss and conductivity (Fig.  S9 ) also suggests a phase transition between 40 o C-50 o C. Figure  4b  shows frequency spectra of dielectric constant, dielectric loss, and loss tangent. Unusually high values of 𝜀𝜀 𝑟𝑟 ′ , similar to those in Refs.  37, 38  , can be seen at low frequencies (970 at 1 Hz and 30 o C), which dramatically decrease by more than one order at higher frequencies. Such a strong dependence of dielectric permittivity, particularly at low frequencies, is not a favorable sign of a ferroelectric nature of the material.', 'The peak value of loss tangent shifts toward higher frequency as the temperature is increased (~1 Hz for 10 o C to ~200 Hz for 70 o C). Moreover, the loss tangent starts increasing with temperature at &gt;100 Hz, and below this frequency the loss tangent decreases with increasing temperature. More work is expected to be done in the future to understand this phenomenon. As shown in Fig.  S8 , the Nyquist plots of impedance spectra exhibit two distinct chargetransport regimes associated with two semicircles. This is particularly obvious at higher temperatures. The first semicircle in the high-frequency regime arises from fast electron transport, whereas the second semicircle in the low-frequency regime may be attributed to slow ionic migration to the contact interface. Different models have been applied to fit the spectra to gain insight on the physical processes. Here, we employ the model previously used by Yang et al.  38  and Beilsten-Edmands et al.  5  in their studies of perovskite materials, to explain our measured data. It is understood that this simplified model will not capture all the subtleties but does explain the dominant processes.']</t>
         </is>
       </c>
-      <c r="AF210" t="inlineStr"/>
+      <c r="AF210" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Substantiated",
+  "explanation": "The reference article supports the claim of two characteristic relaxation frequencies in the dielectric loss spectra, with a low-frequency component attributed to ionic relaxation and a high-frequency component possibly related to electronic conduction. Excerpt 1 mentions a 'low-/high-frequency boundary' at ~10^3 Hz, which is consistent with the statement's frequency range of &lt;10^4 Hz for the low-frequency component. Additionally, Excerpt 3 discusses two distinct charge-transport regimes in the impedance spectra, which can be related to the high-frequency component mentioned in the statement."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="211">
       <c r="A211" t="inlineStr">
@@ -31098,7 +32653,17 @@
           <t>['5 ). Since the cooling is not as large as in PMIP1 there is more water vapour in the atmosphere and evaporation still occurs along the path of the storm track, which explains the signature in precipitation.\n\nMid-Holocene\nChanges are modest compared to those of the LGM, but reflect the sensitivity of the climate system to changes in the mean seasonal cycle of insolation. In particular, there is nearly no simulated change in annual mean temperature or precipitation for the Mid-Holocene, consistent with no change in global annual mean insolation. The major changes for this period compared to present correspond to an enhanced (reduced) seasonal cycle of temperature in the NH (SH). The continental warming favours the deepening of the JJAS thermal low over land, which intensifies the low level    winds and moisture transport from the tropical ocean to the continent, and thereby intensifies monsoon system in the tropical regions  (Kutzbach et al., 1993; Joussaume et al., 1999) . All models simulate an amplification of the mean seasonal cycle of NH surface temperature.', 'Figures  9c  and  d   Results from the PMIP2 OA simulations suggest a reduction of about 20% to 42 % over Africa, except for one model that produces a slight enhancement of precipitation (+16%). Several PMIP1 SSTf simulations produce a larger reduction in precipitation, up to a 62%. The spread of PMIP1 SSTc results is even larger (10 to 80%). Over North India, similar conclusions can be drawn (Fig.  9d ). These results show that there is no specific differences between the different sets of simulations, suggesting that the change in precipitation is mostly due to the reduction in the mean water vapour associated to the large-scale cooling across the tropical regions, the reduction in evaporation, changes in the residence time of water in the atmosphere and to changes in water vapour advection  (Yanase and Abe-Ouchi, 2007) . \n\nAfrican and Indian monsoons at the Mid-Holocene\nThe change in MH precipitation over West Africa has been a key focus of PMIP1.', 'Figure  9a  shows that the response of PMIP2 OA MH simulation in JJAS ranges from 0.2 mm/d to 1.6 mm/d (5 to 140%). Both OA and OAV simulations tend to produce larger precipitation changes in this region than PMIP1 SSTf experiments. This increase in precipitation is due to the response of the ocean and the building up of warmer conditions in the subtropics and mid latitudes in the Atlantic north of the equator and colder conditions in the Southern Hemisphere (Fig.  6 ). This strengthens the cross equatorial flow and favours the maintenance of the ITCZ to the north of its present day position in West Africa and the nearby ocean  (Kutzbach and Liu, 1997; Braconnot et al., 2000; Zhao et al., 2005) . The expansion of the area influenced by the Afro-Asian summer monsoon during MH is one of the most striking features shown by palaeoenvironmental data (Fig.  10 ), and thus this region has become one of the major focus for model evaluation in PMIP  (McAvaney et al., 2001) .']</t>
         </is>
       </c>
-      <c r="AF211" t="inlineStr"/>
+      <c r="AF211" t="inlineStr">
+        <is>
+          <t>Here is my evaluation:
+```
+{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article does not support the claim that some mid-Holocene model simulations show evidence of drier conditions below ca. 10°N in response to a northward shift in the monsoon. The excerpts actually suggest an amplification or intensification of the African monsoon at the Mid-Holocene, with increased precipitation over West Africa (Excerpt 3)."
+}
+```</t>
+        </is>
+      </c>
     </row>
     <row r="212">
       <c r="A212" t="inlineStr">
@@ -31238,7 +32803,14 @@
           <t>['However, with increasing density [Fig.  1(b) ] E f will pass E eq at a given density, and then E f serves as a new starting point for the hopping transport. With increasing density E f moves closer to E t , leading to an enhanced mobility for larger densities. The relative positions of E f and E eq are crucial to explain the temperature dependence of the charge transport  [11, 12] . Upon cooling down, E eq moves deeper into the tail of the Gaussian DOS, leading to a non-Arrhenius temperature dependence given by ln / 1=T 2 in case of low densities  [5] . For sufficiently high densities [Fig.  1(b)] , meaning E f &gt; E eq , it has been demonstrated by Coehoorn that also within the Gaussian disorder model the transport is governed by an Arrhenius-like ln / 1=T behavior  [12] , as often observed in organic transistors  [13, 14] . Experimentally, the question whether the transport in organic semiconductors is better described by a ln / 1=T 2 or ln / 1=T [Eq.', 'Recently, also the dependence of h on the carrier density in a PPV derivative has been investigated by a combined study on polymeric diodes and field-effect transistors  [8] . It has been demonstrated that the hole mobility is constant for charge carrier densities typically &lt;10 22 m ÿ3 and increases with a power law with density for carrier densities &gt;10 22 m ÿ3 . In contrast to the earlier assumption  [4]  the enhancement of the mobility at higher voltages in SCL diodes at room temperature has been shown to be totally due to the increase of the carrier density instead of the electric field  [9] . However, at lower temperatures the field dependence of the mobility becomes increasingly more important. Therefore, a transport model has been developed that incorporates both the effect of carrier density and electric field on the mobility  [10] . The occurrence of two regimes in the density dependence of the mobility is governed by the amount of charge carriers in FIG.  1 . (a) The hopping in a Gaussian DOS is schematically represented for low carrier densities.', 'As expected, the materials with a higher mobility also show weaker temperature dependence due to the reduced disorder. In Fig.  3 (b) the Arrhenius plot is extrapolated to T ! 1. Remarkably, again all measured mobilities originate from nearly one point, again 0 30 10 cm 2 =V s. The occurrence of a single value for 0 for such a large variety of organic semiconductors is surprising since its value is expected to be governed by the amount of electronic overlap between the chain segments. This result would indicate that the packing and resulting wave function overlap would be very similar for the materials studied here. However, it should be noted that the measured mobilities for the conjugated polymers are an average between both intrachain and interchain hopping processes. For intrachain hopping the hopping distance and localization length are about equal, leading to a T ! 1 mobility in a Gaussian DOS of  [22]  0 ea 2 ph  (3)  with a the hopping distance and ph the attempt-to-escape frequency.']</t>
         </is>
       </c>
-      <c r="AF212" t="inlineStr"/>
+      <c r="AF212" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Substantiated",
+  "explanation": "The reference article supports the statement that at high charge carrier densities, a universal Arrhenius-like temperature dependence has been observed for disordered conjugated polymers. Excerpt 1 mentions that for sufficiently high densities, the transport is governed by an Arrhenius-like behavior, which aligns with the citation statement."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="213">
       <c r="A213" t="inlineStr">
@@ -31378,7 +32950,14 @@
           <t>['We present one example. In  [7] , we constructed a fourband tight-binding model for HgTe. It is a zero-gap system, but by opening a gap with uniaxial pressure, it becomes a band insulator. The question here is whether it is a simple insulator or a topological insulator (i.e. QSH). In fact, from the parities of the bands below the Fermi energy E F from the four-band model in  [7] , the Z 2 topological number ν turns out to be even. This disagrees with the result in  [18] . The reason for the disagreement is the following. This model only has four bands near the Fermi energy E F , and the other bands well below E F are discarded. In HgTe, one doubly-degenerate band just below the Fermi energy has a trivial Z 2 topological number, while the other discarded bands deep below the Fermi energy have a nontrivial Z 2 topological number; this leads to the seemingly contradicting results.', 'A crossing of two such energy bands has co-dimension three; namely, by tuning three parameters one can make two bands degenerate  [20, 21] . To see this, let us consider a 2 × 2 Hamiltonian matrix H = a c c * b , (8) where a, b are real functions of k and m, and c is a complex function of k and m. A necessary condition for the two eigenvalues to be identical consists of three conditions a = b, Re c = 0 and Im c = 0, i.e. the co-dimension is three  [20] . These three conditions determine a curve in the 4D space (m, k x , k y and k z ). Thus for generic m there will be in general a point (or points) k where the eigenvalues are degenerate. When m is changed continuously the k point moves in the k space, and the system remains gapless. It will be revealed later how the system can open a gap and run into either the QSH or the insulating phases. On the other hand, for k = G/2, band crossing cannot occur in general.', "At the phase transition, the Z 2 topological number must change, which necessitates the closing of the gap at some wavevector k. There are various kinds of band crossing when we introduce a number of parameters; nevertheless, to study the phase transition, we restrict ourselves to 'generic' band crossing, and exclude band crossing achieved only by tuning more than one parameter. To be specific, we consider a Hamiltonian matrix H (k) = h ↑↑ (k) h ↑↓ (k) h ↓↑ (k) h ↓↓ (k) , (6) where k = (k x , k y , k z ). We assume that the spectrum of the Hamiltonian has no extra degeneracies other than those imposed by symmetry. We also assume that the Fermi energy E F lies within a gap of the Hamiltonian. The T-symmetry implies, H (k) = σ y H T (-k)σ y , (7) i.e. h ↑↑ (k) = h T ↓↓ (-k), h ↑↓ (k) = -h T ↑↓ (-k) and h ↓↑ (k) = -h T ↓↑ (-k)."]</t>
         </is>
       </c>
-      <c r="AF213" t="inlineStr"/>
+      <c r="AF213" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article does not discuss Weyl semimetals or the topological protection of degeneracies. Instead, it focuses on phase transitions between quantum spin Hall and insulator phases in 3D systems, which is unrelated to the statement about Weyl semimetals."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="214">
       <c r="A214" t="inlineStr">
@@ -31520,7 +33099,14 @@
           <t>['1 ). Here we investigate how this process, a momentum space manifestation of Klein tunneling  [22] , affects the magnetic quantum oscillations of the density of states (de Haas-van Alphen effect), providing a unique thermodynamic signature of the topologically protected band structure (an alternative to proposed transport signatures  [9, [23] [24] [25] ). Because the quantum oscillations are governed by extremal cross sections of the Fermi surface, one might wonder whether some symmetry is required to align the extremal cross section with the Weyl point, so that it becomes observable. Our analysis shows that a magnetic field axis for this alignment exists generically, because of the Möbius strip topology of the projective plane. We first consider Klein tunneling through a single type-II Weyl point, and then turn to pairs of Weyl cones of opposite helicity, which can be combined in topologically distinct ways  [8] -with a qualitatively different dependence on the Klein tunneling probability.', 'Experimentally, Klein tunneling through a type-II Weyl point can be detected in measurements of the de Haas-van Alphen effect in the magnetic susceptibility. With sufficient doping WTe 2 would produce disconnected type-II Weyl cones near the Fermi energy  [9, 41] , while they are connected in undoped LaAlGe  [15] . Klein tunneling is a powerful diagnostic for such topologically distinct Fermi surfaces.', 'While in graphene the high symmetry of the honeycomb lattice keeps the cone upright, strain providing only a weak tilt  [13] , the tilting can be strong in 3D Weyl semimetals. This leads to a natural division of Weyl cones into two topologically distinct types  [9] . In type I the cone is only weakly tilted so that the electronlike states and holelike states occupy separate energy ranges, above or below the Weyl point. In type II the cone has tipped over so that electron and hole states coexist in energy. Many experimental realizations of a type-II Weyl semimetal have recently been reported  [14] [15] [16] [17] [18] [19] [20] [21] . In a magnetic field the coexisting electron and hole pockets of a type-II Weyl semimetal are coupled by tunneling through the Weyl point (Fig.  1 ).']</t>
         </is>
       </c>
-      <c r="AF214" t="inlineStr"/>
+      <c r="AF214" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Substantiated",
+  "explanation": "The reference article discusses Klein tunneling in a type-II Weyl semimetal, which is one of the phenomena mentioned in the citation statement. The excerpts and abstract provide evidence that the authors investigated the effects of Klein tunneling on magnetic quantum oscillations and thermodynamic properties, supporting the claim made in the citing article."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="215">
       <c r="A215" t="inlineStr">
@@ -31660,7 +33246,14 @@
           <t>['In summary, we have demonstrated that the CRISPR-Cas9 system can be used to cure a genetic disease in mouse by directly correcting the genetic defect through NHEJ-or HDRmediated gene editing. In the future, it would be of interest to investigate whether similar gene-correction strategies could be used for mutation correction in a setting related to human diseases, such as human stem cells.', 'Impressively, by directly injecting Cas9 mRNA and single-guide RNAs (sgRNAs) into zygotes, mice or rats carrying mutations in transgenes or multiple endogenous genes can be generated in one step  (Li et al., 2013a (Li et al., , 2013b;; Shen et al., 2013; Wang et al., 2013; Yang et al., 2013) , indicating that the CRISPR-Cas9 system can be used as an effective tool for genome engineering  (Gaj et al., 2013) . Nevertheless, successful correction of disease-causing mutations in animal models via the CRISPR-Cas9 system has not yet been demonstrated. In this study, we report the efficient correction of a mutant gene in a mouse disease model by zygote injection of CRISPR-Cas9, and we report subsequent successful transmission of the corrected trait to the next generation. We chose a mouse model of dominant cataract disorder caused by a defined mutation in the Crygc gene  (Zhao et al., 2010) . These mice carry a 1 bp deletion in exon 3 of Crygc.', 'Taken together, our data suggest that while supplying exogenous oligos may not be necessary, the exogenous oligonucleotide could serve as an optional template for repairing the mutant gene, especially when the endogenous allele cannot be used as the template (as in homozygous genetic diseases). In this study, 24 mice were cured of cataracts using the CRISPR-Cas9 system. To further confirm the correction of the disease, we performed histological analysis of lenses prepared from repaired and control cataract mice. As shown in Figure  1I  and Figure  S2H , control cataract mice showed pathological changes in the equatorial region of their entire eyes, but the cataract-free mice that were cured via HDR or NHEJ-mediated gene editing (two or three mice, respectively) exhibited normal histological features. One major hindrance to the therapeutic application of the CRISPR-Cas9 system is the potential for offtarget mutations; we therefore examined off-target effects in the repaired mice.']</t>
         </is>
       </c>
-      <c r="AF215" t="inlineStr"/>
+      <c r="AF215" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Substantiated",
+  "explanation": "The reference article demonstrates the use of the CRISPR-Cas9 system to correct a genetic disease in mice, showing that the system can be used to efficiently correct genetic defects. This directly supports the statement that the CRISPR-Cas system represents a promising approach for correction of diverse genetic defects."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="216">
       <c r="A216" t="inlineStr">
@@ -31800,7 +33393,14 @@
           <t>['In our studies, the contrast was achieved by patterning metallic resonators on a polymeric substrate, and the metamaterial sheets crumpled or flattened out on solvent exchange which induced solvation and desolvation of the films, and consequently reversible self-folding at differentially cross-linked hinges. The ability to create stimuli-responsive metamaterials offers the possibility for the realization of adaptive optical and electromagnetic coatings. Kim et al. have shown that differentially cross-linked NIPAM bistrips with lateral swelling heterogeneities show interesting thermally responsive shape transformations (Figure  4B )  [52, 53] , which could potentially be utilized to create novel stimuli-responsive structures. Spatial heterogeneities can also be achieved by doping NIPAM with carbon nanotubes (CNTs) which were used to realize thermal stimuli responsive NIPAM/LDPE bilayer folding (Figure  4C ) and offer the possibility for optically responsive folding owing to the strong absorption of the CNTs in the near infrared  [54] .', 'Introduction\nStimuli responsive materials are expected to play an important role in the creation of multi-functional, smart, reconfigurable, mechanized, and biomimetic structures at a variety of length scales  [1 ] . Self-folding broadly refers to a class of self-assembly systems in which structures curve or fold-up either spontaneously or in response to a stimulus. In the perfect sense of the term, self-folding materials are composed of multiple interconnected units that fold up without any active human control. Selffolding of biomolecules such as proteins is an essential feature of the internal machinery of a cell and a variety of supramolecular and origami inspired strategies have been developed to create synthetic stimuli responsive selffolding molecular structures ranging from self-folding cavitands  [2, 3]  to foldamers  [4, 5]  to DNA boxes  [6] . Folding in these systems is typically mediated by relatively weak interactions such as hydrogen bonds which can be broken or formed.', 'Reversible folding has been achieved with electric and optical signals, pH, ionic strength and solvent exchange while predominantly one-way triggered actuation has been achieved in response to a range of biochemical stimuli. To create biochemically responsive reversible self-folding structures, it would be necessary to utilize thin bi-layers or bi-strips composed of novel polymers such as glucose  [63]  or antigen responsive  [64]  gels. In doing so, it may be possible to create a range of biosensing actuators to enable autonomous functions and biomimetic behaviors. Additionally, while such stimuli responsive structures have been demonstrated at the molecular and the 100 mm to 1 cm length scales, the intermediate 0.1 to 1 mm scale remains relatively unexplored, mainly owing to challenges in patterning polymers and hydrogels with these dimensions. It is noteworthy that self-folding methods work at these size scales and 100 nm scaled metallic self-folding polyhedra have already been achieved,  [65]  but similarly sized stimuli responsive polymeric self-folding structures have yet to be demonstrated.']</t>
         </is>
       </c>
-      <c r="AF216" t="inlineStr"/>
+      <c r="AF216" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article does not provide evidence of discussing other methods of light stimuli-responsive origami. The abstract and provided excerpts focus on stimuli-responsive self-folding using thin polymer films, but do not mention recent reviews of light stimuli-responsive origami."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="217">
       <c r="A217" t="inlineStr">
@@ -31940,7 +33540,14 @@
           <t>['The two hypothetical mechanisms are (1) increased amplification of standing and short wavelength Rossby waves (called "quasi-resonant" circulation regimes) and (  2 ) weakening of fast-moving Rossby waves and associated storms. Note that the two mechanisms are active areas of research, and as such their theoretical basis in either the observed or future climate is not established. However, the two hypotheses would be consistent with nonlinear increases in extreme heat events. Furthermore, the hypotheses complement one another as both account for reduced summer weather variability at synoptic time scales, and there is some evidence that both are occurring in boreal summer  [21] .\n\n"Resonant" Circulation Regimes\nPlanetary wave influence on midlatitude weather in all seasons is a topic of active research. In the boreal midlatitude summer, amplifying interactions among standing (quasistationary) Rossby waves and fast-moving (free) Rossby waves of similar wavenumber (e.g., 6-8) have been proposed as being critical in producing long-standing heatwaves and other extreme events  [17, 18, 20, 21, 23, 37, 44] .', 'Beyond an incipient theoretical basis for quasi-resonance and its link to heat extremes, some observational evidence for it exists  [21] ; however, the evidence remains mixed, and its detection is potentially sensitive to how quasi-resonance is measured  [43, 46] . Thus, considerable scientific work remains to establish anything more than an associative link to changes in heat extremes.\n\nWeakened Zonal Winds and Summer Storms\nIncreases in midlatitude extreme heat events have also been loosely attributed to weaker zonal flow  [21]  and reduced summer storms  [21, [23] [24] [25] . The proposed mechanism is that transient fast-moving waves slow and weaken in response to a weakened equator-to-pole temperature gradient from Arctic amplification  [21, [23] [24] [25] 47] , which reduces baroclinicity  [25, 43] . Coumou et al.  [23]  report that a combination of weaker waves with slower phase speeds has reduced eddy kinetic energy (EKE, a quantity of transient systems) by a striking two standard deviations, a departure climate models do not project under large radiative forcing until approximately 2100.', 'How well does persistence associated with the large-scale dynamical mechanisms explain heat wave evolution, relative to the predictions associated with existing, more localized, theories of heat wave evolution (e.g., Miralles et al.  [32] )? While only representing a single model and location, the analysis of Teng et al.  [54]  of projected heatwaves over the Great Plains is important because it partitioned both planetary wave and land surface factors, concluding that only the latter could explain projected increases in heat waves there. The question of causation of any changes in midlatitude dynamics is even more challenging. Changes in the summer midlatitudes and Arctic may share a common mechanism, perhaps in the tropics (e.g., Ding et al.  [55] ). Petoukhov et al.  [17]  and Hoskins and Woolings  [40]   summer 2011 heatwave in the USA. The quasi-resonant patterns with a strong contribution from zonal wave numbers m = 6 (b, c) and m = 7 (a) are clearly seen. From Petoukhov et al.']</t>
         </is>
       </c>
-      <c r="AF217" t="inlineStr"/>
+      <c r="AF217" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article does not support the statement about changes in atmospheric circulation patterns related to planetary waves being responsible for detected changes in correlation in some regions. The article discusses the relationship between heat events and atmospheric circulation, but it does not provide evidence or mention the specific topic of changes in correlation in some regions due to changes in planetary waves."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="218">
       <c r="A218" t="inlineStr">
@@ -32080,7 +33687,14 @@
           <t>['This would contribute to the lower PCE value of the one-step processed sample. The signal from PbCl -is found to be very low and fairly constant, indicating that the PbCl 2 precursor is almost absent. In sample A (Figure  7a ), the perovskite layer is very compact, The strong decrease in R A within the perovskite layer indicates that the perovskite formation is inhomogeneous with a more efficient conversion at the bottom part of the perovskite layer, while more Pb X I Y species are present at the interface with the HTM not bound into the perovskite structure. In sample B, R B is fairly stable within the perovskite layer, indicating an efficient and homogeneous perovskite conversion which well fits with the high PCE values. The raise of R B indicated some iodine diffusion toward the HTM. In sample C, similarly to sample B, R C displays a constant value in the perovskite layer.\n\nCONCLUSIONS\nThis work has explored in detail the morphology, composition, and interfaces in PSCs deposited by different methodologies and external conditions by combining multiple advanced characterization tools.', '2.4. Perovskite Conversion Efficiency. Composition analysis with EDX, XPS, and ToF-SIMS have revealed iodine diffusion leading to an inhomogeneous lead/iodine ratio, with marked composition differences between in the capping perovskite layer and the one embedded into the mesoporous TiO 2 layer. It is then crucial to establish whether the constituent elements of the perovskite are present in the desired perovskite form (i.e., CH 3 NH 3 PbI 3 ) or in other forms (PbI 3 or PbI 2 , etc.) as this would allow to compare the perovskite conversion efficiency associated with the each conversion method and environment and determine ionic diffusion testified by the presence of strong signals from iodine fragments.', 'To do this, we selected from the ToF-SIMS profiles the most characteristic fragment from the crystallized perovskite (Pb 2 I 3 -, which is totally absent outside the perovskite layer) and a second fragment PbI 3 -which has the strongest intensity in the perovskite layer, but it is thought to be found also where iodine and lead are bound to form isolated PbI 3 (i.e., not converted into the perovskite structure). The profiles obtained in each sample together with the ratio between PbI 3 and the (smoothed) Pb 2 I 3 -signals (named R i ) are displayed in Figure  7 . In a homogeneous perovskite layer R i would be constant; an increase in R i is an indication of higher abundance of PbI 3 not in the perovskite form. In sample D (single step, Figure  7d ), PbI 3 signal displays a remarkable raise in the mesoporous TiO 2 matrix indicating a possible iodine diffusion into the TiO 2 scaffold not efficiently forming the perovskite structure (in agreement with STEM results).']</t>
         </is>
       </c>
-      <c r="AF218" t="inlineStr"/>
+      <c r="AF218" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article does not mention the influence of different terminations at grain boundaries and interstitials on the optoelectronic properties of perovskite grains, which is the specific claim attributed to this reference. Instead, it focuses on the analysis of interfaces and composition in perovskite solar cells using various characterization techniques."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="219">
       <c r="A219" t="inlineStr">
@@ -32220,7 +33834,14 @@
           <t>['635 Ma (Fig.  3 ). The long duration (&gt;55 m.y.) of the Sturtian glacial epoch implies a relatively short Cryogenian nonglacial interlude (&lt;25 m.y.), consistent with a repeated trigger for glaciation related to the tectonic background conditions that drive weathering and the consumption of CO 2 on 1-10 m.y. time scales  (Mills et al., 2011) . This updated Neoproterozoic chronology provides new constraints to test and refi ne climate models of a long-duration glacial epoch and the nature of a relatively short nonglacial interlude. The Os i data presented here confi rm enhanced weathering of juvenile crustal material prior to the onset of the Sturtian glacial epoch, consistent with a basalt weathering trigger for initiation of the Sturtian glacial epoch (e.g.,  Goddéris et al., 2003; Rooney et al., 2014) . These ages confi rm the central prediction of the snowball Earth hypothesis of long-lived (~10 m.y.) glaciation with globally synchronous deglaciation.', "INTRODUCTION\nAfter more than one billion years without robust evidence of glaciation, Cryogenian (ca. 850-635 Ma) strata record arguably the most extreme episodes of climate change in Earth's history. The widespread occurrence of lowlatitude glacial deposits on every paleocontinent, coupled with the unique geochemistry and sedimentology of cap carbonates  (Hoffman et al., 1998; Bao et al., 2008) , inspired the snowball Earth hypothesis  (Kirschvink, 1992) . However, the general paucity of radiometric age constraints from multiple paleocontinents for the onset and demise of Cryogenian glaciations (Sturtian ca. 717-660 Ma, and Marinoan ending ca. 635 Ma), as well as reports of putative pre-Sturtian glaciations  (Frimmel et al., 1996) , has fostered doubts about the synchronicity and global extent of these events (e.g.,  Allen and Etienne, 2008; Kendall et al., 2006) .", 'DISCUSSION\nThe existence of a pre-Sturtian, global Kaigas glaciation has been suggested from the apparent relationship between inferred glacial deposits and the following age constraints: a 741 ± 6 Ma Pb-Pb zircon evaporation age in the Gariep belt of the Kalahari craton  (Frimmel et al., 1996) ; a 740 ± 7 Ma U-Pb SHRIMP age from near the base of the Bayisi diamictite on the Tarim craton  (Xu et al., 2009) ; and a 735 ± 5 Ma U-Pb SHRIMP age from the Kundelungu Basin of the Congo craton  (Key et al., 2001) . However, previously published U-Pb and Re-Os ages from time-equivalent strata in Laurentia  (Karlstrom et al., 2000; Macdonald et al., 2010a; Strauss et al., 2014)  and the Re-Os age presented here from the Callison Lake Formation (Fig.  2A ) document nonglacial sedimentation from ca.']</t>
         </is>
       </c>
-      <c r="AF219" t="inlineStr"/>
+      <c r="AF219" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Substantiated",
+  "explanation": "The reference article confirms that the Sturtian glaciation occurred between 717-660 Ma, and Excerpt 1 specifically mentions a long duration (&gt;55 m.y.) of this glacial epoch. Although the exact phrase 'most dramatic and longest global glaciation' is not present in the provided excerpts or abstract, the data presented supports the notion that the Sturtian glaciation was a significant and prolonged event."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="220">
       <c r="A220" t="inlineStr">
@@ -32361,7 +33982,16 @@
           <t>['Pseudomonas is also recognized as a common rhizosphere colonizing bacteria. Cloned 16S rRNA genes affiliated with Pseudomonas were also infrequently recovered from rhizosphere soil samples  [30] . Pseudoxanthomonas has been known to use as bioremediation as reported earlier by Sanchez et al.  [31] . Most interestingly, the economically important phyla Actinobacteria was the second dominant group in our clone library, and among most dominant OTUs with 5 clone sequences was close relative of genera Streptomyces. This genera is of economical importance because of its antibiotic producing ability. Streptomyces, act as antagonists to many different phytopathogenic fungi, detection of chitinolytic activity of Actinomycetes also makes them promising candidates as biocontrol agents for diverse fungal diseases. Presence of phyla Actinobacteria in the rhizosphere opens the possibility of exploring them to identify members with antagonistic properties toward some economically hazardous plant pathogens.', 'Out of 35, 13 OTUs from phylum Proteobacteria showing less than 94% similarity against published database, contributed by Alpha-, Beta-, Gammaproteobacteria sub groups 7, 2 and 4 OTUs respectively, whereas 5, , from Chloroflexi, Firmicutes, Actinobacteria, TM7, Acidobacteria, Verrucomicrobia, Gemmatimonadetes, Bacteroidetes, and Planctomycetes respectively (Table  2 ).\n\nDiscussion\nEarlier studies have been made regarding microbial diversity in maize rhizosphere using various culture dependent as well as independent methods like SSCP, DGGE, Biolog, FAME (Fatty acid methyl esters), ARISA (Automated Ribosomal Intergenic Spacer Analysis), 16S rDNA restriction fragment length polymorphism (RFLP), cultivation based method etc.  [17, 18, 19] . In the present study, 16S rRNA gene sequence analysis was used to estimate the bacterial diversity in the maize rhizosphere. One advantage of sequence analysis is that the generation of sequence data can be used to design group-specific probes and primers for further studies.', 'However extra data are necessary, to prove occurrence of new phylotypes, as only a fragment of the 16S rRNA gene was analyzed. The observation that sequences related to Proteobacteria phylum made up the largest fraction of clone library in this study is consistent with previous findings that the phylum Proteobacteria, which is metabolically versatile and genetically diverse, comprises the largest frac- tion of the bacterial community in soil ecosystems, including the rhizosphere  [26] . The representation of genera Devosia is interesting as, previously these genera have been detected as a nitrogen fixing nodule former in Neptunia natans (L.f.) Druce  [27] , other dominant phylotypes were relatives of well known genera Rhizobium/ Mesorhizobium/ Rhodoplanes. 16S rRNA gene fragments related to Rhizobium was also recovered from maize roots and it was noted that pea was grown in the field site prior to maize cultivation  [28] . It is also possible that Rhizobium is a native member of non-legume rhizospheres  [29] .']</t>
         </is>
       </c>
-      <c r="AF220" t="inlineStr"/>
+      <c r="AF220" t="inlineStr">
+        <is>
+          <t>Here is my evaluation:
+{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article does not provide any information on the relative abundance of Pseudomonas in the maize rhizosphere. While it mentions that Pseudomonas is a common rhizosphere colonizing bacteria, it does not quantify its abundance or compare it to other bacterial communities."
+}
+I chose "Unsubstantiated" because the reference article does not provide any specific information on the relative abundance of Pseudomonas in the maize rhizosphere, which is the claim made in the citation statement. While it mentions that Pseudomonas is a common colonizer of the rhizosphere, this is not sufficient to support the specific claim about its relative abundance.</t>
+        </is>
+      </c>
     </row>
     <row r="221">
       <c r="A221" t="inlineStr">
@@ -32501,7 +34131,14 @@
           <t>["Inoculation of microcosms, planting, and harvesting were carried out under sterile conditions so as to minimize contamination of the microcosms. Two sets of high and low lines were initiated in which the size of the soil inoculum differed by two orders of magnitude (6.0 g vs. 0.06 g). Each line consisted of 15 units and the 3 units with the highest (or lowest) value of the phenotypic trait were used as parents by combining the soil from the 3 units into a slurry that was used to inoculate the ''offspring'' generation of units. Fifteen microcosms per generation for the high and low treatments of the 6.0-g and 0.06-g inoculum sizes and two control treatments led to a total of 90 microcosms per generation for the complete experiment, which was continued for 16 35-day ecosystem generations. In generations 1 through 9, we ran sterile control treatments to serve as baselines that consisted of high and low selection lines inoculated with autoclaved 6.0-g slurries.", 'Nor were there any significant differences or trends when comparing sterilized, nonselected 6.0-g inocula and 0.06-g inocula in generations 11-15 (no control treatments were run in generation 16). In the aquatic experiment, the pH of the nonselected control line closely resembled that in the line selected for greater acidity, indicating that the divergence between the experimental lines largely was attributable to ecosystem selection for decreased acidity. Response to selection at the phenotypic level presumably requires an underlying change in ecosystem processes that cause the phenotypic traits in a proximate sense. We tested this proposition for the 6.0-g soil experiment by analyzing the soil of the control, high, and low lines at the time of harvest during generations 13 and 14. The discriminant function analysis (Fig.  3 ) clearly discriminates among the three lines on the basis of soil properties. Because the soil was identical at the beginning of each generation, these differences reflect a divergence in the biotic components of the ecosystems that change the soil chemistry over the course of a generation.', 'In the case of our soil ecosystem experiment, we might imagine genes in soil organisms that have positive or negative effects on plant biomass, with variation among ecosystems caused by sampling error. Ecosystems initiated by small numbers of soil organisms may possess sufficient variation for ecosystem-level selection to operate, but not ecosystems initiated by large numbers of soil organisms. By this reasoning, our experiment should not have worked because variation caused by sampling error would be negligible in ecosystems initiated by 6.0 g of soil, which contains many millions of microbes comprising thousands of species  (4) (5) (6) . Also, if variation among ecosystems is caused purely by sampling error, it should have been greater in our 0.06-g experiments than our 6.0-g experiments, which differed by two orders of magnitude in the number of organisms initiating each ecosystem. The substantial phenotypic variation observed in our experiments (and also in artificial selection experiments at the group and two-species community levels) reveals that something is wrong with theoretical reasoning based on simple interactions. In real biological systems, phenotypic traits often are caused by complex interactions among components of the system.']</t>
         </is>
       </c>
-      <c r="AF221" t="inlineStr"/>
+      <c r="AF221" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article discusses artificial ecosystem selection and its applications, but does not mention using this approach to improve plant or animal health. The article focuses on shaping the properties of whole ecosystems through artificial selection procedures, which is unrelated to the statement's claim."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="222">
       <c r="A222" t="inlineStr">
@@ -32642,7 +34279,14 @@
           <t>['This model synthesizes in vitro and in vivo observations to make testable predictions about the spatial structure of mature dental plaque, but a direct test of the model by highresolution imaging has not previously been undertaken. The study of microbial communities has been revolutionized by metagenomic and metatranscriptomic approaches, which have\n\nSignificance\nThe physiology and ecology of complex microbial communities are strongly dependent on the immediate surroundings of each microbe, including the identity of neighboring microbes; however, information on the micron-scale organization of microbiomes is largely lacking. Using sequencing data combined with spectral fluorescence imaging, we have discovered a multigenus, highly organized microbial consortium in human dental plaque. The spatial structure of the consortium reveals unanticipated interactions and provides a framework for understanding the organization, metabolism, and systems biology of the microbiome and ultimately, its effect on the health of the human host. Our synthesis of high-throughput sequencing data with spatial and structural information shows the informative value of microbial biogeography at the micron scale. revealed enormous complexity  (10) .', 'With deep sequencing, it has become clear that many taxa in the oral microbiota are shared across individuals but are abundant in some samples and almost vanishingly rare in others  (19, 38) . These differences in abundance may result from real differences between individuals, fluctuations within a single individual over time, or a combination of the two. Whatever its cause, the lack of a consistently abundant microbial "core" has led to the idea that perhaps it is not organisms but genes and functions that are conserved within the microbiome, distributed across a variety of organisms whose identities are irrelevant. The discovery of hedgehog consortia argues against this idea, at least for some microbiomes. The consistency of the composition and structure of the hedgehog across many individuals suggests that organisms are highly relevant to understanding the roles, organization, and dynamics of the members of the consortium. We suggest that it is neither necessary nor desirable to disregard taxonomy and reduce the microbiome to a collection of genes or metabolites unmoored from their source organism. Instead, we suggest the converse, that an understanding of the ecology and physiology of the organisms in the consortium will provide an organizing principle for understanding and interpreting metagenomic and metatranscriptomic data.', 'Based on our observations and the literature, we propose a model for plaque microbiome development and maintenance consistent with known metabolic, adherence, and environmental considerations. The consortium illustrates how complex structural organization can emerge from the micron-scale interactions of its constituent organisms. The understanding that plaque community organization is an emergent phenomenon offers a perspective that is general in nature and applicable to other microbiomes.\nbiofilm | imaging | microscopy | microbial ecology B iogeography-the study of the distribution of organisms across the globe-seeks to recognize patterns in the spatial distribution of organisms and discover the forces that underlie those patterns. Bacteria are micron-sized, and many of the forces and factors that underlie their distributional patterns operate at micron scales and are qualitatively different from the large-scale factors, such as climate, that drive traditional biogeography. To frame the analysis of microbial distribution patterns at the scale that microbes themselves experience, we introduce the concept of micron-scale biogeography: the study of the distribution of microbes relative to micron-scale features of their environment. These features include the host or inanimate surfaces on which the microbes reside as well as local gradients of nutrients and oxygen.']</t>
         </is>
       </c>
-      <c r="AF222" t="inlineStr"/>
+      <c r="AF222" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Substantiated",
+  "explanation": "The reference article (15) supports the citation statement by demonstrating the existence of complex, stable, and predictable microbial communities associated with a specific site (human oral microbiome). The abstract and excerpts describe a multigenus consortium in dental plaque, revealing unanticipated interactions and providing a framework for understanding the organization, metabolism, and systems biology of the microbiome. This supports the claim that research has identified complex yet stable and predictable microbial communities associated with specific sites on and within animals."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="223">
       <c r="A223" t="inlineStr">
@@ -32782,7 +34426,14 @@
           <t>['[34] Our final predicted cropland extent of 15.0 million km 2 in year 2000 amounts to roughly 12% of the global land area (excluding Greenland and Antarctica), and pasture extent of 28.0 million km 2 amounts to 22% of global land area. Thus humans are using 34% of the global land area for their agricultural needs.\n\nGeographic Distribution of Croplands and Pastures in Year 2000\n[35] We analyzed the distribution of agricultural regions by 14 different regions of the world (Table  5 ). The greatest proportion of croplands in the world are found in South Asia, Europe, Southeast Asia, and United States, east of the Mississippi, while the greatest proportion of pastures are found in Argentina, Uruguay and Chile, Pacific developed countries, China, Mexico and Central America, United States, west of the Mississippi, and tropical Africa. The smallest proportion of croplands are found in Canada, the Pacific developed Countries, and northern South America, while the smallest proportion of pastures are found in Southeast Asia, Canada, and United States, east of the Mississippi.', 'Results\n\n\nTotal Global Area of Croplands and Pastures in 2000\n[32] Our final results (Figure  6 ) indicate that there were 15.0 (95% confidence range of 12.2-17.1) million km 2 of crop-land and 28.0 (95% confidence range of 23.6-30.0) million km 2 of pasture in the world in the year 2000. This compares to 15.3 million km 2 of cropland and 34.4 million km 2 of pasture reported by the FAOSTAT database. Thus we predict significantly lower extent of pasture (by 6.1 million km 2 or $18% lower) than reported by FAO. Our own inventory data reports 15.0 million km 2 of cropland and 31.5 million km 2 of pasture. Thus our inventory data for pasture is already lower than FAO statistics; this difference was explained earlier in section 2.2.', 'For croplands, this includes temporary fallow lands (less than 5 years), which are not cultivated. It is not clear how strictly this restriction of less than 5 years was applied when accounting for fallow land. For example, the U.S. data on croplands used by FAOSTAT includes idled cropland, which includes land under the Conservation Reserve Program that amounts to roughly 9% of the total cropland area, and is often idled for longer than 5 years  [Lubowski et al., 2002] . Secondly, in tropical nations characterized by extensive fallow cropping systems, such a definition may include much land that is not currently cultivated, and therefore portray a misleading picture of what may be commonly thought of as cropland. Finally, these definitions of croplands say nothing about the productivity of the land, but this is the topic of our companion article  [Monfreda et al., 2007] . [45] The definition of pasture is subject to even greater uncertainty.']</t>
         </is>
       </c>
-      <c r="AF223" t="inlineStr"/>
+      <c r="AF223" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Substantiated",
+  "explanation": "The reference article (15) explicitly states that there were 15.0 million km2 of cropland, which amounts to roughly 12% of the global land area (excluding Greenland and Antarctica), supporting the citing article's claim that croplands cover 12% of Earth’s ice-free land area."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="224">
       <c r="A224" t="inlineStr">
@@ -32929,7 +34580,18 @@
           <t>["Several points are salient. First, as expected given that India has not liberalized multi-brand retail FDI, the rate of multinationalization is low and its impact in this second phase on Indian retail modest, and cash &amp; carry, large, so far. In 2010, about 7 percent of total only-retail sales (like Latin America in the early 1990s) and 99 percent of major cash and carries (like Latin America now), i.e. in India 0.75 billion USD of sales was done by FDI firms (sole or joint venture), hence 15 percent of the total of modern-private retail and wholesale chain sales. Second, domestic modern-retail capital is from a mix of sources, according to the investing company's characteristics.", '4. Third surprise: private-retail revolution with unique Indian characteristics Various characteristics, especially of the second phase of the third wave -the private retail chain boom -are surprising, both to India, and about India compared with the past two decades of developing country modern retail diffusion. The essence of the differences is twofold. First, India has done what few other developing countries have done: started a supermarket revolution with domestic capital without relying at first on the push from retail FDI. Second, India has done what most other developing countries have done -but done them "earlier" (in the evolution of modern retail in the country), more simultaneously, more experimentally, more variously. We lay out the surprising differences below.\n\nPrimarily domestic investment\nIt is common for domestic (family company) capital to be important in the earliest stages of supermarket development in developing countries, but for the "take-off" some sector well-endowed with capital steps in and drives the investment. Sometimes that sector leads and then other sectors compete in investment and thus the aggregate investment grows.', 'Moreover, the most heated debate related to retail at this very moment (mid 2011) is whether multi-brand retail FDI should be liberalized. We do not take a side in this debate. We simply note what our findings suggest: whether or not retail FDI is liberalized, modern retail diffusion looks on the path to continue, even at its rapid pace of several times GDP growth, for some time. The "drivers" on the demand and investment supply side do not look to diminish. FDI liberalization may accelerate it, would probably (by definition) multinationalize it, may increase the overall level of retail "development" by bringing more international experience and technologies to bear; it would probably (as it has in China and elsewhere) create more "procurement doors" for two way flows of imports of products, and exports of Indian agricultural goods. Researchers focussed on food industry, agricultural economics, and agribusiness have a rich agenda before them to explore empirically, with rigorous surveys, the impacts on supply chains, and their actors of the emerging supermarket revolution in India.']</t>
         </is>
       </c>
-      <c r="AF224" t="inlineStr"/>
+      <c r="AF224" t="inlineStr">
+        <is>
+          <t>Here is my evaluation:
+```
+{
+  "label": "Substantiated",
+  "explanation": "The reference article supports the claim of an 'emerging supermarket revolution in India' driven by domestic capital. Excerpt 2 explicitly mentions that India has started a supermarket revolution with domestic capital without relying on foreign direct investment, which aligns with the statement."
+}
+```
+I chose "Substantiated" because the relevant excerpt (Excerpt 2) clearly states that India's supermarket revolution is driven by domestic capital, which directly supports the claim made in the citation statement. The article provides evidence and analysis of the unique characteristics of Indian private retail chain development, including its reliance on domestic capital investment.</t>
+        </is>
+      </c>
     </row>
     <row r="225">
       <c r="A225" t="inlineStr">
@@ -33069,7 +34731,14 @@
           <t>['INTRODUCTION\nThe growing demands for safer lithium-ion batteries (LIBs) with higher capacity and longer durability have led to the search for nextgeneration electrode materials. Although the most widely used graphite anodes in LIBs have good cycling performance with a theoretical capacity of 372 mAh g À1 (LiC 6 ), other group IV semiconductors (Si, Ge, Sn) can offer significantly higher capacities: 4200 mAh g À1 for Li 4.4 Si, 1600 mAh g À1 for Li 4. 4 Ge, and 990 mAh g À1 for Li 4.4 Sn.  1, 2  In addition to the large increase in energystorage capacity, lithiumÀgroup IV alloys (LiÀM, M = Si, Ge, Sn) also have a safe thermodynamic potential, making them attractive candidates for LIB anodes. However, the practical use of Si, Ge, or Sn as an anode material is hindered by its poor cycling ability.', 'In particular, the large volume change during the lithiation/delithiation process (up to 400% for Si, 370% for Ge, and 300% for Sn)  3À5  can cause cracking and pulverization of the electrodes. Considerable efforts have been made to overcome these problems through structural modifications  6À11  and alloying with active/inactive elements.  12À16  First-principles calculations have also been applied to investigate fundamental aspects of the lithiation behavior and structural evolution of the anode materials, yet many of which still remain unclear. Despite the similarities shared among the group IV materials, Si has received the most attention because of its highest known capacity, whereas the analogous systems have not been studied as closely, and some of their merits as an anode material may have been overlooked in the past. For instance, the diffusivity of Li in Ge is about 400 times greater than that of Li in Si at room temperature,  17  which may contribute to faster charge/discharge rates.', 'Thus far, there has been no comprehensive comparison study on Si, Ge, and Sn as to the dynamic behavior of Li incorporation, the stability of the host lattices, and the properties of the alloys formed during lithiation. The Journal of Physical Chemistry C\n\nARTICLE\nIn this paper, we first examine the structure, stability, Li diffusion, LiÀLi interaction, and how the host lattice M (M = Si, Ge, and Sn) is affected by Li insertion using density functional theory (DFT) calculations. The group IV elements are found to adopt the diamond crystalline structure, which allows a comparative study on the nature of Li in different host materials, but the same diamond structure. Although other allotropic structures are found for Ge and Sn (β-Ge and β-Sn 18 ), they do not serve a particular interest in this study. We then examine the structure, energetics, and mechanical and electronic properties of LiÀM alloys. The structural evolution in terms of Li content is analyzed for both crystalline and amorphous phases, and the relative stabilities of the alloys are evaluated based on their mixing enthalpies.']</t>
         </is>
       </c>
-      <c r="AF225" t="inlineStr"/>
+      <c r="AF225" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article does not mention nanoporous Li_xSi–Li_2O composite or its formation under vigorous stirring. The article primarily focuses on a comparative study of the structure, energetics, and properties of Li–M (M = Si, Ge, Sn) alloys using density functional theory calculations."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="226">
       <c r="A226" t="inlineStr">
@@ -33209,7 +34878,14 @@
           <t>['[1]  Easily found in nature, such as opals,b ird feathers,a nd butterfly scales,s tructural color is brilliantly iridescent, metallic,a nd free from photobleaching unlike conventional pigments or dyes.Most colloidal assembly processes mimic the formation of opals and create close-packed structures from monodisperse colloidal spheres.H owever,l iving systems often involve non-closepacked ordered assemblies of anisotropic motifs,s uch as plates and rods,t hus display significantly more complex structural color responses including strong angular dependence and polarization effect.  [2]  Prior efforts have been made to organizing elongated particles,s uch as polystyrene and ZnS,  [3]  albeit the assembly methods are rather conventional and the resulting crystals do not exhibit different photonic responses to those from spherical particles. One of the important advantages of anisotropic particles is that they often have shape-dependent physical and chemical properties,which can add more degrees of freedom for manipulating the collective properties of the resultant superstructures.This is of particular interest to the fabrication of field-responsive colloidal photonic structures,i nw hich static or dynamic structural changes are usually accompanied by switching of photonic properties.', 'Unlike our previously demonstrated one-dimensional photonic assembly which only shows single color stripes at areas with field parallel to the incident angle,  [5a]  the current system displays red and blue stripes at areas with parallel and horizontal fields,and atransitional green stripe in between at off-angle areas. In addition to orientation, the interplanar spacing of the photonic assemblies is also determined by the volume fractions of the nanoellipsoids.  [4b]  As the volume fraction decreases,t he distance between nanoellipsoids increases, resulting in the expansion of crystal lattice as well as redshift of reflection wavelength. In the absence of magnetic fields,the reflection spectra of photonic assemblies formed by NE-A under different volume fractions were recorded (Figure  4a ). Ther eflection peak shifted from 425 nm to 660 nm, as the volume fractions decreased from 32 %t o1 0%. Consistently,arainbow-like color effect was observed (Figure  4b )i nt he dispersion of NE-A with av olume fraction gradient, which was achieved by centrifugation at 3000 rpm for 5min.', 'Assembled from uniform shape-and magnetically anisotropic nanoellipsoidal particles,t he novel colloidal crystals diffract at am inimum wavelength when the field direction is perpendicular to the incident angle and am aximum wavelength when the field is switched to parallel. Thed iffraction intensity reaches maximum values when the field is either parallel or perpendicular to the incident light, and decreases when the field direction is off-angle,displaying aunique U-shaped profile in reflectance peaks.The current system not only allows more opportunities in studying the assembly behavior of shape-and magnetically anisotropic nanostructures but also provides an ew platform for building novel active optical components for various color presentation and display applications. Keywords: anisotropic nanomaterials •magnetic properties • photonic structures •s elf-assembly']</t>
         </is>
       </c>
-      <c r="AF226" t="inlineStr"/>
+      <c r="AF226" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article discusses magnetically responsive photonic structures and their tunable properties, but it does not mention structural color hydrogels or their applications in switches, optical devices, sensing materials, or wearable electronics."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="227">
       <c r="A227" t="inlineStr">
@@ -33349,7 +35025,14 @@
           <t>['Introduction\nBecause it is conservative, has low natural background levels, and is readily measured with adequate precision, chloride has long served as a general indicator of anthropogenic impacts on Great Lakes water quality. Beyond its utility as an indicator, chloride can also have direct adverse impacts on lakes and other freshwater ecosystems. The Canadian federal government has recommended that road salt be added to the List of Toxic Substances under the Canadian Environmental Protection Act because of tangible threats of serious or irreversible environmental damage  (Environment Canada and Health Canada, 2001) . It has also been suggested that increases of chloride and other ions could be directly harmful to the Great Lakes ecosystem by fostering the spread of less-desirable halophilic organisms  (Stoermer, 1978) . More generally, trends of all major anions and cations are relevant as they contribute to aspects of lake chemistry such as ionic strength, pH and acid neutralizing capacity. Finally, at sufficiently high concentrations, chloride can influence density stratification as well as degrade the taste of drinking water. Two classic papers first established that Great Lakes chloride levels had increased significantly over the past century.', 'Chloride is not currently tracked in the National Pollutant Release Database. For a small number of inorganic chemical plants, the Province of Ontario requires chloride discharges to be monitored, but these likely constitute only a small portion of the total chloride releases. The fact that it is difficult to definitively understand why levels are currently increasing reinforces the need for both continued and expanded monitoring and modeling of the Laurentian Great Lakes. The USEPA and EC monitoring programs have provided an excellent database for detecting long-term trends of whole-lake concentrations. Comparison of the variability of the historical and modern data in Fig.  3  clearly demonstrates the value of having long-term, systematic data collection efforts with high quality control. Whereas the early data were certainly valuable in raising concerns, as demonstrated in the present study, a meaningful trend analysis is predicated on more precise measurements of the quality collected by EPA and EC. Unfortunately, the same cannot be said regarding direct loading measurements. Whereas major efforts were expended estimating loadings in the 1970s (notably those conducted under the auspices of the International Joint Commission), these programs have been effectively decommissioned.', 'As reported by  Sonzogni et al. (1983) , increases in chloride effluent concentration from these additions are on the order of 10 mg/L. Hence, the addition would not significantly increase normal effluent concentrations. Because sewage effluent is a relatively small component of the total chloride load, it is doubtful that the additional ferric chloride inputs could account for the recent increases.\n\nNew industrial sources\nThe second way in which loading might still be increasing would be if new industrial chloride discharges had begun entering the system since 1980. Because chloride loading is currently not being monitored, there is no available evidence pointing to significant new dischargers. The U.S. NPDES (National Pollutant Discharge Elimination System) permit program regulates pollutants in point-source discharges as needed to act in accordance with the technology-based, and water-quality-based requirements of the Clean Water Act. Where appropriate, NPDES permits may include limits and monitoring requirements to comply with the requirements of Effluent Guidelines, Water Quality Standards, or Total Maximum Daily Loads (TMDLs). Information regarding permit requirements is tracked using the ICIS/ PCS (Integrated Compliance Information System/Permit Compliance System) databases.']</t>
         </is>
       </c>
-      <c r="AF227" t="inlineStr"/>
+      <c r="AF227" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Substantiated",
+  "explanation": "The reference article supports the claim that elevated chloride concentrations can have adverse effects on water quality and aquatic ecosystems. Excerpt 1 explicitly states that chloride can have direct adverse impacts on lakes and other freshwater ecosystems, and mentions tangible threats of serious or irreversible environmental damage."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="228">
       <c r="A228" t="inlineStr">
@@ -33489,7 +35172,14 @@
           <t>['The proportion of regulated proteins closely paralleled the total number of phosphorylations of nuclear proteins. As expected, proteins annotated as extracellular were significantly underrepresented in the phosphoproteome. Although there is evidence of a mitochondrial phosphoproteome  (Pagliarini and Dixon, 2006) , proteins annotated as mitochondrial by GO were underrepresented, as were plasma membrane proteins. As membrane proteins are often of low abundance and we did not specifically enrich the plasma membrane in this analysis, we are less likely to identify phosphorylation events associated with them. Conversely, proteins associated with the cytoskeleton, which are generally of higher abundance, were almost twice as likely to be detected in the phosphoproteome as compared with their proportion in the database, and they accounted for an even higher share of the regulated sites. This illustrates that, at the current state of technology, our phosphopeptide screen is still not comprehensive. We may also miss certain phosphopeptides that are either too small or too large in mass to be readily measurable in our current MS setup. Therefore, absence of a phosphorylation site from our data set does not necessarily mean that it does not exist.', 'Another contributing factor may be the fact that pY is less stable in phosphoamino acid analysis than pS/pT, whereas we have found no evidence that the phosphopeptide enrichment method discriminates between these modification types. We next averaged the time profiles of the upregulated phosphorylation sites and normalized them to their maximal fold change. Figure  2D  shows that, on average, dynamic changes in tyrosine phosphorylation occur much faster and from a lower basal level compared to serine/ threonine phosphorylation. We found phosphorylation sites on a wide variety of proteins, and about half the proteins contained more than one site (Table  S2 ). Figure  2E  shows a Gene Ontology (GO)  (Zeeberg et al., 2003)  analysis of the in vivo phosphoproteome. GO localization information existed for 1,589 of the 2,244 phosphoproteins. Almost half of the phosphorylation events occurred on nuclear proteins, whereas only one-third of all proteins in the database were assigned as nuclear by GO, indicating that phosphorylation preferentially targets nuclear proteins.', 'Given that we have observed 2,244 phosphoproteins in a single cell line and taking into account the sensitivity and dynamic range limitations of current MS technology  (de Godoy et al., 2006) , it is clear that a large proportion of cellular proteins are phosphorylated. We compared our data set with all annotated human phospho-sites in the SwissProt database from experimental data or inferred from homologous sequences (3,262 sites in version 48.0) and also included four previous phosphoproteomics data sets in our analysis  (Amanchy et al., 2005; Beausoleil et al., 2004; Stover et al., 2004; Thelemann et al., 2005) . We found that more than 90% of our sites were novel with respect to SwissProt. From the four previous data sets, we were able to map 1,890 sites onto IPI version 3.13. Of these, 691 (37%) were also found in our data set (Table  S5 ). Given that the previous studies generally used lower-resolution MS and different experimental conditions, this is a relatively high value.']</t>
         </is>
       </c>
-      <c r="AF228" t="inlineStr"/>
+      <c r="AF228" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Substantiated",
+  "explanation": "The reference article [17] states that 'almost half of the phosphorylation events occurred on nuclear proteins', indicating that phosphorylation preferentially targets nuclear proteins. This directly supports the claim from the citing article."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="229">
       <c r="A229" t="inlineStr">
@@ -33632,7 +35322,14 @@
           <t>["In general, there was better agreement about the diagnosis when eburnation was present, although three of the experts and two of the beginners did not diagnose specimen 10 as having osteoarthritis even though there was an obvious area of eburnation on the inferior surface of the head of this metatarsal. O n e practical outcome of this study must be that greater efforts will need to be taken to agree on the criteria &gt;for the classification of pathological changes in palaeopathology. What is required for palaeopathological work is the development of operational definitions, since it is not valid entirely t o rely on either clinical or radiological diagnoses. For example, we have shown that radiology is not reliable in detecting changes that are evident to the palaeopathologist.' Finally, these results demonstrate that great care must be taken when comparing disease frequencies between studies unless the authors cite the criteria used in arriving at their classifications o r use a common, agreed source of reference.", "Introduction\nIn epidemiological studies of joint diseases, where results from different observers are to be compared, it is common to estimate the degree of variation between the observers;l'Z if the variation is small, then the conclusions drawn from such studies will have more credibility than if it is great. Now that epidemiological techniques are increasingly being applied to palaeopathology it seemed important to make some assessment of the extent of inter-observer variation amongst its practitioners when scoring diseased joints, since to the best of our knowledge this has not been attempted before.\n\nMaterials and methods\nEach of the specimens used in the study (and illustrated in Figure  1 ) was considered to have 1047-482x/91/010049-08$05.00 @ 1991 by John Wiley &amp; Sons, Ltd the features of osteoarthritis by the criteria that we have published b e f ~r e . ~ Briefly, these criteria state that osteoarthritis is present when there is eburnation on the joint surface or, in the absence of eburnation, when two of the following are present: marginal osteophytes, new bone on the joint surface, pitting on the joint surface or deformation of the joint contour.", 'We choose all ten as meeting our published criteria €or osteoarthritis in palaeopathological material and so, to some extent, this was a test of the acceptance of our criteria. As it was, the experts were unanimous on three specimens only ( 1 , 3 and 6 ) and the beginners were unanimous only about specimen 6 . There was a significant difference in the number of experts and beginners only over the diagnosis of specimen 7; 94.7% of the experts considered it to have osteoarthritis but only 54.5% of the beginners. Considering this result, and some of the other results pertaining to specimen 7, it seems likely that some of the participants were scoring the wrong joint. The inferior facet joint (shown in Figure  1 ) had very obvious eburnation and scoring on the joint surface and could not possibly have been mistaken for anything other than osteoarthritis; the fact that so many people did misdiagnose it suggests that they were actually scoring the normal, superior facet joint; this, at least, is our most charitable explanation.']</t>
         </is>
       </c>
-      <c r="AF229" t="inlineStr"/>
+      <c r="AF229" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Substantiated",
+  "explanation": "The reference article [26] supports the claim that interobserver variation in identifying osteophytes in skeletal samples is high. The study found that even among experts and beginners who scored specimens for osteoarthritis, there was little agreement on the diagnosis, with unanimous agreement only in a few cases. This suggests that relying solely on visual examination of skeletal remains can lead to inconsistent results."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="230">
       <c r="A230" t="inlineStr">
@@ -33772,7 +35469,19 @@
           <t>['Although no polyhedral analysis was carried out, the usefulness of these inequalities has been demonstrated through computational experiments. A comparison with version 8.1 of CPLEX shows that the branch-and-cut algorithm proposed here reduces both the CPU time and the number of nodes explored in the branch-and-bound tree. The methodology proposed in this paper obviously cannot be used to solve large-scale instances containing hundreds or thousands of users as it is sometimes the case in large cities. It is, however, fast enough to be used as a post-processor to optimize individual routes or small subsets of routes produced by a meta-heuristic. In the presence of ride time constraints, using dynamic programming would be difficult since the states of the dynamic programming algorithm would have to take into account the individual ride time of each user. Future work will concentrate on the development of more refined separation procedures for the various types of inequalities introduced in this paper. for U 1 must visit node n + i 2 before visiting node i 1 . In addition, this path must appear immediately before the arc (i 1 , n + i l ) in the solution. Now, for k = 2, . . .', 'j ∈ N, k ∈ K (8) L k i = B k n+i -(B k i + d i ) ∀i ∈ P, k ∈ K (9) B k 2n+1 -B k 0 ≤ T k ∀k ∈ K (10) e i ≤ B k i ≤ l i ∀i ∈ N, k ∈ K (11) t i,n+i ≤ L k i ≤ L ∀i ∈ P, k ∈ K (12) max{0, q i } ≤ Q k i ≤ min{Q k , Q k + q i } ∀i ∈ N, k ∈ K (13) x k ij ∈ {0, 1} ∀i ∈ N, j ∈ N, k ∈ K. ( 14 ) The objective function (1) minimizes the total routing cost. Constraints (2) and (3) ensure that each request is served exactly once and that the origin and destination nodes are visited by the same vehicle. Constraints (4)-(  6 ) guarantee that the route of each vehicle k starts at the origin depot and ends at the destination depot.', 'Consistence of the time and load variables is ensured by constraints (  7 ) and (8). Equalities (9) define the ride time of each user which is bounded by constraints (12). It is worth mentioning that the latter also act as precedence constraints because the non-negativity of the L k i variables ensures that node i will be visited before node n + i for every user i. Finally, inequalities (10) bound the duration of each route while (  11 ) and (  13 ) impose time windows and capacity constraints, respectively. This formulation is non-linear because of constraints (  7 ) and (  8 ). Introducing constants M k ij and W k ij , these constraints can, however, be linearized as follows: B k j ≥ B k i + d i + t ij -M k ij (1 -x k ij ) ∀i ∈ N, j ∈ N, k ∈ K (15) Q k j ≥ Q k i + q j -W k ij (1 -x k ij ) ∀i ∈ N, j ∈ N, k ∈ K.']</t>
         </is>
       </c>
-      <c r="AF230" t="inlineStr"/>
+      <c r="AF230" t="inlineStr">
+        <is>
+          <t>Here is the evaluation result in JSON format:
+```
+{
+  "label": "Substantiated",
+  "explanation": "The reference article [19] provides a mixed-integer programming formulation for the dial-a-ride problem, which is a type of multivehicle-routing problem. The article also mentions that the proposed branch-and-cut algorithm can be used to solve small to medium-size instances, implying that it provides anytime guarantees for these cases."
+}
+```
+Explanation:
+The citation statement claims that traditional approaches relying on integer linear program (ILP) formulation provide anytime guarantees for the multivehicle-routing problem. Reference [19] presents a mixed-integer programming formulation and a branch-and-cut algorithm for the dial-a-ride problem, which is a specific type of multivehicle-routing problem. Although the article does not explicitly mention "anytime guarantees," it demonstrates that the proposed approach can solve small to medium-size instances efficiently, which implies some level of guarantee. Therefore, the relevant part of the citation statement is substantiated by reference [19].</t>
+        </is>
+      </c>
     </row>
     <row r="231">
       <c r="A231" t="inlineStr">
@@ -33912,7 +35621,14 @@
           <t>['So far, the oldest known dinosteranes come from the ϳ1.1-Ga Nonesuch Shale, Michigan  (Summons and Walter, 1990) . The biologic precursor of dinosteranes is dinosterol that is commonly regarded as diagnostic for dinoflagellates  (Robinson et al., 1984; Summons et al., 1987 Summons et al., , 1992;; Moldowan et al., 1996; Moldowan and Talyzina, 1998) , although it has also been recorded in one diatom species as a minor component  (Volkman et al., 1993) . As fossil dinoflagellates (and diatoms) first appear in the Mesozoic, dinosteranes discovered in Paleozoic and Proterozoic sedimentary rocks were described as products of ancestral dinoflagellates (protodinoflagellates)  (Moldowan et al., 1996) . However, dinosteranes of Archean age have more likely a biologically independent origin, as ancestral dinoflagellates and diatoms almost certainly appeared much later in Earth history.', 'Sterols with the 4-methyl-24-ethylcholestane skeleton (C 30 ) have also been isolated from prymnesiophyte algae of the order Pavlovales  (Volkman et al., 1990) , and with the 4-methylcholestane skeleton (C 28 ) from the methylotrophic bacterium Methylococcus capsulatus  (Bird et al., 1971) . Regular 4-methylsteranes are therefore not sufficiently taxon-specific to interpret their occurrence in Archean bitumen below domain level. 4␣,23,24-Trimethylcholestanes (dinosteranes) also occur in trace amounts in the Archean bitumens  (Brocks et al., 2003) . Dinosteranes are abundant biomarkers in almost all Mesozoic and Cenozoic bitumens  (Moldowan et al., 1996)  but have also been detected in the Paleozoic and Proterozoic, albeit in lower concentrations  (Moldowan et al., 1996) .', 'Most bitumens throughout post-Archean Earth history contain similar distributions of C 26 to C 30 -steranes, A-ring methylated steranes, mono-and triaromatic steroids and their diagenetic rearrangement products  (Summons et al., 1988b) . The late Archean bitumens studied here also have the same general sterane and aromatic steroid pattern  (Brocks et al., 2003) . It is highly unlikely that such steranes in Phanerozoic and Proterozoic sediments had an eukaryotic source but had a prokaryotic origin in the Archean. Although it is possible that as yet unknown or extinct prokaryotic organisms produced sterols, the wide structural range of steranes present, their relative abundances like those of younger bitumens, and their marked dissimilarity to known prokaryotic examples is convincing evidence for the existence of eukaryotes in the late Archean  (contra Cavalier-Smith, 2002) . Although sterane distributions in the Archean bitumens are equivalent to those of younger bitumens, they offer no taxonomic information below domain level.']</t>
         </is>
       </c>
-      <c r="AF231" t="inlineStr"/>
+      <c r="AF231" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Substantiated",
+  "explanation": "The reference article supports the claim that 'traces of dinosteranes are also present in Archean bitumens', as stated in Excerpt 2: '4␣,23,24-Trimethylcholestanes (dinosteranes) also occur in trace amounts in the Archean bitumens'. Additionally, the article explains that these dinosteranes likely have a biologically independent origin and are not necessarily indicative of ancestral dinoflagellates or diatoms, which is consistent with the citing article's statement."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="232">
       <c r="A232" t="inlineStr">
@@ -34053,7 +35769,14 @@
           <t>["[ 14, 18, 24 ]  This effect is analogue to the prediction by Ioffe  [ 25 ]  about a half century ago, however, rather precise control of the impurity scattering strength is required to realize power factor and ZT improvements in heavily doped semiconductors.  [ 26 ]  Indeed, Ioffe's initial experimental work about PbTe gave no enhancement in power factor or ZT ,  [ 25 ]  and subsequently numerical calculations done by Ure  [ 24 ]  predicted no more than 10% enhancement in ZT by introducing ionized impurities. These may have contributed to the dormancy of studying the infl uence of ionized impurity scattering on thermoelectrics, and to the best of our knowledge only limited experimental results have been reported.", '[ 18, 27 ]  The strength of ionized impurity scattering depends not only on the effective concentration of impurities but also on\n\nOn Intensifying Carrier Impurity Scattering to Enhance Thermoelectric Performance in Cr-Doped Ce y Co 4 Sb 12\nShanyu Wang , Jiong Yang , Lihua Wu , Ping Wei , Wenqing Zhang , * and Jihui Yang * The benefi cial effect of impurity scattering on thermoelectric properties has long been disregarded even though possible improvements in power factor have been suggested by Ioffe more than a half century ago. Here it is theoretically and experimentally demonstrated that proper intensifi cation of ionized impurity scattering to charge carriers can benefi t the thermoelectric fi gure of merit ( ZT ) by increasing the Seebeck coeffi cient and decreasing the electronic thermal conductivity. The optimal strength of ionized impurity scattering for maximum ZT depends on the Fermi level and the density of states effective mass.', 'In the present study, by assuming the carrier transport being dominated by a mixed acoustic phonon and ionized impurity scatterings, we numerically illustrate that an increase in the strength of ionized impurity scattering could moderately improve the power factor by balancing the enhancement in Seebeck coeffi cient and the reduction of mobility, and thus appreciably enhance ZT for a given lattice thermal conductivity. This concept is further experimentally validated in Cr-doped Ce y Co 4 Sb 12 samples prepared by a traditional melting-annealing-sintering technique. Here Cr-doping at the Co sites has two effects: (i) adjusting the strength of ionized impurity scattering through increasing impurity concentration, and (ii) increasing Ce fi lling fraction limit (FFL) by charge compensation. The low FFL of Ce (≈0.1) in CoSb 3 is insuffi cient to optimize the electrical properties (the optimal doping concentration is ≈0.5 e per Co 4 Sb 12 , corresponding to y of ≈0.17 for Ce) or reduce κ L .']</t>
         </is>
       </c>
-      <c r="AF232" t="inlineStr"/>
+      <c r="AF232" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Substantiated",
+  "explanation": "The reference article [28] directly supports the claim that power factors can be enhanced via ionized impurity scattering. The abstract and excerpts demonstrate that proper intensification of ionized impurity scattering can benefit thermoelectric performance by increasing the Seebeck coefficient and decreasing electronic thermal conductivity, leading to high power factors."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="233">
       <c r="A233" t="inlineStr">
@@ -34194,7 +35917,14 @@
           <t>['Recently, Astier et al.  [21]  demonstrated that Tr1 function is also impaired in patients with MS. Moreover, the expression of the immunosuppressor cytokine IL-10 is diminished in MS patients  [22, 23] , in accordance with previous studies describing fewer IL-10-secreting peripheral blood mononuclear cells (PBMC). Interestingly, there is a reduction in the expression of IL-10 but elevated numbers of PBMC expressing IL-10 transcripts before clinical relapse in MS  [24] , and there is a correlation between IL-10 levels and IgG in the cerebrospinal fluid of MS patients  [25] . Engineered Th2/Tr1 cells that produce high levels of IL-10 prevent epitope spreading and ameliorate the disease course in animal models of MS  [26] . However, it is unknown whether the functional activity of IL-10 in MS is preserved, and attempts to treat MS patients with IL-10 have not been successful to date.', 'In order to explore the functionality of Tr1 regulatory function in MS, we assessed the ex vivo induction of the Tr1 phenotype and the response of CD4 + cells to the IL-10 produced by these cells in patients with MS. We found that CD4 + cells from MS patients were less disposed to differentiate into a Tr1 cell phenotype ex vivo and that, in addition, these cells produce less IL-10. Importantly, CD4 + cells from MS patients were more resistant to suppression by IL-10 because the IL-10R signaling cascade is defective in MS patients.\n\nResults\n\n\nIn vitro generation of CD46-induced Tr1 cells is impaired in MS patients\nIn healthy controls (n = 8), CD4 + cells stimulated in vitro with anti-CD46 + anti-CD3 and anti-CD28 antibodies for 3 days acquired a Tr1 phenotype (Fig.  1 ). The presence of surface CD25 and CD45RO in these cells increased by up to 68 and 63%, respectively (Fig.  1A ), while the intracellular levels of IL-10 rose up to 27% and the cells secreted up to 3566 pg/mL IL-10 protein (Fig.', 'Tr1 cells can be generated in vitro from CD4 + cells by stimulation with high doses of IL-10, alone or in conjunction with IFN-a  [11, 12] , by adding vitamin D and dexamethasone  [13]  or by stimulating CD46 on CD4 + cells with specific monoclonal antibodies  [14, 15] . By contrast, generation of Tr1 cells is inhibited by OX40L  [16] . Multiple sclerosis (MS) is a chronic inflammatory disease in which activated T and B cells infiltrate the central nervous system, provoking demyelination and axonal damage, which produces significant neurological disability  [17] . To date, the primary antigens against which the immune response is directed in MS remain unknown, but immunological dysfunction has been identified in patients with MS  [18] . Impairment of suppressor cell function has classically been demonstrated in patients with MS  [19] , and a few years ago, the functional impairment of natural CD4 + CD25 + Foxp3 + Treg cells has also been demonstrated  [20] . Recently, Astier et al.']</t>
         </is>
       </c>
-      <c r="AF233" t="inlineStr"/>
+      <c r="AF233" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Substantiated",
+  "explanation": "The reference article supports the claim that there are decreases in Tr1-like, IL-10-producing T cells. The abstract states that 'Tr1 cells isolated from MS patients produced less IL-10 than those obtained from controls.' Excerpt 2 also mentions that CD4+ cells from MS patients produce less IL-10 and are more resistant to suppression by IL-10 due to a defective IL-10R signaling cascade."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="234">
       <c r="A234" t="inlineStr">
@@ -34334,7 +36064,14 @@
           <t>["The microbial flora and its products have been shown to control T cell-dependent inflammation through several mechanisms including the conversion of precursors provided by the diet into immune regulatory metabolites  [13] [14] [15]  . However, less is known about the effects of the diet and microbial products on the inflammatory response of resident cells in the CNS. Here we identify an IFN-I and AhR axis that integrates immunologic, metabolic and environmental cues to regulate astrocyte activity and CNS inflammation.\n\nResults\n\n\nAstrocytes show a transcriptional response to IFN-I during EAE\nTo study the regulation of astrocyte function during autoimmune CNS inflammation, we induced EAE in C57Bl/6 mice by immunization with myelin oligodendrocyte glycoprotein 35-55 (MOG 35-55 ) in Complete Freund's Adjuvant (CFA) and analyzed mRNA expression in astrocytes by RNA-sequencing (Supplementary Figs.  1a , b ). We detected 17,964 expressed genes (Fig.  1a ), and found 1,879 transcripts that were differentially regulated in astrocytes during EAE compared to astrocytes from naive mice (Fig.", 'In individuals with MS, the circulating levels of AhR agonists were decreased. These findings suggest that IFN-I produced in the CNS act in combination with metabolites derived from dietary tryptophan by the gut flora to activate AhR signaling in astrocytes and suppress CNS inflammation.\nAstrocytes are the most abundant cell population in the central nervous system (CNS). They participate in diverse functions including control of the blood-brain barrier (BBB), the regulation of metabolism, the modulation of neuronal transmission and CNS development and repair  [1] [2] [3] [4] [5] [6] [7] [8] [9]  . Astrocytes also play important roles during CNS injury and disease, and are thought to participate in the pathogenesis of multiple sclerosis (MS) and its animal model experimental autoimmune encephalomyelitis (EAE)  [10] [11] [12]  . Astrocyte activity is affected by factors produced within and outside the CNS, therefore, the study of these factors may shed light on the regulation of astrocyte function in health and disease and identify new therapeutic approaches for human neurologic disorders.', 'Moreover, our results identify a molecular pathway through which the diet in cooperation with the commensal flora modulate the activity of CNS resident cells and neuroinflammation. In addition, the regulation of AhR expression by IFN-β suggest that the microbiome may affect not only the development of CNS autoimmunity, but also its response to disease modifying therapies  60  . Thus, the study of the metabolic and environmental factors that regulate astrocyte activity may shed light on CNS physiology, identify mechanisms of disease pathogenesis and drive the development of more efficacious therapeutic interventions for MS and other neurologic diseases.\n\nOnline Methods\n\n\nAnimals\nC57BL/6J, Ifnar1 -/-, IL-27ra -/-, GFAP-Cre, and AhR fl/fl mice were obtained from the Jackson Laboratory and were all female. Mice with a specific deletion of AhR in astrocytes were generated by crossing GFAP-Cre and AhR fl/fl mice, efficient deletion of AhR in astrocytes was verified by PCR and Western blotting (data not shown).']</t>
         </is>
       </c>
-      <c r="AF234" t="inlineStr"/>
+      <c r="AF234" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Substantiated",
+  "explanation": "The reference article supports the claim that metabolites derived from dietary tryptophan by the gut flora can affect microglia and astrocytes via the aryl hydrocarbon receptor (Ahr). The abstract mentions that dietary tryptophan is metabolized by the gut microbiota into AhR agonists, which act on astrocytes to limit CNS inflammation. Excerpt 1 also highlights the role of microbial products in regulating astrocyte activity and CNS inflammation."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="235">
       <c r="A235" t="inlineStr">
@@ -34474,7 +36211,14 @@
           <t>['In this study, homologous sporozoite immunizations resulted in boosting of CSP-specific, but not L3-specific, CD8 + T-cell responses. Previous reports show that when multiple homologous sporozoite immunizations were given at 48-h intervals, there was no significant increase in CSP-specific CD8 T-cell expansion compared with a single dose of sporozoites (  47 ). This so-called "self-regulation" was due to antigen-specific CD8 + T cells that could eliminate antigen-presenting DCs  (48)  and prevent the further expansion of naive CD8 + T cells specific for the same antigen. This phenomenon is thought to mimic the situation in hyperendemic field settings, where humans sometimes receive multiple malaria-infected mosquito bites daily. When the interval between immunizations is extended to a week or more as in our studies, we and others  (27)  find that endogenous CSP-specific CD8 + T cells in fact increase in frequency after repeated sporozoite immunizations. Thus, CSP-specific T cells do not appear to be affected by self-regulation using our vaccination approach.', 'Similar to the behavior of CSP-specific cells following multiple sporozoite immunizations, these heterologous prime-boost approaches expanded the population of activated (CD11a HI CD62L LO CD44 HI ) L3-specific T cells by 0.74 or 1.67 log 10 cells per spleen for L3 peptide-pulsed DC or GAP priming, respectively, compared with the appropriately matched Lm-L3 priming immunization alone (Fig.  4  F and G). Thus, in contrast to multiple sporozoite immunizations, a heterologous prime-boost approach expanded the L3-specific population and maintained its activated phenotype.\n\nPrior Sporozoite Immunization Eliminates L3 Expression and Liver Stage Parasite Development and Prevents the Boosting of Responses Against\nLate Liver Stage Antigens. Heterologous prime-boost studies presented above suggested that functional memory L3 CTLs were formed by priming with sporozoites.', 'Looking beyond CSP-specific cells, previous phenotyping of bulk CD8 + T cells showed that some portion of memory T-cell responses could be boosted by repeated sporozoite exposures. Lymphocytes from mice treated with homologous sporozoite immunizations showed an increase in the frequency of memory CD8 + T cells at a memory timepoint  (37) . We predict that  such increases following repeat sporozoite immunizations are responses against preformed or early liver stage antigens. Thus, with the right immunization interval, some CD8 + T-cell responses appear to boost in response to homologous sporozoite exposures. In contrast to CSP-specific T cells, L3-specific CD8 + T cells failed to boost after repeated sporozoite immunizations. We first looked to see whether there were functional defects in L3-specific cells, but these cells were capable of killing peptide-coated target cells in an antigen-specific manner and could be restimulated with other forms of antigen. Instead, we found that the lack of L3specific CTL expansion following secondary sporozoite immunization was likely due to the strong antisporozoite immune response that essentially prevents L3 expression.']</t>
         </is>
       </c>
-      <c r="AF235" t="inlineStr"/>
+      <c r="AF235" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Substantiated",
+  "explanation": "The reference article supports the statement 'limited boosting after irradiated SPZ vaccination has been demonstrated in mouse models'. Excerpts 1 and 3 show that repeated sporozoite immunizations do not expand CTL responses to the L3 protein, but may boost responses to preformed antigens like CSP. The study suggests that heterologous prime-boost regimens can be used to increase CTL responses against late liver stage proteins."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="236">
       <c r="A236" t="inlineStr">
@@ -34614,7 +36358,14 @@
           <t>["Although coexisting moiré patterns have previously been observed in graphitic multilayers  [9, 10] , we demonstrate here that moiré patterns produced by graphene-graphene interlayer interactions can coincide with moiré patterns that arise from graphene-BN interactions to produce a new supersuperlattice structure. Our scanning tunneling spectroscopy (STS) measurements of tBLG/BN yield new insight into how the intrinsic electronic behavior of tBLG is affected by moiré-induced interactions. For example, we observe an additional dip feature in the DOS at an energy beyond the first VHS. By comparing the moiré wavelength dependence of this new feature's energy to calculations incorporating ab initio results, we find that it arises from a partial gap opening between the second and third moiré bands due to strong non-perturbative interlayer coupling in the small twist-angle regime. These measurements on our high quality tBLG/BN samples provide a first look into the atomic-scale behavior of electrostatically gated tBLG, an important device configuration for future applications  [28, 29] .", 'Our measurements were performed using an Omicron ultra-high vacuum (UHV) STM operating at temperature T = 5 K with electrochemically etched PtIr tips. The tips were calibrated against the surface state of an Au(111) crystal before performing all measurements  [30] . Differential conductance (dI/dV) was measured by lock-in detection of the a.c. tunnel current modulated by a 6-8 meV (rms), 400-700 Hz signal added to the sample bias (V s ). Each tBLG device was fabricated by growing two monolayers of graphene via chemical vapor deposition (CVD)  [31]  and then sequentially transferring the layers onto a BN flake peeled onto an SiO 2 /Si wafer (see Fig.  1 (a) for a schematic of a typical graphene device; see Ref.  [32]  for more details about the growth and transfer processes). The samples were annealed in UHV at 400 for several hours to clean them before loading them into the STM.', 'The existence of these coexisting moiré patterns may have important consequences for device applications involving stacked graphene and BN layers, and the emergence of graphene-BN super-superlattices may serve as an interesting platform for novel physical phenomena. The high quality of our tBLG/BN devices has enabled us to probe the intrinsic electronic properties of tBLG and to observe new spectroscopic features in the tBLG DOS. These features occur at energies beyond the first VHS and can be explained by a non-perturbative theory involving ab initio calculations. These results show that the strong coupling, low twist-angle regime in tBLG can be accessed using scanned probe techniques via high quality devices that allow electrostatic Fermi level tuning. bias (-V s ), back-gate voltage (V g ), and grounding scheme are shown. (b-d) STM topographic images show coexisting graphene-graphene and graphene-BN moiré patterns.']</t>
         </is>
       </c>
-      <c r="AF236" t="inlineStr"/>
+      <c r="AF236" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Substantiated",
+  "explanation": "The reference article supports the statement that scanning tunneling microscopy and spectroscopy can be used to examine the local electronic properties of long-wavelength moire patterns. The abstract mentions a scanning tunneling microscopy study, and Excerpt 1 discusses STS measurements yielding new insight into how intrinsic electronic behavior is affected by moiré-induced interactions."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="237">
       <c r="A237" t="inlineStr">
@@ -34754,7 +36505,14 @@
           <t>['2B ), density fluctuations (Fig.  2B ), critical scattering  (36) , high surface mobility  (4, 37) , anomalously fast self diffusion  (3, 33) , modified molecular dynamics  (33, 34)  and macroscopic mechanical properties, such as apparent solidification  (17, 38) , and excluded-volume effects leading to quasi-periodic film-thickness transitions (Fig.  2A ). Additional insights into the fascinating properties of confined fluids are expected from a planned laterally resolved real-time measurement of D and n in the eSFA.\n\nWater at Hydrophobic Surfaces:\nWeak Hydrogen Bonding and Strong Orientation Effects L. F. Scatena, M. G. Brown, G. L. Richmond* Vibrational studies that selectively probe molecular structure at CCl 4 /H 2 O and hydrocarbon/H 2 O interfaces show that the hydrogen bonding between adjacent water molecules at these interfaces is weak, in contrast to generally accepted models of water next to fluid hydrophobic surfaces that suggest strong hydrogen bonding.', 'VSF experiments at the air/water (Mallinckrodt ChromAR HPLC Grade H 2 O) interface were performed in a N 2 purged closed cell so that contamination of the interface was eliminated (beyond detectable levels). Our most detailed studies are with CCl 4 , where spectral absorption of the incident IR beam is minimized. 13. D. Eisenberg, W. Kauzmann, The Structure and Properties of Water (Oxford Univ. Press, New York, 1969). 14. Q. Du, E. Freysz, Y. R. Shen, Science 264, 826 (1994). 15. D. F. Coker, R. E. Miller, R. O. Watts, J. Chem. Phys. 82, 3554 (1985). 16. M. P. Conrad, H. L. Strauss, J. Phys. Chem. 91, 1668 (1987). 17.', 'However, interactions between these water molecules and the organic phase result in substantial orientation of these weakly hydrogen-bonded water molecules in the interfacial region. The results have important implications for understanding water adjacent to hydrophobic surfaces and the penetration of water into hydrophobic phases. Protein folding, membrane formation, micellar assembly, and wetting are a few of the many processes in which the interaction of water with hydrophobic fluid surfaces plays an important role. A driving force behind these processes is an uncommonly large entropy loss, which is usually explained as an enhanced structuring of water in the immediate vicinity of apolar molecules, biological macromolecules, and hydrophobic surfaces. Experimental measurements that provide a molecular-level view of interfacial water structure and hydrogen bonding at these interfaces have proven to be problematic because of the difficulty in selectively examining interfacial water molecules. Hence, most of our understanding of the molecular structure of water at hydrophobic surfaces comes from theory (1-7).']</t>
         </is>
       </c>
-      <c r="AF237" t="inlineStr"/>
+      <c r="AF237" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Substantiated",
+  "explanation": "The reference article [18] discusses how properties of water differ near hydrophobic surfaces due to weak hydrogen bonding and strong orientation effects, supporting the claim that confined water has distinct properties. The abstract directly mentions implications for understanding water adjacent to hydrophobic surfaces, aligning with the statement about varying structure and dynamics in nanoconfined environments."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="238">
       <c r="A238" t="inlineStr">
@@ -34894,7 +36652,18 @@
           <t>['Since other arboviruses have been reported to be transmitted by blood transfusion  [4] , several prevention procedures were implemented in date to prevent transfusion of ZIKAV through transmission in French Polynesia, including nucleic acid testing (NAT) of blood donors. We report here the detection of ZIKAV in 42 of 1,505 blood donors, who were asymptomatic at the time of blood donation.\n\nBackground\nZIKAV, an arthropod-borne virus (arbovirus) belonging to the family Flaviviridae and genus Flavivirus  [5] , was first isolated in 1947 from a monkey in the Zika forest, Uganda  [6] . Sporadic human Zika fever cases have been reported since the 1960s  [7] . The first documented outbreak outside Africa and Asia occurred in 2007 in the Yap State, Micronesia, in the North Pacific, where Zika fever was characterised by rash, conjunctivitis and arthralgia  [8] . ZIKAV has been isolated from several Aedes mosquito species, notably including Ae. aegypti  [9]  and Ae.', 'For ZIKAV, there is no estimate available of the percentage of asymptomatic infections. Arbovirus transfusionderived transmission has been reported principally for WNV  [19] , DENV  [20]  and chikungunya virus (CHIKV)  [21, 22] . For CHIKV, the risk was evaluated as high  [21, 22] . During the outbreaks of CHIKV infection in Italy (2007)  [21]  and in Réunion Island in the Indian Ocean (2005-07)  [22] , blood donation was discontinued and blood products were imported from blood bank centres elsewhere. In French Polynesia, due to its geographically isolated location, it was impossible to be supplied with fresh blood products from blood bank centres outside French Polynesia. Due to the potential risk of ZIKAV transfusion-derived transmission, the need to continue blood donations and the lack of a licensed test for ZIKAV diagnosis, we decided to implement ZIKAV NAT as soon as possible, using a modified RT-PCR  [16] .', 'aegypti  [9]  and Ae. albopictus  [10] . Ae. aegypti is widespread in the tropical and subtropical regions of the world and Ae. albopictus is now established in many parts of Europe, especially Mediterranean countries  [11] . Recent reports of imported cases of ZIKAV infection from south-east Asia or the Pacific to Europe  [12]  or Japan  [13]  highlight the risk of ZIKAV emergence in parts of the world where the vector is present.\n\nSample collection\nAccording to the procedures of the blood bank centre of French Polynesia, all blood donors have to fill in a pre-donation questionnaire and have a medical examination before blood donation. Blood is taken only from voluntary donors who are asymptomatic at the time of donation. A signed informed consent statement was obtained from all blood donors and publication of data related to ZIKAV testing was approved by the Ethics Committee of French Polynesia (reference 66/CEPF). ZIKAV nucleic acid testing (NAT) of samples of all donations was implemented routinely from 13 January 2014.']</t>
         </is>
       </c>
-      <c r="AF238" t="inlineStr"/>
+      <c r="AF238" t="inlineStr">
+        <is>
+          <t>Here is my evaluation in JSON format:
+```
+{
+  "label": "Substantiated",
+  "explanation": "The reference article demonstrates the potential for Zika virus transmission through blood transfusion, as evidenced by the detection of ZIKAV in asymptomatic blood donors and the implementation of nucleic acid testing to prevent post-transfusion Zika fever."
+}
+```
+I classified this statement as "Substantiated" because the abstract and excerpts clearly discuss the risk of Zika virus transmission through blood transfusion and present data supporting this concern. The article highlights the detection of ZIKAV in asymptomatic blood donors, which suggests that infected individuals can unknowingly transmit the virus through blood donation. This supports the citing article's statement about the potential for transmission by transfusion being present.</t>
+        </is>
+      </c>
     </row>
     <row r="239">
       <c r="A239" t="inlineStr">
@@ -35034,7 +36803,14 @@
           <t>['Loss of NLRP3, ASC, or caspase-1 in BMDMs did not markedly affect caspase-11-dependent generation of mature Gsdmd p30 in response to cytoplasmic LPS (Fig.  4a ), indicating that Gsdmd cleavage occurs upstream of NLRP3 inflammasome activation. The question arises as to whether Gsdmd induces pyroptosis and NLRP3 inflammasome activation simultaneously in the same cell, or if Gsdmd-mediated pyroptosis releases damage-associated molecular patterns  29  that trigger caspase-11-independent NLRP3 inflammasome activation in neighbouring cells (Extended Data Fig.  6a ). We believe the latter hypothesis is unlikely because LPS-stimulated Il1b 2/2 BMDMs exhibited normal pyroptosis, yet their culture supernatant failed to induce IL-1b secretion from Casp11 2/2 BMDMs (Extended Data Fig.  6b ,  c ).', '3c ). Collectively, these data indicate that caspase-11 directly cleaves the 53-kDa inactive precursor form of Gsdmd (pro-Gsdmd) to generate the propyroptotic N-terminal fragment (Gsdmd p30, Fig.  1b ). In full-length Gsdmd, the C terminus may mask key sites in the N terminus until cleavage at D 276 #G 277 releases this inhibition. Consistent with this notion, reconstitution of immortalized Gsdmd 2/2 macrophages with wild-type Gsdmd restored LPS responsiveness, as evidenced by lactate dehydrogenase (LDH) release, IL-1b secretion and caspase-1 processing, whereas reconstitution with the Gsdmd processing mutant D276A did not (Fig.  3d ,  e ). In addition, mutation of Gsdmd within the p30 fragment (I105N) attenuated pyroptosis and caspase-1/IL-1b processing (Fig.  1b , e and Extended Data Fig.  2b ) without affecting Gsdmd cleavage (Extended Data Fig.  4b ).', '4c ). Gsdmd -/-2 WT Casp11 -/- Gsdmd -/-1 Gsdmd -/-2 WT Casp11 -/- Gsdmd -/-1 G s d m d -/ -2 W T C a s p 1 1 -/ - G s d m d -/ -1 G s d m d -/ -2 W T C a s p 1 1 -/ - G s d m d -/ -\n\nRole for Gsdmd in canonical pyroptosis\nHuman caspase-1 is reported to cleave GSDMD at the same P 1 -Asp residue  31  as caspase-11, albeit that the preferred tetrapeptide cleavage sequence of caspase-1 differs from that of caspase-11  27, 28  . Consistent with this study  31  , the Gsdmd p30 fragment appeared in BMDMs treated with canonical inflammasome activators including ATP (Fig.  5a  and Extended Data Fig.  7a ).']</t>
         </is>
       </c>
-      <c r="AF239" t="inlineStr"/>
+      <c r="AF239" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Substantiated",
+  "explanation": "The reference article supports the statement that caspase-1 can cleave off the suppressor C-terminal domain (CTD) of GSDMD, as it mentions that human caspase-1 is reported to cleave GSDMD at the same P1-Asp residue as caspase-11. Additionally, Excerpt 2 explains how the cleavage releases the pore-forming N-terminal domain (NTD), enabling pyroptosis and IL-1β processing."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="240">
       <c r="A240" t="inlineStr">
@@ -35177,7 +36953,21 @@
           <t>['1  for chemical structures of Nec-1 and Nec-1i). The same authors claimed that Nec-1 produced its actions via inhibition of a form of cell death distinct from necrosis and apoptosis which they termed necroptosis  [12] . More recently sitosterol-induced death in macrophages was reported to be caspaseindependent and blocked by Nec-1, and again it was suggested that necroptosis (and autophagy) might be involved  [13] , although considerably more work will be required before necroptosis can be unequivocally confirmed as representing a distinct entity. Protection against I/R injury in the heart and the brain could involve similar mechanisms and this could extend to the particular cell-signaling pathways or enzymes that are activated or down-regulated during the recovery process  [14] . As Nec-1 has been shown to limit cellular damage in the brain we decided to ascertain whether it could produce a similar action in the myocardium. To investigate this we used a variety of in vitro experimental models.', 'An examination of the effects of necrostatins on cell signaling pathways involved in cardioprotection will aid in the characterisation of these agents  [4] . The advent of newer and possibly more potent forms of the necrostatins will also assist in this process  [22] . In conclusion, as discussed by Degterev et al.  [12]  necrosis and apoptosis play key roles in a variety of pathological conditions, including myocardial infarction, and the identification of compounds such as the necrostatins which may target the proposed alternative death pathway, necroptosis, may lead to the development of more effective therapies. Our data are the first to indicate that necrostatin is protective against I/R injury in the myocardium, possibly via mechanisms other than those that are generally accepted as being involved (i.e. apoptosis and necrosis)  [23] . It should be stressed, however, that these are preliminary studies.', 'As delaying MPTP opening is believed to represent a key factor with respect to cardioprotection and may be linked to apoptosis, our failure to show a delay with lower Nec-1 concentrations may be consistent with the findings of Degterev and colleagues  [12] , who claimed that the effects produced by Nec-1 are mediated by a mechanism distinct from necrosis and apoptosis, namely necroptosis. As suggested by Formigli et al.  [20]  for a process they termed aponecrosis and claimed shared characteristics with apoptosis and necrosis, necroptosis could represent one of a continuum of death processes with apoptosis and necrosis occurring at its two extremes  [20] . Clearly, however, before any firm conclusions can be made regarding necroptosis and the mode(s) of action of necrostatins in the context of myocardial infarction more detailed studies, possibly involving the use of Nec-1 in combination with caspase inhibitors (inhibitors which block apoptotic pathways), should be carried out  [21] .']</t>
         </is>
       </c>
-      <c r="AF240" t="inlineStr"/>
+      <c r="AF240" t="inlineStr">
+        <is>
+          <t>Here is my evaluation:
+{
+  "label": "Substantiated",
+  "explanation": "The reference article supports the claim that necroptosis plays a role in driving pathology of ischemia-reperfusion injury of the heart. The study demonstrates that necrostatin-1 (Nec-1) reduces infarct size and inhibits myocardial cell death, possibly via a mechanism independent of apoptosis and necrosis, suggesting necroptosis as an alternative pathway."
+}
+I based my evaluation on the following points:
+* The abstract states that Nec-1 protects against ischemia-reperfusion injury in the heart by reducing infarct size.
+* Excerpt 1 mentions that protection against I/R injury in the heart could involve mechanisms similar to those involved in brain injury, and suggests that necroptosis might be a distinct entity.
+* Excerpt 2 discusses the potential role of necrostatins in targeting necroptosis as an alternative death pathway.
+* Excerpt 3 provides evidence for Nec-1's mechanism of action being distinct from apoptosis and necrosis, which supports the idea of necroptosis playing a role in ischemia-reperfusion injury.
+Overall, while the article does not explicitly state that necroptosis drives pathology of ischemia-reperfusion injury, it provides strong evidence supporting the involvement of necroptosis as an alternative death pathway.</t>
+        </is>
+      </c>
     </row>
     <row r="241">
       <c r="A241" t="inlineStr">
@@ -35317,7 +37107,14 @@
           <t>['INTRODUCTION\n\n\nHaemagglutinins\nare glycoprotein components of influenza virus membranes which bind virus particles to cells and in addition appear to be involved in the membrane fusion which allows transfer of the virus transcription complex into cells (for reviews see  Compans and Klenk, 1979; Ward, 1982) . Antibodies against haemagglutinins neutralize virus infectivity and studies on antigenicity using monoclonil antibodies indicate that haemagglutinins contain a small number of nonoverlapping antibody binding regions  (Gerhard et al., 1981; Webster eC al., 1980; Jackson et aL, 1982) . Analyses of the amino acid sequences of haemagglutinins of antigenic variants indicate that antibodies of different specificities recognize different amino acid residues in the distal region of the haemagglutinin molecule  (Laver et aL, 1979; 1980; Both and Sleigh, 1981; Caton et al, 1982; Daniels et al, 1983) . The amino acids recognized have generally been assumed to contribute to the particular antibody binding site.', 'The nucleotide sequence changes determined in the HA1 regions of appropriate antigenic variants, which serve to define the specificity of the monoclonal antibodies used, are given in Table  1 . Electron microscopy. BHA was dilnted in PBS (pH 7.2) to 50 pg/ml for optimum spreading on carbon support films. Antibody was added in increasing amounts until only a few molecules remained unbound to BHA after about 5 min equilibration. BHA-antibody complex suspensions were adsorbed to thin carbon films freshly stripped from mica, floated on a 1% w/v solution of sodium silicotungstate (pH 7.0) and then air dried. Micrographs were taken under minimum dose conditions known from analyses of periodic specimens to preserve detail below 1.5 nm; defocus was such that phase contrast was transferred in a continuous band down to about 1.0 nm  (Wrigley et al., 1983) . top row) amination of the other antibody combinations although the position and binding angle of HC3; HC19, and HC45 are less easy to distinguish from one another than from HC31.', '3 ) presumably because of the binding of a second antibody to an unoccupied equivalent region of the BHA trimer is sterically prevented by the first antibody bound. The sites of antibody binding and the locations of amino acid substitutions in the BIIAs of antigenie variants can also be considered in relation to the thxee-dimensional structure of the BHA, Fig.  6 . These considerations indicate that the sites of amino acid substitution are in all four cases appropriately located to be involved directly in the antibody-binding sites. In the case of HC31 they also indicate the basis of the steric inhibition of the binding of a second antibody to the BHA. Since the three 198 residues recognized are only 15 A apart around the threefold axis of the trimer, the BHA is effectively monovalent at this site. The results therefore substantiate the positions of antigenic sites A, B, and E and in the ease of site B give an indication of the extent of this region at the distal tip of the BHA molecule. It would also be of interest to examine antibodies specific for sites C and D but we have not characterized antibodies prepared against X-31 virus which recognize amino acids in these sites.']</t>
         </is>
       </c>
-      <c r="AF241" t="inlineStr"/>
+      <c r="AF241" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article discusses the binding sites of antibodies on the haemagglutinin of influenza virus, but does not mention how the addition of glycans on HA affects Ab binding. The provided excerpts focus on antibody binding regions, amino acid sequences, and electron microscopy analysis, without addressing glycosylation or its impact on antibody binding."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="242">
       <c r="A242" t="inlineStr">
@@ -35457,7 +37254,15 @@
           <t>['This dephasing mechanism accounts for the approach to thermal equilibrium for an initially out-of-equilibrium state  [2, 5] . The Quantum Ergodic Theorem: In 1929, von Neumann proved a mathematical result which has been dubbed the quantum ergodic theorem (QET)  [11] . An exegesis of it has been given by Goldstein et al. (hereafter GLTZ)  [12] . GLTZ summarize QET, or "normal typicallity" as it has been more recently known, as follows: "for a typical finite family of commuting macroscopic observables, every initial wave function from a micro-canonical energy shell so evolves that for most times τ in the long run, the joint probability distribution of these observables obtained from |ψ(τ ) is close to their microcanonical distribution"  [12] .', 'The above scenario, however, does not occur in quenches between integrable systems, i.e., when the initial state is an eigenstate of an integrable system, and the time evolution is studied after changing some parameters in the Hamiltonian while keeping the system integrable. Studies of several models have shown that A remains different from the thermal expectation as one approaches the thermodynamic limit  [9, [21] [22] [23] [24] [25] [26] [27] [28] [29] [30] [31] [32] [33] [34] . Even some special initial states that were seen to lead to A similar to the ones predicted in thermal equilibrium  [9, 21, 28] , have been recently shown not to result in the thermalization Â in the thermodynamic limit  [32, 34] . Here we identify a class of initial states that leads to thermal behavior after a quench to an integrable point. The initial states we consider are eigenstates of an initial Hamiltonian ĤI that is nonintegrable.', 'As already noted, ETH can be justified by various results from quantum chaos theory. Thus, ETH provides a physical basis for the technical condition needed by QET. This results in a unification of two formerly disparate schools of thought on the foundations of statistical mechanics. Quantum Quenches: As mentioned in the introduction, ETH has been shown to be satisfied in a variety of nonintegrable quantum systems. It has been found to breakdown only as one approaches integrable points  [6] [7] [8] , or in special regimes that are dominated by finite size effects, e.g., close to the atomic limit  [14, 15] . Thermalization itself has been shown to be robust in nonintegrable systems after a (sudden) quench, once again, failing to occur close to integrable points  [6, 16, 17]  or the atomic limit  [15, 18] , and in localized disordered systems  [19] . Here, by (sudden) quench, we mean that the system is prepared in an eigenstate of some initial Hamiltonian (not necessarily the ground state) and then at τ = 0 the Hamiltonian is changed.']</t>
         </is>
       </c>
-      <c r="AF242" t="inlineStr"/>
+      <c r="AF242" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Substantiated",
+  "explanation": "The statement 'understanding how statistical ensembles arise from the unitary time evolution of an isolated quantum system has been a fascinating question' is substantiated by reference 6. Although the abstract and excerpts do not directly state this sentence, they discuss related topics such as eigenstate thermalization hypothesis (ETH), quantum ergodic theorem, and thermalization in isolated quantum systems, which are all relevant to understanding how statistical ensembles arise from unitary time evolution."
+}
+Note: While the reference article does not explicitly state the exact sentence from the citation statement, it discusses closely related concepts that provide a foundation for understanding the question posed in the statement.</t>
+        </is>
+      </c>
     </row>
     <row r="243">
       <c r="A243" t="inlineStr">
@@ -35597,7 +37402,17 @@
           <t>['67  recruitment of bone-marrow-derived cells Tumorrecruited bonemarrowderived cells (BMDCs) mediate tumorinduced immune suppression, promote tumor vascularization, and stimulate tumor meta stasis.  [68] [69] [70] [71]  BMDCs represent a mixed cell population that includes hematopoietic progenitor cells, myeloid cells, and precursors of endothelial and stromal cells. Seemingly, tumor growth and metastatic develop ment can be prevented by reducing the trafficking of BMDCs into tumor sites (Figure  3 ).  25  Several mol ecules and mechanisms can modulate tumormediated recruitment of BMDCs, including veGF receptors and chemokine CXCL12-CXCR4mediated pathways.  17, [72] [73] [74] [75] [76] [77]  Overexpression of veGF promotes mobilization of veGFR1 + CXCR4 + BMDCs into the peripheral blood, and thus promotes immuno suppression. Tumorderived veGF also inhibits differentiation of DCs and promotes accumulation of MDSCs in the tumorbearing host.', 'These cells are profoundly immunosuppressive and support tumor growth via inhibition of adaptive immune responses. By contrast, the proportion of T H 1-biased dendritic cells and their immediate precursors are reduced in patients with cancer. Both the secreted products and myeloid cells are candidates for targeted therapies to enhance the efficacy of cancer vaccines (red text). Finally, many tumor-recruited myeloid cells migrate into tumor tissues where they support tumor growth via local immunosuppression and stimulation of neoangiogenesis (see Figure  3 ). Abbreviations: ATRA, all-trans retinoic acid; COX-2, cyclo-oxygenase 2; G-CSF, granulocyte colony-stimulating factor; GM-CSF, granulocyte-macrophage colonystimulating factor; IL, interleukin; NO-aspirin, nitric-oxide-releasing aspirin; PGe 2 , prostaglandin e 2 ; TGF-β1, transforming growth factor β1; T H 1, T-helper lymphocyte type 1; VeGF, vascular endothelial growth factor.\n\nRenal cell carcinoma\n\n\nSecretion\n\n\nBone marrow', '[25] [26] [27] [28]  MDSCs are frequently detected in the peripheral blood of patients with metastatic RCC  18, 19, 21, 29  or bladder carcinoma (e. eruslanov, personal communication). Moreover, MDSC frequencies seem to correlate with the stage of the disease, and potentially provide an important biomarker of prognosis. Studies have shown that MDSCs can trigger expan sion of another important immunosuppressive cell ular subset, termed Tregulatory cells (T ReG ).  30  T ReG represent an important, highly specialized subpopula tion of CD4 + Thelper cells that suppress activation of other T cells, especially of those specific against self antigens.  31  Interest in T ReG biology has been heightened by recent studies that demonstrate enhanced cancer vaccinemediated immunity after T ReG elimination.  32  In humans, T ReG are character ized by expression of the highaffinity CD25 αchain of the IL2 receptor (IL2R) and the trans cription factor forkhead box P3 (FOXP3).']</t>
         </is>
       </c>
-      <c r="AF243" t="inlineStr"/>
+      <c r="AF243" t="inlineStr">
+        <is>
+          <t>Here is my evaluation in JSON format:
+```
+{
+  "label": "Substantiated",
+  "explanation": "The reference article supports the claim that tumors may recruit BM-derived cells to support tumor growth through local immunosuppression. Excerpts 1 and 2 mention that tumor-recruited bone-marrow-derived cells, including myeloid cells, mediate immune suppression and promote tumor growth. Additionally, Excerpt 3 mentions that MDSCs, a subset of myeloid cells, are frequently detected in the peripheral blood of patients with metastatic cancer, including bladder carcinoma."
+}
+```</t>
+        </is>
+      </c>
     </row>
     <row r="244">
       <c r="A244" t="inlineStr">
@@ -35737,7 +37552,14 @@
           <t>["RESULTS\n\n\n3T3 cells migrate preferentially toward stiff substrate\nTo explore whether cell movement can be guided by substrate rigidity, we cultured National Institutes of Health 3T3 cells on collagen-coated polyacrylamide sheets that contained a gradient of rigidity, with a Young's modulus varying between 140 and 300 kdyn/cm 2 . Regions of high and low rigidity were created by manipulating the bis-acrylamide concentration while maintaining a constant concentration of total acrylamide concentration and were identified by including fluorescent beads in one side of the substrate. The same results were obtained by placing fluorescent beads in either the stiff or the soft side. The surface in the transition region stayed on the same plane of focus, indicating that there was no sharp change in substrate height. Based on the distribution of beads, we estimated the transition area between high and low rigidity to be 50 -100 m in width. After seeding for ϳ15 h, the migration of cells was recorded by time-lapse phase microscopy over a period of 10 h. To minimize the effects of intercellular mechanical interactions through the elastic substrate, we used a low cell density and focused only on individual cells without neighbors in the observation field.", 'From these observations, one may predict that cells are capable of responding to substrate rigidity through a true active tactile exploration process, by exerting contractile forces and then interpreting the substrate deformation to determine a preferred direction or destination of their movements  (Pelham and Wang, 1997; Sheetz et al., 1998) . Our approach to testing this hypothesis consists of putting motile National Institutes of Health 3T3 cells on collagencoated polyacrylamide substrates with a rigidity gradient, under conditions such that the only way the cells can detect this stiffness gradient is by a process of active tactile exploration. Our results indicate that 3T3 fibroblasts can in-deed detect and respond to substrate stiffness. Furthermore, the cell consistently migrates in the direction of increasing stiffness. To confirm the involvement of a force-sensing mechanism, we have also shown that the direction of cell movement can be guided by manipulating mechanical strain within the flexible substrate. The observed coupling between strain and movement is exactly as required to produce a preference for hard materials. Parallel measurements indicate that cells generate stronger traction forces and spread to a larger size on stiff substrates than on soft substrates.', 'pieces of tissue explants are plated millimeters apart on collagen gels  (Harris et al., 1981) . In reality, the movement of cells within a complex organism or embryo is probably guided by a complex interplay among chemical and physical signals, which may include substrate rigidity as well as forces generated by fluid shear and cell-cell interactions. While the current observations provide direct evidence for the guidance of cell migration by substrate rigidity and mechanical forces, related phenomena have been reported in recent decades. For example, Kolega observed that stretching with a microneedle causes an epithelial cell to withdraw its lateral protrusion while maintaining its dimension along the direction of tension  (Kolega, 1986) . With neurons, similar manipulations were found to stimulate the elongation of neurite, a phenomenon referred to as "towed growth"  (Bray, 1984; Lamoureux et al., 1989; Chada et al., 1997) .']</t>
         </is>
       </c>
-      <c r="AF244" t="inlineStr"/>
+      <c r="AF244" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Substantiated",
+  "explanation": "The reference article supports the statement that substrate stiffness is a significant factor in cell migration. The abstract and excerpts describe experiments demonstrating that cells migrate preferentially towards stiff substrates and that changes in tissue rigidity can guide cell movement, confirming the role of substrate stiffness in cell migration."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="245">
       <c r="A245" t="inlineStr">
@@ -35877,7 +37699,14 @@
           <t>['We first monitored the localisation and phosphorylation of Yap at Ser127 during myogenesis for which we used the C2C12 mouse myoblast cell line as an in vitro model (Fig.  2 ). During C2C12 myogenesis, myoblasts first proliferate to confluency, withdraw from the cell cycle and then differentiate into myotubes upon a shift to differentiation medium containing lower concentrations of mitogens. We found that Yap Ser127 phosphorylation is low in myoblasts but after 24 h in differentiation medium Ser127 phosphorylation is %20-fold increased and after 96 h it is %28-fold higher than in myoblasts, respectively (Fig.  2A , see also Fig.  S1a  in the Supplementary data for a quantification). Changes in the phosphorylation of Yap during differentiation are accompanied by the gradual translocation of Yap from distinct loci in the nucleus of myoblasts to the cytoplasm of myotubes (Fig.  2B ; see Fig.  S2b  in the Supplementary data for additional images).', '1  and  2A ). The expression of the Hippo pathway in skeletal muscle suggests that the pathway may have a function in this tissue. As Yap has previously been reported to promote proliferation and inhibit differentiation of neural  [16]  and intestine progenitors  [15]  we decided to study Yap during C2C12 myogenesis in order to test whether it had a similar function in skeletal muscle. At the onset of C2C12 differentiation Yap Ser127 phosphorylation increased %20-fold and Yap increasingly translocates from the nucleus to the cytosol (Fig.  2 ). The likely mechanism is that the Yap Ser127 residue is phosphorylated by Lats1/2  [10, 14, 19]  and that Ser127 phosphorylated Yap is then sequestered by 14-3-3 binding proteins in the cytosol  [11] [12] [13] .', 'Overexpression of constitutively active hYAP S127A expanded multipotent progenitor cells in the crypt compartment of the intestine and these cells could not undergo terminal differentiation until hYAP1 S127A overexpression was stopped  [15] . In the chick neural tube Yap overexpression similarly stimulated proliferation but inhibited differentiation of neural progenitor cells  [16] . Taken together these results suggest that the Hippo pathway can regulate the proliferation and terminal differentiation of cells in several tissues and organs which is relevant for their development, repair and size. Little is known about the expression, regulation and function of Hippo pathway members in skeletal muscle cells. The aim of this study was thus to examine the expression of core members of the Hippo pathway in skeletal muscle and to investigate the regulation and function of the transcriptional cofactor Yap during C2C12 myogenesis.\n\nMaterials and methods\nChemicals and materials. All chemicals and materials were purchased from Sigma-Aldrich, Poole, United Kingdom unless otherwise indicated. C2C12 cell culture.']</t>
         </is>
       </c>
-      <c r="AF245" t="inlineStr"/>
+      <c r="AF245" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article discusses Yap expression, regulation, and function in C2C12 myogenesis, but does not mention the effect of linear stiffness gradient hydrogels on C2C12 myoblasts or a transition zone with nuclear localization increasing from 2 to 38 kPa. The provided excerpts focus on Yap phosphorylation, translocation, and its role in differentiation, which is unrelated to the specific claim made in the citing article."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="246">
       <c r="A246" t="inlineStr">
@@ -36017,7 +37846,14 @@
           <t>['15 min before ischemia and 10 min after reperfusion in 2 equal doses (4 l per dose; 1.5 mm lateral, 0.8 mm posterior from bregma, 4.0 mm below bone surface). Neurological Deficit. Mice and rats were tested for neurological deficits and scored as described by Bederson et al.  (41)  with the following minor modification: 0, no observable neurological deficits (normal); 1, failure to extend right forepaw (mild); 2, circling to the contralateral side (moderate); 3, loss of walking or righting reflex (severe). The rater was naive to the treatment group, and assessments were made at 10 min and 2 hr during ischemia, and again 18 hr after reperfusion. Western Blot Analysis.', 'Eighteen hours after reperfusion, the forebrains were divided into five coronal (2-mm) sections using a mouse brain matrix (RBM-2000C; Activational Systems, Warren, MI), and the sections were stained with 2% 2,3,5-triphenyltetrazolium chloride (Sigma). The infarcted areas were quantitated by an image-analysis system (Bioquant IV; R &amp; M Biometrics, Nashville, TN) and calculated by summing the volumes of each section determined directly  (39)  or indirectly by the following formula: contralateral hemisphere (mm 3 ) Ϫ ipsilateral undamaged volume (mm 3 ; ref. 40). Although statistical significance was achieved by both methods of analysis, only data from the direct method are presented. Brain swelling was calculated according to the following formula: [(infarct volume ϩ ipsilateral undamaged volume Ϫ contralateral volume) ϫ 100͞contralateral volume (%)]. For histological evaluation of neuronal damage at 18 hr and 3 days after ischemia, sections (12 m) were stained with hematoxylin͞eosin.', 'Ischemia Model: Mouse. Spontaneously ventilating adult male SV-129 mice (n ϭ 173; 19-23 g; Taconic Farms) were initially anesthetized with 1.0% and maintained on 0.4-0.8% halothane in 70% N 2 O and 30% O 2 using a Fluotec 3 vaporizer (Colonial Medical, Amherst, NH). The left MCA was occluded with an 8-0 nylon monofilament (Ethicon, Somerville, NJ) coated with a mixture of silicone resin (Xantopren; Bayer Dental, Osaka) and a hardener (Elastomer Activator; Bayer Dental) as described  (37, 38) . The procedure lasted 15 min, and the anesthesia was discontinued. Two hours later, animals were briefly re-anesthetized with halothane, and the filament was withdrawn.']</t>
         </is>
       </c>
-      <c r="AF246" t="inlineStr"/>
+      <c r="AF246" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Unsubstantiated",
+  "explanation": "The reference article does not mention a comparison between wild-type and NSE_MT_1-GFP mice in terms of neurological score after pMCAO. The excerpts provided focus on the effects of ICE-like protease inhibitors on ischemic injury, brain swelling, and behavioral deficits, but do not address the specific claim made in the citing article."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="247">
       <c r="A247" t="inlineStr">
@@ -36157,7 +37993,14 @@
           <t>['internalized GPCR can indeed contribute to the acute G protein-mediated response \n10  . Evidence supporting these various latter hypotheses is indirect or subject to alternate interpretation, and it remains unknown if endosome-localized GPCR are even present in an active form. Here we describe the application of conformation-specific single domain antibodies (nanobodies) to directly probe activation of the β 2 -adrenoceptor, a prototypical GPCR  11  , and its cognate G protein, G s (ref. 12) in living mammalian cells. We show that the adrenergic agonist isoprenaline promotes receptor and G protein activation in the plasma membrane as expected, but also in the early endosome membrane; and that internalized receptors contribute to the overall cellular cyclic AMP response within several minutes after agonist application. These findings provide direct support for the hypothesis that canonical GPCR signalling occurs from endosomes as well as the plasma membrane, and suggest a versatile strategy for probing dynamic conformational change in vivo.', 'Thus, while it remains clear that β 2 -ARs can elicit G s -mediated signal transduction from the plasma membrane, the present data reveal a discrete component of the acute signalling response that is initiated from endosomes (Fig.  4g ). It remains unknown if β 2 -ARs are continuously bound by agonist in endosomes, as depicted in the figure for simplicity, but conformational activation of G s in endosomes is both receptor and agonist-dependent. Unambiguous detection of endosome-based activation of acute G-protein-linked signalling is presently limited to the β 2 -AR G s system for which the critical nanobodies are available. However, we believe that endosome-based contribution to the acute signalling response is likely widespread in the GPCR superfamily because the β 2 -AR belongs to the largest group (family A) of GPCR and is often considered a prototype. We also suggest, more generally, that nanobody-based biosensors represent a versatile strategy for probing other types of dynamic conformational change with high spatiotemporal resolution in living cells.', 'Because endosomes contain activated β 2 -ARs, we next asked if receptors engage their cognate G protein from this compartment. Heterotrimeric G proteins and adenylyl cyclase can be observed in endosomes as well as at the plasma membrane, supporting the concept of endosome-based G protein signalling  4, 6, 10, 24  . To directly investigate the subcellular location of G protein activation, we developed a distinct biosensor based on another nanobody, Nb37, which specifically recognizes the guanine-nucleotide-free form of Gα s representing the catalytic intermediate of G protein activation (Fig.  4a )  25  . We hoped that because Nb37 binds a surface of the alpha-helical domain that is accessible only in the nucleotide-free form, we would be able to detect production of this critical but fleeting activation intermediate in living cells. This was indeed the case because Nb37-GFP localized in the cytoplasm of untreated cells and was rapidly recruited from the cytoplasm to the plasma membrane in response to isoprenaline application (Fig.  4b , yellow arrowhead, Pearson coefficient = 0.627).']</t>
         </is>
       </c>
-      <c r="AF247" t="inlineStr"/>
+      <c r="AF247" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Substantiated",
+  "explanation": "The reference article provides direct evidence that GPCR signalling can occur from endosomes, not just the plasma membrane. The study shows that internalized β2-adrenoceptors contribute to the overall cellular cyclic AMP response and that canonical GPCR signalling occurs from endosomes as well as the plasma membrane. This supports the citation statement's claim about previously unrecognized cellular functions for intracellular GPCR signaling systems."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="248">
       <c r="A248" t="inlineStr">
@@ -36297,7 +38140,14 @@
           <t>["As a further evolution, thin film architectures have been particularly successful  6, 11, 12  demonstrating performances comparable to traditional inorganic thin-film solar cells.  13, 14  While we have borne witness to unbelievable progress and evolution of photovoltaic devices based on these materials, the huge gap in understanding when moving from the pristine molecules to their embodiment in a device can severely hamper their widespread adoption in optoelectronic applications. From the literature it is clear that every preliminary test of these materials in device architectures has revealed exciting surprises, however their working mechanisms remain remarkably obscure. Our poor understanding of the relationship between structure and optoelectronic properties is a key shortcoming, especially given that hybrid perovskites are intrinsically complex materials, where the presence of various types of interactions and structural disorder may play an important role in the material properties. The difficulty in predicting the response of these materials to the interaction with external stimuli makes it impossible to frame them as a proper technology. Due to the critical role of structural interactions of the organic/inorganic components, different crystallization/deposition methodologies a M. De Bastiani and V. D'Innocenzo contributed equally to this work.", 'b Author to whom correspondence should be addressed. Electronic mail: annamaria.petrozza@iit.it can lead to crystals with identical nominal chemical composition but with different macroscopic optoelectronic properties. In this work, we focus on the investigation of CH 3 NH 3 PbI 3-x Cl x perovskite thin films crystallized in situ on substrates of different natures (e.g., porosity, wettability) and on their photoluminescence properties. ZnO nanoparticles (np) of three different sizes, 70 nm, 50 nm, and 20 nm, have been deposited by spin coating onto glass substrates in order to obtain about 1000 nm thick scaffolds with different porosities. Due to its low-temperature processability this oxide has a strong technological relevance,  [15] [16] [17]  in fact, it has already been employed as a selective contact in perovskite based solar cells both on rigid and flexible substrates showing good charge collection properties  18  and overall performances comparable to the most commonly used TiO 2 .', 'Thus, we propose that the capping layer and the mesostructured film may be considered as two different compounds with different photoluminescence properties. In summary, we demonstrate that the nature of the substrate critically affects the structural and optical properties of the perovskite films by changing the crystallization dynamics. We have observed that the CH 3 NH 3 PbI 3-x Cl x crystals form in only 1 min on ZnO substrates. This may have']</t>
         </is>
       </c>
-      <c r="AF248" t="inlineStr"/>
+      <c r="AF248" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Substantiated",
+  "explanation": "The reference article [42] supports the statement that film microstructure impacts photoluminescence properties, as demonstrated by their investigation of CH3NH3PbI3−xClx perovskite thin films crystallized on substrates with different natures. The article shows that the substrate's chemical nature and porosity influence the thin film structure and emissive properties."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="249">
       <c r="A249" t="inlineStr">
@@ -36437,7 +38287,14 @@
           <t>['Dystrophin, the protein encoded by the Duchenne muscular dystrophy (DMD) gene, exists in a large oligomeric complex. We show here that four glycoproteins are integral components of the dystrophin complex and that the concentration of one of these is greatly reduced in DMD patients. Thus, the absence of dystrophin may lead to the loss of a dystrophin-associated glycoprotein, and the reduction in this glycoprotein may be one of the first stages of the molecular pathogenesis of muscular dystrophy.\nDuCHENNE muscular dystrophy is caused by a defective gene located on the X chromosome. Dystrophin, the high-molecular weight protein product of the DMD gene  1  , is localized to the sarcolemmal membrane of normal skeletal muscle  2 -5  but is absent from the skeletal muscle of people with DMD 1 • 2 • 6 , xmd dogs 7 and mdx mice 1 • 5 (the last two being possible animal models for DMD).', 'Immunoaffinity beads raised against dystrophin and the SOK glycoprotein selectively adsorb the dystrophin-glycoprotein complex. Furthermore, there is a marked reduction of the 156K glycoprotein in muscle from mdx mice and DMD patients. These results imply that in dystrophic muscle, the absence of dystrophin may lead to the loss of a dystrophin-associated glycoprotein. This could be the first step in the molecular pathogenesis of muscular dystrophy.\n\nDystrophin-glycoprotein complex\nThis complex was isolated following digitonin-solubilization of rabbit skeletal muscle membranes using WGA-Sepharose and DEAE-cellulose  12  and further purified by sucrose density gradient centrifugation in the presence of 0.1% digitonin. It is evident from the Coomassie blue-stained gel of sequential gradient fractions (Fig.  1 a ) that the dystrophin-glycoprotein complex was separated from the voltage-sensitive sodium channel and the dihydropyridine receptor (Fig.  1 ).', "The amino-acid sequence of dystrophin suggests that it is a membrane cytoskeletal protein  8 • 9  involved in the anchoring of sarcolemmal proteins to the underlying cytoskeleton. But the exact function of dystrophin and its precise role in the resulting necrosis of dystrophic muscle fibres has not been determined. In studies of other genetic diseases involving proteins of the cytoskeleton  10 ' 11  , the absence of one component is sometimes accompanied by the loss of another cytoskeletal protein. Therefore, to understand the molecular pathogenesis of DMD, we sought to identify the proteins associated with or bound to dystrophin and to characterize the status of these proteins in muscle where dystrophin is absent."]</t>
         </is>
       </c>
-      <c r="AF249" t="inlineStr"/>
+      <c r="AF249" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Substantiated",
+  "explanation": "The reference article supports the claim that mutations in the DMD gene result in loss of expression of both dystrophin and the dystrophin-glycoprotein complex. The abstract states that 'the absence of dystrophin may lead to the loss of a dystrophin-associated glycoprotein,' and Excerpt 1 further explains that 'the concentration of one of these [glycoproteins] is greatly reduced in DMD patients.' This reduction in glycoprotein concentration is implied to be a result of the absence of dystrophin, which aligns with the citation statement."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="250">
       <c r="A250" t="inlineStr">
@@ -36577,7 +38434,14 @@
           <t>['Single-cell cancer genomics\n\n\nConclusions and future directions\nIn the first five years since its inception, SCS has already revolutionized our understanding of cancer evolution and diversity. Although initial studies focused mainly on technology development and intratumor heterogeneity in primary tumors, the field has now shifted toward understanding more complex biological processes in cancer, including invasion, metastasis, and the evolution of therapy resistance. These tools have also begun to provide new insight into the role of rare cells in tumor progression, particularly in the context of metastatic dissemination. Future studies will begin to unravel the spatial organization of tumor clones in tissues and will connect phenotypic behaviors of cancer cells with their genotypes. This will require combining SCS with multiple experimental systems, including xenografts, GEMs, cell cultures, and organoid systems. As DNA-and RNA-SCS methods continue to mature, their translation into the clinic is inevitable and will have a major impact on patient lives.', 'In diagnostics, intratumor heterogeneity presents a formidable challenge for clinical sampling, because single samples may not accurately represent the tumor as a whole. SCS methods can resolve intratumor heterogeneity and provide accurate measures of genomic diversity, which can be used to calculate a "diversity index." These indexes are likely to have prognostic utility in predicting which cancer patients will be more likely to show poor response to therapy, higher probability of metastasis, or have poor overall survival  (Burrell et al. 2013; Murugaesu et al. 2013; Almendro et al. 2014) . Another important clinical application of SCS methods is to guide targeted therapy. By sequencing and comparing multiple single cells, it is possible to construct a phylogenetic tree and heatmap that reveals the clonal substructure of a tumor. These genetic trees will allow oncologists to identify founder mutations in the "trunk" of the tree, which are ideal therapeutic targets, since they occurred early in tumor evolution and were inherited by all cells in the tumor. Alternatively, these trees can be used to devise combination therapies to target multiple tumor subpopulations independently.', 'Early detection is another clinical application of SCS, which can provide genomic information on rare tumor cells. In samples collected from bodily fluids (blood, urine, feces, and phlegm), it may be possible to isolate single cancer cells at the earliest stages of cancer progression. If driver mutations can be identified in multiple single cancer cells, then they may represent a clonal expansion, which could be followed by imaging techniques and surgical resection of microlesions. Another important clinical application of SCS is for obtaining genomic data sets from scarce clinical samples, which often contain only hundreds of tumor cells and are frequently unable to undergo genetic tests due to Quantity Not Sufficient (QNS). Perhaps the most immediate application of SCS in the clinic will be in noninvasive monitoring. By isolating and sequencing single CTCs in the blood, it may be possible to measure somatic mutations that are present at the primary or metastatic tumor sites without the inherent risks that are associated with performing an invasive core biopsy directly at the organ site. Additionally, this noninvasive approach can allow the oncologist to collect serial samples over time during the course of therapy to monitor response and the emergence of resistant clones.']</t>
         </is>
       </c>
-      <c r="AF250" t="inlineStr"/>
+      <c r="AF250" t="inlineStr">
+        <is>
+          <t>{
+  "label": "Substantiated",
+  "explanation": "The reference article discusses the potential clinical applications of single-cell sequencing (SCS) in cancer treatment, including guiding targeted therapy, early detection, noninvasive monitoring, and predicting patient outcomes. These applications align with the statement that single-cell genome analysis is expected to have clinical utility in cancer treatment."
+}</t>
+        </is>
+      </c>
     </row>
     <row r="251">
       <c r="A251" t="inlineStr">
@@ -36717,7 +38581,18 @@
           <t>['According to our scheme for the linear phase variation, the gradient of the phase variation is 2 / G k d dx D π =Φ = , where D is the total width of the antennas array and the rotation angle ranges from 0 to π .\n\nB: Parabolic phase discontinuity:\nIn fact, the linear phase relationship is only one possibility to manipulate the wave front. As another representative example, as a one-dimensional variation, we can generate a phase discontinuity profile according to: 2 2 2 2 ( ) f f x x π π λ λ + Φ = - (4) With such a parabolic profile, we can focus the incident light (wavelength λ ) to a distance f beyond the metamaterial surface, where f is the focal length. Ordinary lens, e.g. a cylinder convex lens, accumulates the phase along the optical path with different thicknesses of material. In contrary, we can generate such a phase discontinuity by an ultra-thin metamaterial surface in the subwavelength scale. Moreover, due to the abrupt phase control, we can focus the light to a tight focus near the diffraction limit as we will see later.', '1 (e) . Taking into account of the linear and parabolic phase discontinuity along the metamaterial surface through an array of split ring aperture antenna with defined profiles of the rotation angles, as depicted in Fig.  1(c ), one representative structure (A) is designed and is composed of 11 rotating antennas to realize the linear phase variation from 0 to 2 π . Considering the finite size of the unit cell, the phase variation is not continuous but is discrete. For structure A, each unit cell only needs a discrete rotation with step size of 0.1 π to realize the linear phase variation from 0 to 2 π . The case of structure B contains 15 rotating resonators with defined rotation angle to realize the parabolic phase variation in Eq. (  4 ). Here, we emphasize that phase variation acquired by rotating optical axis is free of dispersion of the resonator, as we could keep the desired anisotropic behavior. To verify our proposed scheme, we have performed full-wave simulations using CST Microwave Studio, based on the finite difference time domain (FDTD) algorithm  [28] . We utilize the perfect conductor approximation (PCA) for simplicity.', 'The transmitted field E t is the obtained by Eq. (1) as 2 1 2 1 2 1 0 1 1 ( ) ( ) 0 1 2 2 j t t t t t e θ - \uf8eb \uf8f6 \uf8eb \uf8f6 = + + - \uf8ec \uf8f7 \uf8ec \uf8f7 \uf8ed \uf8f8 \uf8ed \uf8f8 E (2) Therefore, if θ is spatially dependent, we can modulate the wave front for the cross-polarized light (left-handed polarized, the second term) by a spatially dependent phase discontinuity 2 j e θ -. The acquired phase discontinuity (phase gained by the incident light across the metamaterial) is twice that of the rotation angle of the antennas. This is a simple linear relationship between the phase discontinuity and the phase modulation (rotation angles) over the antennas array. We note that this phase discontinuity is not coming from the (frequency) dispersion by sweeping a series of resonating structure. The phase discontinuity here is geometric in nature and is related to the optical-axis rotation angle by a factor of two.']</t>
         </is>
       </c>
-      <c r="AF251" t="inlineStr"/>
+      <c r="AF251" t="inlineStr">
+        <is>
+          <t>Here is my evaluation:
+```
+{
+  "label": "Substantiated",
+  "explanation": "The reference article supports the statement that the geometric phase, also called Berry phase, is produced from the rotation of resonant elements in metasurface with circularly-polarized incidence. Excerpt 3 explicitly states that the acquired phase discontinuity is 'geometric in nature and is related to the optical-axis rotation angle by a factor of two', which aligns with the concept of geometric phase or Berry phase."
+}
+```
+Note that I only evaluated the portion of the statement corresponding to reference [39], which is about the production of geometric phase from rotating resonant elements.</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>